<commit_message>
Ahora si que esta el excel
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
@@ -1342,6 +1342,90 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1364,90 +1448,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1564,43 +1564,43 @@
                   <c:v>46.769999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.47</c:v>
+                  <c:v>43.47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45.47</c:v>
+                  <c:v>42.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2005,8 +2005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AB99" sqref="AB99"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,22 +2035,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="101" t="s">
+      <c r="J2" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="102"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="102"/>
-      <c r="S2" s="102"/>
-      <c r="T2" s="102"/>
-      <c r="U2" s="102"/>
-      <c r="V2" s="102"/>
-      <c r="W2" s="103"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="97"/>
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="97"/>
+      <c r="V2" s="97"/>
+      <c r="W2" s="98"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
@@ -2121,7 +2121,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="102" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="41" t="s">
@@ -2162,7 +2162,7 @@
       <c r="W4" s="20"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="108"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="48" t="s">
         <v>59</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="W5" s="22"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="108"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="48" t="s">
         <v>75</v>
       </c>
@@ -2236,8 +2236,8 @@
       <c r="W6" s="22"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="108"/>
-      <c r="C7" s="116" t="s">
+      <c r="B7" s="103"/>
+      <c r="C7" s="111" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="44" t="s">
@@ -2275,8 +2275,8 @@
       <c r="W7" s="22"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="108"/>
-      <c r="C8" s="116"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="48" t="s">
         <v>62</v>
       </c>
@@ -2312,8 +2312,8 @@
       <c r="W8" s="22"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="112"/>
-      <c r="C9" s="117"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="112"/>
       <c r="D9" s="45" t="s">
         <v>63</v>
       </c>
@@ -2349,7 +2349,7 @@
       <c r="W9" s="24"/>
     </row>
     <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="109" t="s">
+      <c r="B10" s="104" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="53" t="s">
@@ -2388,7 +2388,7 @@
       <c r="W10" s="26"/>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="110"/>
+      <c r="B11" s="105"/>
       <c r="C11" s="48" t="s">
         <v>66</v>
       </c>
@@ -2425,7 +2425,7 @@
       <c r="W11" s="60"/>
     </row>
     <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="110"/>
+      <c r="B12" s="105"/>
       <c r="C12" s="48" t="s">
         <v>67</v>
       </c>
@@ -2462,7 +2462,7 @@
       <c r="W12" s="60"/>
     </row>
     <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="111"/>
+      <c r="B13" s="106"/>
       <c r="C13" s="47" t="s">
         <v>120</v>
       </c>
@@ -2497,7 +2497,7 @@
       <c r="W13" s="71"/>
     </row>
     <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="111"/>
+      <c r="B14" s="106"/>
       <c r="C14" s="47" t="s">
         <v>118</v>
       </c>
@@ -2532,7 +2532,7 @@
       <c r="W14" s="71"/>
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="111"/>
+      <c r="B15" s="106"/>
       <c r="C15" s="47" t="s">
         <v>68</v>
       </c>
@@ -2569,7 +2569,7 @@
       <c r="W15" s="71"/>
     </row>
     <row r="16" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="107" t="s">
+      <c r="B16" s="102" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="67" t="s">
@@ -2588,13 +2588,17 @@
       </c>
       <c r="I16" s="59">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J16" s="72">
         <v>0</v>
       </c>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
+      <c r="K16" s="87">
+        <v>2</v>
+      </c>
+      <c r="L16" s="87">
+        <v>1</v>
+      </c>
       <c r="M16" s="27"/>
       <c r="N16" s="27"/>
       <c r="O16" s="27"/>
@@ -2608,7 +2612,7 @@
       <c r="W16" s="29"/>
     </row>
     <row r="17" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="108"/>
+      <c r="B17" s="103"/>
       <c r="C17" s="48" t="s">
         <v>36</v>
       </c>
@@ -2645,8 +2649,8 @@
       <c r="W17" s="32"/>
     </row>
     <row r="18" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="108"/>
-      <c r="C18" s="115" t="s">
+      <c r="B18" s="103"/>
+      <c r="C18" s="110" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="48" t="s">
@@ -2684,8 +2688,8 @@
       <c r="W18" s="32"/>
     </row>
     <row r="19" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="108"/>
-      <c r="C19" s="115"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="110"/>
       <c r="D19" s="48" t="s">
         <v>39</v>
       </c>
@@ -2721,8 +2725,8 @@
       <c r="W19" s="32"/>
     </row>
     <row r="20" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="108"/>
-      <c r="C20" s="96" t="s">
+      <c r="B20" s="103"/>
+      <c r="C20" s="124" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="48" t="s">
@@ -2760,8 +2764,8 @@
       <c r="W20" s="32"/>
     </row>
     <row r="21" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="108"/>
-      <c r="C21" s="96"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="124"/>
       <c r="D21" s="48" t="s">
         <v>34</v>
       </c>
@@ -2797,8 +2801,8 @@
       <c r="W21" s="32"/>
     </row>
     <row r="22" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="108"/>
-      <c r="C22" s="96"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="124"/>
       <c r="D22" s="48" t="s">
         <v>35</v>
       </c>
@@ -2834,8 +2838,8 @@
       <c r="W22" s="32"/>
     </row>
     <row r="23" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="108"/>
-      <c r="C23" s="96"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="48" t="s">
         <v>40</v>
       </c>
@@ -2871,8 +2875,8 @@
       <c r="W23" s="32"/>
     </row>
     <row r="24" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="108"/>
-      <c r="C24" s="96"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="124"/>
       <c r="D24" s="48" t="s">
         <v>41</v>
       </c>
@@ -2908,8 +2912,8 @@
       <c r="W24" s="32"/>
     </row>
     <row r="25" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="108"/>
-      <c r="C25" s="96"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="124"/>
       <c r="D25" s="48" t="s">
         <v>42</v>
       </c>
@@ -2945,8 +2949,8 @@
       <c r="W25" s="32"/>
     </row>
     <row r="26" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="108"/>
-      <c r="C26" s="96"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="124"/>
       <c r="D26" s="48" t="s">
         <v>43</v>
       </c>
@@ -2982,8 +2986,8 @@
       <c r="W26" s="32"/>
     </row>
     <row r="27" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="108"/>
-      <c r="C27" s="96"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="124"/>
       <c r="D27" s="48" t="s">
         <v>44</v>
       </c>
@@ -3019,8 +3023,8 @@
       <c r="W27" s="32"/>
     </row>
     <row r="28" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="108"/>
-      <c r="C28" s="96"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="124"/>
       <c r="D28" s="48" t="s">
         <v>45</v>
       </c>
@@ -3056,8 +3060,8 @@
       <c r="W28" s="32"/>
     </row>
     <row r="29" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="108"/>
-      <c r="C29" s="96"/>
+      <c r="B29" s="103"/>
+      <c r="C29" s="124"/>
       <c r="D29" s="48" t="s">
         <v>46</v>
       </c>
@@ -3093,8 +3097,8 @@
       <c r="W29" s="32"/>
     </row>
     <row r="30" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="108"/>
-      <c r="C30" s="96"/>
+      <c r="B30" s="103"/>
+      <c r="C30" s="124"/>
       <c r="D30" s="48" t="s">
         <v>47</v>
       </c>
@@ -3130,8 +3134,8 @@
       <c r="W30" s="32"/>
     </row>
     <row r="31" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="108"/>
-      <c r="C31" s="96"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="124"/>
       <c r="D31" s="48" t="s">
         <v>48</v>
       </c>
@@ -3167,8 +3171,8 @@
       <c r="W31" s="32"/>
     </row>
     <row r="32" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="108"/>
-      <c r="C32" s="96"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="124"/>
       <c r="D32" s="48" t="s">
         <v>49</v>
       </c>
@@ -3204,8 +3208,8 @@
       <c r="W32" s="32"/>
     </row>
     <row r="33" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="108"/>
-      <c r="C33" s="96"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="124"/>
       <c r="D33" s="48" t="s">
         <v>50</v>
       </c>
@@ -3241,8 +3245,8 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="108"/>
-      <c r="C34" s="96"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="124"/>
       <c r="D34" s="48" t="s">
         <v>51</v>
       </c>
@@ -3278,8 +3282,8 @@
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="108"/>
-      <c r="C35" s="96"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="124"/>
       <c r="D35" s="48" t="s">
         <v>52</v>
       </c>
@@ -3315,8 +3319,8 @@
       <c r="W35" s="32"/>
     </row>
     <row r="36" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="108"/>
-      <c r="C36" s="96"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="124"/>
       <c r="D36" s="54" t="s">
         <v>111</v>
       </c>
@@ -3352,7 +3356,7 @@
       <c r="W36" s="32"/>
     </row>
     <row r="37" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="108"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="51" t="s">
         <v>53</v>
       </c>
@@ -3389,7 +3393,7 @@
       <c r="W37" s="32"/>
     </row>
     <row r="38" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="108"/>
+      <c r="B38" s="103"/>
       <c r="C38" s="51" t="s">
         <v>55</v>
       </c>
@@ -3426,7 +3430,7 @@
       <c r="W38" s="32"/>
     </row>
     <row r="39" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="108"/>
+      <c r="B39" s="103"/>
       <c r="C39" s="51" t="s">
         <v>56</v>
       </c>
@@ -3463,7 +3467,7 @@
       <c r="W39" s="32"/>
     </row>
     <row r="40" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="108"/>
+      <c r="B40" s="103"/>
       <c r="C40" s="58" t="s">
         <v>112</v>
       </c>
@@ -3500,10 +3504,10 @@
       <c r="W40" s="32"/>
     </row>
     <row r="41" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="98" t="s">
+      <c r="B41" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="94" t="s">
+      <c r="C41" s="122" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="52" t="s">
@@ -3526,25 +3530,25 @@
       <c r="J41" s="87">
         <v>0.45</v>
       </c>
-      <c r="K41" s="123">
+      <c r="K41" s="90">
         <v>0.5</v>
       </c>
-      <c r="L41" s="123"/>
-      <c r="M41" s="123"/>
-      <c r="N41" s="123"/>
-      <c r="O41" s="123"/>
-      <c r="P41" s="124"/>
-      <c r="Q41" s="124"/>
-      <c r="R41" s="124"/>
-      <c r="S41" s="124"/>
-      <c r="T41" s="124"/>
-      <c r="U41" s="124"/>
-      <c r="V41" s="124"/>
-      <c r="W41" s="125"/>
+      <c r="L41" s="90"/>
+      <c r="M41" s="90"/>
+      <c r="N41" s="90"/>
+      <c r="O41" s="90"/>
+      <c r="P41" s="91"/>
+      <c r="Q41" s="91"/>
+      <c r="R41" s="91"/>
+      <c r="S41" s="91"/>
+      <c r="T41" s="91"/>
+      <c r="U41" s="91"/>
+      <c r="V41" s="91"/>
+      <c r="W41" s="92"/>
     </row>
     <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="99"/>
-      <c r="C42" s="95"/>
+      <c r="B42" s="94"/>
+      <c r="C42" s="123"/>
       <c r="D42" s="51" t="s">
         <v>21</v>
       </c>
@@ -3580,8 +3584,8 @@
       <c r="W42" s="32"/>
     </row>
     <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="99"/>
-      <c r="C43" s="95"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="123"/>
       <c r="D43" s="51" t="s">
         <v>22</v>
       </c>
@@ -3617,8 +3621,8 @@
       <c r="W43" s="32"/>
     </row>
     <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="99"/>
-      <c r="C44" s="95"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="123"/>
       <c r="D44" s="51" t="s">
         <v>23</v>
       </c>
@@ -3654,8 +3658,8 @@
       <c r="W44" s="32"/>
     </row>
     <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="99"/>
-      <c r="C45" s="95"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="123"/>
       <c r="D45" s="51" t="s">
         <v>24</v>
       </c>
@@ -3691,8 +3695,8 @@
       <c r="W45" s="32"/>
     </row>
     <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="99"/>
-      <c r="C46" s="95"/>
+      <c r="B46" s="94"/>
+      <c r="C46" s="123"/>
       <c r="D46" s="51" t="s">
         <v>25</v>
       </c>
@@ -3728,8 +3732,8 @@
       <c r="W46" s="32"/>
     </row>
     <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="99"/>
-      <c r="C47" s="95"/>
+      <c r="B47" s="94"/>
+      <c r="C47" s="123"/>
       <c r="D47" s="51" t="s">
         <v>26</v>
       </c>
@@ -3765,8 +3769,8 @@
       <c r="W47" s="32"/>
     </row>
     <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="99"/>
-      <c r="C48" s="95"/>
+      <c r="B48" s="94"/>
+      <c r="C48" s="123"/>
       <c r="D48" s="51" t="s">
         <v>27</v>
       </c>
@@ -3802,8 +3806,8 @@
       <c r="W48" s="32"/>
     </row>
     <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="99"/>
-      <c r="C49" s="95"/>
+      <c r="B49" s="94"/>
+      <c r="C49" s="123"/>
       <c r="D49" s="51" t="s">
         <v>28</v>
       </c>
@@ -3839,8 +3843,8 @@
       <c r="W49" s="32"/>
     </row>
     <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="99"/>
-      <c r="C50" s="95"/>
+      <c r="B50" s="94"/>
+      <c r="C50" s="123"/>
       <c r="D50" s="51" t="s">
         <v>29</v>
       </c>
@@ -3876,8 +3880,8 @@
       <c r="W50" s="32"/>
     </row>
     <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="99"/>
-      <c r="C51" s="95"/>
+      <c r="B51" s="94"/>
+      <c r="C51" s="123"/>
       <c r="D51" s="51" t="s">
         <v>30</v>
       </c>
@@ -3913,8 +3917,8 @@
       <c r="W51" s="32"/>
     </row>
     <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="99"/>
-      <c r="C52" s="95"/>
+      <c r="B52" s="94"/>
+      <c r="C52" s="123"/>
       <c r="D52" s="51" t="s">
         <v>31</v>
       </c>
@@ -3950,8 +3954,8 @@
       <c r="W52" s="32"/>
     </row>
     <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="99"/>
-      <c r="C53" s="95"/>
+      <c r="B53" s="94"/>
+      <c r="C53" s="123"/>
       <c r="D53" s="51" t="s">
         <v>77</v>
       </c>
@@ -3987,8 +3991,8 @@
       <c r="W53" s="32"/>
     </row>
     <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="99"/>
-      <c r="C54" s="95"/>
+      <c r="B54" s="94"/>
+      <c r="C54" s="123"/>
       <c r="D54" s="51" t="s">
         <v>78</v>
       </c>
@@ -4024,8 +4028,8 @@
       <c r="W54" s="32"/>
     </row>
     <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="99"/>
-      <c r="C55" s="95"/>
+      <c r="B55" s="94"/>
+      <c r="C55" s="123"/>
       <c r="D55" s="51" t="s">
         <v>78</v>
       </c>
@@ -4061,8 +4065,8 @@
       <c r="W55" s="32"/>
     </row>
     <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="99"/>
-      <c r="C56" s="95"/>
+      <c r="B56" s="94"/>
+      <c r="C56" s="123"/>
       <c r="D56" s="51" t="s">
         <v>79</v>
       </c>
@@ -4098,8 +4102,8 @@
       <c r="W56" s="32"/>
     </row>
     <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="99"/>
-      <c r="C57" s="95"/>
+      <c r="B57" s="94"/>
+      <c r="C57" s="123"/>
       <c r="D57" s="51" t="s">
         <v>80</v>
       </c>
@@ -4135,8 +4139,8 @@
       <c r="W57" s="32"/>
     </row>
     <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="99"/>
-      <c r="C58" s="95"/>
+      <c r="B58" s="94"/>
+      <c r="C58" s="123"/>
       <c r="D58" s="51" t="s">
         <v>81</v>
       </c>
@@ -4172,8 +4176,8 @@
       <c r="W58" s="32"/>
     </row>
     <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="99"/>
-      <c r="C59" s="95"/>
+      <c r="B59" s="94"/>
+      <c r="C59" s="123"/>
       <c r="D59" s="51" t="s">
         <v>82</v>
       </c>
@@ -4209,8 +4213,8 @@
       <c r="W59" s="32"/>
     </row>
     <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="99"/>
-      <c r="C60" s="95"/>
+      <c r="B60" s="94"/>
+      <c r="C60" s="123"/>
       <c r="D60" s="51" t="s">
         <v>83</v>
       </c>
@@ -4246,8 +4250,8 @@
       <c r="W60" s="32"/>
     </row>
     <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="99"/>
-      <c r="C61" s="95"/>
+      <c r="B61" s="94"/>
+      <c r="C61" s="123"/>
       <c r="D61" s="51" t="s">
         <v>84</v>
       </c>
@@ -4283,8 +4287,8 @@
       <c r="W61" s="32"/>
     </row>
     <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="99"/>
-      <c r="C62" s="95"/>
+      <c r="B62" s="94"/>
+      <c r="C62" s="123"/>
       <c r="D62" s="51" t="s">
         <v>85</v>
       </c>
@@ -4320,8 +4324,8 @@
       <c r="W62" s="32"/>
     </row>
     <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="99"/>
-      <c r="C63" s="95"/>
+      <c r="B63" s="94"/>
+      <c r="C63" s="123"/>
       <c r="D63" s="51" t="s">
         <v>86</v>
       </c>
@@ -4357,8 +4361,8 @@
       <c r="W63" s="32"/>
     </row>
     <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="99"/>
-      <c r="C64" s="95"/>
+      <c r="B64" s="94"/>
+      <c r="C64" s="123"/>
       <c r="D64" s="51" t="s">
         <v>87</v>
       </c>
@@ -4394,8 +4398,8 @@
       <c r="W64" s="32"/>
     </row>
     <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="99"/>
-      <c r="C65" s="95"/>
+      <c r="B65" s="94"/>
+      <c r="C65" s="123"/>
       <c r="D65" s="51" t="s">
         <v>88</v>
       </c>
@@ -4431,8 +4435,8 @@
       <c r="W65" s="32"/>
     </row>
     <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="99"/>
-      <c r="C66" s="95"/>
+      <c r="B66" s="94"/>
+      <c r="C66" s="123"/>
       <c r="D66" s="51" t="s">
         <v>89</v>
       </c>
@@ -4468,8 +4472,8 @@
       <c r="W66" s="32"/>
     </row>
     <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="99"/>
-      <c r="C67" s="95"/>
+      <c r="B67" s="94"/>
+      <c r="C67" s="123"/>
       <c r="D67" s="51" t="s">
         <v>94</v>
       </c>
@@ -4505,8 +4509,8 @@
       <c r="W67" s="32"/>
     </row>
     <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="99"/>
-      <c r="C68" s="95"/>
+      <c r="B68" s="94"/>
+      <c r="C68" s="123"/>
       <c r="D68" s="51" t="s">
         <v>95</v>
       </c>
@@ -4542,8 +4546,8 @@
       <c r="W68" s="32"/>
     </row>
     <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="99"/>
-      <c r="C69" s="95"/>
+      <c r="B69" s="94"/>
+      <c r="C69" s="123"/>
       <c r="D69" s="51" t="s">
         <v>96</v>
       </c>
@@ -4579,8 +4583,8 @@
       <c r="W69" s="32"/>
     </row>
     <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="99"/>
-      <c r="C70" s="95"/>
+      <c r="B70" s="94"/>
+      <c r="C70" s="123"/>
       <c r="D70" s="51" t="s">
         <v>97</v>
       </c>
@@ -4616,8 +4620,8 @@
       <c r="W70" s="32"/>
     </row>
     <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="99"/>
-      <c r="C71" s="95"/>
+      <c r="B71" s="94"/>
+      <c r="C71" s="123"/>
       <c r="D71" s="51" t="s">
         <v>98</v>
       </c>
@@ -4653,8 +4657,8 @@
       <c r="W71" s="32"/>
     </row>
     <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="99"/>
-      <c r="C72" s="95"/>
+      <c r="B72" s="94"/>
+      <c r="C72" s="123"/>
       <c r="D72" s="51" t="s">
         <v>99</v>
       </c>
@@ -4690,8 +4694,8 @@
       <c r="W72" s="32"/>
     </row>
     <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="99"/>
-      <c r="C73" s="95"/>
+      <c r="B73" s="94"/>
+      <c r="C73" s="123"/>
       <c r="D73" s="51" t="s">
         <v>100</v>
       </c>
@@ -4727,8 +4731,8 @@
       <c r="W73" s="32"/>
     </row>
     <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="99"/>
-      <c r="C74" s="95"/>
+      <c r="B74" s="94"/>
+      <c r="C74" s="123"/>
       <c r="D74" s="51" t="s">
         <v>101</v>
       </c>
@@ -4764,8 +4768,8 @@
       <c r="W74" s="32"/>
     </row>
     <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="99"/>
-      <c r="C75" s="95"/>
+      <c r="B75" s="94"/>
+      <c r="C75" s="123"/>
       <c r="D75" s="51" t="s">
         <v>102</v>
       </c>
@@ -4801,8 +4805,8 @@
       <c r="W75" s="32"/>
     </row>
     <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="99"/>
-      <c r="C76" s="95"/>
+      <c r="B76" s="94"/>
+      <c r="C76" s="123"/>
       <c r="D76" s="51" t="s">
         <v>103</v>
       </c>
@@ -4838,8 +4842,8 @@
       <c r="W76" s="32"/>
     </row>
     <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="99"/>
-      <c r="C77" s="95"/>
+      <c r="B77" s="94"/>
+      <c r="C77" s="123"/>
       <c r="D77" s="51" t="s">
         <v>104</v>
       </c>
@@ -4875,8 +4879,8 @@
       <c r="W77" s="32"/>
     </row>
     <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="99"/>
-      <c r="C78" s="95"/>
+      <c r="B78" s="94"/>
+      <c r="C78" s="123"/>
       <c r="D78" s="51" t="s">
         <v>105</v>
       </c>
@@ -4912,8 +4916,8 @@
       <c r="W78" s="32"/>
     </row>
     <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="99"/>
-      <c r="C79" s="95"/>
+      <c r="B79" s="94"/>
+      <c r="C79" s="123"/>
       <c r="D79" s="51" t="s">
         <v>106</v>
       </c>
@@ -4949,8 +4953,8 @@
       <c r="W79" s="32"/>
     </row>
     <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="99"/>
-      <c r="C80" s="95"/>
+      <c r="B80" s="94"/>
+      <c r="C80" s="123"/>
       <c r="D80" s="51" t="s">
         <v>107</v>
       </c>
@@ -4986,8 +4990,8 @@
       <c r="W80" s="32"/>
     </row>
     <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="99"/>
-      <c r="C81" s="95"/>
+      <c r="B81" s="94"/>
+      <c r="C81" s="123"/>
       <c r="D81" s="51" t="s">
         <v>90</v>
       </c>
@@ -5023,8 +5027,8 @@
       <c r="W81" s="32"/>
     </row>
     <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="99"/>
-      <c r="C82" s="95"/>
+      <c r="B82" s="94"/>
+      <c r="C82" s="123"/>
       <c r="D82" s="51" t="s">
         <v>91</v>
       </c>
@@ -5060,8 +5064,8 @@
       <c r="W82" s="32"/>
     </row>
     <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="99"/>
-      <c r="C83" s="95"/>
+      <c r="B83" s="94"/>
+      <c r="C83" s="123"/>
       <c r="D83" s="51" t="s">
         <v>114</v>
       </c>
@@ -5099,8 +5103,8 @@
       <c r="W83" s="89"/>
     </row>
     <row r="84" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="99"/>
-      <c r="C84" s="100" t="s">
+      <c r="B84" s="94"/>
+      <c r="C84" s="95" t="s">
         <v>37</v>
       </c>
       <c r="D84" s="48" t="s">
@@ -5138,8 +5142,8 @@
       <c r="W84" s="32"/>
     </row>
     <row r="85" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="99"/>
-      <c r="C85" s="100"/>
+      <c r="B85" s="94"/>
+      <c r="C85" s="95"/>
       <c r="D85" s="54" t="s">
         <v>70</v>
       </c>
@@ -5175,8 +5179,8 @@
       <c r="W85" s="32"/>
     </row>
     <row r="86" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="99"/>
-      <c r="C86" s="100"/>
+      <c r="B86" s="94"/>
+      <c r="C86" s="95"/>
       <c r="D86" s="54" t="s">
         <v>71</v>
       </c>
@@ -5212,8 +5216,8 @@
       <c r="W86" s="32"/>
     </row>
     <row r="87" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="99"/>
-      <c r="C87" s="100"/>
+      <c r="B87" s="94"/>
+      <c r="C87" s="95"/>
       <c r="D87" s="54" t="s">
         <v>72</v>
       </c>
@@ -5249,8 +5253,8 @@
       <c r="W87" s="32"/>
     </row>
     <row r="88" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="99"/>
-      <c r="C88" s="100"/>
+      <c r="B88" s="94"/>
+      <c r="C88" s="95"/>
       <c r="D88" s="54" t="s">
         <v>73</v>
       </c>
@@ -5286,8 +5290,8 @@
       <c r="W88" s="60"/>
     </row>
     <row r="89" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="99"/>
-      <c r="C89" s="100"/>
+      <c r="B89" s="94"/>
+      <c r="C89" s="95"/>
       <c r="D89" s="54" t="s">
         <v>74</v>
       </c>
@@ -5323,7 +5327,7 @@
       <c r="W89" s="32"/>
     </row>
     <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="99"/>
+      <c r="B90" s="94"/>
       <c r="C90" s="85" t="s">
         <v>125</v>
       </c>
@@ -5360,7 +5364,7 @@
       <c r="W90" s="89"/>
     </row>
     <row r="91" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="99"/>
+      <c r="B91" s="94"/>
       <c r="C91" s="77" t="s">
         <v>113</v>
       </c>
@@ -5397,7 +5401,7 @@
       <c r="W91" s="32"/>
     </row>
     <row r="92" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="118" t="s">
+      <c r="B92" s="113" t="s">
         <v>92</v>
       </c>
       <c r="C92" s="40" t="s">
@@ -5436,7 +5440,7 @@
       <c r="W92" s="69"/>
     </row>
     <row r="93" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="119"/>
+      <c r="B93" s="114"/>
       <c r="C93" s="43" t="s">
         <v>119</v>
       </c>
@@ -5471,8 +5475,8 @@
       <c r="W93" s="68"/>
     </row>
     <row r="94" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="120"/>
-      <c r="C94" s="97" t="s">
+      <c r="B94" s="115"/>
+      <c r="C94" s="125" t="s">
         <v>108</v>
       </c>
       <c r="D94" s="44" t="s">
@@ -5510,8 +5514,8 @@
       <c r="W94" s="60"/>
     </row>
     <row r="95" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B95" s="121"/>
-      <c r="C95" s="97"/>
+      <c r="B95" s="116"/>
+      <c r="C95" s="125"/>
       <c r="D95" s="44" t="s">
         <v>109</v>
       </c>
@@ -5547,7 +5551,7 @@
       <c r="W95" s="60"/>
     </row>
     <row r="96" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="122"/>
+      <c r="B96" s="117"/>
       <c r="C96" s="46" t="s">
         <v>116</v>
       </c>
@@ -5584,7 +5588,7 @@
       <c r="W96" s="66"/>
     </row>
     <row r="97" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="98" t="s">
+      <c r="B97" s="93" t="s">
         <v>93</v>
       </c>
       <c r="C97" s="65" t="s">
@@ -5623,7 +5627,7 @@
       <c r="W97" s="29"/>
     </row>
     <row r="98" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B98" s="121"/>
+      <c r="B98" s="116"/>
       <c r="C98" s="56" t="s">
         <v>131</v>
       </c>
@@ -5660,7 +5664,7 @@
       <c r="W98" s="32"/>
     </row>
     <row r="99" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B99" s="121"/>
+      <c r="B99" s="116"/>
       <c r="C99" s="56" t="s">
         <v>130</v>
       </c>
@@ -5697,7 +5701,7 @@
       <c r="W99" s="32"/>
     </row>
     <row r="100" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B100" s="121"/>
+      <c r="B100" s="116"/>
       <c r="C100" s="56" t="s">
         <v>129</v>
       </c>
@@ -5734,7 +5738,7 @@
       <c r="W100" s="32"/>
     </row>
     <row r="101" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B101" s="121"/>
+      <c r="B101" s="116"/>
       <c r="C101" s="56" t="s">
         <v>128</v>
       </c>
@@ -5771,7 +5775,7 @@
       <c r="W101" s="32"/>
     </row>
     <row r="102" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="122"/>
+      <c r="B102" s="117"/>
       <c r="C102" s="46" t="s">
         <v>127</v>
       </c>
@@ -5808,21 +5812,21 @@
       <c r="W102" s="36"/>
     </row>
     <row r="103" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="113" t="s">
+      <c r="B103" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C103" s="114"/>
-      <c r="D103" s="114"/>
-      <c r="E103" s="114"/>
-      <c r="F103" s="114"/>
-      <c r="G103" s="114"/>
+      <c r="C103" s="109"/>
+      <c r="D103" s="109"/>
+      <c r="E103" s="109"/>
+      <c r="F103" s="109"/>
+      <c r="G103" s="109"/>
       <c r="H103" s="17">
         <f t="shared" ref="H103:W103" si="4">SUM(H4:H102)</f>
         <v>48.72</v>
       </c>
       <c r="I103" s="17">
         <f t="shared" si="4"/>
-        <v>3.25</v>
+        <v>6.25</v>
       </c>
       <c r="J103" s="17">
         <f t="shared" si="4"/>
@@ -5830,11 +5834,11 @@
       </c>
       <c r="K103" s="17">
         <f t="shared" si="4"/>
-        <v>1.3</v>
+        <v>3.3</v>
       </c>
       <c r="L103" s="17">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M103" s="17">
         <f t="shared" si="4"/>
@@ -5890,22 +5894,22 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
-      <c r="J104" s="104" t="s">
+      <c r="J104" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="K104" s="105"/>
-      <c r="L104" s="105"/>
-      <c r="M104" s="105"/>
-      <c r="N104" s="105"/>
-      <c r="O104" s="105"/>
-      <c r="P104" s="105"/>
-      <c r="Q104" s="105"/>
-      <c r="R104" s="105"/>
-      <c r="S104" s="105"/>
-      <c r="T104" s="105"/>
-      <c r="U104" s="105"/>
-      <c r="V104" s="105"/>
-      <c r="W104" s="106"/>
+      <c r="K104" s="100"/>
+      <c r="L104" s="100"/>
+      <c r="M104" s="100"/>
+      <c r="N104" s="100"/>
+      <c r="O104" s="100"/>
+      <c r="P104" s="100"/>
+      <c r="Q104" s="100"/>
+      <c r="R104" s="100"/>
+      <c r="S104" s="100"/>
+      <c r="T104" s="100"/>
+      <c r="U104" s="100"/>
+      <c r="V104" s="100"/>
+      <c r="W104" s="101"/>
     </row>
     <row r="105" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="78" t="s">
@@ -5949,65 +5953,65 @@
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="90" t="s">
+      <c r="H106" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="I106" s="93"/>
+      <c r="I106" s="121"/>
       <c r="J106" s="10">
         <f>H103-J103</f>
         <v>46.769999999999996</v>
       </c>
       <c r="K106" s="10">
         <f>J106-K103</f>
-        <v>45.47</v>
+        <v>43.47</v>
       </c>
       <c r="L106" s="10">
         <f>K106-L103</f>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="M106" s="10">
         <f>L106-M103</f>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="N106" s="10">
         <f t="shared" ref="N106:W106" si="5">M106-N103</f>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="O106" s="10">
         <f t="shared" si="5"/>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="P106" s="10">
         <f t="shared" si="5"/>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="Q106" s="10">
         <f t="shared" si="5"/>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="R106" s="10">
         <f t="shared" si="5"/>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="S106" s="10">
         <f t="shared" si="5"/>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="T106" s="10">
         <f t="shared" si="5"/>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="U106" s="10">
         <f t="shared" si="5"/>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="V106" s="10">
         <f t="shared" si="5"/>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
       <c r="W106" s="10">
         <f t="shared" si="5"/>
-        <v>45.47</v>
+        <v>42.47</v>
       </c>
     </row>
     <row r="107" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6052,27 +6056,27 @@
         <v>15</v>
       </c>
       <c r="F108" s="3"/>
-      <c r="H108" s="90" t="s">
+      <c r="H108" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="I108" s="91"/>
-      <c r="J108" s="90">
+      <c r="I108" s="119"/>
+      <c r="J108" s="118">
         <f>H103-I103</f>
-        <v>45.47</v>
-      </c>
-      <c r="K108" s="91"/>
-      <c r="L108" s="91"/>
-      <c r="M108" s="91"/>
-      <c r="N108" s="91"/>
-      <c r="O108" s="91"/>
-      <c r="P108" s="91"/>
-      <c r="Q108" s="91"/>
-      <c r="R108" s="91"/>
-      <c r="S108" s="91"/>
-      <c r="T108" s="91"/>
-      <c r="U108" s="91"/>
-      <c r="V108" s="91"/>
-      <c r="W108" s="92"/>
+        <v>42.47</v>
+      </c>
+      <c r="K108" s="119"/>
+      <c r="L108" s="119"/>
+      <c r="M108" s="119"/>
+      <c r="N108" s="119"/>
+      <c r="O108" s="119"/>
+      <c r="P108" s="119"/>
+      <c r="Q108" s="119"/>
+      <c r="R108" s="119"/>
+      <c r="S108" s="119"/>
+      <c r="T108" s="119"/>
+      <c r="U108" s="119"/>
+      <c r="V108" s="119"/>
+      <c r="W108" s="120"/>
     </row>
     <row r="109" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B109" s="3"/>
@@ -6152,6 +6156,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="J108:W108"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="C41:C83"/>
+    <mergeCell ref="C20:C36"/>
+    <mergeCell ref="C94:C95"/>
     <mergeCell ref="B41:B91"/>
     <mergeCell ref="C84:C89"/>
     <mergeCell ref="J2:W2"/>
@@ -6164,12 +6174,6 @@
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="B92:B96"/>
     <mergeCell ref="B97:B102"/>
-    <mergeCell ref="J108:W108"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="C41:C83"/>
-    <mergeCell ref="C20:C36"/>
-    <mergeCell ref="C94:C95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizado el excel, captura de pantalla dia 2
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Enti\MAP\The_Legend_of_Radev\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MSI-D\Documents\MAP_LegendOfRadev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -576,6 +576,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="39">
     <border>
@@ -1087,7 +1093,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1360,6 +1366,84 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1384,82 +1468,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1582,37 +1597,37 @@
                   <c:v>36.32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.82</c:v>
+                  <c:v>32.326999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1672,7 +1687,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1804,6 +1818,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1839,6 +1870,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2017,28 +2065,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M98" sqref="M98:M100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>126</v>
       </c>
@@ -2046,25 +2094,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="105" t="s">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
-      <c r="P2" s="106"/>
-      <c r="Q2" s="106"/>
-      <c r="R2" s="106"/>
-      <c r="S2" s="106"/>
-      <c r="T2" s="106"/>
-      <c r="U2" s="106"/>
-      <c r="V2" s="106"/>
-      <c r="W2" s="107"/>
-    </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="100"/>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
@@ -2132,8 +2180,8 @@
         <v>43081</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="111" t="s">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="104" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="89" t="s">
@@ -2199,8 +2247,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="112"/>
+    <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="105"/>
       <c r="C5" s="46" t="s">
         <v>59</v>
       </c>
@@ -2262,8 +2310,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="112"/>
+    <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="105"/>
       <c r="C6" s="46" t="s">
         <v>75</v>
       </c>
@@ -2280,7 +2328,7 @@
       </c>
       <c r="I6" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.96</v>
       </c>
       <c r="J6" s="71">
         <v>0</v>
@@ -2288,8 +2336,12 @@
       <c r="K6" s="71">
         <v>0</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
+      <c r="L6" s="71">
+        <v>0</v>
+      </c>
+      <c r="M6" s="48">
+        <v>0.96</v>
+      </c>
       <c r="N6" s="28"/>
       <c r="O6" s="28"/>
       <c r="P6" s="28"/>
@@ -2301,9 +2353,9 @@
       <c r="V6" s="19"/>
       <c r="W6" s="20"/>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="112"/>
-      <c r="C7" s="120" t="s">
+    <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="105"/>
+      <c r="C7" s="113" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="42" t="s">
@@ -2329,8 +2381,12 @@
       <c r="K7" s="71">
         <v>0</v>
       </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
+      <c r="L7" s="71">
+        <v>0</v>
+      </c>
+      <c r="M7" s="71">
+        <v>0</v>
+      </c>
       <c r="N7" s="28"/>
       <c r="O7" s="28"/>
       <c r="P7" s="28"/>
@@ -2342,9 +2398,9 @@
       <c r="V7" s="19"/>
       <c r="W7" s="20"/>
     </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="112"/>
-      <c r="C8" s="120"/>
+    <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="105"/>
+      <c r="C8" s="113"/>
       <c r="D8" s="46" t="s">
         <v>62</v>
       </c>
@@ -2368,8 +2424,12 @@
       <c r="K8" s="71">
         <v>0</v>
       </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
+      <c r="L8" s="71">
+        <v>0</v>
+      </c>
+      <c r="M8" s="71">
+        <v>0</v>
+      </c>
       <c r="N8" s="28"/>
       <c r="O8" s="28"/>
       <c r="P8" s="28"/>
@@ -2381,9 +2441,9 @@
       <c r="V8" s="19"/>
       <c r="W8" s="20"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="116"/>
-      <c r="C9" s="121"/>
+    <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="109"/>
+      <c r="C9" s="114"/>
       <c r="D9" s="43" t="s">
         <v>63</v>
       </c>
@@ -2407,8 +2467,12 @@
       <c r="K9" s="72">
         <v>0</v>
       </c>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
+      <c r="L9" s="72">
+        <v>0</v>
+      </c>
+      <c r="M9" s="72">
+        <v>0</v>
+      </c>
       <c r="N9" s="32"/>
       <c r="O9" s="32"/>
       <c r="P9" s="32"/>
@@ -2420,8 +2484,8 @@
       <c r="V9" s="21"/>
       <c r="W9" s="22"/>
     </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="113" t="s">
+    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="106" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="51" t="s">
@@ -2440,7 +2504,7 @@
       </c>
       <c r="I10" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="J10" s="73">
         <v>0</v>
@@ -2448,8 +2512,12 @@
       <c r="K10" s="73">
         <v>0</v>
       </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
+      <c r="L10" s="73">
+        <v>0</v>
+      </c>
+      <c r="M10" s="128">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="N10" s="35"/>
       <c r="O10" s="35"/>
       <c r="P10" s="35"/>
@@ -2461,8 +2529,8 @@
       <c r="V10" s="23"/>
       <c r="W10" s="24"/>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="114"/>
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="107"/>
       <c r="C11" s="46" t="s">
         <v>66</v>
       </c>
@@ -2487,8 +2555,12 @@
       <c r="K11" s="71">
         <v>0</v>
       </c>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="L11" s="71">
+        <v>0</v>
+      </c>
+      <c r="M11" s="71">
+        <v>0</v>
+      </c>
       <c r="N11" s="28"/>
       <c r="O11" s="28"/>
       <c r="P11" s="28"/>
@@ -2500,8 +2572,8 @@
       <c r="V11" s="28"/>
       <c r="W11" s="58"/>
     </row>
-    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="114"/>
+    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="107"/>
       <c r="C12" s="46" t="s">
         <v>67</v>
       </c>
@@ -2526,8 +2598,12 @@
       <c r="K12" s="71">
         <v>0</v>
       </c>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
+      <c r="L12" s="71">
+        <v>0</v>
+      </c>
+      <c r="M12" s="71">
+        <v>0</v>
+      </c>
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
       <c r="P12" s="28"/>
@@ -2539,8 +2615,8 @@
       <c r="V12" s="28"/>
       <c r="W12" s="58"/>
     </row>
-    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="115"/>
+    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="108"/>
       <c r="C13" s="45" t="s">
         <v>120</v>
       </c>
@@ -2565,8 +2641,12 @@
       <c r="K13" s="74">
         <v>0</v>
       </c>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
+      <c r="L13" s="74">
+        <v>0</v>
+      </c>
+      <c r="M13" s="74">
+        <v>0</v>
+      </c>
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
@@ -2578,8 +2658,8 @@
       <c r="V13" s="31"/>
       <c r="W13" s="69"/>
     </row>
-    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="115"/>
+    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="108"/>
       <c r="C14" s="45" t="s">
         <v>118</v>
       </c>
@@ -2604,8 +2684,12 @@
       <c r="K14" s="74">
         <v>0</v>
       </c>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
+      <c r="L14" s="74">
+        <v>0</v>
+      </c>
+      <c r="M14" s="74">
+        <v>0</v>
+      </c>
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
@@ -2617,8 +2701,8 @@
       <c r="V14" s="31"/>
       <c r="W14" s="69"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="115"/>
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="108"/>
       <c r="C15" s="45" t="s">
         <v>68</v>
       </c>
@@ -2643,8 +2727,12 @@
       <c r="K15" s="74">
         <v>0</v>
       </c>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
+      <c r="L15" s="74">
+        <v>0</v>
+      </c>
+      <c r="M15" s="74">
+        <v>0</v>
+      </c>
       <c r="N15" s="31"/>
       <c r="O15" s="31"/>
       <c r="P15" s="31"/>
@@ -2656,8 +2744,8 @@
       <c r="V15" s="31"/>
       <c r="W15" s="69"/>
     </row>
-    <row r="16" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="111" t="s">
+    <row r="16" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="104" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="65" t="s">
@@ -2721,8 +2809,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="112"/>
+    <row r="17" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="105"/>
       <c r="C17" s="46" t="s">
         <v>36</v>
       </c>
@@ -2739,7 +2827,7 @@
       </c>
       <c r="I17" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.083</v>
       </c>
       <c r="J17" s="71">
         <v>0</v>
@@ -2747,8 +2835,12 @@
       <c r="K17" s="71">
         <v>0</v>
       </c>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="L17" s="71">
+        <v>0</v>
+      </c>
+      <c r="M17" s="48">
+        <v>1.083</v>
+      </c>
       <c r="N17" s="28"/>
       <c r="O17" s="28"/>
       <c r="P17" s="29"/>
@@ -2760,9 +2852,9 @@
       <c r="V17" s="29"/>
       <c r="W17" s="30"/>
     </row>
-    <row r="18" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="112"/>
-      <c r="C18" s="119" t="s">
+    <row r="18" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="105"/>
+      <c r="C18" s="112" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="46" t="s">
@@ -2788,8 +2880,12 @@
       <c r="K18" s="71">
         <v>0</v>
       </c>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
+      <c r="L18" s="71">
+        <v>0</v>
+      </c>
+      <c r="M18" s="71">
+        <v>0</v>
+      </c>
       <c r="N18" s="28"/>
       <c r="O18" s="28"/>
       <c r="P18" s="29"/>
@@ -2801,9 +2897,9 @@
       <c r="V18" s="29"/>
       <c r="W18" s="30"/>
     </row>
-    <row r="19" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="112"/>
-      <c r="C19" s="119"/>
+    <row r="19" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="105"/>
+      <c r="C19" s="112"/>
       <c r="D19" s="46" t="s">
         <v>39</v>
       </c>
@@ -2819,7 +2915,7 @@
       </c>
       <c r="I19" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J19" s="71">
         <v>0</v>
@@ -2827,8 +2923,12 @@
       <c r="K19" s="71">
         <v>0</v>
       </c>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
+      <c r="L19" s="71">
+        <v>0</v>
+      </c>
+      <c r="M19" s="48">
+        <v>0.15</v>
+      </c>
       <c r="N19" s="28"/>
       <c r="O19" s="28"/>
       <c r="P19" s="29"/>
@@ -2840,9 +2940,9 @@
       <c r="V19" s="29"/>
       <c r="W19" s="30"/>
     </row>
-    <row r="20" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="112"/>
-      <c r="C20" s="100" t="s">
+    <row r="20" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="105"/>
+      <c r="C20" s="126" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="46" t="s">
@@ -2868,8 +2968,12 @@
       <c r="K20" s="71">
         <v>0</v>
       </c>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
+      <c r="L20" s="71">
+        <v>0</v>
+      </c>
+      <c r="M20" s="71">
+        <v>0</v>
+      </c>
       <c r="N20" s="28"/>
       <c r="O20" s="28"/>
       <c r="P20" s="29"/>
@@ -2881,9 +2985,9 @@
       <c r="V20" s="29"/>
       <c r="W20" s="30"/>
     </row>
-    <row r="21" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="112"/>
-      <c r="C21" s="100"/>
+    <row r="21" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="105"/>
+      <c r="C21" s="126"/>
       <c r="D21" s="46" t="s">
         <v>34</v>
       </c>
@@ -2907,8 +3011,12 @@
       <c r="K21" s="71">
         <v>0</v>
       </c>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
+      <c r="L21" s="71">
+        <v>0</v>
+      </c>
+      <c r="M21" s="71">
+        <v>0</v>
+      </c>
       <c r="N21" s="28"/>
       <c r="O21" s="28"/>
       <c r="P21" s="29"/>
@@ -2920,9 +3028,9 @@
       <c r="V21" s="29"/>
       <c r="W21" s="30"/>
     </row>
-    <row r="22" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="112"/>
-      <c r="C22" s="100"/>
+    <row r="22" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="105"/>
+      <c r="C22" s="126"/>
       <c r="D22" s="46" t="s">
         <v>35</v>
       </c>
@@ -2946,8 +3054,12 @@
       <c r="K22" s="71">
         <v>0</v>
       </c>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
+      <c r="L22" s="71">
+        <v>0</v>
+      </c>
+      <c r="M22" s="71">
+        <v>0</v>
+      </c>
       <c r="N22" s="28"/>
       <c r="O22" s="28"/>
       <c r="P22" s="29"/>
@@ -2959,9 +3071,9 @@
       <c r="V22" s="29"/>
       <c r="W22" s="30"/>
     </row>
-    <row r="23" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="112"/>
-      <c r="C23" s="100"/>
+    <row r="23" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="105"/>
+      <c r="C23" s="126"/>
       <c r="D23" s="46" t="s">
         <v>40</v>
       </c>
@@ -2985,8 +3097,12 @@
       <c r="K23" s="71">
         <v>0</v>
       </c>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
+      <c r="L23" s="71">
+        <v>0</v>
+      </c>
+      <c r="M23" s="71">
+        <v>0</v>
+      </c>
       <c r="N23" s="28"/>
       <c r="O23" s="28"/>
       <c r="P23" s="29"/>
@@ -2998,9 +3114,9 @@
       <c r="V23" s="29"/>
       <c r="W23" s="30"/>
     </row>
-    <row r="24" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="112"/>
-      <c r="C24" s="100"/>
+    <row r="24" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="105"/>
+      <c r="C24" s="126"/>
       <c r="D24" s="46" t="s">
         <v>41</v>
       </c>
@@ -3024,8 +3140,12 @@
       <c r="K24" s="71">
         <v>0</v>
       </c>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
+      <c r="L24" s="71">
+        <v>0</v>
+      </c>
+      <c r="M24" s="71">
+        <v>0</v>
+      </c>
       <c r="N24" s="28"/>
       <c r="O24" s="28"/>
       <c r="P24" s="29"/>
@@ -3037,9 +3157,9 @@
       <c r="V24" s="29"/>
       <c r="W24" s="30"/>
     </row>
-    <row r="25" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="112"/>
-      <c r="C25" s="100"/>
+    <row r="25" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="105"/>
+      <c r="C25" s="126"/>
       <c r="D25" s="46" t="s">
         <v>42</v>
       </c>
@@ -3063,8 +3183,12 @@
       <c r="K25" s="71">
         <v>0</v>
       </c>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
+      <c r="L25" s="71">
+        <v>0</v>
+      </c>
+      <c r="M25" s="71">
+        <v>0</v>
+      </c>
       <c r="N25" s="28"/>
       <c r="O25" s="28"/>
       <c r="P25" s="29"/>
@@ -3076,9 +3200,9 @@
       <c r="V25" s="29"/>
       <c r="W25" s="30"/>
     </row>
-    <row r="26" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="112"/>
-      <c r="C26" s="100"/>
+    <row r="26" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="105"/>
+      <c r="C26" s="126"/>
       <c r="D26" s="46" t="s">
         <v>43</v>
       </c>
@@ -3102,8 +3226,12 @@
       <c r="K26" s="71">
         <v>0</v>
       </c>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
+      <c r="L26" s="71">
+        <v>0</v>
+      </c>
+      <c r="M26" s="71">
+        <v>0</v>
+      </c>
       <c r="N26" s="28"/>
       <c r="O26" s="28"/>
       <c r="P26" s="29"/>
@@ -3115,9 +3243,9 @@
       <c r="V26" s="29"/>
       <c r="W26" s="30"/>
     </row>
-    <row r="27" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="112"/>
-      <c r="C27" s="100"/>
+    <row r="27" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="105"/>
+      <c r="C27" s="126"/>
       <c r="D27" s="46" t="s">
         <v>44</v>
       </c>
@@ -3141,8 +3269,12 @@
       <c r="K27" s="71">
         <v>0</v>
       </c>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
+      <c r="L27" s="71">
+        <v>0</v>
+      </c>
+      <c r="M27" s="71">
+        <v>0</v>
+      </c>
       <c r="N27" s="28"/>
       <c r="O27" s="28"/>
       <c r="P27" s="29"/>
@@ -3154,9 +3286,9 @@
       <c r="V27" s="29"/>
       <c r="W27" s="30"/>
     </row>
-    <row r="28" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="112"/>
-      <c r="C28" s="100"/>
+    <row r="28" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="105"/>
+      <c r="C28" s="126"/>
       <c r="D28" s="46" t="s">
         <v>45</v>
       </c>
@@ -3180,8 +3312,12 @@
       <c r="K28" s="71">
         <v>0</v>
       </c>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
+      <c r="L28" s="71">
+        <v>0</v>
+      </c>
+      <c r="M28" s="71">
+        <v>0</v>
+      </c>
       <c r="N28" s="28"/>
       <c r="O28" s="28"/>
       <c r="P28" s="29"/>
@@ -3193,9 +3329,9 @@
       <c r="V28" s="29"/>
       <c r="W28" s="30"/>
     </row>
-    <row r="29" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="112"/>
-      <c r="C29" s="100"/>
+    <row r="29" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="105"/>
+      <c r="C29" s="126"/>
       <c r="D29" s="46" t="s">
         <v>46</v>
       </c>
@@ -3219,8 +3355,12 @@
       <c r="K29" s="71">
         <v>0</v>
       </c>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
+      <c r="L29" s="71">
+        <v>0</v>
+      </c>
+      <c r="M29" s="71">
+        <v>0</v>
+      </c>
       <c r="N29" s="28"/>
       <c r="O29" s="28"/>
       <c r="P29" s="29"/>
@@ -3232,9 +3372,9 @@
       <c r="V29" s="29"/>
       <c r="W29" s="30"/>
     </row>
-    <row r="30" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="112"/>
-      <c r="C30" s="100"/>
+    <row r="30" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="105"/>
+      <c r="C30" s="126"/>
       <c r="D30" s="46" t="s">
         <v>47</v>
       </c>
@@ -3258,8 +3398,12 @@
       <c r="K30" s="71">
         <v>0</v>
       </c>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
+      <c r="L30" s="71">
+        <v>0</v>
+      </c>
+      <c r="M30" s="71">
+        <v>0</v>
+      </c>
       <c r="N30" s="28"/>
       <c r="O30" s="28"/>
       <c r="P30" s="29"/>
@@ -3271,9 +3415,9 @@
       <c r="V30" s="29"/>
       <c r="W30" s="30"/>
     </row>
-    <row r="31" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="112"/>
-      <c r="C31" s="100"/>
+    <row r="31" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="105"/>
+      <c r="C31" s="126"/>
       <c r="D31" s="46" t="s">
         <v>48</v>
       </c>
@@ -3297,8 +3441,12 @@
       <c r="K31" s="71">
         <v>0</v>
       </c>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
+      <c r="L31" s="71">
+        <v>0</v>
+      </c>
+      <c r="M31" s="71">
+        <v>0</v>
+      </c>
       <c r="N31" s="28"/>
       <c r="O31" s="28"/>
       <c r="P31" s="29"/>
@@ -3310,9 +3458,9 @@
       <c r="V31" s="29"/>
       <c r="W31" s="30"/>
     </row>
-    <row r="32" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="112"/>
-      <c r="C32" s="100"/>
+    <row r="32" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="105"/>
+      <c r="C32" s="126"/>
       <c r="D32" s="46" t="s">
         <v>49</v>
       </c>
@@ -3336,8 +3484,12 @@
       <c r="K32" s="71">
         <v>0</v>
       </c>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
+      <c r="L32" s="71">
+        <v>0</v>
+      </c>
+      <c r="M32" s="71">
+        <v>0</v>
+      </c>
       <c r="N32" s="28"/>
       <c r="O32" s="28"/>
       <c r="P32" s="29"/>
@@ -3349,9 +3501,9 @@
       <c r="V32" s="29"/>
       <c r="W32" s="30"/>
     </row>
-    <row r="33" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="112"/>
-      <c r="C33" s="100"/>
+    <row r="33" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="105"/>
+      <c r="C33" s="126"/>
       <c r="D33" s="46" t="s">
         <v>50</v>
       </c>
@@ -3375,8 +3527,12 @@
       <c r="K33" s="71">
         <v>0</v>
       </c>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
+      <c r="L33" s="71">
+        <v>0</v>
+      </c>
+      <c r="M33" s="71">
+        <v>0</v>
+      </c>
       <c r="N33" s="28"/>
       <c r="O33" s="28"/>
       <c r="P33" s="29"/>
@@ -3388,9 +3544,9 @@
       <c r="V33" s="29"/>
       <c r="W33" s="30"/>
     </row>
-    <row r="34" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="112"/>
-      <c r="C34" s="100"/>
+    <row r="34" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="105"/>
+      <c r="C34" s="126"/>
       <c r="D34" s="46" t="s">
         <v>51</v>
       </c>
@@ -3414,8 +3570,12 @@
       <c r="K34" s="71">
         <v>0</v>
       </c>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
+      <c r="L34" s="71">
+        <v>0</v>
+      </c>
+      <c r="M34" s="71">
+        <v>0</v>
+      </c>
       <c r="N34" s="28"/>
       <c r="O34" s="28"/>
       <c r="P34" s="29"/>
@@ -3427,9 +3587,9 @@
       <c r="V34" s="29"/>
       <c r="W34" s="30"/>
     </row>
-    <row r="35" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="112"/>
-      <c r="C35" s="100"/>
+    <row r="35" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="105"/>
+      <c r="C35" s="126"/>
       <c r="D35" s="46" t="s">
         <v>52</v>
       </c>
@@ -3453,8 +3613,12 @@
       <c r="K35" s="71">
         <v>0</v>
       </c>
-      <c r="L35" s="28"/>
-      <c r="M35" s="28"/>
+      <c r="L35" s="71">
+        <v>0</v>
+      </c>
+      <c r="M35" s="71">
+        <v>0</v>
+      </c>
       <c r="N35" s="28"/>
       <c r="O35" s="28"/>
       <c r="P35" s="29"/>
@@ -3466,9 +3630,9 @@
       <c r="V35" s="29"/>
       <c r="W35" s="30"/>
     </row>
-    <row r="36" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="112"/>
-      <c r="C36" s="100"/>
+    <row r="36" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="105"/>
+      <c r="C36" s="126"/>
       <c r="D36" s="52" t="s">
         <v>111</v>
       </c>
@@ -3492,8 +3656,12 @@
       <c r="K36" s="71">
         <v>0</v>
       </c>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
+      <c r="L36" s="71">
+        <v>0</v>
+      </c>
+      <c r="M36" s="71">
+        <v>0</v>
+      </c>
       <c r="N36" s="28"/>
       <c r="O36" s="28"/>
       <c r="P36" s="29"/>
@@ -3505,8 +3673,8 @@
       <c r="V36" s="29"/>
       <c r="W36" s="30"/>
     </row>
-    <row r="37" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="112"/>
+    <row r="37" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="105"/>
       <c r="C37" s="49" t="s">
         <v>53</v>
       </c>
@@ -3531,8 +3699,12 @@
       <c r="K37" s="71">
         <v>0</v>
       </c>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
+      <c r="L37" s="71">
+        <v>0</v>
+      </c>
+      <c r="M37" s="71">
+        <v>0</v>
+      </c>
       <c r="N37" s="28"/>
       <c r="O37" s="28"/>
       <c r="P37" s="29"/>
@@ -3544,8 +3716,8 @@
       <c r="V37" s="29"/>
       <c r="W37" s="30"/>
     </row>
-    <row r="38" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="112"/>
+    <row r="38" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="105"/>
       <c r="C38" s="49" t="s">
         <v>55</v>
       </c>
@@ -3570,8 +3742,12 @@
       <c r="K38" s="71">
         <v>0</v>
       </c>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
+      <c r="L38" s="71">
+        <v>0</v>
+      </c>
+      <c r="M38" s="71">
+        <v>0</v>
+      </c>
       <c r="N38" s="28"/>
       <c r="O38" s="28"/>
       <c r="P38" s="29"/>
@@ -3583,8 +3759,8 @@
       <c r="V38" s="29"/>
       <c r="W38" s="30"/>
     </row>
-    <row r="39" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="112"/>
+    <row r="39" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="105"/>
       <c r="C39" s="49" t="s">
         <v>56</v>
       </c>
@@ -3609,7 +3785,7 @@
       <c r="K39" s="71">
         <v>0</v>
       </c>
-      <c r="L39" s="127">
+      <c r="L39" s="94">
         <v>0.5</v>
       </c>
       <c r="M39" s="48">
@@ -3646,8 +3822,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="112"/>
+    <row r="40" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="105"/>
       <c r="C40" s="56" t="s">
         <v>112</v>
       </c>
@@ -3675,7 +3851,9 @@
       <c r="L40" s="71">
         <v>0</v>
       </c>
-      <c r="M40" s="28"/>
+      <c r="M40" s="71">
+        <v>0</v>
+      </c>
       <c r="N40" s="28"/>
       <c r="O40" s="28"/>
       <c r="P40" s="29"/>
@@ -3687,11 +3865,11 @@
       <c r="V40" s="29"/>
       <c r="W40" s="30"/>
     </row>
-    <row r="41" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="102" t="s">
+    <row r="41" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="98" t="s">
+      <c r="C41" s="124" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="50" t="s">
@@ -3754,9 +3932,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="103"/>
-      <c r="C42" s="99"/>
+    <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="96"/>
+      <c r="C42" s="125"/>
       <c r="D42" s="49" t="s">
         <v>21</v>
       </c>
@@ -3783,7 +3961,9 @@
       <c r="L42" s="71">
         <v>0</v>
       </c>
-      <c r="M42" s="28"/>
+      <c r="M42" s="71">
+        <v>0</v>
+      </c>
       <c r="N42" s="28"/>
       <c r="O42" s="28"/>
       <c r="P42" s="29"/>
@@ -3795,9 +3975,9 @@
       <c r="V42" s="29"/>
       <c r="W42" s="30"/>
     </row>
-    <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="103"/>
-      <c r="C43" s="99"/>
+    <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="96"/>
+      <c r="C43" s="125"/>
       <c r="D43" s="49" t="s">
         <v>22</v>
       </c>
@@ -3824,7 +4004,9 @@
       <c r="L43" s="71">
         <v>0</v>
       </c>
-      <c r="M43" s="28"/>
+      <c r="M43" s="71">
+        <v>0</v>
+      </c>
       <c r="N43" s="28"/>
       <c r="O43" s="28"/>
       <c r="P43" s="29"/>
@@ -3836,9 +4018,9 @@
       <c r="V43" s="29"/>
       <c r="W43" s="30"/>
     </row>
-    <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="103"/>
-      <c r="C44" s="99"/>
+    <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="96"/>
+      <c r="C44" s="125"/>
       <c r="D44" s="49" t="s">
         <v>23</v>
       </c>
@@ -3865,7 +4047,9 @@
       <c r="L44" s="71">
         <v>0</v>
       </c>
-      <c r="M44" s="28"/>
+      <c r="M44" s="71">
+        <v>0</v>
+      </c>
       <c r="N44" s="28"/>
       <c r="O44" s="28"/>
       <c r="P44" s="29"/>
@@ -3877,9 +4061,9 @@
       <c r="V44" s="29"/>
       <c r="W44" s="30"/>
     </row>
-    <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="103"/>
-      <c r="C45" s="99"/>
+    <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="96"/>
+      <c r="C45" s="125"/>
       <c r="D45" s="49" t="s">
         <v>24</v>
       </c>
@@ -3906,7 +4090,9 @@
       <c r="L45" s="71">
         <v>0</v>
       </c>
-      <c r="M45" s="28"/>
+      <c r="M45" s="71">
+        <v>0</v>
+      </c>
       <c r="N45" s="28"/>
       <c r="O45" s="28"/>
       <c r="P45" s="29"/>
@@ -3918,9 +4104,9 @@
       <c r="V45" s="29"/>
       <c r="W45" s="30"/>
     </row>
-    <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="103"/>
-      <c r="C46" s="99"/>
+    <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="96"/>
+      <c r="C46" s="125"/>
       <c r="D46" s="49" t="s">
         <v>25</v>
       </c>
@@ -3947,7 +4133,9 @@
       <c r="L46" s="71">
         <v>0</v>
       </c>
-      <c r="M46" s="28"/>
+      <c r="M46" s="71">
+        <v>0</v>
+      </c>
       <c r="N46" s="28"/>
       <c r="O46" s="28"/>
       <c r="P46" s="29"/>
@@ -3959,9 +4147,9 @@
       <c r="V46" s="29"/>
       <c r="W46" s="30"/>
     </row>
-    <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="103"/>
-      <c r="C47" s="99"/>
+    <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="96"/>
+      <c r="C47" s="125"/>
       <c r="D47" s="49" t="s">
         <v>26</v>
       </c>
@@ -3988,7 +4176,9 @@
       <c r="L47" s="71">
         <v>0</v>
       </c>
-      <c r="M47" s="28"/>
+      <c r="M47" s="71">
+        <v>0</v>
+      </c>
       <c r="N47" s="28"/>
       <c r="O47" s="28"/>
       <c r="P47" s="29"/>
@@ -4000,9 +4190,9 @@
       <c r="V47" s="29"/>
       <c r="W47" s="30"/>
     </row>
-    <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="103"/>
-      <c r="C48" s="99"/>
+    <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="96"/>
+      <c r="C48" s="125"/>
       <c r="D48" s="49" t="s">
         <v>27</v>
       </c>
@@ -4029,7 +4219,9 @@
       <c r="L48" s="71">
         <v>0</v>
       </c>
-      <c r="M48" s="28"/>
+      <c r="M48" s="71">
+        <v>0</v>
+      </c>
       <c r="N48" s="28"/>
       <c r="O48" s="28"/>
       <c r="P48" s="29"/>
@@ -4041,9 +4233,9 @@
       <c r="V48" s="29"/>
       <c r="W48" s="30"/>
     </row>
-    <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="103"/>
-      <c r="C49" s="99"/>
+    <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="96"/>
+      <c r="C49" s="125"/>
       <c r="D49" s="49" t="s">
         <v>28</v>
       </c>
@@ -4070,7 +4262,9 @@
       <c r="L49" s="71">
         <v>0</v>
       </c>
-      <c r="M49" s="28"/>
+      <c r="M49" s="71">
+        <v>0</v>
+      </c>
       <c r="N49" s="28"/>
       <c r="O49" s="28"/>
       <c r="P49" s="29"/>
@@ -4082,9 +4276,9 @@
       <c r="V49" s="29"/>
       <c r="W49" s="30"/>
     </row>
-    <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="103"/>
-      <c r="C50" s="99"/>
+    <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="96"/>
+      <c r="C50" s="125"/>
       <c r="D50" s="49" t="s">
         <v>29</v>
       </c>
@@ -4111,7 +4305,9 @@
       <c r="L50" s="71">
         <v>0</v>
       </c>
-      <c r="M50" s="28"/>
+      <c r="M50" s="71">
+        <v>0</v>
+      </c>
       <c r="N50" s="28"/>
       <c r="O50" s="28"/>
       <c r="P50" s="29"/>
@@ -4123,9 +4319,9 @@
       <c r="V50" s="29"/>
       <c r="W50" s="30"/>
     </row>
-    <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="103"/>
-      <c r="C51" s="99"/>
+    <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="96"/>
+      <c r="C51" s="125"/>
       <c r="D51" s="49" t="s">
         <v>30</v>
       </c>
@@ -4152,7 +4348,9 @@
       <c r="L51" s="71">
         <v>0</v>
       </c>
-      <c r="M51" s="28"/>
+      <c r="M51" s="71">
+        <v>0</v>
+      </c>
       <c r="N51" s="28"/>
       <c r="O51" s="28"/>
       <c r="P51" s="29"/>
@@ -4164,9 +4362,9 @@
       <c r="V51" s="29"/>
       <c r="W51" s="30"/>
     </row>
-    <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="103"/>
-      <c r="C52" s="99"/>
+    <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="96"/>
+      <c r="C52" s="125"/>
       <c r="D52" s="49" t="s">
         <v>31</v>
       </c>
@@ -4193,7 +4391,9 @@
       <c r="L52" s="71">
         <v>0</v>
       </c>
-      <c r="M52" s="28"/>
+      <c r="M52" s="71">
+        <v>0</v>
+      </c>
       <c r="N52" s="28"/>
       <c r="O52" s="28"/>
       <c r="P52" s="29"/>
@@ -4205,9 +4405,9 @@
       <c r="V52" s="29"/>
       <c r="W52" s="30"/>
     </row>
-    <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="103"/>
-      <c r="C53" s="99"/>
+    <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="96"/>
+      <c r="C53" s="125"/>
       <c r="D53" s="49" t="s">
         <v>77</v>
       </c>
@@ -4234,7 +4434,9 @@
       <c r="L53" s="71">
         <v>0</v>
       </c>
-      <c r="M53" s="28"/>
+      <c r="M53" s="71">
+        <v>0</v>
+      </c>
       <c r="N53" s="28"/>
       <c r="O53" s="28"/>
       <c r="P53" s="29"/>
@@ -4246,9 +4448,9 @@
       <c r="V53" s="29"/>
       <c r="W53" s="30"/>
     </row>
-    <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="103"/>
-      <c r="C54" s="99"/>
+    <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="96"/>
+      <c r="C54" s="125"/>
       <c r="D54" s="49" t="s">
         <v>78</v>
       </c>
@@ -4275,7 +4477,9 @@
       <c r="L54" s="71">
         <v>0</v>
       </c>
-      <c r="M54" s="28"/>
+      <c r="M54" s="71">
+        <v>0</v>
+      </c>
       <c r="N54" s="28"/>
       <c r="O54" s="28"/>
       <c r="P54" s="29"/>
@@ -4287,9 +4491,9 @@
       <c r="V54" s="29"/>
       <c r="W54" s="30"/>
     </row>
-    <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="103"/>
-      <c r="C55" s="99"/>
+    <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="96"/>
+      <c r="C55" s="125"/>
       <c r="D55" s="49" t="s">
         <v>78</v>
       </c>
@@ -4316,7 +4520,9 @@
       <c r="L55" s="71">
         <v>0</v>
       </c>
-      <c r="M55" s="28"/>
+      <c r="M55" s="71">
+        <v>0</v>
+      </c>
       <c r="N55" s="28"/>
       <c r="O55" s="28"/>
       <c r="P55" s="29"/>
@@ -4328,9 +4534,9 @@
       <c r="V55" s="29"/>
       <c r="W55" s="30"/>
     </row>
-    <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="103"/>
-      <c r="C56" s="99"/>
+    <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="96"/>
+      <c r="C56" s="125"/>
       <c r="D56" s="49" t="s">
         <v>79</v>
       </c>
@@ -4357,7 +4563,9 @@
       <c r="L56" s="71">
         <v>0</v>
       </c>
-      <c r="M56" s="28"/>
+      <c r="M56" s="71">
+        <v>0</v>
+      </c>
       <c r="N56" s="28"/>
       <c r="O56" s="28"/>
       <c r="P56" s="29"/>
@@ -4369,9 +4577,9 @@
       <c r="V56" s="29"/>
       <c r="W56" s="30"/>
     </row>
-    <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="103"/>
-      <c r="C57" s="99"/>
+    <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="96"/>
+      <c r="C57" s="125"/>
       <c r="D57" s="49" t="s">
         <v>80</v>
       </c>
@@ -4398,7 +4606,9 @@
       <c r="L57" s="71">
         <v>0</v>
       </c>
-      <c r="M57" s="28"/>
+      <c r="M57" s="71">
+        <v>0</v>
+      </c>
       <c r="N57" s="28"/>
       <c r="O57" s="28"/>
       <c r="P57" s="29"/>
@@ -4410,9 +4620,9 @@
       <c r="V57" s="29"/>
       <c r="W57" s="30"/>
     </row>
-    <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="103"/>
-      <c r="C58" s="99"/>
+    <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="96"/>
+      <c r="C58" s="125"/>
       <c r="D58" s="49" t="s">
         <v>81</v>
       </c>
@@ -4439,7 +4649,9 @@
       <c r="L58" s="71">
         <v>0</v>
       </c>
-      <c r="M58" s="28"/>
+      <c r="M58" s="71">
+        <v>0</v>
+      </c>
       <c r="N58" s="28"/>
       <c r="O58" s="28"/>
       <c r="P58" s="29"/>
@@ -4451,9 +4663,9 @@
       <c r="V58" s="29"/>
       <c r="W58" s="30"/>
     </row>
-    <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="103"/>
-      <c r="C59" s="99"/>
+    <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="96"/>
+      <c r="C59" s="125"/>
       <c r="D59" s="49" t="s">
         <v>82</v>
       </c>
@@ -4480,7 +4692,9 @@
       <c r="L59" s="71">
         <v>0</v>
       </c>
-      <c r="M59" s="28"/>
+      <c r="M59" s="71">
+        <v>0</v>
+      </c>
       <c r="N59" s="28"/>
       <c r="O59" s="28"/>
       <c r="P59" s="29"/>
@@ -4492,9 +4706,9 @@
       <c r="V59" s="29"/>
       <c r="W59" s="30"/>
     </row>
-    <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="103"/>
-      <c r="C60" s="99"/>
+    <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="96"/>
+      <c r="C60" s="125"/>
       <c r="D60" s="49" t="s">
         <v>83</v>
       </c>
@@ -4521,7 +4735,9 @@
       <c r="L60" s="71">
         <v>0</v>
       </c>
-      <c r="M60" s="28"/>
+      <c r="M60" s="71">
+        <v>0</v>
+      </c>
       <c r="N60" s="28"/>
       <c r="O60" s="28"/>
       <c r="P60" s="29"/>
@@ -4533,9 +4749,9 @@
       <c r="V60" s="29"/>
       <c r="W60" s="30"/>
     </row>
-    <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="103"/>
-      <c r="C61" s="99"/>
+    <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="96"/>
+      <c r="C61" s="125"/>
       <c r="D61" s="49" t="s">
         <v>84</v>
       </c>
@@ -4562,7 +4778,9 @@
       <c r="L61" s="71">
         <v>0</v>
       </c>
-      <c r="M61" s="28"/>
+      <c r="M61" s="71">
+        <v>0</v>
+      </c>
       <c r="N61" s="28"/>
       <c r="O61" s="28"/>
       <c r="P61" s="29"/>
@@ -4574,9 +4792,9 @@
       <c r="V61" s="29"/>
       <c r="W61" s="30"/>
     </row>
-    <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="103"/>
-      <c r="C62" s="99"/>
+    <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="96"/>
+      <c r="C62" s="125"/>
       <c r="D62" s="49" t="s">
         <v>85</v>
       </c>
@@ -4603,7 +4821,9 @@
       <c r="L62" s="71">
         <v>0</v>
       </c>
-      <c r="M62" s="28"/>
+      <c r="M62" s="71">
+        <v>0</v>
+      </c>
       <c r="N62" s="28"/>
       <c r="O62" s="28"/>
       <c r="P62" s="29"/>
@@ -4615,9 +4835,9 @@
       <c r="V62" s="29"/>
       <c r="W62" s="30"/>
     </row>
-    <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="103"/>
-      <c r="C63" s="99"/>
+    <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="96"/>
+      <c r="C63" s="125"/>
       <c r="D63" s="49" t="s">
         <v>86</v>
       </c>
@@ -4644,7 +4864,9 @@
       <c r="L63" s="71">
         <v>0</v>
       </c>
-      <c r="M63" s="28"/>
+      <c r="M63" s="71">
+        <v>0</v>
+      </c>
       <c r="N63" s="28"/>
       <c r="O63" s="28"/>
       <c r="P63" s="29"/>
@@ -4656,9 +4878,9 @@
       <c r="V63" s="29"/>
       <c r="W63" s="30"/>
     </row>
-    <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="103"/>
-      <c r="C64" s="99"/>
+    <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="96"/>
+      <c r="C64" s="125"/>
       <c r="D64" s="49" t="s">
         <v>87</v>
       </c>
@@ -4685,7 +4907,9 @@
       <c r="L64" s="71">
         <v>0</v>
       </c>
-      <c r="M64" s="28"/>
+      <c r="M64" s="71">
+        <v>0</v>
+      </c>
       <c r="N64" s="28"/>
       <c r="O64" s="28"/>
       <c r="P64" s="29"/>
@@ -4697,9 +4921,9 @@
       <c r="V64" s="29"/>
       <c r="W64" s="30"/>
     </row>
-    <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="103"/>
-      <c r="C65" s="99"/>
+    <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="96"/>
+      <c r="C65" s="125"/>
       <c r="D65" s="49" t="s">
         <v>88</v>
       </c>
@@ -4726,7 +4950,9 @@
       <c r="L65" s="71">
         <v>0</v>
       </c>
-      <c r="M65" s="28"/>
+      <c r="M65" s="71">
+        <v>0</v>
+      </c>
       <c r="N65" s="28"/>
       <c r="O65" s="28"/>
       <c r="P65" s="29"/>
@@ -4738,9 +4964,9 @@
       <c r="V65" s="29"/>
       <c r="W65" s="30"/>
     </row>
-    <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="103"/>
-      <c r="C66" s="99"/>
+    <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="96"/>
+      <c r="C66" s="125"/>
       <c r="D66" s="49" t="s">
         <v>89</v>
       </c>
@@ -4767,7 +4993,9 @@
       <c r="L66" s="71">
         <v>0</v>
       </c>
-      <c r="M66" s="28"/>
+      <c r="M66" s="71">
+        <v>0</v>
+      </c>
       <c r="N66" s="28"/>
       <c r="O66" s="28"/>
       <c r="P66" s="29"/>
@@ -4779,9 +5007,9 @@
       <c r="V66" s="29"/>
       <c r="W66" s="30"/>
     </row>
-    <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="103"/>
-      <c r="C67" s="99"/>
+    <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="96"/>
+      <c r="C67" s="125"/>
       <c r="D67" s="49" t="s">
         <v>94</v>
       </c>
@@ -4808,7 +5036,9 @@
       <c r="L67" s="71">
         <v>0</v>
       </c>
-      <c r="M67" s="28"/>
+      <c r="M67" s="71">
+        <v>0</v>
+      </c>
       <c r="N67" s="28"/>
       <c r="O67" s="28"/>
       <c r="P67" s="29"/>
@@ -4820,9 +5050,9 @@
       <c r="V67" s="29"/>
       <c r="W67" s="30"/>
     </row>
-    <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="103"/>
-      <c r="C68" s="99"/>
+    <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="96"/>
+      <c r="C68" s="125"/>
       <c r="D68" s="49" t="s">
         <v>95</v>
       </c>
@@ -4849,7 +5079,9 @@
       <c r="L68" s="71">
         <v>0</v>
       </c>
-      <c r="M68" s="28"/>
+      <c r="M68" s="71">
+        <v>0</v>
+      </c>
       <c r="N68" s="28"/>
       <c r="O68" s="28"/>
       <c r="P68" s="29"/>
@@ -4861,9 +5093,9 @@
       <c r="V68" s="29"/>
       <c r="W68" s="30"/>
     </row>
-    <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="103"/>
-      <c r="C69" s="99"/>
+    <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="96"/>
+      <c r="C69" s="125"/>
       <c r="D69" s="49" t="s">
         <v>96</v>
       </c>
@@ -4890,7 +5122,9 @@
       <c r="L69" s="71">
         <v>0</v>
       </c>
-      <c r="M69" s="28"/>
+      <c r="M69" s="71">
+        <v>0</v>
+      </c>
       <c r="N69" s="28"/>
       <c r="O69" s="28"/>
       <c r="P69" s="29"/>
@@ -4902,9 +5136,9 @@
       <c r="V69" s="29"/>
       <c r="W69" s="30"/>
     </row>
-    <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="103"/>
-      <c r="C70" s="99"/>
+    <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="96"/>
+      <c r="C70" s="125"/>
       <c r="D70" s="49" t="s">
         <v>97</v>
       </c>
@@ -4931,7 +5165,9 @@
       <c r="L70" s="71">
         <v>0</v>
       </c>
-      <c r="M70" s="28"/>
+      <c r="M70" s="71">
+        <v>0</v>
+      </c>
       <c r="N70" s="28"/>
       <c r="O70" s="28"/>
       <c r="P70" s="29"/>
@@ -4943,9 +5179,9 @@
       <c r="V70" s="29"/>
       <c r="W70" s="30"/>
     </row>
-    <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="103"/>
-      <c r="C71" s="99"/>
+    <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="96"/>
+      <c r="C71" s="125"/>
       <c r="D71" s="49" t="s">
         <v>98</v>
       </c>
@@ -4972,7 +5208,9 @@
       <c r="L71" s="71">
         <v>0</v>
       </c>
-      <c r="M71" s="28"/>
+      <c r="M71" s="71">
+        <v>0</v>
+      </c>
       <c r="N71" s="28"/>
       <c r="O71" s="28"/>
       <c r="P71" s="29"/>
@@ -4984,9 +5222,9 @@
       <c r="V71" s="29"/>
       <c r="W71" s="30"/>
     </row>
-    <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="103"/>
-      <c r="C72" s="99"/>
+    <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="96"/>
+      <c r="C72" s="125"/>
       <c r="D72" s="49" t="s">
         <v>99</v>
       </c>
@@ -5013,7 +5251,9 @@
       <c r="L72" s="71">
         <v>0</v>
       </c>
-      <c r="M72" s="28"/>
+      <c r="M72" s="71">
+        <v>0</v>
+      </c>
       <c r="N72" s="28"/>
       <c r="O72" s="28"/>
       <c r="P72" s="29"/>
@@ -5025,9 +5265,9 @@
       <c r="V72" s="29"/>
       <c r="W72" s="30"/>
     </row>
-    <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="103"/>
-      <c r="C73" s="99"/>
+    <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="96"/>
+      <c r="C73" s="125"/>
       <c r="D73" s="49" t="s">
         <v>100</v>
       </c>
@@ -5054,7 +5294,9 @@
       <c r="L73" s="71">
         <v>0</v>
       </c>
-      <c r="M73" s="28"/>
+      <c r="M73" s="71">
+        <v>0</v>
+      </c>
       <c r="N73" s="28"/>
       <c r="O73" s="28"/>
       <c r="P73" s="29"/>
@@ -5066,9 +5308,9 @@
       <c r="V73" s="29"/>
       <c r="W73" s="30"/>
     </row>
-    <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="103"/>
-      <c r="C74" s="99"/>
+    <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="96"/>
+      <c r="C74" s="125"/>
       <c r="D74" s="49" t="s">
         <v>101</v>
       </c>
@@ -5095,7 +5337,9 @@
       <c r="L74" s="71">
         <v>0</v>
       </c>
-      <c r="M74" s="28"/>
+      <c r="M74" s="71">
+        <v>0</v>
+      </c>
       <c r="N74" s="28"/>
       <c r="O74" s="28"/>
       <c r="P74" s="29"/>
@@ -5107,9 +5351,9 @@
       <c r="V74" s="29"/>
       <c r="W74" s="30"/>
     </row>
-    <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="103"/>
-      <c r="C75" s="99"/>
+    <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="96"/>
+      <c r="C75" s="125"/>
       <c r="D75" s="49" t="s">
         <v>102</v>
       </c>
@@ -5136,7 +5380,9 @@
       <c r="L75" s="71">
         <v>0</v>
       </c>
-      <c r="M75" s="28"/>
+      <c r="M75" s="71">
+        <v>0</v>
+      </c>
       <c r="N75" s="28"/>
       <c r="O75" s="28"/>
       <c r="P75" s="29"/>
@@ -5148,9 +5394,9 @@
       <c r="V75" s="29"/>
       <c r="W75" s="30"/>
     </row>
-    <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="103"/>
-      <c r="C76" s="99"/>
+    <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="96"/>
+      <c r="C76" s="125"/>
       <c r="D76" s="49" t="s">
         <v>103</v>
       </c>
@@ -5177,7 +5423,9 @@
       <c r="L76" s="71">
         <v>0</v>
       </c>
-      <c r="M76" s="28"/>
+      <c r="M76" s="71">
+        <v>0</v>
+      </c>
       <c r="N76" s="28"/>
       <c r="O76" s="28"/>
       <c r="P76" s="29"/>
@@ -5189,9 +5437,9 @@
       <c r="V76" s="29"/>
       <c r="W76" s="30"/>
     </row>
-    <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="103"/>
-      <c r="C77" s="99"/>
+    <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="96"/>
+      <c r="C77" s="125"/>
       <c r="D77" s="49" t="s">
         <v>104</v>
       </c>
@@ -5218,7 +5466,9 @@
       <c r="L77" s="71">
         <v>0</v>
       </c>
-      <c r="M77" s="28"/>
+      <c r="M77" s="71">
+        <v>0</v>
+      </c>
       <c r="N77" s="28"/>
       <c r="O77" s="28"/>
       <c r="P77" s="29"/>
@@ -5230,9 +5480,9 @@
       <c r="V77" s="29"/>
       <c r="W77" s="30"/>
     </row>
-    <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="103"/>
-      <c r="C78" s="99"/>
+    <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="96"/>
+      <c r="C78" s="125"/>
       <c r="D78" s="49" t="s">
         <v>105</v>
       </c>
@@ -5259,7 +5509,9 @@
       <c r="L78" s="71">
         <v>0</v>
       </c>
-      <c r="M78" s="28"/>
+      <c r="M78" s="71">
+        <v>0</v>
+      </c>
       <c r="N78" s="28"/>
       <c r="O78" s="28"/>
       <c r="P78" s="29"/>
@@ -5271,9 +5523,9 @@
       <c r="V78" s="29"/>
       <c r="W78" s="30"/>
     </row>
-    <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="103"/>
-      <c r="C79" s="99"/>
+    <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="96"/>
+      <c r="C79" s="125"/>
       <c r="D79" s="49" t="s">
         <v>106</v>
       </c>
@@ -5300,7 +5552,9 @@
       <c r="L79" s="71">
         <v>0</v>
       </c>
-      <c r="M79" s="28"/>
+      <c r="M79" s="71">
+        <v>0</v>
+      </c>
       <c r="N79" s="28"/>
       <c r="O79" s="28"/>
       <c r="P79" s="29"/>
@@ -5312,9 +5566,9 @@
       <c r="V79" s="29"/>
       <c r="W79" s="30"/>
     </row>
-    <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="103"/>
-      <c r="C80" s="99"/>
+    <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="96"/>
+      <c r="C80" s="125"/>
       <c r="D80" s="49" t="s">
         <v>107</v>
       </c>
@@ -5341,7 +5595,9 @@
       <c r="L80" s="71">
         <v>0</v>
       </c>
-      <c r="M80" s="28"/>
+      <c r="M80" s="71">
+        <v>0</v>
+      </c>
       <c r="N80" s="28"/>
       <c r="O80" s="28"/>
       <c r="P80" s="29"/>
@@ -5353,9 +5609,9 @@
       <c r="V80" s="29"/>
       <c r="W80" s="30"/>
     </row>
-    <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="103"/>
-      <c r="C81" s="99"/>
+    <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="96"/>
+      <c r="C81" s="125"/>
       <c r="D81" s="49" t="s">
         <v>90</v>
       </c>
@@ -5382,7 +5638,9 @@
       <c r="L81" s="71">
         <v>0</v>
       </c>
-      <c r="M81" s="28"/>
+      <c r="M81" s="71">
+        <v>0</v>
+      </c>
       <c r="N81" s="28"/>
       <c r="O81" s="28"/>
       <c r="P81" s="29"/>
@@ -5394,9 +5652,9 @@
       <c r="V81" s="29"/>
       <c r="W81" s="30"/>
     </row>
-    <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="103"/>
-      <c r="C82" s="99"/>
+    <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="96"/>
+      <c r="C82" s="125"/>
       <c r="D82" s="49" t="s">
         <v>91</v>
       </c>
@@ -5423,7 +5681,9 @@
       <c r="L82" s="71">
         <v>0</v>
       </c>
-      <c r="M82" s="28"/>
+      <c r="M82" s="71">
+        <v>0</v>
+      </c>
       <c r="N82" s="28"/>
       <c r="O82" s="28"/>
       <c r="P82" s="29"/>
@@ -5435,9 +5695,9 @@
       <c r="V82" s="29"/>
       <c r="W82" s="30"/>
     </row>
-    <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="103"/>
-      <c r="C83" s="99"/>
+    <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="96"/>
+      <c r="C83" s="125"/>
       <c r="D83" s="49" t="s">
         <v>114</v>
       </c>
@@ -5498,9 +5758,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="103"/>
-      <c r="C84" s="104" t="s">
+    <row r="84" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="96"/>
+      <c r="C84" s="97" t="s">
         <v>37</v>
       </c>
       <c r="D84" s="46" t="s">
@@ -5526,8 +5786,12 @@
       <c r="K84" s="71">
         <v>0</v>
       </c>
-      <c r="L84" s="28"/>
-      <c r="M84" s="28"/>
+      <c r="L84" s="71">
+        <v>0</v>
+      </c>
+      <c r="M84" s="71">
+        <v>0</v>
+      </c>
       <c r="N84" s="28"/>
       <c r="O84" s="28"/>
       <c r="P84" s="28"/>
@@ -5539,9 +5803,9 @@
       <c r="V84" s="29"/>
       <c r="W84" s="30"/>
     </row>
-    <row r="85" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="103"/>
-      <c r="C85" s="104"/>
+    <row r="85" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="96"/>
+      <c r="C85" s="97"/>
       <c r="D85" s="52" t="s">
         <v>70</v>
       </c>
@@ -5565,8 +5829,12 @@
       <c r="K85" s="71">
         <v>0</v>
       </c>
-      <c r="L85" s="28"/>
-      <c r="M85" s="28"/>
+      <c r="L85" s="71">
+        <v>0</v>
+      </c>
+      <c r="M85" s="71">
+        <v>0</v>
+      </c>
       <c r="N85" s="28"/>
       <c r="O85" s="28"/>
       <c r="P85" s="28"/>
@@ -5578,9 +5846,9 @@
       <c r="V85" s="29"/>
       <c r="W85" s="30"/>
     </row>
-    <row r="86" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="103"/>
-      <c r="C86" s="104"/>
+    <row r="86" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="96"/>
+      <c r="C86" s="97"/>
       <c r="D86" s="52" t="s">
         <v>71</v>
       </c>
@@ -5604,8 +5872,12 @@
       <c r="K86" s="71">
         <v>0</v>
       </c>
-      <c r="L86" s="28"/>
-      <c r="M86" s="28"/>
+      <c r="L86" s="71">
+        <v>0</v>
+      </c>
+      <c r="M86" s="71">
+        <v>0</v>
+      </c>
       <c r="N86" s="28"/>
       <c r="O86" s="28"/>
       <c r="P86" s="28"/>
@@ -5617,9 +5889,9 @@
       <c r="V86" s="29"/>
       <c r="W86" s="30"/>
     </row>
-    <row r="87" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="103"/>
-      <c r="C87" s="104"/>
+    <row r="87" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="96"/>
+      <c r="C87" s="97"/>
       <c r="D87" s="52" t="s">
         <v>72</v>
       </c>
@@ -5643,8 +5915,12 @@
       <c r="K87" s="71">
         <v>0</v>
       </c>
-      <c r="L87" s="28"/>
-      <c r="M87" s="28"/>
+      <c r="L87" s="71">
+        <v>0</v>
+      </c>
+      <c r="M87" s="71">
+        <v>0</v>
+      </c>
       <c r="N87" s="28"/>
       <c r="O87" s="28"/>
       <c r="P87" s="28"/>
@@ -5656,9 +5932,9 @@
       <c r="V87" s="29"/>
       <c r="W87" s="30"/>
     </row>
-    <row r="88" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="103"/>
-      <c r="C88" s="104"/>
+    <row r="88" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="96"/>
+      <c r="C88" s="97"/>
       <c r="D88" s="52" t="s">
         <v>73</v>
       </c>
@@ -5682,8 +5958,12 @@
       <c r="K88" s="71">
         <v>0</v>
       </c>
-      <c r="L88" s="28"/>
-      <c r="M88" s="28"/>
+      <c r="L88" s="71">
+        <v>0</v>
+      </c>
+      <c r="M88" s="71">
+        <v>0</v>
+      </c>
       <c r="N88" s="28"/>
       <c r="O88" s="28"/>
       <c r="P88" s="28"/>
@@ -5695,9 +5975,9 @@
       <c r="V88" s="28"/>
       <c r="W88" s="58"/>
     </row>
-    <row r="89" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="103"/>
-      <c r="C89" s="104"/>
+    <row r="89" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="96"/>
+      <c r="C89" s="97"/>
       <c r="D89" s="52" t="s">
         <v>74</v>
       </c>
@@ -5721,8 +6001,12 @@
       <c r="K89" s="71">
         <v>0</v>
       </c>
-      <c r="L89" s="28"/>
-      <c r="M89" s="28"/>
+      <c r="L89" s="71">
+        <v>0</v>
+      </c>
+      <c r="M89" s="71">
+        <v>0</v>
+      </c>
       <c r="N89" s="28"/>
       <c r="O89" s="28"/>
       <c r="P89" s="28"/>
@@ -5734,8 +6018,8 @@
       <c r="V89" s="29"/>
       <c r="W89" s="30"/>
     </row>
-    <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="103"/>
+    <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="96"/>
       <c r="C90" s="83" t="s">
         <v>125</v>
       </c>
@@ -5797,8 +6081,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="103"/>
+    <row r="91" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="96"/>
       <c r="C91" s="75" t="s">
         <v>113</v>
       </c>
@@ -5823,8 +6107,12 @@
       <c r="K91" s="71">
         <v>0</v>
       </c>
-      <c r="L91" s="28"/>
-      <c r="M91" s="28"/>
+      <c r="L91" s="71">
+        <v>0</v>
+      </c>
+      <c r="M91" s="71">
+        <v>0</v>
+      </c>
       <c r="N91" s="28"/>
       <c r="O91" s="28"/>
       <c r="P91" s="28"/>
@@ -5836,8 +6124,8 @@
       <c r="V91" s="29"/>
       <c r="W91" s="30"/>
     </row>
-    <row r="92" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="122" t="s">
+    <row r="92" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="115" t="s">
         <v>92</v>
       </c>
       <c r="C92" s="38" t="s">
@@ -5864,8 +6152,12 @@
       <c r="K92" s="70">
         <v>0</v>
       </c>
-      <c r="L92" s="25"/>
-      <c r="M92" s="25"/>
+      <c r="L92" s="70">
+        <v>0</v>
+      </c>
+      <c r="M92" s="70">
+        <v>0</v>
+      </c>
       <c r="N92" s="25"/>
       <c r="O92" s="25"/>
       <c r="P92" s="25"/>
@@ -5877,8 +6169,8 @@
       <c r="V92" s="25"/>
       <c r="W92" s="67"/>
     </row>
-    <row r="93" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="123"/>
+    <row r="93" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="116"/>
       <c r="C93" s="41" t="s">
         <v>119</v>
       </c>
@@ -5897,10 +6189,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J93" s="73"/>
-      <c r="K93" s="73"/>
-      <c r="L93" s="35"/>
-      <c r="M93" s="35"/>
+      <c r="J93" s="73">
+        <v>0</v>
+      </c>
+      <c r="K93" s="73">
+        <v>0</v>
+      </c>
+      <c r="L93" s="73">
+        <v>0</v>
+      </c>
+      <c r="M93" s="73">
+        <v>0</v>
+      </c>
       <c r="N93" s="35"/>
       <c r="O93" s="35"/>
       <c r="P93" s="35"/>
@@ -5912,9 +6212,9 @@
       <c r="V93" s="35"/>
       <c r="W93" s="66"/>
     </row>
-    <row r="94" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="124"/>
-      <c r="C94" s="101" t="s">
+    <row r="94" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="117"/>
+      <c r="C94" s="127" t="s">
         <v>108</v>
       </c>
       <c r="D94" s="42" t="s">
@@ -5940,8 +6240,12 @@
       <c r="K94" s="71">
         <v>0</v>
       </c>
-      <c r="L94" s="28"/>
-      <c r="M94" s="28"/>
+      <c r="L94" s="71">
+        <v>0</v>
+      </c>
+      <c r="M94" s="71">
+        <v>0</v>
+      </c>
       <c r="N94" s="28"/>
       <c r="O94" s="28"/>
       <c r="P94" s="28"/>
@@ -5953,9 +6257,9 @@
       <c r="V94" s="28"/>
       <c r="W94" s="58"/>
     </row>
-    <row r="95" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B95" s="125"/>
-      <c r="C95" s="101"/>
+    <row r="95" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B95" s="118"/>
+      <c r="C95" s="127"/>
       <c r="D95" s="42" t="s">
         <v>109</v>
       </c>
@@ -5979,8 +6283,12 @@
       <c r="K95" s="71">
         <v>0</v>
       </c>
-      <c r="L95" s="28"/>
-      <c r="M95" s="28"/>
+      <c r="L95" s="71">
+        <v>0</v>
+      </c>
+      <c r="M95" s="71">
+        <v>0</v>
+      </c>
       <c r="N95" s="28"/>
       <c r="O95" s="28"/>
       <c r="P95" s="28"/>
@@ -5992,8 +6300,8 @@
       <c r="V95" s="29"/>
       <c r="W95" s="58"/>
     </row>
-    <row r="96" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="126"/>
+    <row r="96" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="119"/>
       <c r="C96" s="44" t="s">
         <v>116</v>
       </c>
@@ -6010,7 +6318,7 @@
       </c>
       <c r="I96" s="59">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J96" s="72">
         <v>0</v>
@@ -6018,8 +6326,12 @@
       <c r="K96" s="72">
         <v>0</v>
       </c>
-      <c r="L96" s="32"/>
-      <c r="M96" s="32"/>
+      <c r="L96" s="72">
+        <v>0</v>
+      </c>
+      <c r="M96" s="129">
+        <v>0.75</v>
+      </c>
       <c r="N96" s="32"/>
       <c r="O96" s="32"/>
       <c r="P96" s="32"/>
@@ -6031,8 +6343,8 @@
       <c r="V96" s="32"/>
       <c r="W96" s="64"/>
     </row>
-    <row r="97" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="102" t="s">
+    <row r="97" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="95" t="s">
         <v>93</v>
       </c>
       <c r="C97" s="63" t="s">
@@ -6051,7 +6363,7 @@
       </c>
       <c r="I97" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="J97" s="70">
         <v>0</v>
@@ -6059,8 +6371,12 @@
       <c r="K97" s="70">
         <v>0</v>
       </c>
-      <c r="L97" s="25"/>
-      <c r="M97" s="25"/>
+      <c r="L97" s="70">
+        <v>0</v>
+      </c>
+      <c r="M97" s="87">
+        <v>0.46700000000000003</v>
+      </c>
       <c r="N97" s="26"/>
       <c r="O97" s="26"/>
       <c r="P97" s="26"/>
@@ -6072,8 +6388,8 @@
       <c r="V97" s="26"/>
       <c r="W97" s="27"/>
     </row>
-    <row r="98" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B98" s="125"/>
+    <row r="98" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B98" s="118"/>
       <c r="C98" s="54" t="s">
         <v>131</v>
       </c>
@@ -6098,8 +6414,12 @@
       <c r="K98" s="71">
         <v>0</v>
       </c>
-      <c r="L98" s="28"/>
-      <c r="M98" s="28"/>
+      <c r="L98" s="71">
+        <v>0</v>
+      </c>
+      <c r="M98" s="130">
+        <v>0</v>
+      </c>
       <c r="N98" s="29"/>
       <c r="O98" s="29"/>
       <c r="P98" s="29"/>
@@ -6111,8 +6431,8 @@
       <c r="V98" s="29"/>
       <c r="W98" s="30"/>
     </row>
-    <row r="99" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B99" s="125"/>
+    <row r="99" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B99" s="118"/>
       <c r="C99" s="54" t="s">
         <v>130</v>
       </c>
@@ -6137,8 +6457,12 @@
       <c r="K99" s="71">
         <v>0</v>
       </c>
-      <c r="L99" s="28"/>
-      <c r="M99" s="28"/>
+      <c r="L99" s="71">
+        <v>0</v>
+      </c>
+      <c r="M99" s="130">
+        <v>0</v>
+      </c>
       <c r="N99" s="29"/>
       <c r="O99" s="29"/>
       <c r="P99" s="29"/>
@@ -6150,8 +6474,8 @@
       <c r="V99" s="29"/>
       <c r="W99" s="30"/>
     </row>
-    <row r="100" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B100" s="125"/>
+    <row r="100" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B100" s="118"/>
       <c r="C100" s="54" t="s">
         <v>129</v>
       </c>
@@ -6176,8 +6500,12 @@
       <c r="K100" s="71">
         <v>0</v>
       </c>
-      <c r="L100" s="28"/>
-      <c r="M100" s="28"/>
+      <c r="L100" s="71">
+        <v>0</v>
+      </c>
+      <c r="M100" s="130">
+        <v>0</v>
+      </c>
       <c r="N100" s="29"/>
       <c r="O100" s="29"/>
       <c r="P100" s="29"/>
@@ -6189,8 +6517,8 @@
       <c r="V100" s="29"/>
       <c r="W100" s="30"/>
     </row>
-    <row r="101" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B101" s="125"/>
+    <row r="101" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B101" s="118"/>
       <c r="C101" s="54" t="s">
         <v>128</v>
       </c>
@@ -6215,8 +6543,12 @@
       <c r="K101" s="71">
         <v>0</v>
       </c>
-      <c r="L101" s="28"/>
-      <c r="M101" s="28"/>
+      <c r="L101" s="71">
+        <v>0</v>
+      </c>
+      <c r="M101" s="71">
+        <v>0</v>
+      </c>
       <c r="N101" s="29"/>
       <c r="O101" s="29"/>
       <c r="P101" s="29"/>
@@ -6228,8 +6560,8 @@
       <c r="V101" s="29"/>
       <c r="W101" s="30"/>
     </row>
-    <row r="102" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="126"/>
+    <row r="102" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="119"/>
       <c r="C102" s="44" t="s">
         <v>127</v>
       </c>
@@ -6254,8 +6586,12 @@
       <c r="K102" s="72">
         <v>0</v>
       </c>
-      <c r="L102" s="32"/>
-      <c r="M102" s="32"/>
+      <c r="L102" s="72">
+        <v>0</v>
+      </c>
+      <c r="M102" s="72">
+        <v>0</v>
+      </c>
       <c r="N102" s="32"/>
       <c r="O102" s="32"/>
       <c r="P102" s="33"/>
@@ -6267,22 +6603,22 @@
       <c r="V102" s="33"/>
       <c r="W102" s="34"/>
     </row>
-    <row r="103" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="117" t="s">
+    <row r="103" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="C103" s="118"/>
-      <c r="D103" s="118"/>
-      <c r="E103" s="118"/>
-      <c r="F103" s="118"/>
-      <c r="G103" s="118"/>
+      <c r="C103" s="111"/>
+      <c r="D103" s="111"/>
+      <c r="E103" s="111"/>
+      <c r="F103" s="111"/>
+      <c r="G103" s="111"/>
       <c r="H103" s="17">
         <f t="shared" ref="H103:W103" si="4">SUM(H4:H102)</f>
         <v>48.72</v>
       </c>
       <c r="I103" s="17">
         <f t="shared" si="4"/>
-        <v>12.9</v>
+        <v>16.393000000000001</v>
       </c>
       <c r="J103" s="17">
         <f t="shared" si="4"/>
@@ -6298,7 +6634,7 @@
       </c>
       <c r="M103" s="17">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>3.9929999999999999</v>
       </c>
       <c r="N103" s="17">
         <f t="shared" si="4"/>
@@ -6341,7 +6677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -6350,24 +6686,24 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
-      <c r="J104" s="108" t="s">
+      <c r="J104" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="K104" s="109"/>
-      <c r="L104" s="109"/>
-      <c r="M104" s="109"/>
-      <c r="N104" s="109"/>
-      <c r="O104" s="109"/>
-      <c r="P104" s="109"/>
-      <c r="Q104" s="109"/>
-      <c r="R104" s="109"/>
-      <c r="S104" s="109"/>
-      <c r="T104" s="109"/>
-      <c r="U104" s="109"/>
-      <c r="V104" s="109"/>
-      <c r="W104" s="110"/>
-    </row>
-    <row r="105" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K104" s="102"/>
+      <c r="L104" s="102"/>
+      <c r="M104" s="102"/>
+      <c r="N104" s="102"/>
+      <c r="O104" s="102"/>
+      <c r="P104" s="102"/>
+      <c r="Q104" s="102"/>
+      <c r="R104" s="102"/>
+      <c r="S104" s="102"/>
+      <c r="T104" s="102"/>
+      <c r="U104" s="102"/>
+      <c r="V104" s="102"/>
+      <c r="W104" s="103"/>
+    </row>
+    <row r="105" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B105" s="76" t="s">
         <v>124</v>
       </c>
@@ -6391,7 +6727,7 @@
       <c r="O105" s="9"/>
       <c r="P105" s="9"/>
     </row>
-    <row r="106" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B106" s="82" t="s">
         <v>16</v>
       </c>
@@ -6401,18 +6737,18 @@
       </c>
       <c r="D106" s="36">
         <f>SUM(I98:I102,I91:I96,I9,I7,I40)</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E106" s="36">
         <f>SUM(C106,-D106)</f>
-        <v>12.27</v>
+        <v>11.52</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="94" t="s">
+      <c r="H106" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="I106" s="97"/>
+      <c r="I106" s="123"/>
       <c r="J106" s="10">
         <f>H103-J103</f>
         <v>46.769999999999996</v>
@@ -6427,50 +6763,50 @@
       </c>
       <c r="M106" s="10">
         <f>L106-M103</f>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="N106" s="10">
         <f t="shared" ref="N106:W106" si="5">M106-N103</f>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="O106" s="10">
         <f t="shared" si="5"/>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="P106" s="10">
         <f t="shared" si="5"/>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="Q106" s="10">
         <f t="shared" si="5"/>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="R106" s="10">
         <f t="shared" si="5"/>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="S106" s="10">
         <f t="shared" si="5"/>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="T106" s="10">
         <f t="shared" si="5"/>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="U106" s="10">
         <f t="shared" si="5"/>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="V106" s="10">
         <f t="shared" si="5"/>
-        <v>35.82</v>
+        <v>32.326999999999998</v>
       </c>
       <c r="W106" s="10">
         <f t="shared" si="5"/>
-        <v>35.82</v>
-      </c>
-    </row>
-    <row r="107" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>32.326999999999998</v>
+      </c>
+    </row>
+    <row r="107" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B107" s="80" t="s">
         <v>15</v>
       </c>
@@ -6480,11 +6816,11 @@
       </c>
       <c r="D107" s="5">
         <f>SUM(I97,I84:I89,I17:I36,I10:I15,I8,I5:I6,I90,I4)</f>
-        <v>1.6500000000000001</v>
+        <v>4.3929999999999998</v>
       </c>
       <c r="E107" s="5">
         <f>SUM(C107,-D107)</f>
-        <v>16.549999999999994</v>
+        <v>13.806999999999992</v>
       </c>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
@@ -6495,7 +6831,7 @@
       <c r="L107" s="3"/>
       <c r="M107" s="3"/>
     </row>
-    <row r="108" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="80" t="s">
         <v>17</v>
       </c>
@@ -6512,29 +6848,29 @@
         <v>5.5</v>
       </c>
       <c r="F108" s="3"/>
-      <c r="H108" s="94" t="s">
+      <c r="H108" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="I108" s="95"/>
-      <c r="J108" s="94">
+      <c r="I108" s="121"/>
+      <c r="J108" s="120">
         <f>H103-I103</f>
-        <v>35.82</v>
-      </c>
-      <c r="K108" s="95"/>
-      <c r="L108" s="95"/>
-      <c r="M108" s="95"/>
-      <c r="N108" s="95"/>
-      <c r="O108" s="95"/>
-      <c r="P108" s="95"/>
-      <c r="Q108" s="95"/>
-      <c r="R108" s="95"/>
-      <c r="S108" s="95"/>
-      <c r="T108" s="95"/>
-      <c r="U108" s="95"/>
-      <c r="V108" s="95"/>
-      <c r="W108" s="96"/>
-    </row>
-    <row r="109" spans="2:23" x14ac:dyDescent="0.25">
+        <v>32.326999999999998</v>
+      </c>
+      <c r="K108" s="121"/>
+      <c r="L108" s="121"/>
+      <c r="M108" s="121"/>
+      <c r="N108" s="121"/>
+      <c r="O108" s="121"/>
+      <c r="P108" s="121"/>
+      <c r="Q108" s="121"/>
+      <c r="R108" s="121"/>
+      <c r="S108" s="121"/>
+      <c r="T108" s="121"/>
+      <c r="U108" s="121"/>
+      <c r="V108" s="121"/>
+      <c r="W108" s="122"/>
+    </row>
+    <row r="109" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
@@ -6548,7 +6884,7 @@
       <c r="L109" s="3"/>
       <c r="M109" s="3"/>
     </row>
-    <row r="110" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -6562,7 +6898,7 @@
       <c r="L110" s="3"/>
       <c r="M110" s="3"/>
     </row>
-    <row r="111" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
@@ -6576,42 +6912,48 @@
       <c r="L111" s="3"/>
       <c r="M111" s="3"/>
     </row>
-    <row r="112" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B117" s="7"/>
     </row>
-    <row r="118" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B118" s="7"/>
     </row>
-    <row r="119" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B119" s="7"/>
     </row>
-    <row r="120" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B124" s="7"/>
     </row>
-    <row r="125" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B125" s="7"/>
     </row>
-    <row r="126" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B126" s="7"/>
     </row>
-    <row r="127" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B127" s="7"/>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="J108:W108"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="C41:C83"/>
+    <mergeCell ref="C20:C36"/>
+    <mergeCell ref="C94:C95"/>
     <mergeCell ref="B41:B91"/>
     <mergeCell ref="C84:C89"/>
     <mergeCell ref="J2:W2"/>
@@ -6624,12 +6966,6 @@
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="B92:B96"/>
     <mergeCell ref="B97:B102"/>
-    <mergeCell ref="J108:W108"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="C41:C83"/>
-    <mergeCell ref="C20:C36"/>
-    <mergeCell ref="C94:C95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6643,7 +6979,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6655,7 +6991,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado excel + screenshot 3 diciembre
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
@@ -521,7 +521,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -582,6 +582,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="39">
     <border>
@@ -1093,7 +1099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1369,6 +1375,39 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1444,37 +1483,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1600,34 +1609,34 @@
                   <c:v>32.326999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>30.826999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2065,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98:M100"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N81" sqref="N81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2095,22 +2104,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="98" t="s">
+      <c r="J2" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="99"/>
-      <c r="W2" s="100"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="110"/>
+      <c r="V2" s="110"/>
+      <c r="W2" s="111"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
@@ -2181,7 +2190,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="115" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="89" t="s">
@@ -2248,7 +2257,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="105"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="46" t="s">
         <v>59</v>
       </c>
@@ -2311,7 +2320,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="105"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="46" t="s">
         <v>75</v>
       </c>
@@ -2342,7 +2351,9 @@
       <c r="M6" s="48">
         <v>0.96</v>
       </c>
-      <c r="N6" s="28"/>
+      <c r="N6" s="48">
+        <v>0</v>
+      </c>
       <c r="O6" s="28"/>
       <c r="P6" s="28"/>
       <c r="Q6" s="19"/>
@@ -2354,8 +2365,8 @@
       <c r="W6" s="20"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="105"/>
-      <c r="C7" s="113" t="s">
+      <c r="B7" s="116"/>
+      <c r="C7" s="124" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="42" t="s">
@@ -2387,7 +2398,9 @@
       <c r="M7" s="71">
         <v>0</v>
       </c>
-      <c r="N7" s="28"/>
+      <c r="N7" s="71">
+        <v>0</v>
+      </c>
       <c r="O7" s="28"/>
       <c r="P7" s="28"/>
       <c r="Q7" s="19"/>
@@ -2399,8 +2412,8 @@
       <c r="W7" s="20"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="105"/>
-      <c r="C8" s="113"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="124"/>
       <c r="D8" s="46" t="s">
         <v>62</v>
       </c>
@@ -2430,7 +2443,9 @@
       <c r="M8" s="71">
         <v>0</v>
       </c>
-      <c r="N8" s="28"/>
+      <c r="N8" s="131">
+        <v>0</v>
+      </c>
       <c r="O8" s="28"/>
       <c r="P8" s="28"/>
       <c r="Q8" s="19"/>
@@ -2442,8 +2457,8 @@
       <c r="W8" s="20"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="109"/>
-      <c r="C9" s="114"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="125"/>
       <c r="D9" s="43" t="s">
         <v>63</v>
       </c>
@@ -2473,7 +2488,9 @@
       <c r="M9" s="72">
         <v>0</v>
       </c>
-      <c r="N9" s="32"/>
+      <c r="N9" s="72">
+        <v>0</v>
+      </c>
       <c r="O9" s="32"/>
       <c r="P9" s="32"/>
       <c r="Q9" s="21"/>
@@ -2485,7 +2502,7 @@
       <c r="W9" s="22"/>
     </row>
     <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="117" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="51" t="s">
@@ -2515,10 +2532,12 @@
       <c r="L10" s="73">
         <v>0</v>
       </c>
-      <c r="M10" s="128">
+      <c r="M10" s="95">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="N10" s="35"/>
+      <c r="N10" s="95">
+        <v>0</v>
+      </c>
       <c r="O10" s="35"/>
       <c r="P10" s="35"/>
       <c r="Q10" s="35"/>
@@ -2530,7 +2549,7 @@
       <c r="W10" s="24"/>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="107"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="46" t="s">
         <v>66</v>
       </c>
@@ -2561,7 +2580,9 @@
       <c r="M11" s="71">
         <v>0</v>
       </c>
-      <c r="N11" s="28"/>
+      <c r="N11" s="71">
+        <v>0</v>
+      </c>
       <c r="O11" s="28"/>
       <c r="P11" s="28"/>
       <c r="Q11" s="28"/>
@@ -2573,7 +2594,7 @@
       <c r="W11" s="58"/>
     </row>
     <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="107"/>
+      <c r="B12" s="118"/>
       <c r="C12" s="46" t="s">
         <v>67</v>
       </c>
@@ -2604,7 +2625,9 @@
       <c r="M12" s="71">
         <v>0</v>
       </c>
-      <c r="N12" s="28"/>
+      <c r="N12" s="71">
+        <v>0</v>
+      </c>
       <c r="O12" s="28"/>
       <c r="P12" s="28"/>
       <c r="Q12" s="28"/>
@@ -2616,7 +2639,7 @@
       <c r="W12" s="58"/>
     </row>
     <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="108"/>
+      <c r="B13" s="119"/>
       <c r="C13" s="45" t="s">
         <v>120</v>
       </c>
@@ -2647,7 +2670,9 @@
       <c r="M13" s="74">
         <v>0</v>
       </c>
-      <c r="N13" s="31"/>
+      <c r="N13" s="74">
+        <v>0</v>
+      </c>
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
       <c r="Q13" s="31"/>
@@ -2659,7 +2684,7 @@
       <c r="W13" s="69"/>
     </row>
     <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="108"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="45" t="s">
         <v>118</v>
       </c>
@@ -2690,7 +2715,9 @@
       <c r="M14" s="74">
         <v>0</v>
       </c>
-      <c r="N14" s="31"/>
+      <c r="N14" s="74">
+        <v>0</v>
+      </c>
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
       <c r="Q14" s="31"/>
@@ -2702,7 +2729,7 @@
       <c r="W14" s="69"/>
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="108"/>
+      <c r="B15" s="119"/>
       <c r="C15" s="45" t="s">
         <v>68</v>
       </c>
@@ -2733,7 +2760,9 @@
       <c r="M15" s="74">
         <v>0</v>
       </c>
-      <c r="N15" s="31"/>
+      <c r="N15" s="74">
+        <v>0</v>
+      </c>
       <c r="O15" s="31"/>
       <c r="P15" s="31"/>
       <c r="Q15" s="31"/>
@@ -2745,7 +2774,7 @@
       <c r="W15" s="69"/>
     </row>
     <row r="16" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="115" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="65" t="s">
@@ -2810,7 +2839,7 @@
       </c>
     </row>
     <row r="17" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="105"/>
+      <c r="B17" s="116"/>
       <c r="C17" s="46" t="s">
         <v>36</v>
       </c>
@@ -2841,7 +2870,9 @@
       <c r="M17" s="48">
         <v>1.083</v>
       </c>
-      <c r="N17" s="28"/>
+      <c r="N17" s="48">
+        <v>0</v>
+      </c>
       <c r="O17" s="28"/>
       <c r="P17" s="29"/>
       <c r="Q17" s="29"/>
@@ -2853,8 +2884,8 @@
       <c r="W17" s="30"/>
     </row>
     <row r="18" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="105"/>
-      <c r="C18" s="112" t="s">
+      <c r="B18" s="116"/>
+      <c r="C18" s="123" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="46" t="s">
@@ -2886,7 +2917,9 @@
       <c r="M18" s="71">
         <v>0</v>
       </c>
-      <c r="N18" s="28"/>
+      <c r="N18" s="71">
+        <v>0</v>
+      </c>
       <c r="O18" s="28"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
@@ -2898,8 +2931,8 @@
       <c r="W18" s="30"/>
     </row>
     <row r="19" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="105"/>
-      <c r="C19" s="112"/>
+      <c r="B19" s="116"/>
+      <c r="C19" s="123"/>
       <c r="D19" s="46" t="s">
         <v>39</v>
       </c>
@@ -2929,7 +2962,9 @@
       <c r="M19" s="48">
         <v>0.15</v>
       </c>
-      <c r="N19" s="28"/>
+      <c r="N19" s="48">
+        <v>0</v>
+      </c>
       <c r="O19" s="28"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="29"/>
@@ -2941,8 +2976,8 @@
       <c r="W19" s="30"/>
     </row>
     <row r="20" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="105"/>
-      <c r="C20" s="126" t="s">
+      <c r="B20" s="116"/>
+      <c r="C20" s="104" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="46" t="s">
@@ -2960,7 +2995,7 @@
       </c>
       <c r="I20" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J20" s="71">
         <v>0</v>
@@ -2974,7 +3009,9 @@
       <c r="M20" s="71">
         <v>0</v>
       </c>
-      <c r="N20" s="28"/>
+      <c r="N20" s="48">
+        <v>1.1499999999999999</v>
+      </c>
       <c r="O20" s="28"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="29"/>
@@ -2986,8 +3023,8 @@
       <c r="W20" s="30"/>
     </row>
     <row r="21" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="105"/>
-      <c r="C21" s="126"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="104"/>
       <c r="D21" s="46" t="s">
         <v>34</v>
       </c>
@@ -3017,7 +3054,9 @@
       <c r="M21" s="71">
         <v>0</v>
       </c>
-      <c r="N21" s="28"/>
+      <c r="N21" s="71">
+        <v>0</v>
+      </c>
       <c r="O21" s="28"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="29"/>
@@ -3029,8 +3068,8 @@
       <c r="W21" s="30"/>
     </row>
     <row r="22" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="105"/>
-      <c r="C22" s="126"/>
+      <c r="B22" s="116"/>
+      <c r="C22" s="104"/>
       <c r="D22" s="46" t="s">
         <v>35</v>
       </c>
@@ -3046,7 +3085,7 @@
       </c>
       <c r="I22" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="J22" s="71">
         <v>0</v>
@@ -3060,7 +3099,9 @@
       <c r="M22" s="71">
         <v>0</v>
       </c>
-      <c r="N22" s="28"/>
+      <c r="N22" s="94">
+        <v>0.35</v>
+      </c>
       <c r="O22" s="28"/>
       <c r="P22" s="29"/>
       <c r="Q22" s="29"/>
@@ -3072,8 +3113,8 @@
       <c r="W22" s="30"/>
     </row>
     <row r="23" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="105"/>
-      <c r="C23" s="126"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="104"/>
       <c r="D23" s="46" t="s">
         <v>40</v>
       </c>
@@ -3103,7 +3144,9 @@
       <c r="M23" s="71">
         <v>0</v>
       </c>
-      <c r="N23" s="28"/>
+      <c r="N23" s="71">
+        <v>0</v>
+      </c>
       <c r="O23" s="28"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="29"/>
@@ -3115,8 +3158,8 @@
       <c r="W23" s="30"/>
     </row>
     <row r="24" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="105"/>
-      <c r="C24" s="126"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="104"/>
       <c r="D24" s="46" t="s">
         <v>41</v>
       </c>
@@ -3146,7 +3189,9 @@
       <c r="M24" s="71">
         <v>0</v>
       </c>
-      <c r="N24" s="28"/>
+      <c r="N24" s="71">
+        <v>0</v>
+      </c>
       <c r="O24" s="28"/>
       <c r="P24" s="29"/>
       <c r="Q24" s="29"/>
@@ -3158,8 +3203,8 @@
       <c r="W24" s="30"/>
     </row>
     <row r="25" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="105"/>
-      <c r="C25" s="126"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="104"/>
       <c r="D25" s="46" t="s">
         <v>42</v>
       </c>
@@ -3189,7 +3234,9 @@
       <c r="M25" s="71">
         <v>0</v>
       </c>
-      <c r="N25" s="28"/>
+      <c r="N25" s="71">
+        <v>0</v>
+      </c>
       <c r="O25" s="28"/>
       <c r="P25" s="29"/>
       <c r="Q25" s="29"/>
@@ -3201,8 +3248,8 @@
       <c r="W25" s="30"/>
     </row>
     <row r="26" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="105"/>
-      <c r="C26" s="126"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="104"/>
       <c r="D26" s="46" t="s">
         <v>43</v>
       </c>
@@ -3232,7 +3279,9 @@
       <c r="M26" s="71">
         <v>0</v>
       </c>
-      <c r="N26" s="28"/>
+      <c r="N26" s="71">
+        <v>0</v>
+      </c>
       <c r="O26" s="28"/>
       <c r="P26" s="29"/>
       <c r="Q26" s="29"/>
@@ -3244,8 +3293,8 @@
       <c r="W26" s="30"/>
     </row>
     <row r="27" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="105"/>
-      <c r="C27" s="126"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="104"/>
       <c r="D27" s="46" t="s">
         <v>44</v>
       </c>
@@ -3275,7 +3324,9 @@
       <c r="M27" s="71">
         <v>0</v>
       </c>
-      <c r="N27" s="28"/>
+      <c r="N27" s="71">
+        <v>0</v>
+      </c>
       <c r="O27" s="28"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="29"/>
@@ -3287,8 +3338,8 @@
       <c r="W27" s="30"/>
     </row>
     <row r="28" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="105"/>
-      <c r="C28" s="126"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="104"/>
       <c r="D28" s="46" t="s">
         <v>45</v>
       </c>
@@ -3318,7 +3369,9 @@
       <c r="M28" s="71">
         <v>0</v>
       </c>
-      <c r="N28" s="28"/>
+      <c r="N28" s="71">
+        <v>0</v>
+      </c>
       <c r="O28" s="28"/>
       <c r="P28" s="29"/>
       <c r="Q28" s="29"/>
@@ -3330,8 +3383,8 @@
       <c r="W28" s="30"/>
     </row>
     <row r="29" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="105"/>
-      <c r="C29" s="126"/>
+      <c r="B29" s="116"/>
+      <c r="C29" s="104"/>
       <c r="D29" s="46" t="s">
         <v>46</v>
       </c>
@@ -3361,7 +3414,9 @@
       <c r="M29" s="71">
         <v>0</v>
       </c>
-      <c r="N29" s="28"/>
+      <c r="N29" s="71">
+        <v>0</v>
+      </c>
       <c r="O29" s="28"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="29"/>
@@ -3373,8 +3428,8 @@
       <c r="W29" s="30"/>
     </row>
     <row r="30" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="105"/>
-      <c r="C30" s="126"/>
+      <c r="B30" s="116"/>
+      <c r="C30" s="104"/>
       <c r="D30" s="46" t="s">
         <v>47</v>
       </c>
@@ -3404,7 +3459,9 @@
       <c r="M30" s="71">
         <v>0</v>
       </c>
-      <c r="N30" s="28"/>
+      <c r="N30" s="71">
+        <v>0</v>
+      </c>
       <c r="O30" s="28"/>
       <c r="P30" s="29"/>
       <c r="Q30" s="29"/>
@@ -3416,8 +3473,8 @@
       <c r="W30" s="30"/>
     </row>
     <row r="31" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="105"/>
-      <c r="C31" s="126"/>
+      <c r="B31" s="116"/>
+      <c r="C31" s="104"/>
       <c r="D31" s="46" t="s">
         <v>48</v>
       </c>
@@ -3447,7 +3504,9 @@
       <c r="M31" s="71">
         <v>0</v>
       </c>
-      <c r="N31" s="28"/>
+      <c r="N31" s="71">
+        <v>0</v>
+      </c>
       <c r="O31" s="28"/>
       <c r="P31" s="29"/>
       <c r="Q31" s="29"/>
@@ -3459,8 +3518,8 @@
       <c r="W31" s="30"/>
     </row>
     <row r="32" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="105"/>
-      <c r="C32" s="126"/>
+      <c r="B32" s="116"/>
+      <c r="C32" s="104"/>
       <c r="D32" s="46" t="s">
         <v>49</v>
       </c>
@@ -3490,7 +3549,9 @@
       <c r="M32" s="71">
         <v>0</v>
       </c>
-      <c r="N32" s="28"/>
+      <c r="N32" s="71">
+        <v>0</v>
+      </c>
       <c r="O32" s="28"/>
       <c r="P32" s="29"/>
       <c r="Q32" s="29"/>
@@ -3502,8 +3563,8 @@
       <c r="W32" s="30"/>
     </row>
     <row r="33" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="105"/>
-      <c r="C33" s="126"/>
+      <c r="B33" s="116"/>
+      <c r="C33" s="104"/>
       <c r="D33" s="46" t="s">
         <v>50</v>
       </c>
@@ -3533,7 +3594,9 @@
       <c r="M33" s="71">
         <v>0</v>
       </c>
-      <c r="N33" s="28"/>
+      <c r="N33" s="71">
+        <v>0</v>
+      </c>
       <c r="O33" s="28"/>
       <c r="P33" s="29"/>
       <c r="Q33" s="29"/>
@@ -3545,8 +3608,8 @@
       <c r="W33" s="30"/>
     </row>
     <row r="34" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="105"/>
-      <c r="C34" s="126"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="104"/>
       <c r="D34" s="46" t="s">
         <v>51</v>
       </c>
@@ -3576,7 +3639,9 @@
       <c r="M34" s="71">
         <v>0</v>
       </c>
-      <c r="N34" s="28"/>
+      <c r="N34" s="71">
+        <v>0</v>
+      </c>
       <c r="O34" s="28"/>
       <c r="P34" s="29"/>
       <c r="Q34" s="29"/>
@@ -3588,8 +3653,8 @@
       <c r="W34" s="30"/>
     </row>
     <row r="35" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="105"/>
-      <c r="C35" s="126"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="104"/>
       <c r="D35" s="46" t="s">
         <v>52</v>
       </c>
@@ -3619,7 +3684,9 @@
       <c r="M35" s="71">
         <v>0</v>
       </c>
-      <c r="N35" s="28"/>
+      <c r="N35" s="71">
+        <v>0</v>
+      </c>
       <c r="O35" s="28"/>
       <c r="P35" s="29"/>
       <c r="Q35" s="29"/>
@@ -3631,8 +3698,8 @@
       <c r="W35" s="30"/>
     </row>
     <row r="36" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="105"/>
-      <c r="C36" s="126"/>
+      <c r="B36" s="116"/>
+      <c r="C36" s="104"/>
       <c r="D36" s="52" t="s">
         <v>111</v>
       </c>
@@ -3662,7 +3729,9 @@
       <c r="M36" s="71">
         <v>0</v>
       </c>
-      <c r="N36" s="28"/>
+      <c r="N36" s="71">
+        <v>0</v>
+      </c>
       <c r="O36" s="28"/>
       <c r="P36" s="29"/>
       <c r="Q36" s="29"/>
@@ -3674,7 +3743,7 @@
       <c r="W36" s="30"/>
     </row>
     <row r="37" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="105"/>
+      <c r="B37" s="116"/>
       <c r="C37" s="49" t="s">
         <v>53</v>
       </c>
@@ -3705,7 +3774,9 @@
       <c r="M37" s="71">
         <v>0</v>
       </c>
-      <c r="N37" s="28"/>
+      <c r="N37" s="71">
+        <v>0</v>
+      </c>
       <c r="O37" s="28"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="29"/>
@@ -3717,7 +3788,7 @@
       <c r="W37" s="30"/>
     </row>
     <row r="38" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="105"/>
+      <c r="B38" s="116"/>
       <c r="C38" s="49" t="s">
         <v>55</v>
       </c>
@@ -3748,7 +3819,9 @@
       <c r="M38" s="71">
         <v>0</v>
       </c>
-      <c r="N38" s="28"/>
+      <c r="N38" s="71">
+        <v>0</v>
+      </c>
       <c r="O38" s="28"/>
       <c r="P38" s="29"/>
       <c r="Q38" s="29"/>
@@ -3760,7 +3833,7 @@
       <c r="W38" s="30"/>
     </row>
     <row r="39" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="105"/>
+      <c r="B39" s="116"/>
       <c r="C39" s="49" t="s">
         <v>56</v>
       </c>
@@ -3823,7 +3896,7 @@
       </c>
     </row>
     <row r="40" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="105"/>
+      <c r="B40" s="116"/>
       <c r="C40" s="56" t="s">
         <v>112</v>
       </c>
@@ -3854,7 +3927,9 @@
       <c r="M40" s="71">
         <v>0</v>
       </c>
-      <c r="N40" s="28"/>
+      <c r="N40" s="71">
+        <v>0</v>
+      </c>
       <c r="O40" s="28"/>
       <c r="P40" s="29"/>
       <c r="Q40" s="29"/>
@@ -3866,10 +3941,10 @@
       <c r="W40" s="30"/>
     </row>
     <row r="41" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="95" t="s">
+      <c r="B41" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="124" t="s">
+      <c r="C41" s="102" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="50" t="s">
@@ -3933,8 +4008,8 @@
       </c>
     </row>
     <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="96"/>
-      <c r="C42" s="125"/>
+      <c r="B42" s="107"/>
+      <c r="C42" s="103"/>
       <c r="D42" s="49" t="s">
         <v>21</v>
       </c>
@@ -3964,7 +4039,9 @@
       <c r="M42" s="71">
         <v>0</v>
       </c>
-      <c r="N42" s="28"/>
+      <c r="N42" s="71">
+        <v>0</v>
+      </c>
       <c r="O42" s="28"/>
       <c r="P42" s="29"/>
       <c r="Q42" s="29"/>
@@ -3976,8 +4053,8 @@
       <c r="W42" s="30"/>
     </row>
     <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="96"/>
-      <c r="C43" s="125"/>
+      <c r="B43" s="107"/>
+      <c r="C43" s="103"/>
       <c r="D43" s="49" t="s">
         <v>22</v>
       </c>
@@ -4007,7 +4084,9 @@
       <c r="M43" s="71">
         <v>0</v>
       </c>
-      <c r="N43" s="28"/>
+      <c r="N43" s="71">
+        <v>0</v>
+      </c>
       <c r="O43" s="28"/>
       <c r="P43" s="29"/>
       <c r="Q43" s="29"/>
@@ -4019,8 +4098,8 @@
       <c r="W43" s="30"/>
     </row>
     <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="96"/>
-      <c r="C44" s="125"/>
+      <c r="B44" s="107"/>
+      <c r="C44" s="103"/>
       <c r="D44" s="49" t="s">
         <v>23</v>
       </c>
@@ -4050,7 +4129,9 @@
       <c r="M44" s="71">
         <v>0</v>
       </c>
-      <c r="N44" s="28"/>
+      <c r="N44" s="71">
+        <v>0</v>
+      </c>
       <c r="O44" s="28"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="29"/>
@@ -4062,8 +4143,8 @@
       <c r="W44" s="30"/>
     </row>
     <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="96"/>
-      <c r="C45" s="125"/>
+      <c r="B45" s="107"/>
+      <c r="C45" s="103"/>
       <c r="D45" s="49" t="s">
         <v>24</v>
       </c>
@@ -4093,7 +4174,9 @@
       <c r="M45" s="71">
         <v>0</v>
       </c>
-      <c r="N45" s="28"/>
+      <c r="N45" s="71">
+        <v>0</v>
+      </c>
       <c r="O45" s="28"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="29"/>
@@ -4105,8 +4188,8 @@
       <c r="W45" s="30"/>
     </row>
     <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="96"/>
-      <c r="C46" s="125"/>
+      <c r="B46" s="107"/>
+      <c r="C46" s="103"/>
       <c r="D46" s="49" t="s">
         <v>25</v>
       </c>
@@ -4136,7 +4219,9 @@
       <c r="M46" s="71">
         <v>0</v>
       </c>
-      <c r="N46" s="28"/>
+      <c r="N46" s="71">
+        <v>0</v>
+      </c>
       <c r="O46" s="28"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
@@ -4148,8 +4233,8 @@
       <c r="W46" s="30"/>
     </row>
     <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="96"/>
-      <c r="C47" s="125"/>
+      <c r="B47" s="107"/>
+      <c r="C47" s="103"/>
       <c r="D47" s="49" t="s">
         <v>26</v>
       </c>
@@ -4179,7 +4264,9 @@
       <c r="M47" s="71">
         <v>0</v>
       </c>
-      <c r="N47" s="28"/>
+      <c r="N47" s="71">
+        <v>0</v>
+      </c>
       <c r="O47" s="28"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
@@ -4191,8 +4278,8 @@
       <c r="W47" s="30"/>
     </row>
     <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="96"/>
-      <c r="C48" s="125"/>
+      <c r="B48" s="107"/>
+      <c r="C48" s="103"/>
       <c r="D48" s="49" t="s">
         <v>27</v>
       </c>
@@ -4222,7 +4309,9 @@
       <c r="M48" s="71">
         <v>0</v>
       </c>
-      <c r="N48" s="28"/>
+      <c r="N48" s="71">
+        <v>0</v>
+      </c>
       <c r="O48" s="28"/>
       <c r="P48" s="29"/>
       <c r="Q48" s="29"/>
@@ -4234,8 +4323,8 @@
       <c r="W48" s="30"/>
     </row>
     <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="96"/>
-      <c r="C49" s="125"/>
+      <c r="B49" s="107"/>
+      <c r="C49" s="103"/>
       <c r="D49" s="49" t="s">
         <v>28</v>
       </c>
@@ -4265,7 +4354,9 @@
       <c r="M49" s="71">
         <v>0</v>
       </c>
-      <c r="N49" s="28"/>
+      <c r="N49" s="71">
+        <v>0</v>
+      </c>
       <c r="O49" s="28"/>
       <c r="P49" s="29"/>
       <c r="Q49" s="29"/>
@@ -4277,8 +4368,8 @@
       <c r="W49" s="30"/>
     </row>
     <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="96"/>
-      <c r="C50" s="125"/>
+      <c r="B50" s="107"/>
+      <c r="C50" s="103"/>
       <c r="D50" s="49" t="s">
         <v>29</v>
       </c>
@@ -4308,7 +4399,9 @@
       <c r="M50" s="71">
         <v>0</v>
       </c>
-      <c r="N50" s="28"/>
+      <c r="N50" s="71">
+        <v>0</v>
+      </c>
       <c r="O50" s="28"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
@@ -4320,8 +4413,8 @@
       <c r="W50" s="30"/>
     </row>
     <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="96"/>
-      <c r="C51" s="125"/>
+      <c r="B51" s="107"/>
+      <c r="C51" s="103"/>
       <c r="D51" s="49" t="s">
         <v>30</v>
       </c>
@@ -4351,7 +4444,9 @@
       <c r="M51" s="71">
         <v>0</v>
       </c>
-      <c r="N51" s="28"/>
+      <c r="N51" s="71">
+        <v>0</v>
+      </c>
       <c r="O51" s="28"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="29"/>
@@ -4363,8 +4458,8 @@
       <c r="W51" s="30"/>
     </row>
     <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="96"/>
-      <c r="C52" s="125"/>
+      <c r="B52" s="107"/>
+      <c r="C52" s="103"/>
       <c r="D52" s="49" t="s">
         <v>31</v>
       </c>
@@ -4394,7 +4489,9 @@
       <c r="M52" s="71">
         <v>0</v>
       </c>
-      <c r="N52" s="28"/>
+      <c r="N52" s="71">
+        <v>0</v>
+      </c>
       <c r="O52" s="28"/>
       <c r="P52" s="29"/>
       <c r="Q52" s="29"/>
@@ -4406,8 +4503,8 @@
       <c r="W52" s="30"/>
     </row>
     <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="96"/>
-      <c r="C53" s="125"/>
+      <c r="B53" s="107"/>
+      <c r="C53" s="103"/>
       <c r="D53" s="49" t="s">
         <v>77</v>
       </c>
@@ -4437,7 +4534,9 @@
       <c r="M53" s="71">
         <v>0</v>
       </c>
-      <c r="N53" s="28"/>
+      <c r="N53" s="71">
+        <v>0</v>
+      </c>
       <c r="O53" s="28"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="29"/>
@@ -4449,8 +4548,8 @@
       <c r="W53" s="30"/>
     </row>
     <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="96"/>
-      <c r="C54" s="125"/>
+      <c r="B54" s="107"/>
+      <c r="C54" s="103"/>
       <c r="D54" s="49" t="s">
         <v>78</v>
       </c>
@@ -4480,7 +4579,9 @@
       <c r="M54" s="71">
         <v>0</v>
       </c>
-      <c r="N54" s="28"/>
+      <c r="N54" s="71">
+        <v>0</v>
+      </c>
       <c r="O54" s="28"/>
       <c r="P54" s="29"/>
       <c r="Q54" s="29"/>
@@ -4492,8 +4593,8 @@
       <c r="W54" s="30"/>
     </row>
     <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="96"/>
-      <c r="C55" s="125"/>
+      <c r="B55" s="107"/>
+      <c r="C55" s="103"/>
       <c r="D55" s="49" t="s">
         <v>78</v>
       </c>
@@ -4523,7 +4624,9 @@
       <c r="M55" s="71">
         <v>0</v>
       </c>
-      <c r="N55" s="28"/>
+      <c r="N55" s="71">
+        <v>0</v>
+      </c>
       <c r="O55" s="28"/>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
@@ -4535,8 +4638,8 @@
       <c r="W55" s="30"/>
     </row>
     <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="96"/>
-      <c r="C56" s="125"/>
+      <c r="B56" s="107"/>
+      <c r="C56" s="103"/>
       <c r="D56" s="49" t="s">
         <v>79</v>
       </c>
@@ -4566,7 +4669,9 @@
       <c r="M56" s="71">
         <v>0</v>
       </c>
-      <c r="N56" s="28"/>
+      <c r="N56" s="71">
+        <v>0</v>
+      </c>
       <c r="O56" s="28"/>
       <c r="P56" s="29"/>
       <c r="Q56" s="29"/>
@@ -4578,8 +4683,8 @@
       <c r="W56" s="30"/>
     </row>
     <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="96"/>
-      <c r="C57" s="125"/>
+      <c r="B57" s="107"/>
+      <c r="C57" s="103"/>
       <c r="D57" s="49" t="s">
         <v>80</v>
       </c>
@@ -4609,7 +4714,9 @@
       <c r="M57" s="71">
         <v>0</v>
       </c>
-      <c r="N57" s="28"/>
+      <c r="N57" s="71">
+        <v>0</v>
+      </c>
       <c r="O57" s="28"/>
       <c r="P57" s="29"/>
       <c r="Q57" s="29"/>
@@ -4621,8 +4728,8 @@
       <c r="W57" s="30"/>
     </row>
     <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="96"/>
-      <c r="C58" s="125"/>
+      <c r="B58" s="107"/>
+      <c r="C58" s="103"/>
       <c r="D58" s="49" t="s">
         <v>81</v>
       </c>
@@ -4652,7 +4759,9 @@
       <c r="M58" s="71">
         <v>0</v>
       </c>
-      <c r="N58" s="28"/>
+      <c r="N58" s="71">
+        <v>0</v>
+      </c>
       <c r="O58" s="28"/>
       <c r="P58" s="29"/>
       <c r="Q58" s="29"/>
@@ -4664,8 +4773,8 @@
       <c r="W58" s="30"/>
     </row>
     <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="96"/>
-      <c r="C59" s="125"/>
+      <c r="B59" s="107"/>
+      <c r="C59" s="103"/>
       <c r="D59" s="49" t="s">
         <v>82</v>
       </c>
@@ -4695,7 +4804,9 @@
       <c r="M59" s="71">
         <v>0</v>
       </c>
-      <c r="N59" s="28"/>
+      <c r="N59" s="71">
+        <v>0</v>
+      </c>
       <c r="O59" s="28"/>
       <c r="P59" s="29"/>
       <c r="Q59" s="29"/>
@@ -4707,8 +4818,8 @@
       <c r="W59" s="30"/>
     </row>
     <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="96"/>
-      <c r="C60" s="125"/>
+      <c r="B60" s="107"/>
+      <c r="C60" s="103"/>
       <c r="D60" s="49" t="s">
         <v>83</v>
       </c>
@@ -4738,7 +4849,9 @@
       <c r="M60" s="71">
         <v>0</v>
       </c>
-      <c r="N60" s="28"/>
+      <c r="N60" s="71">
+        <v>0</v>
+      </c>
       <c r="O60" s="28"/>
       <c r="P60" s="29"/>
       <c r="Q60" s="29"/>
@@ -4750,8 +4863,8 @@
       <c r="W60" s="30"/>
     </row>
     <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="96"/>
-      <c r="C61" s="125"/>
+      <c r="B61" s="107"/>
+      <c r="C61" s="103"/>
       <c r="D61" s="49" t="s">
         <v>84</v>
       </c>
@@ -4781,7 +4894,9 @@
       <c r="M61" s="71">
         <v>0</v>
       </c>
-      <c r="N61" s="28"/>
+      <c r="N61" s="71">
+        <v>0</v>
+      </c>
       <c r="O61" s="28"/>
       <c r="P61" s="29"/>
       <c r="Q61" s="29"/>
@@ -4793,8 +4908,8 @@
       <c r="W61" s="30"/>
     </row>
     <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="96"/>
-      <c r="C62" s="125"/>
+      <c r="B62" s="107"/>
+      <c r="C62" s="103"/>
       <c r="D62" s="49" t="s">
         <v>85</v>
       </c>
@@ -4824,7 +4939,9 @@
       <c r="M62" s="71">
         <v>0</v>
       </c>
-      <c r="N62" s="28"/>
+      <c r="N62" s="71">
+        <v>0</v>
+      </c>
       <c r="O62" s="28"/>
       <c r="P62" s="29"/>
       <c r="Q62" s="29"/>
@@ -4836,8 +4953,8 @@
       <c r="W62" s="30"/>
     </row>
     <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="96"/>
-      <c r="C63" s="125"/>
+      <c r="B63" s="107"/>
+      <c r="C63" s="103"/>
       <c r="D63" s="49" t="s">
         <v>86</v>
       </c>
@@ -4867,7 +4984,9 @@
       <c r="M63" s="71">
         <v>0</v>
       </c>
-      <c r="N63" s="28"/>
+      <c r="N63" s="71">
+        <v>0</v>
+      </c>
       <c r="O63" s="28"/>
       <c r="P63" s="29"/>
       <c r="Q63" s="29"/>
@@ -4879,8 +4998,8 @@
       <c r="W63" s="30"/>
     </row>
     <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="96"/>
-      <c r="C64" s="125"/>
+      <c r="B64" s="107"/>
+      <c r="C64" s="103"/>
       <c r="D64" s="49" t="s">
         <v>87</v>
       </c>
@@ -4910,7 +5029,9 @@
       <c r="M64" s="71">
         <v>0</v>
       </c>
-      <c r="N64" s="28"/>
+      <c r="N64" s="71">
+        <v>0</v>
+      </c>
       <c r="O64" s="28"/>
       <c r="P64" s="29"/>
       <c r="Q64" s="29"/>
@@ -4922,8 +5043,8 @@
       <c r="W64" s="30"/>
     </row>
     <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="96"/>
-      <c r="C65" s="125"/>
+      <c r="B65" s="107"/>
+      <c r="C65" s="103"/>
       <c r="D65" s="49" t="s">
         <v>88</v>
       </c>
@@ -4953,7 +5074,9 @@
       <c r="M65" s="71">
         <v>0</v>
       </c>
-      <c r="N65" s="28"/>
+      <c r="N65" s="71">
+        <v>0</v>
+      </c>
       <c r="O65" s="28"/>
       <c r="P65" s="29"/>
       <c r="Q65" s="29"/>
@@ -4965,8 +5088,8 @@
       <c r="W65" s="30"/>
     </row>
     <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="96"/>
-      <c r="C66" s="125"/>
+      <c r="B66" s="107"/>
+      <c r="C66" s="103"/>
       <c r="D66" s="49" t="s">
         <v>89</v>
       </c>
@@ -4996,7 +5119,9 @@
       <c r="M66" s="71">
         <v>0</v>
       </c>
-      <c r="N66" s="28"/>
+      <c r="N66" s="71">
+        <v>0</v>
+      </c>
       <c r="O66" s="28"/>
       <c r="P66" s="29"/>
       <c r="Q66" s="29"/>
@@ -5008,8 +5133,8 @@
       <c r="W66" s="30"/>
     </row>
     <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="96"/>
-      <c r="C67" s="125"/>
+      <c r="B67" s="107"/>
+      <c r="C67" s="103"/>
       <c r="D67" s="49" t="s">
         <v>94</v>
       </c>
@@ -5039,7 +5164,9 @@
       <c r="M67" s="71">
         <v>0</v>
       </c>
-      <c r="N67" s="28"/>
+      <c r="N67" s="71">
+        <v>0</v>
+      </c>
       <c r="O67" s="28"/>
       <c r="P67" s="29"/>
       <c r="Q67" s="29"/>
@@ -5051,8 +5178,8 @@
       <c r="W67" s="30"/>
     </row>
     <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="96"/>
-      <c r="C68" s="125"/>
+      <c r="B68" s="107"/>
+      <c r="C68" s="103"/>
       <c r="D68" s="49" t="s">
         <v>95</v>
       </c>
@@ -5082,7 +5209,9 @@
       <c r="M68" s="71">
         <v>0</v>
       </c>
-      <c r="N68" s="28"/>
+      <c r="N68" s="71">
+        <v>0</v>
+      </c>
       <c r="O68" s="28"/>
       <c r="P68" s="29"/>
       <c r="Q68" s="29"/>
@@ -5094,8 +5223,8 @@
       <c r="W68" s="30"/>
     </row>
     <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="96"/>
-      <c r="C69" s="125"/>
+      <c r="B69" s="107"/>
+      <c r="C69" s="103"/>
       <c r="D69" s="49" t="s">
         <v>96</v>
       </c>
@@ -5125,7 +5254,9 @@
       <c r="M69" s="71">
         <v>0</v>
       </c>
-      <c r="N69" s="28"/>
+      <c r="N69" s="71">
+        <v>0</v>
+      </c>
       <c r="O69" s="28"/>
       <c r="P69" s="29"/>
       <c r="Q69" s="29"/>
@@ -5137,8 +5268,8 @@
       <c r="W69" s="30"/>
     </row>
     <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="96"/>
-      <c r="C70" s="125"/>
+      <c r="B70" s="107"/>
+      <c r="C70" s="103"/>
       <c r="D70" s="49" t="s">
         <v>97</v>
       </c>
@@ -5168,7 +5299,9 @@
       <c r="M70" s="71">
         <v>0</v>
       </c>
-      <c r="N70" s="28"/>
+      <c r="N70" s="71">
+        <v>0</v>
+      </c>
       <c r="O70" s="28"/>
       <c r="P70" s="29"/>
       <c r="Q70" s="29"/>
@@ -5180,8 +5313,8 @@
       <c r="W70" s="30"/>
     </row>
     <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="96"/>
-      <c r="C71" s="125"/>
+      <c r="B71" s="107"/>
+      <c r="C71" s="103"/>
       <c r="D71" s="49" t="s">
         <v>98</v>
       </c>
@@ -5211,7 +5344,9 @@
       <c r="M71" s="71">
         <v>0</v>
       </c>
-      <c r="N71" s="28"/>
+      <c r="N71" s="71">
+        <v>0</v>
+      </c>
       <c r="O71" s="28"/>
       <c r="P71" s="29"/>
       <c r="Q71" s="29"/>
@@ -5223,8 +5358,8 @@
       <c r="W71" s="30"/>
     </row>
     <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="96"/>
-      <c r="C72" s="125"/>
+      <c r="B72" s="107"/>
+      <c r="C72" s="103"/>
       <c r="D72" s="49" t="s">
         <v>99</v>
       </c>
@@ -5254,7 +5389,9 @@
       <c r="M72" s="71">
         <v>0</v>
       </c>
-      <c r="N72" s="28"/>
+      <c r="N72" s="71">
+        <v>0</v>
+      </c>
       <c r="O72" s="28"/>
       <c r="P72" s="29"/>
       <c r="Q72" s="29"/>
@@ -5266,8 +5403,8 @@
       <c r="W72" s="30"/>
     </row>
     <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="96"/>
-      <c r="C73" s="125"/>
+      <c r="B73" s="107"/>
+      <c r="C73" s="103"/>
       <c r="D73" s="49" t="s">
         <v>100</v>
       </c>
@@ -5297,7 +5434,9 @@
       <c r="M73" s="71">
         <v>0</v>
       </c>
-      <c r="N73" s="28"/>
+      <c r="N73" s="71">
+        <v>0</v>
+      </c>
       <c r="O73" s="28"/>
       <c r="P73" s="29"/>
       <c r="Q73" s="29"/>
@@ -5309,8 +5448,8 @@
       <c r="W73" s="30"/>
     </row>
     <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="96"/>
-      <c r="C74" s="125"/>
+      <c r="B74" s="107"/>
+      <c r="C74" s="103"/>
       <c r="D74" s="49" t="s">
         <v>101</v>
       </c>
@@ -5340,7 +5479,9 @@
       <c r="M74" s="71">
         <v>0</v>
       </c>
-      <c r="N74" s="28"/>
+      <c r="N74" s="71">
+        <v>0</v>
+      </c>
       <c r="O74" s="28"/>
       <c r="P74" s="29"/>
       <c r="Q74" s="29"/>
@@ -5352,8 +5493,8 @@
       <c r="W74" s="30"/>
     </row>
     <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="96"/>
-      <c r="C75" s="125"/>
+      <c r="B75" s="107"/>
+      <c r="C75" s="103"/>
       <c r="D75" s="49" t="s">
         <v>102</v>
       </c>
@@ -5383,7 +5524,9 @@
       <c r="M75" s="71">
         <v>0</v>
       </c>
-      <c r="N75" s="28"/>
+      <c r="N75" s="71">
+        <v>0</v>
+      </c>
       <c r="O75" s="28"/>
       <c r="P75" s="29"/>
       <c r="Q75" s="29"/>
@@ -5395,8 +5538,8 @@
       <c r="W75" s="30"/>
     </row>
     <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="96"/>
-      <c r="C76" s="125"/>
+      <c r="B76" s="107"/>
+      <c r="C76" s="103"/>
       <c r="D76" s="49" t="s">
         <v>103</v>
       </c>
@@ -5426,7 +5569,9 @@
       <c r="M76" s="71">
         <v>0</v>
       </c>
-      <c r="N76" s="28"/>
+      <c r="N76" s="71">
+        <v>0</v>
+      </c>
       <c r="O76" s="28"/>
       <c r="P76" s="29"/>
       <c r="Q76" s="29"/>
@@ -5438,8 +5583,8 @@
       <c r="W76" s="30"/>
     </row>
     <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="96"/>
-      <c r="C77" s="125"/>
+      <c r="B77" s="107"/>
+      <c r="C77" s="103"/>
       <c r="D77" s="49" t="s">
         <v>104</v>
       </c>
@@ -5469,7 +5614,9 @@
       <c r="M77" s="71">
         <v>0</v>
       </c>
-      <c r="N77" s="28"/>
+      <c r="N77" s="71">
+        <v>0</v>
+      </c>
       <c r="O77" s="28"/>
       <c r="P77" s="29"/>
       <c r="Q77" s="29"/>
@@ -5481,8 +5628,8 @@
       <c r="W77" s="30"/>
     </row>
     <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="96"/>
-      <c r="C78" s="125"/>
+      <c r="B78" s="107"/>
+      <c r="C78" s="103"/>
       <c r="D78" s="49" t="s">
         <v>105</v>
       </c>
@@ -5512,7 +5659,9 @@
       <c r="M78" s="71">
         <v>0</v>
       </c>
-      <c r="N78" s="28"/>
+      <c r="N78" s="71">
+        <v>0</v>
+      </c>
       <c r="O78" s="28"/>
       <c r="P78" s="29"/>
       <c r="Q78" s="29"/>
@@ -5524,8 +5673,8 @@
       <c r="W78" s="30"/>
     </row>
     <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="96"/>
-      <c r="C79" s="125"/>
+      <c r="B79" s="107"/>
+      <c r="C79" s="103"/>
       <c r="D79" s="49" t="s">
         <v>106</v>
       </c>
@@ -5555,7 +5704,9 @@
       <c r="M79" s="71">
         <v>0</v>
       </c>
-      <c r="N79" s="28"/>
+      <c r="N79" s="71">
+        <v>0</v>
+      </c>
       <c r="O79" s="28"/>
       <c r="P79" s="29"/>
       <c r="Q79" s="29"/>
@@ -5567,8 +5718,8 @@
       <c r="W79" s="30"/>
     </row>
     <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="96"/>
-      <c r="C80" s="125"/>
+      <c r="B80" s="107"/>
+      <c r="C80" s="103"/>
       <c r="D80" s="49" t="s">
         <v>107</v>
       </c>
@@ -5598,7 +5749,9 @@
       <c r="M80" s="71">
         <v>0</v>
       </c>
-      <c r="N80" s="28"/>
+      <c r="N80" s="71">
+        <v>0</v>
+      </c>
       <c r="O80" s="28"/>
       <c r="P80" s="29"/>
       <c r="Q80" s="29"/>
@@ -5610,8 +5763,8 @@
       <c r="W80" s="30"/>
     </row>
     <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="96"/>
-      <c r="C81" s="125"/>
+      <c r="B81" s="107"/>
+      <c r="C81" s="103"/>
       <c r="D81" s="49" t="s">
         <v>90</v>
       </c>
@@ -5641,7 +5794,9 @@
       <c r="M81" s="71">
         <v>0</v>
       </c>
-      <c r="N81" s="28"/>
+      <c r="N81" s="71">
+        <v>0</v>
+      </c>
       <c r="O81" s="28"/>
       <c r="P81" s="29"/>
       <c r="Q81" s="29"/>
@@ -5653,8 +5808,8 @@
       <c r="W81" s="30"/>
     </row>
     <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="96"/>
-      <c r="C82" s="125"/>
+      <c r="B82" s="107"/>
+      <c r="C82" s="103"/>
       <c r="D82" s="49" t="s">
         <v>91</v>
       </c>
@@ -5684,7 +5839,9 @@
       <c r="M82" s="71">
         <v>0</v>
       </c>
-      <c r="N82" s="28"/>
+      <c r="N82" s="71">
+        <v>0</v>
+      </c>
       <c r="O82" s="28"/>
       <c r="P82" s="29"/>
       <c r="Q82" s="29"/>
@@ -5696,8 +5853,8 @@
       <c r="W82" s="30"/>
     </row>
     <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="96"/>
-      <c r="C83" s="125"/>
+      <c r="B83" s="107"/>
+      <c r="C83" s="103"/>
       <c r="D83" s="49" t="s">
         <v>114</v>
       </c>
@@ -5759,8 +5916,8 @@
       </c>
     </row>
     <row r="84" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="96"/>
-      <c r="C84" s="97" t="s">
+      <c r="B84" s="107"/>
+      <c r="C84" s="108" t="s">
         <v>37</v>
       </c>
       <c r="D84" s="46" t="s">
@@ -5792,7 +5949,9 @@
       <c r="M84" s="71">
         <v>0</v>
       </c>
-      <c r="N84" s="28"/>
+      <c r="N84" s="71">
+        <v>0</v>
+      </c>
       <c r="O84" s="28"/>
       <c r="P84" s="28"/>
       <c r="Q84" s="28"/>
@@ -5804,8 +5963,8 @@
       <c r="W84" s="30"/>
     </row>
     <row r="85" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="96"/>
-      <c r="C85" s="97"/>
+      <c r="B85" s="107"/>
+      <c r="C85" s="108"/>
       <c r="D85" s="52" t="s">
         <v>70</v>
       </c>
@@ -5835,7 +5994,9 @@
       <c r="M85" s="71">
         <v>0</v>
       </c>
-      <c r="N85" s="28"/>
+      <c r="N85" s="71">
+        <v>0</v>
+      </c>
       <c r="O85" s="28"/>
       <c r="P85" s="28"/>
       <c r="Q85" s="28"/>
@@ -5847,8 +6008,8 @@
       <c r="W85" s="30"/>
     </row>
     <row r="86" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="96"/>
-      <c r="C86" s="97"/>
+      <c r="B86" s="107"/>
+      <c r="C86" s="108"/>
       <c r="D86" s="52" t="s">
         <v>71</v>
       </c>
@@ -5878,7 +6039,9 @@
       <c r="M86" s="71">
         <v>0</v>
       </c>
-      <c r="N86" s="28"/>
+      <c r="N86" s="71">
+        <v>0</v>
+      </c>
       <c r="O86" s="28"/>
       <c r="P86" s="28"/>
       <c r="Q86" s="28"/>
@@ -5890,8 +6053,8 @@
       <c r="W86" s="30"/>
     </row>
     <row r="87" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="96"/>
-      <c r="C87" s="97"/>
+      <c r="B87" s="107"/>
+      <c r="C87" s="108"/>
       <c r="D87" s="52" t="s">
         <v>72</v>
       </c>
@@ -5921,7 +6084,9 @@
       <c r="M87" s="71">
         <v>0</v>
       </c>
-      <c r="N87" s="28"/>
+      <c r="N87" s="71">
+        <v>0</v>
+      </c>
       <c r="O87" s="28"/>
       <c r="P87" s="28"/>
       <c r="Q87" s="28"/>
@@ -5933,8 +6098,8 @@
       <c r="W87" s="30"/>
     </row>
     <row r="88" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="96"/>
-      <c r="C88" s="97"/>
+      <c r="B88" s="107"/>
+      <c r="C88" s="108"/>
       <c r="D88" s="52" t="s">
         <v>73</v>
       </c>
@@ -5964,7 +6129,9 @@
       <c r="M88" s="71">
         <v>0</v>
       </c>
-      <c r="N88" s="28"/>
+      <c r="N88" s="71">
+        <v>0</v>
+      </c>
       <c r="O88" s="28"/>
       <c r="P88" s="28"/>
       <c r="Q88" s="28"/>
@@ -5976,8 +6143,8 @@
       <c r="W88" s="58"/>
     </row>
     <row r="89" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="96"/>
-      <c r="C89" s="97"/>
+      <c r="B89" s="107"/>
+      <c r="C89" s="108"/>
       <c r="D89" s="52" t="s">
         <v>74</v>
       </c>
@@ -6007,7 +6174,9 @@
       <c r="M89" s="71">
         <v>0</v>
       </c>
-      <c r="N89" s="28"/>
+      <c r="N89" s="71">
+        <v>0</v>
+      </c>
       <c r="O89" s="28"/>
       <c r="P89" s="28"/>
       <c r="Q89" s="28"/>
@@ -6019,7 +6188,7 @@
       <c r="W89" s="30"/>
     </row>
     <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="96"/>
+      <c r="B90" s="107"/>
       <c r="C90" s="83" t="s">
         <v>125</v>
       </c>
@@ -6082,7 +6251,7 @@
       </c>
     </row>
     <row r="91" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="96"/>
+      <c r="B91" s="107"/>
       <c r="C91" s="75" t="s">
         <v>113</v>
       </c>
@@ -6113,7 +6282,9 @@
       <c r="M91" s="71">
         <v>0</v>
       </c>
-      <c r="N91" s="28"/>
+      <c r="N91" s="71">
+        <v>0</v>
+      </c>
       <c r="O91" s="28"/>
       <c r="P91" s="28"/>
       <c r="Q91" s="28"/>
@@ -6125,7 +6296,7 @@
       <c r="W91" s="30"/>
     </row>
     <row r="92" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="115" t="s">
+      <c r="B92" s="126" t="s">
         <v>92</v>
       </c>
       <c r="C92" s="38" t="s">
@@ -6158,7 +6329,9 @@
       <c r="M92" s="70">
         <v>0</v>
       </c>
-      <c r="N92" s="25"/>
+      <c r="N92" s="70">
+        <v>0</v>
+      </c>
       <c r="O92" s="25"/>
       <c r="P92" s="25"/>
       <c r="Q92" s="25"/>
@@ -6170,7 +6343,7 @@
       <c r="W92" s="67"/>
     </row>
     <row r="93" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="116"/>
+      <c r="B93" s="127"/>
       <c r="C93" s="41" t="s">
         <v>119</v>
       </c>
@@ -6201,7 +6374,9 @@
       <c r="M93" s="73">
         <v>0</v>
       </c>
-      <c r="N93" s="35"/>
+      <c r="N93" s="73">
+        <v>0</v>
+      </c>
       <c r="O93" s="35"/>
       <c r="P93" s="35"/>
       <c r="Q93" s="35"/>
@@ -6213,8 +6388,8 @@
       <c r="W93" s="66"/>
     </row>
     <row r="94" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="117"/>
-      <c r="C94" s="127" t="s">
+      <c r="B94" s="128"/>
+      <c r="C94" s="105" t="s">
         <v>108</v>
       </c>
       <c r="D94" s="42" t="s">
@@ -6246,7 +6421,9 @@
       <c r="M94" s="71">
         <v>0</v>
       </c>
-      <c r="N94" s="28"/>
+      <c r="N94" s="71">
+        <v>0</v>
+      </c>
       <c r="O94" s="28"/>
       <c r="P94" s="28"/>
       <c r="Q94" s="28"/>
@@ -6258,8 +6435,8 @@
       <c r="W94" s="58"/>
     </row>
     <row r="95" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B95" s="118"/>
-      <c r="C95" s="127"/>
+      <c r="B95" s="129"/>
+      <c r="C95" s="105"/>
       <c r="D95" s="42" t="s">
         <v>109</v>
       </c>
@@ -6289,7 +6466,9 @@
       <c r="M95" s="71">
         <v>0</v>
       </c>
-      <c r="N95" s="28"/>
+      <c r="N95" s="71">
+        <v>0</v>
+      </c>
       <c r="O95" s="28"/>
       <c r="P95" s="28"/>
       <c r="Q95" s="28"/>
@@ -6301,7 +6480,7 @@
       <c r="W95" s="58"/>
     </row>
     <row r="96" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="119"/>
+      <c r="B96" s="130"/>
       <c r="C96" s="44" t="s">
         <v>116</v>
       </c>
@@ -6329,10 +6508,12 @@
       <c r="L96" s="72">
         <v>0</v>
       </c>
-      <c r="M96" s="129">
+      <c r="M96" s="96">
         <v>0.75</v>
       </c>
-      <c r="N96" s="32"/>
+      <c r="N96" s="96">
+        <v>0</v>
+      </c>
       <c r="O96" s="32"/>
       <c r="P96" s="32"/>
       <c r="Q96" s="32"/>
@@ -6344,7 +6525,7 @@
       <c r="W96" s="64"/>
     </row>
     <row r="97" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="95" t="s">
+      <c r="B97" s="106" t="s">
         <v>93</v>
       </c>
       <c r="C97" s="63" t="s">
@@ -6377,7 +6558,9 @@
       <c r="M97" s="87">
         <v>0.46700000000000003</v>
       </c>
-      <c r="N97" s="26"/>
+      <c r="N97" s="87">
+        <v>0</v>
+      </c>
       <c r="O97" s="26"/>
       <c r="P97" s="26"/>
       <c r="Q97" s="26"/>
@@ -6389,7 +6572,7 @@
       <c r="W97" s="27"/>
     </row>
     <row r="98" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B98" s="118"/>
+      <c r="B98" s="129"/>
       <c r="C98" s="54" t="s">
         <v>131</v>
       </c>
@@ -6417,10 +6600,12 @@
       <c r="L98" s="71">
         <v>0</v>
       </c>
-      <c r="M98" s="130">
-        <v>0</v>
-      </c>
-      <c r="N98" s="29"/>
+      <c r="M98" s="97">
+        <v>0</v>
+      </c>
+      <c r="N98" s="97">
+        <v>0</v>
+      </c>
       <c r="O98" s="29"/>
       <c r="P98" s="29"/>
       <c r="Q98" s="29"/>
@@ -6432,7 +6617,7 @@
       <c r="W98" s="30"/>
     </row>
     <row r="99" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B99" s="118"/>
+      <c r="B99" s="129"/>
       <c r="C99" s="54" t="s">
         <v>130</v>
       </c>
@@ -6460,10 +6645,12 @@
       <c r="L99" s="71">
         <v>0</v>
       </c>
-      <c r="M99" s="130">
-        <v>0</v>
-      </c>
-      <c r="N99" s="29"/>
+      <c r="M99" s="97">
+        <v>0</v>
+      </c>
+      <c r="N99" s="97">
+        <v>0</v>
+      </c>
       <c r="O99" s="29"/>
       <c r="P99" s="29"/>
       <c r="Q99" s="29"/>
@@ -6475,7 +6662,7 @@
       <c r="W99" s="30"/>
     </row>
     <row r="100" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B100" s="118"/>
+      <c r="B100" s="129"/>
       <c r="C100" s="54" t="s">
         <v>129</v>
       </c>
@@ -6503,10 +6690,12 @@
       <c r="L100" s="71">
         <v>0</v>
       </c>
-      <c r="M100" s="130">
-        <v>0</v>
-      </c>
-      <c r="N100" s="29"/>
+      <c r="M100" s="97">
+        <v>0</v>
+      </c>
+      <c r="N100" s="97">
+        <v>0</v>
+      </c>
       <c r="O100" s="29"/>
       <c r="P100" s="29"/>
       <c r="Q100" s="29"/>
@@ -6518,7 +6707,7 @@
       <c r="W100" s="30"/>
     </row>
     <row r="101" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B101" s="118"/>
+      <c r="B101" s="129"/>
       <c r="C101" s="54" t="s">
         <v>128</v>
       </c>
@@ -6549,7 +6738,9 @@
       <c r="M101" s="71">
         <v>0</v>
       </c>
-      <c r="N101" s="29"/>
+      <c r="N101" s="71">
+        <v>0</v>
+      </c>
       <c r="O101" s="29"/>
       <c r="P101" s="29"/>
       <c r="Q101" s="29"/>
@@ -6561,7 +6752,7 @@
       <c r="W101" s="30"/>
     </row>
     <row r="102" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="119"/>
+      <c r="B102" s="130"/>
       <c r="C102" s="44" t="s">
         <v>127</v>
       </c>
@@ -6592,7 +6783,9 @@
       <c r="M102" s="72">
         <v>0</v>
       </c>
-      <c r="N102" s="32"/>
+      <c r="N102" s="72">
+        <v>0</v>
+      </c>
       <c r="O102" s="32"/>
       <c r="P102" s="33"/>
       <c r="Q102" s="33"/>
@@ -6604,21 +6797,21 @@
       <c r="W102" s="34"/>
     </row>
     <row r="103" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="110" t="s">
+      <c r="B103" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="C103" s="111"/>
-      <c r="D103" s="111"/>
-      <c r="E103" s="111"/>
-      <c r="F103" s="111"/>
-      <c r="G103" s="111"/>
+      <c r="C103" s="122"/>
+      <c r="D103" s="122"/>
+      <c r="E103" s="122"/>
+      <c r="F103" s="122"/>
+      <c r="G103" s="122"/>
       <c r="H103" s="17">
         <f t="shared" ref="H103:W103" si="4">SUM(H4:H102)</f>
         <v>48.72</v>
       </c>
       <c r="I103" s="17">
         <f t="shared" si="4"/>
-        <v>16.393000000000001</v>
+        <v>17.893000000000001</v>
       </c>
       <c r="J103" s="17">
         <f t="shared" si="4"/>
@@ -6638,7 +6831,7 @@
       </c>
       <c r="N103" s="17">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="O103" s="17">
         <f t="shared" si="4"/>
@@ -6686,22 +6879,22 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
-      <c r="J104" s="101" t="s">
+      <c r="J104" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="K104" s="102"/>
-      <c r="L104" s="102"/>
-      <c r="M104" s="102"/>
-      <c r="N104" s="102"/>
-      <c r="O104" s="102"/>
-      <c r="P104" s="102"/>
-      <c r="Q104" s="102"/>
-      <c r="R104" s="102"/>
-      <c r="S104" s="102"/>
-      <c r="T104" s="102"/>
-      <c r="U104" s="102"/>
-      <c r="V104" s="102"/>
-      <c r="W104" s="103"/>
+      <c r="K104" s="113"/>
+      <c r="L104" s="113"/>
+      <c r="M104" s="113"/>
+      <c r="N104" s="113"/>
+      <c r="O104" s="113"/>
+      <c r="P104" s="113"/>
+      <c r="Q104" s="113"/>
+      <c r="R104" s="113"/>
+      <c r="S104" s="113"/>
+      <c r="T104" s="113"/>
+      <c r="U104" s="113"/>
+      <c r="V104" s="113"/>
+      <c r="W104" s="114"/>
     </row>
     <row r="105" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B105" s="76" t="s">
@@ -6745,10 +6938,10 @@
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="120" t="s">
+      <c r="H106" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="I106" s="123"/>
+      <c r="I106" s="101"/>
       <c r="J106" s="10">
         <f>H103-J103</f>
         <v>46.769999999999996</v>
@@ -6767,43 +6960,43 @@
       </c>
       <c r="N106" s="10">
         <f t="shared" ref="N106:W106" si="5">M106-N103</f>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
       <c r="O106" s="10">
         <f t="shared" si="5"/>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
       <c r="P106" s="10">
         <f t="shared" si="5"/>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
       <c r="Q106" s="10">
         <f t="shared" si="5"/>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
       <c r="R106" s="10">
         <f t="shared" si="5"/>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
       <c r="S106" s="10">
         <f t="shared" si="5"/>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
       <c r="T106" s="10">
         <f t="shared" si="5"/>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
       <c r="U106" s="10">
         <f t="shared" si="5"/>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
       <c r="V106" s="10">
         <f t="shared" si="5"/>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
       <c r="W106" s="10">
         <f t="shared" si="5"/>
-        <v>32.326999999999998</v>
+        <v>30.826999999999998</v>
       </c>
     </row>
     <row r="107" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6816,11 +7009,11 @@
       </c>
       <c r="D107" s="5">
         <f>SUM(I97,I84:I89,I17:I36,I10:I15,I8,I5:I6,I90,I4)</f>
-        <v>4.3929999999999998</v>
+        <v>5.8929999999999998</v>
       </c>
       <c r="E107" s="5">
         <f>SUM(C107,-D107)</f>
-        <v>13.806999999999992</v>
+        <v>12.306999999999992</v>
       </c>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
@@ -6848,27 +7041,27 @@
         <v>5.5</v>
       </c>
       <c r="F108" s="3"/>
-      <c r="H108" s="120" t="s">
+      <c r="H108" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="I108" s="121"/>
-      <c r="J108" s="120">
+      <c r="I108" s="99"/>
+      <c r="J108" s="98">
         <f>H103-I103</f>
-        <v>32.326999999999998</v>
-      </c>
-      <c r="K108" s="121"/>
-      <c r="L108" s="121"/>
-      <c r="M108" s="121"/>
-      <c r="N108" s="121"/>
-      <c r="O108" s="121"/>
-      <c r="P108" s="121"/>
-      <c r="Q108" s="121"/>
-      <c r="R108" s="121"/>
-      <c r="S108" s="121"/>
-      <c r="T108" s="121"/>
-      <c r="U108" s="121"/>
-      <c r="V108" s="121"/>
-      <c r="W108" s="122"/>
+        <v>30.826999999999998</v>
+      </c>
+      <c r="K108" s="99"/>
+      <c r="L108" s="99"/>
+      <c r="M108" s="99"/>
+      <c r="N108" s="99"/>
+      <c r="O108" s="99"/>
+      <c r="P108" s="99"/>
+      <c r="Q108" s="99"/>
+      <c r="R108" s="99"/>
+      <c r="S108" s="99"/>
+      <c r="T108" s="99"/>
+      <c r="U108" s="99"/>
+      <c r="V108" s="99"/>
+      <c r="W108" s="100"/>
     </row>
     <row r="109" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B109" s="3"/>
@@ -6948,12 +7141,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J108:W108"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="C41:C83"/>
-    <mergeCell ref="C20:C36"/>
-    <mergeCell ref="C94:C95"/>
     <mergeCell ref="B41:B91"/>
     <mergeCell ref="C84:C89"/>
     <mergeCell ref="J2:W2"/>
@@ -6966,6 +7153,12 @@
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="B92:B96"/>
     <mergeCell ref="B97:B102"/>
+    <mergeCell ref="J108:W108"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="C41:C83"/>
+    <mergeCell ref="C20:C36"/>
+    <mergeCell ref="C94:C95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizado el excel y screenshot 5/12
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MSI-D\Documents\MAP_LegendOfRadev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,12 +575,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -593,7 +587,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,7 +1102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1354,9 +1348,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1381,19 +1372,43 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1471,37 +1486,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1633,28 +1636,28 @@
                   <c:v>29.726999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.726999999999997</c:v>
+                  <c:v>29.696999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.726999999999997</c:v>
+                  <c:v>29.696999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.726999999999997</c:v>
+                  <c:v>29.696999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.726999999999997</c:v>
+                  <c:v>29.696999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29.726999999999997</c:v>
+                  <c:v>29.696999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29.726999999999997</c:v>
+                  <c:v>29.696999999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.726999999999997</c:v>
+                  <c:v>29.696999999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29.726999999999997</c:v>
+                  <c:v>29.696999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1845,6 +1848,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1880,6 +1900,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2058,28 +2095,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R59" sqref="R59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>126</v>
       </c>
@@ -2087,25 +2124,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="102" t="s">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="104"/>
-    </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="110"/>
+      <c r="V2" s="110"/>
+      <c r="W2" s="111"/>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
@@ -2173,18 +2210,18 @@
         <v>43081</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="108" t="s">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89" t="s">
+      <c r="E4" s="88"/>
+      <c r="F4" s="88" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="12">
@@ -2203,45 +2240,45 @@
       <c r="K4" s="70">
         <v>0</v>
       </c>
-      <c r="L4" s="87">
+      <c r="L4" s="86">
         <v>0.08</v>
       </c>
-      <c r="M4" s="87">
-        <v>0</v>
-      </c>
-      <c r="N4" s="87">
-        <v>0</v>
-      </c>
-      <c r="O4" s="87">
-        <v>0</v>
-      </c>
-      <c r="P4" s="87">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="90">
-        <v>0</v>
-      </c>
-      <c r="R4" s="90">
-        <v>0</v>
-      </c>
-      <c r="S4" s="90">
-        <v>0</v>
-      </c>
-      <c r="T4" s="90">
-        <v>0</v>
-      </c>
-      <c r="U4" s="90">
-        <v>0</v>
-      </c>
-      <c r="V4" s="90">
-        <v>0</v>
-      </c>
-      <c r="W4" s="91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="109"/>
+      <c r="M4" s="86">
+        <v>0</v>
+      </c>
+      <c r="N4" s="86">
+        <v>0</v>
+      </c>
+      <c r="O4" s="86">
+        <v>0</v>
+      </c>
+      <c r="P4" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="89">
+        <v>0</v>
+      </c>
+      <c r="R4" s="89">
+        <v>0</v>
+      </c>
+      <c r="S4" s="89">
+        <v>0</v>
+      </c>
+      <c r="T4" s="89">
+        <v>0</v>
+      </c>
+      <c r="U4" s="89">
+        <v>0</v>
+      </c>
+      <c r="V4" s="89">
+        <v>0</v>
+      </c>
+      <c r="W4" s="90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="116"/>
       <c r="C5" s="46" t="s">
         <v>59</v>
       </c>
@@ -2281,30 +2318,30 @@
       <c r="P5" s="48">
         <v>0</v>
       </c>
-      <c r="Q5" s="92">
-        <v>0</v>
-      </c>
-      <c r="R5" s="92">
-        <v>0</v>
-      </c>
-      <c r="S5" s="92">
-        <v>0</v>
-      </c>
-      <c r="T5" s="92">
-        <v>0</v>
-      </c>
-      <c r="U5" s="92">
-        <v>0</v>
-      </c>
-      <c r="V5" s="92">
-        <v>0</v>
-      </c>
-      <c r="W5" s="93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="109"/>
+      <c r="Q5" s="91">
+        <v>0</v>
+      </c>
+      <c r="R5" s="91">
+        <v>0</v>
+      </c>
+      <c r="S5" s="91">
+        <v>0</v>
+      </c>
+      <c r="T5" s="91">
+        <v>0</v>
+      </c>
+      <c r="U5" s="91">
+        <v>0</v>
+      </c>
+      <c r="V5" s="91">
+        <v>0</v>
+      </c>
+      <c r="W5" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="116"/>
       <c r="C6" s="46" t="s">
         <v>75</v>
       </c>
@@ -2338,8 +2375,12 @@
       <c r="N6" s="48">
         <v>0</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
+      <c r="O6" s="48">
+        <v>0</v>
+      </c>
+      <c r="P6" s="48">
+        <v>0</v>
+      </c>
       <c r="Q6" s="19"/>
       <c r="R6" s="19"/>
       <c r="S6" s="19"/>
@@ -2348,9 +2389,9 @@
       <c r="V6" s="19"/>
       <c r="W6" s="20"/>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="109"/>
-      <c r="C7" s="117" t="s">
+    <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="116"/>
+      <c r="C7" s="124" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="42" t="s">
@@ -2385,8 +2426,12 @@
       <c r="N7" s="71">
         <v>0</v>
       </c>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
+      <c r="O7" s="71">
+        <v>0</v>
+      </c>
+      <c r="P7" s="71">
+        <v>0</v>
+      </c>
       <c r="Q7" s="19"/>
       <c r="R7" s="19"/>
       <c r="S7" s="19"/>
@@ -2395,9 +2440,9 @@
       <c r="V7" s="19"/>
       <c r="W7" s="20"/>
     </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="109"/>
-      <c r="C8" s="117"/>
+    <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="116"/>
+      <c r="C8" s="124"/>
       <c r="D8" s="46" t="s">
         <v>62</v>
       </c>
@@ -2427,11 +2472,15 @@
       <c r="M8" s="71">
         <v>0</v>
       </c>
-      <c r="N8" s="98">
-        <v>0</v>
-      </c>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
+      <c r="N8" s="96">
+        <v>0</v>
+      </c>
+      <c r="O8" s="96">
+        <v>0</v>
+      </c>
+      <c r="P8" s="96">
+        <v>0</v>
+      </c>
       <c r="Q8" s="19"/>
       <c r="R8" s="19"/>
       <c r="S8" s="19"/>
@@ -2440,9 +2489,9 @@
       <c r="V8" s="19"/>
       <c r="W8" s="20"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="113"/>
-      <c r="C9" s="118"/>
+    <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="120"/>
+      <c r="C9" s="125"/>
       <c r="D9" s="43" t="s">
         <v>63</v>
       </c>
@@ -2475,8 +2524,12 @@
       <c r="N9" s="72">
         <v>0</v>
       </c>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
+      <c r="O9" s="72">
+        <v>0</v>
+      </c>
+      <c r="P9" s="72">
+        <v>0</v>
+      </c>
       <c r="Q9" s="21"/>
       <c r="R9" s="21"/>
       <c r="S9" s="21"/>
@@ -2485,8 +2538,8 @@
       <c r="V9" s="21"/>
       <c r="W9" s="22"/>
     </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="110" t="s">
+    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="117" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="51" t="s">
@@ -2516,14 +2569,18 @@
       <c r="L10" s="73">
         <v>0</v>
       </c>
-      <c r="M10" s="95">
+      <c r="M10" s="93">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="N10" s="95">
-        <v>0</v>
-      </c>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
+      <c r="N10" s="93">
+        <v>0</v>
+      </c>
+      <c r="O10" s="93">
+        <v>0</v>
+      </c>
+      <c r="P10" s="93">
+        <v>0</v>
+      </c>
       <c r="Q10" s="35"/>
       <c r="R10" s="35"/>
       <c r="S10" s="35"/>
@@ -2532,8 +2589,8 @@
       <c r="V10" s="23"/>
       <c r="W10" s="24"/>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="111"/>
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="118"/>
       <c r="C11" s="46" t="s">
         <v>66</v>
       </c>
@@ -2567,8 +2624,12 @@
       <c r="N11" s="71">
         <v>0</v>
       </c>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
+      <c r="O11" s="71">
+        <v>0</v>
+      </c>
+      <c r="P11" s="71">
+        <v>0</v>
+      </c>
       <c r="Q11" s="28"/>
       <c r="R11" s="28"/>
       <c r="S11" s="28"/>
@@ -2577,8 +2638,8 @@
       <c r="V11" s="28"/>
       <c r="W11" s="58"/>
     </row>
-    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="111"/>
+    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="118"/>
       <c r="C12" s="46" t="s">
         <v>67</v>
       </c>
@@ -2612,8 +2673,12 @@
       <c r="N12" s="71">
         <v>0</v>
       </c>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
+      <c r="O12" s="71">
+        <v>0</v>
+      </c>
+      <c r="P12" s="71">
+        <v>0</v>
+      </c>
       <c r="Q12" s="28"/>
       <c r="R12" s="28"/>
       <c r="S12" s="28"/>
@@ -2622,8 +2687,8 @@
       <c r="V12" s="28"/>
       <c r="W12" s="58"/>
     </row>
-    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="112"/>
+    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="119"/>
       <c r="C13" s="45" t="s">
         <v>120</v>
       </c>
@@ -2657,8 +2722,12 @@
       <c r="N13" s="74">
         <v>0</v>
       </c>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
+      <c r="O13" s="74">
+        <v>0</v>
+      </c>
+      <c r="P13" s="74">
+        <v>0</v>
+      </c>
       <c r="Q13" s="31"/>
       <c r="R13" s="31"/>
       <c r="S13" s="31"/>
@@ -2667,8 +2736,8 @@
       <c r="V13" s="31"/>
       <c r="W13" s="69"/>
     </row>
-    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="112"/>
+    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="119"/>
       <c r="C14" s="45" t="s">
         <v>118</v>
       </c>
@@ -2702,8 +2771,12 @@
       <c r="N14" s="74">
         <v>0</v>
       </c>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
+      <c r="O14" s="74">
+        <v>0</v>
+      </c>
+      <c r="P14" s="74">
+        <v>0</v>
+      </c>
       <c r="Q14" s="31"/>
       <c r="R14" s="31"/>
       <c r="S14" s="31"/>
@@ -2712,8 +2785,8 @@
       <c r="V14" s="31"/>
       <c r="W14" s="69"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="112"/>
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="119"/>
       <c r="C15" s="45" t="s">
         <v>68</v>
       </c>
@@ -2747,8 +2820,12 @@
       <c r="N15" s="74">
         <v>0</v>
       </c>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
+      <c r="O15" s="74">
+        <v>0</v>
+      </c>
+      <c r="P15" s="74">
+        <v>0</v>
+      </c>
       <c r="Q15" s="31"/>
       <c r="R15" s="31"/>
       <c r="S15" s="31"/>
@@ -2757,8 +2834,8 @@
       <c r="V15" s="31"/>
       <c r="W15" s="69"/>
     </row>
-    <row r="16" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="108" t="s">
+    <row r="16" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="115" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="65" t="s">
@@ -2782,48 +2859,48 @@
       <c r="J16" s="70">
         <v>0</v>
       </c>
-      <c r="K16" s="85">
+      <c r="K16" s="134">
         <v>2</v>
       </c>
-      <c r="L16" s="85">
+      <c r="L16" s="134">
         <v>6.5</v>
       </c>
-      <c r="M16" s="87">
+      <c r="M16" s="86">
         <v>0.25</v>
       </c>
-      <c r="N16" s="87">
-        <v>0</v>
-      </c>
-      <c r="O16" s="87">
-        <v>0</v>
-      </c>
-      <c r="P16" s="87">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="87">
-        <v>0</v>
-      </c>
-      <c r="R16" s="87">
-        <v>0</v>
-      </c>
-      <c r="S16" s="87">
-        <v>0</v>
-      </c>
-      <c r="T16" s="87">
-        <v>0</v>
-      </c>
-      <c r="U16" s="87">
-        <v>0</v>
-      </c>
-      <c r="V16" s="87">
-        <v>0</v>
-      </c>
-      <c r="W16" s="88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="109"/>
+      <c r="N16" s="86">
+        <v>0</v>
+      </c>
+      <c r="O16" s="86">
+        <v>0</v>
+      </c>
+      <c r="P16" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="86">
+        <v>0</v>
+      </c>
+      <c r="R16" s="86">
+        <v>0</v>
+      </c>
+      <c r="S16" s="86">
+        <v>0</v>
+      </c>
+      <c r="T16" s="86">
+        <v>0</v>
+      </c>
+      <c r="U16" s="86">
+        <v>0</v>
+      </c>
+      <c r="V16" s="86">
+        <v>0</v>
+      </c>
+      <c r="W16" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="116"/>
       <c r="C17" s="46" t="s">
         <v>36</v>
       </c>
@@ -2857,8 +2934,12 @@
       <c r="N17" s="48">
         <v>0</v>
       </c>
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
+      <c r="O17" s="48">
+        <v>0</v>
+      </c>
+      <c r="P17" s="48">
+        <v>0</v>
+      </c>
       <c r="Q17" s="29"/>
       <c r="R17" s="29"/>
       <c r="S17" s="29"/>
@@ -2867,9 +2948,9 @@
       <c r="V17" s="29"/>
       <c r="W17" s="30"/>
     </row>
-    <row r="18" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="109"/>
-      <c r="C18" s="116" t="s">
+    <row r="18" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="116"/>
+      <c r="C18" s="123" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="46" t="s">
@@ -2904,8 +2985,12 @@
       <c r="N18" s="71">
         <v>0</v>
       </c>
-      <c r="O18" s="28"/>
-      <c r="P18" s="29"/>
+      <c r="O18" s="71">
+        <v>0</v>
+      </c>
+      <c r="P18" s="71">
+        <v>0</v>
+      </c>
       <c r="Q18" s="29"/>
       <c r="R18" s="29"/>
       <c r="S18" s="29"/>
@@ -2914,9 +2999,9 @@
       <c r="V18" s="29"/>
       <c r="W18" s="30"/>
     </row>
-    <row r="19" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="109"/>
-      <c r="C19" s="116"/>
+    <row r="19" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="116"/>
+      <c r="C19" s="123"/>
       <c r="D19" s="46" t="s">
         <v>39</v>
       </c>
@@ -2949,8 +3034,12 @@
       <c r="N19" s="48">
         <v>0</v>
       </c>
-      <c r="O19" s="28"/>
-      <c r="P19" s="29"/>
+      <c r="O19" s="48">
+        <v>0</v>
+      </c>
+      <c r="P19" s="48">
+        <v>0</v>
+      </c>
       <c r="Q19" s="29"/>
       <c r="R19" s="29"/>
       <c r="S19" s="29"/>
@@ -2959,9 +3048,9 @@
       <c r="V19" s="29"/>
       <c r="W19" s="30"/>
     </row>
-    <row r="20" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="109"/>
-      <c r="C20" s="130" t="s">
+    <row r="20" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="116"/>
+      <c r="C20" s="104" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="46" t="s">
@@ -2996,8 +3085,12 @@
       <c r="N20" s="48">
         <v>1.1499999999999999</v>
       </c>
-      <c r="O20" s="28"/>
-      <c r="P20" s="29"/>
+      <c r="O20" s="48">
+        <v>0</v>
+      </c>
+      <c r="P20" s="48">
+        <v>0</v>
+      </c>
       <c r="Q20" s="29"/>
       <c r="R20" s="29"/>
       <c r="S20" s="29"/>
@@ -3006,9 +3099,9 @@
       <c r="V20" s="29"/>
       <c r="W20" s="30"/>
     </row>
-    <row r="21" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="109"/>
-      <c r="C21" s="130"/>
+    <row r="21" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="116"/>
+      <c r="C21" s="104"/>
       <c r="D21" s="46" t="s">
         <v>34</v>
       </c>
@@ -3041,8 +3134,12 @@
       <c r="N21" s="71">
         <v>0</v>
       </c>
-      <c r="O21" s="28"/>
-      <c r="P21" s="29"/>
+      <c r="O21" s="71">
+        <v>0</v>
+      </c>
+      <c r="P21" s="71">
+        <v>0</v>
+      </c>
       <c r="Q21" s="29"/>
       <c r="R21" s="29"/>
       <c r="S21" s="29"/>
@@ -3051,9 +3148,9 @@
       <c r="V21" s="29"/>
       <c r="W21" s="30"/>
     </row>
-    <row r="22" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="109"/>
-      <c r="C22" s="130"/>
+    <row r="22" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="116"/>
+      <c r="C22" s="104"/>
       <c r="D22" s="46" t="s">
         <v>35</v>
       </c>
@@ -3069,25 +3166,29 @@
       </c>
       <c r="I22" s="55">
         <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
+      <c r="J22" s="71">
+        <v>0</v>
+      </c>
+      <c r="K22" s="71">
+        <v>0</v>
+      </c>
+      <c r="L22" s="71">
+        <v>0</v>
+      </c>
+      <c r="M22" s="71">
+        <v>0</v>
+      </c>
+      <c r="N22" s="132">
         <v>0.35</v>
       </c>
-      <c r="J22" s="71">
-        <v>0</v>
-      </c>
-      <c r="K22" s="71">
-        <v>0</v>
-      </c>
-      <c r="L22" s="71">
-        <v>0</v>
-      </c>
-      <c r="M22" s="71">
-        <v>0</v>
-      </c>
-      <c r="N22" s="94">
-        <v>0.35</v>
-      </c>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
+      <c r="O22" s="132">
+        <v>0</v>
+      </c>
+      <c r="P22" s="133">
+        <v>0.03</v>
+      </c>
       <c r="Q22" s="29"/>
       <c r="R22" s="29"/>
       <c r="S22" s="29"/>
@@ -3096,9 +3197,9 @@
       <c r="V22" s="29"/>
       <c r="W22" s="30"/>
     </row>
-    <row r="23" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="109"/>
-      <c r="C23" s="130"/>
+    <row r="23" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="116"/>
+      <c r="C23" s="104"/>
       <c r="D23" s="46" t="s">
         <v>40</v>
       </c>
@@ -3131,8 +3232,12 @@
       <c r="N23" s="71">
         <v>0</v>
       </c>
-      <c r="O23" s="28"/>
-      <c r="P23" s="29"/>
+      <c r="O23" s="71">
+        <v>0</v>
+      </c>
+      <c r="P23" s="71">
+        <v>0</v>
+      </c>
       <c r="Q23" s="29"/>
       <c r="R23" s="29"/>
       <c r="S23" s="29"/>
@@ -3141,9 +3246,9 @@
       <c r="V23" s="29"/>
       <c r="W23" s="30"/>
     </row>
-    <row r="24" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="109"/>
-      <c r="C24" s="130"/>
+    <row r="24" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="116"/>
+      <c r="C24" s="104"/>
       <c r="D24" s="46" t="s">
         <v>41</v>
       </c>
@@ -3176,8 +3281,12 @@
       <c r="N24" s="71">
         <v>0</v>
       </c>
-      <c r="O24" s="28"/>
-      <c r="P24" s="29"/>
+      <c r="O24" s="71">
+        <v>0</v>
+      </c>
+      <c r="P24" s="71">
+        <v>0</v>
+      </c>
       <c r="Q24" s="29"/>
       <c r="R24" s="29"/>
       <c r="S24" s="29"/>
@@ -3186,9 +3295,9 @@
       <c r="V24" s="29"/>
       <c r="W24" s="30"/>
     </row>
-    <row r="25" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="109"/>
-      <c r="C25" s="130"/>
+    <row r="25" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="116"/>
+      <c r="C25" s="104"/>
       <c r="D25" s="46" t="s">
         <v>42</v>
       </c>
@@ -3221,8 +3330,12 @@
       <c r="N25" s="71">
         <v>0</v>
       </c>
-      <c r="O25" s="28"/>
-      <c r="P25" s="29"/>
+      <c r="O25" s="71">
+        <v>0</v>
+      </c>
+      <c r="P25" s="71">
+        <v>0</v>
+      </c>
       <c r="Q25" s="29"/>
       <c r="R25" s="29"/>
       <c r="S25" s="29"/>
@@ -3231,9 +3344,9 @@
       <c r="V25" s="29"/>
       <c r="W25" s="30"/>
     </row>
-    <row r="26" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="109"/>
-      <c r="C26" s="130"/>
+    <row r="26" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="116"/>
+      <c r="C26" s="104"/>
       <c r="D26" s="46" t="s">
         <v>43</v>
       </c>
@@ -3266,8 +3379,12 @@
       <c r="N26" s="71">
         <v>0</v>
       </c>
-      <c r="O26" s="28"/>
-      <c r="P26" s="29"/>
+      <c r="O26" s="71">
+        <v>0</v>
+      </c>
+      <c r="P26" s="71">
+        <v>0</v>
+      </c>
       <c r="Q26" s="29"/>
       <c r="R26" s="29"/>
       <c r="S26" s="29"/>
@@ -3276,9 +3393,9 @@
       <c r="V26" s="29"/>
       <c r="W26" s="30"/>
     </row>
-    <row r="27" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="109"/>
-      <c r="C27" s="130"/>
+    <row r="27" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="116"/>
+      <c r="C27" s="104"/>
       <c r="D27" s="46" t="s">
         <v>44</v>
       </c>
@@ -3311,8 +3428,12 @@
       <c r="N27" s="71">
         <v>0</v>
       </c>
-      <c r="O27" s="28"/>
-      <c r="P27" s="29"/>
+      <c r="O27" s="71">
+        <v>0</v>
+      </c>
+      <c r="P27" s="71">
+        <v>0</v>
+      </c>
       <c r="Q27" s="29"/>
       <c r="R27" s="29"/>
       <c r="S27" s="29"/>
@@ -3321,9 +3442,9 @@
       <c r="V27" s="29"/>
       <c r="W27" s="30"/>
     </row>
-    <row r="28" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="109"/>
-      <c r="C28" s="130"/>
+    <row r="28" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="116"/>
+      <c r="C28" s="104"/>
       <c r="D28" s="46" t="s">
         <v>45</v>
       </c>
@@ -3356,8 +3477,12 @@
       <c r="N28" s="71">
         <v>0</v>
       </c>
-      <c r="O28" s="28"/>
-      <c r="P28" s="29"/>
+      <c r="O28" s="71">
+        <v>0</v>
+      </c>
+      <c r="P28" s="71">
+        <v>0</v>
+      </c>
       <c r="Q28" s="29"/>
       <c r="R28" s="29"/>
       <c r="S28" s="29"/>
@@ -3366,9 +3491,9 @@
       <c r="V28" s="29"/>
       <c r="W28" s="30"/>
     </row>
-    <row r="29" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="109"/>
-      <c r="C29" s="130"/>
+    <row r="29" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="116"/>
+      <c r="C29" s="104"/>
       <c r="D29" s="46" t="s">
         <v>46</v>
       </c>
@@ -3401,8 +3526,12 @@
       <c r="N29" s="71">
         <v>0</v>
       </c>
-      <c r="O29" s="28"/>
-      <c r="P29" s="29"/>
+      <c r="O29" s="71">
+        <v>0</v>
+      </c>
+      <c r="P29" s="71">
+        <v>0</v>
+      </c>
       <c r="Q29" s="29"/>
       <c r="R29" s="29"/>
       <c r="S29" s="29"/>
@@ -3411,9 +3540,9 @@
       <c r="V29" s="29"/>
       <c r="W29" s="30"/>
     </row>
-    <row r="30" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="109"/>
-      <c r="C30" s="130"/>
+    <row r="30" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="116"/>
+      <c r="C30" s="104"/>
       <c r="D30" s="46" t="s">
         <v>47</v>
       </c>
@@ -3446,8 +3575,12 @@
       <c r="N30" s="71">
         <v>0</v>
       </c>
-      <c r="O30" s="28"/>
-      <c r="P30" s="29"/>
+      <c r="O30" s="71">
+        <v>0</v>
+      </c>
+      <c r="P30" s="71">
+        <v>0</v>
+      </c>
       <c r="Q30" s="29"/>
       <c r="R30" s="29"/>
       <c r="S30" s="29"/>
@@ -3456,9 +3589,9 @@
       <c r="V30" s="29"/>
       <c r="W30" s="30"/>
     </row>
-    <row r="31" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="109"/>
-      <c r="C31" s="130"/>
+    <row r="31" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="116"/>
+      <c r="C31" s="104"/>
       <c r="D31" s="46" t="s">
         <v>48</v>
       </c>
@@ -3491,8 +3624,12 @@
       <c r="N31" s="71">
         <v>0</v>
       </c>
-      <c r="O31" s="28"/>
-      <c r="P31" s="29"/>
+      <c r="O31" s="71">
+        <v>0</v>
+      </c>
+      <c r="P31" s="71">
+        <v>0</v>
+      </c>
       <c r="Q31" s="29"/>
       <c r="R31" s="29"/>
       <c r="S31" s="29"/>
@@ -3501,9 +3638,9 @@
       <c r="V31" s="29"/>
       <c r="W31" s="30"/>
     </row>
-    <row r="32" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="109"/>
-      <c r="C32" s="130"/>
+    <row r="32" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="116"/>
+      <c r="C32" s="104"/>
       <c r="D32" s="46" t="s">
         <v>49</v>
       </c>
@@ -3536,8 +3673,12 @@
       <c r="N32" s="71">
         <v>0</v>
       </c>
-      <c r="O32" s="28"/>
-      <c r="P32" s="29"/>
+      <c r="O32" s="71">
+        <v>0</v>
+      </c>
+      <c r="P32" s="71">
+        <v>0</v>
+      </c>
       <c r="Q32" s="29"/>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
@@ -3546,9 +3687,9 @@
       <c r="V32" s="29"/>
       <c r="W32" s="30"/>
     </row>
-    <row r="33" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="109"/>
-      <c r="C33" s="130"/>
+    <row r="33" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="116"/>
+      <c r="C33" s="104"/>
       <c r="D33" s="46" t="s">
         <v>50</v>
       </c>
@@ -3581,8 +3722,12 @@
       <c r="N33" s="71">
         <v>0</v>
       </c>
-      <c r="O33" s="28"/>
-      <c r="P33" s="29"/>
+      <c r="O33" s="71">
+        <v>0</v>
+      </c>
+      <c r="P33" s="71">
+        <v>0</v>
+      </c>
       <c r="Q33" s="29"/>
       <c r="R33" s="29"/>
       <c r="S33" s="29"/>
@@ -3591,9 +3736,9 @@
       <c r="V33" s="29"/>
       <c r="W33" s="30"/>
     </row>
-    <row r="34" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="109"/>
-      <c r="C34" s="130"/>
+    <row r="34" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="116"/>
+      <c r="C34" s="104"/>
       <c r="D34" s="46" t="s">
         <v>51</v>
       </c>
@@ -3626,8 +3771,12 @@
       <c r="N34" s="71">
         <v>0</v>
       </c>
-      <c r="O34" s="28"/>
-      <c r="P34" s="29"/>
+      <c r="O34" s="71">
+        <v>0</v>
+      </c>
+      <c r="P34" s="71">
+        <v>0</v>
+      </c>
       <c r="Q34" s="29"/>
       <c r="R34" s="29"/>
       <c r="S34" s="29"/>
@@ -3636,9 +3785,9 @@
       <c r="V34" s="29"/>
       <c r="W34" s="30"/>
     </row>
-    <row r="35" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="109"/>
-      <c r="C35" s="130"/>
+    <row r="35" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="116"/>
+      <c r="C35" s="104"/>
       <c r="D35" s="46" t="s">
         <v>52</v>
       </c>
@@ -3671,8 +3820,12 @@
       <c r="N35" s="71">
         <v>0</v>
       </c>
-      <c r="O35" s="28"/>
-      <c r="P35" s="29"/>
+      <c r="O35" s="71">
+        <v>0</v>
+      </c>
+      <c r="P35" s="71">
+        <v>0</v>
+      </c>
       <c r="Q35" s="29"/>
       <c r="R35" s="29"/>
       <c r="S35" s="29"/>
@@ -3681,9 +3834,9 @@
       <c r="V35" s="29"/>
       <c r="W35" s="30"/>
     </row>
-    <row r="36" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="109"/>
-      <c r="C36" s="130"/>
+    <row r="36" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="116"/>
+      <c r="C36" s="104"/>
       <c r="D36" s="52" t="s">
         <v>111</v>
       </c>
@@ -3716,8 +3869,12 @@
       <c r="N36" s="71">
         <v>0</v>
       </c>
-      <c r="O36" s="28"/>
-      <c r="P36" s="29"/>
+      <c r="O36" s="71">
+        <v>0</v>
+      </c>
+      <c r="P36" s="71">
+        <v>0</v>
+      </c>
       <c r="Q36" s="29"/>
       <c r="R36" s="29"/>
       <c r="S36" s="29"/>
@@ -3726,8 +3883,8 @@
       <c r="V36" s="29"/>
       <c r="W36" s="30"/>
     </row>
-    <row r="37" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="109"/>
+    <row r="37" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="116"/>
       <c r="C37" s="49" t="s">
         <v>53</v>
       </c>
@@ -3761,8 +3918,12 @@
       <c r="N37" s="71">
         <v>0</v>
       </c>
-      <c r="O37" s="28"/>
-      <c r="P37" s="29"/>
+      <c r="O37" s="71">
+        <v>0</v>
+      </c>
+      <c r="P37" s="71">
+        <v>0</v>
+      </c>
       <c r="Q37" s="29"/>
       <c r="R37" s="29"/>
       <c r="S37" s="29"/>
@@ -3771,8 +3932,8 @@
       <c r="V37" s="29"/>
       <c r="W37" s="30"/>
     </row>
-    <row r="38" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="109"/>
+    <row r="38" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="116"/>
       <c r="C38" s="49" t="s">
         <v>55</v>
       </c>
@@ -3806,8 +3967,12 @@
       <c r="N38" s="71">
         <v>0</v>
       </c>
-      <c r="O38" s="28"/>
-      <c r="P38" s="29"/>
+      <c r="O38" s="71">
+        <v>0</v>
+      </c>
+      <c r="P38" s="71">
+        <v>0</v>
+      </c>
       <c r="Q38" s="29"/>
       <c r="R38" s="29"/>
       <c r="S38" s="29"/>
@@ -3816,8 +3981,8 @@
       <c r="V38" s="29"/>
       <c r="W38" s="30"/>
     </row>
-    <row r="39" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="109"/>
+    <row r="39" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="116"/>
       <c r="C39" s="49" t="s">
         <v>56</v>
       </c>
@@ -3842,7 +4007,7 @@
       <c r="K39" s="71">
         <v>0</v>
       </c>
-      <c r="L39" s="94">
+      <c r="L39" s="132">
         <v>0.5</v>
       </c>
       <c r="M39" s="48">
@@ -3875,12 +4040,12 @@
       <c r="V39" s="48">
         <v>0</v>
       </c>
-      <c r="W39" s="86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="109"/>
+      <c r="W39" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="116"/>
       <c r="C40" s="56" t="s">
         <v>112</v>
       </c>
@@ -3914,8 +4079,12 @@
       <c r="N40" s="71">
         <v>0</v>
       </c>
-      <c r="O40" s="28"/>
-      <c r="P40" s="29"/>
+      <c r="O40" s="71">
+        <v>0</v>
+      </c>
+      <c r="P40" s="71">
+        <v>0</v>
+      </c>
       <c r="Q40" s="29"/>
       <c r="R40" s="29"/>
       <c r="S40" s="29"/>
@@ -3924,11 +4093,11 @@
       <c r="V40" s="29"/>
       <c r="W40" s="30"/>
     </row>
-    <row r="41" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="99" t="s">
+    <row r="41" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="128" t="s">
+      <c r="C41" s="102" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="50" t="s">
@@ -3948,52 +4117,52 @@
         <f t="shared" ref="I41:I101" si="1">SUM(J41:W41)</f>
         <v>0.95</v>
       </c>
-      <c r="J41" s="85">
+      <c r="J41" s="134">
         <v>0.45</v>
       </c>
-      <c r="K41" s="87">
+      <c r="K41" s="86">
         <v>0.5</v>
       </c>
-      <c r="L41" s="87">
-        <v>0</v>
-      </c>
-      <c r="M41" s="87">
-        <v>0</v>
-      </c>
-      <c r="N41" s="87">
-        <v>0</v>
-      </c>
-      <c r="O41" s="87">
-        <v>0</v>
-      </c>
-      <c r="P41" s="87">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="87">
-        <v>0</v>
-      </c>
-      <c r="R41" s="87">
-        <v>0</v>
-      </c>
-      <c r="S41" s="87">
-        <v>0</v>
-      </c>
-      <c r="T41" s="87">
-        <v>0</v>
-      </c>
-      <c r="U41" s="87">
-        <v>0</v>
-      </c>
-      <c r="V41" s="87">
-        <v>0</v>
-      </c>
-      <c r="W41" s="88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="100"/>
-      <c r="C42" s="129"/>
+      <c r="L41" s="86">
+        <v>0</v>
+      </c>
+      <c r="M41" s="86">
+        <v>0</v>
+      </c>
+      <c r="N41" s="86">
+        <v>0</v>
+      </c>
+      <c r="O41" s="86">
+        <v>0</v>
+      </c>
+      <c r="P41" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="86">
+        <v>0</v>
+      </c>
+      <c r="R41" s="86">
+        <v>0</v>
+      </c>
+      <c r="S41" s="86">
+        <v>0</v>
+      </c>
+      <c r="T41" s="86">
+        <v>0</v>
+      </c>
+      <c r="U41" s="86">
+        <v>0</v>
+      </c>
+      <c r="V41" s="86">
+        <v>0</v>
+      </c>
+      <c r="W41" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="107"/>
+      <c r="C42" s="103"/>
       <c r="D42" s="49" t="s">
         <v>21</v>
       </c>
@@ -4026,8 +4195,12 @@
       <c r="N42" s="71">
         <v>0</v>
       </c>
-      <c r="O42" s="28"/>
-      <c r="P42" s="29"/>
+      <c r="O42" s="71">
+        <v>0</v>
+      </c>
+      <c r="P42" s="71">
+        <v>0</v>
+      </c>
       <c r="Q42" s="29"/>
       <c r="R42" s="29"/>
       <c r="S42" s="29"/>
@@ -4036,9 +4209,9 @@
       <c r="V42" s="29"/>
       <c r="W42" s="30"/>
     </row>
-    <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="100"/>
-      <c r="C43" s="129"/>
+    <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="107"/>
+      <c r="C43" s="103"/>
       <c r="D43" s="49" t="s">
         <v>22</v>
       </c>
@@ -4071,8 +4244,12 @@
       <c r="N43" s="71">
         <v>0</v>
       </c>
-      <c r="O43" s="28"/>
-      <c r="P43" s="29"/>
+      <c r="O43" s="71">
+        <v>0</v>
+      </c>
+      <c r="P43" s="71">
+        <v>0</v>
+      </c>
       <c r="Q43" s="29"/>
       <c r="R43" s="29"/>
       <c r="S43" s="29"/>
@@ -4081,9 +4258,9 @@
       <c r="V43" s="29"/>
       <c r="W43" s="30"/>
     </row>
-    <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="100"/>
-      <c r="C44" s="129"/>
+    <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="107"/>
+      <c r="C44" s="103"/>
       <c r="D44" s="49" t="s">
         <v>23</v>
       </c>
@@ -4116,8 +4293,12 @@
       <c r="N44" s="71">
         <v>0</v>
       </c>
-      <c r="O44" s="28"/>
-      <c r="P44" s="29"/>
+      <c r="O44" s="71">
+        <v>0</v>
+      </c>
+      <c r="P44" s="71">
+        <v>0</v>
+      </c>
       <c r="Q44" s="29"/>
       <c r="R44" s="29"/>
       <c r="S44" s="29"/>
@@ -4126,9 +4307,9 @@
       <c r="V44" s="29"/>
       <c r="W44" s="30"/>
     </row>
-    <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="100"/>
-      <c r="C45" s="129"/>
+    <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="107"/>
+      <c r="C45" s="103"/>
       <c r="D45" s="49" t="s">
         <v>24</v>
       </c>
@@ -4161,8 +4342,12 @@
       <c r="N45" s="71">
         <v>0</v>
       </c>
-      <c r="O45" s="28"/>
-      <c r="P45" s="29"/>
+      <c r="O45" s="71">
+        <v>0</v>
+      </c>
+      <c r="P45" s="71">
+        <v>0</v>
+      </c>
       <c r="Q45" s="29"/>
       <c r="R45" s="29"/>
       <c r="S45" s="29"/>
@@ -4171,9 +4356,9 @@
       <c r="V45" s="29"/>
       <c r="W45" s="30"/>
     </row>
-    <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="100"/>
-      <c r="C46" s="129"/>
+    <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="107"/>
+      <c r="C46" s="103"/>
       <c r="D46" s="49" t="s">
         <v>25</v>
       </c>
@@ -4206,8 +4391,12 @@
       <c r="N46" s="71">
         <v>0</v>
       </c>
-      <c r="O46" s="28"/>
-      <c r="P46" s="29"/>
+      <c r="O46" s="71">
+        <v>0</v>
+      </c>
+      <c r="P46" s="71">
+        <v>0</v>
+      </c>
       <c r="Q46" s="29"/>
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
@@ -4216,9 +4405,9 @@
       <c r="V46" s="29"/>
       <c r="W46" s="30"/>
     </row>
-    <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="100"/>
-      <c r="C47" s="129"/>
+    <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="107"/>
+      <c r="C47" s="103"/>
       <c r="D47" s="49" t="s">
         <v>26</v>
       </c>
@@ -4251,8 +4440,12 @@
       <c r="N47" s="71">
         <v>0</v>
       </c>
-      <c r="O47" s="28"/>
-      <c r="P47" s="29"/>
+      <c r="O47" s="71">
+        <v>0</v>
+      </c>
+      <c r="P47" s="71">
+        <v>0</v>
+      </c>
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
@@ -4261,9 +4454,9 @@
       <c r="V47" s="29"/>
       <c r="W47" s="30"/>
     </row>
-    <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="100"/>
-      <c r="C48" s="129"/>
+    <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="107"/>
+      <c r="C48" s="103"/>
       <c r="D48" s="49" t="s">
         <v>27</v>
       </c>
@@ -4296,8 +4489,12 @@
       <c r="N48" s="71">
         <v>0</v>
       </c>
-      <c r="O48" s="28"/>
-      <c r="P48" s="29"/>
+      <c r="O48" s="71">
+        <v>0</v>
+      </c>
+      <c r="P48" s="71">
+        <v>0</v>
+      </c>
       <c r="Q48" s="29"/>
       <c r="R48" s="29"/>
       <c r="S48" s="29"/>
@@ -4306,9 +4503,9 @@
       <c r="V48" s="29"/>
       <c r="W48" s="30"/>
     </row>
-    <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="100"/>
-      <c r="C49" s="129"/>
+    <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="107"/>
+      <c r="C49" s="103"/>
       <c r="D49" s="49" t="s">
         <v>28</v>
       </c>
@@ -4341,8 +4538,12 @@
       <c r="N49" s="71">
         <v>0</v>
       </c>
-      <c r="O49" s="28"/>
-      <c r="P49" s="29"/>
+      <c r="O49" s="71">
+        <v>0</v>
+      </c>
+      <c r="P49" s="71">
+        <v>0</v>
+      </c>
       <c r="Q49" s="29"/>
       <c r="R49" s="29"/>
       <c r="S49" s="29"/>
@@ -4351,9 +4552,9 @@
       <c r="V49" s="29"/>
       <c r="W49" s="30"/>
     </row>
-    <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="100"/>
-      <c r="C50" s="129"/>
+    <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="107"/>
+      <c r="C50" s="103"/>
       <c r="D50" s="49" t="s">
         <v>29</v>
       </c>
@@ -4386,8 +4587,12 @@
       <c r="N50" s="71">
         <v>0</v>
       </c>
-      <c r="O50" s="28"/>
-      <c r="P50" s="29"/>
+      <c r="O50" s="71">
+        <v>0</v>
+      </c>
+      <c r="P50" s="71">
+        <v>0</v>
+      </c>
       <c r="Q50" s="29"/>
       <c r="R50" s="29"/>
       <c r="S50" s="29"/>
@@ -4396,9 +4601,9 @@
       <c r="V50" s="29"/>
       <c r="W50" s="30"/>
     </row>
-    <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="100"/>
-      <c r="C51" s="129"/>
+    <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="107"/>
+      <c r="C51" s="103"/>
       <c r="D51" s="49" t="s">
         <v>30</v>
       </c>
@@ -4431,8 +4636,12 @@
       <c r="N51" s="71">
         <v>0</v>
       </c>
-      <c r="O51" s="28"/>
-      <c r="P51" s="29"/>
+      <c r="O51" s="71">
+        <v>0</v>
+      </c>
+      <c r="P51" s="71">
+        <v>0</v>
+      </c>
       <c r="Q51" s="29"/>
       <c r="R51" s="29"/>
       <c r="S51" s="29"/>
@@ -4441,9 +4650,9 @@
       <c r="V51" s="29"/>
       <c r="W51" s="30"/>
     </row>
-    <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="100"/>
-      <c r="C52" s="129"/>
+    <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="107"/>
+      <c r="C52" s="103"/>
       <c r="D52" s="49" t="s">
         <v>31</v>
       </c>
@@ -4476,8 +4685,12 @@
       <c r="N52" s="71">
         <v>0</v>
       </c>
-      <c r="O52" s="28"/>
-      <c r="P52" s="29"/>
+      <c r="O52" s="71">
+        <v>0</v>
+      </c>
+      <c r="P52" s="71">
+        <v>0</v>
+      </c>
       <c r="Q52" s="29"/>
       <c r="R52" s="29"/>
       <c r="S52" s="29"/>
@@ -4486,9 +4699,9 @@
       <c r="V52" s="29"/>
       <c r="W52" s="30"/>
     </row>
-    <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="100"/>
-      <c r="C53" s="129"/>
+    <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="107"/>
+      <c r="C53" s="103"/>
       <c r="D53" s="49" t="s">
         <v>77</v>
       </c>
@@ -4521,8 +4734,12 @@
       <c r="N53" s="71">
         <v>0</v>
       </c>
-      <c r="O53" s="28"/>
-      <c r="P53" s="29"/>
+      <c r="O53" s="71">
+        <v>0</v>
+      </c>
+      <c r="P53" s="71">
+        <v>0</v>
+      </c>
       <c r="Q53" s="29"/>
       <c r="R53" s="29"/>
       <c r="S53" s="29"/>
@@ -4531,9 +4748,9 @@
       <c r="V53" s="29"/>
       <c r="W53" s="30"/>
     </row>
-    <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="100"/>
-      <c r="C54" s="129"/>
+    <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="107"/>
+      <c r="C54" s="103"/>
       <c r="D54" s="49" t="s">
         <v>78</v>
       </c>
@@ -4566,8 +4783,12 @@
       <c r="N54" s="71">
         <v>0</v>
       </c>
-      <c r="O54" s="28"/>
-      <c r="P54" s="29"/>
+      <c r="O54" s="71">
+        <v>0</v>
+      </c>
+      <c r="P54" s="71">
+        <v>0</v>
+      </c>
       <c r="Q54" s="29"/>
       <c r="R54" s="29"/>
       <c r="S54" s="29"/>
@@ -4576,9 +4797,9 @@
       <c r="V54" s="29"/>
       <c r="W54" s="30"/>
     </row>
-    <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="100"/>
-      <c r="C55" s="129"/>
+    <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="107"/>
+      <c r="C55" s="103"/>
       <c r="D55" s="49" t="s">
         <v>78</v>
       </c>
@@ -4611,8 +4832,12 @@
       <c r="N55" s="71">
         <v>0</v>
       </c>
-      <c r="O55" s="28"/>
-      <c r="P55" s="29"/>
+      <c r="O55" s="71">
+        <v>0</v>
+      </c>
+      <c r="P55" s="71">
+        <v>0</v>
+      </c>
       <c r="Q55" s="29"/>
       <c r="R55" s="29"/>
       <c r="S55" s="29"/>
@@ -4621,9 +4846,9 @@
       <c r="V55" s="29"/>
       <c r="W55" s="30"/>
     </row>
-    <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="100"/>
-      <c r="C56" s="129"/>
+    <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="107"/>
+      <c r="C56" s="103"/>
       <c r="D56" s="49" t="s">
         <v>79</v>
       </c>
@@ -4656,8 +4881,12 @@
       <c r="N56" s="71">
         <v>0</v>
       </c>
-      <c r="O56" s="28"/>
-      <c r="P56" s="29"/>
+      <c r="O56" s="71">
+        <v>0</v>
+      </c>
+      <c r="P56" s="71">
+        <v>0</v>
+      </c>
       <c r="Q56" s="29"/>
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
@@ -4666,9 +4895,9 @@
       <c r="V56" s="29"/>
       <c r="W56" s="30"/>
     </row>
-    <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="100"/>
-      <c r="C57" s="129"/>
+    <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="107"/>
+      <c r="C57" s="103"/>
       <c r="D57" s="49" t="s">
         <v>80</v>
       </c>
@@ -4701,8 +4930,12 @@
       <c r="N57" s="71">
         <v>0</v>
       </c>
-      <c r="O57" s="28"/>
-      <c r="P57" s="29"/>
+      <c r="O57" s="71">
+        <v>0</v>
+      </c>
+      <c r="P57" s="71">
+        <v>0</v>
+      </c>
       <c r="Q57" s="29"/>
       <c r="R57" s="29"/>
       <c r="S57" s="29"/>
@@ -4711,9 +4944,9 @@
       <c r="V57" s="29"/>
       <c r="W57" s="30"/>
     </row>
-    <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="100"/>
-      <c r="C58" s="129"/>
+    <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="107"/>
+      <c r="C58" s="103"/>
       <c r="D58" s="49" t="s">
         <v>81</v>
       </c>
@@ -4746,8 +4979,12 @@
       <c r="N58" s="71">
         <v>0</v>
       </c>
-      <c r="O58" s="28"/>
-      <c r="P58" s="29"/>
+      <c r="O58" s="71">
+        <v>0</v>
+      </c>
+      <c r="P58" s="71">
+        <v>0</v>
+      </c>
       <c r="Q58" s="29"/>
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
@@ -4756,9 +4993,9 @@
       <c r="V58" s="29"/>
       <c r="W58" s="30"/>
     </row>
-    <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="100"/>
-      <c r="C59" s="129"/>
+    <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="107"/>
+      <c r="C59" s="103"/>
       <c r="D59" s="49" t="s">
         <v>82</v>
       </c>
@@ -4791,8 +5028,12 @@
       <c r="N59" s="71">
         <v>0</v>
       </c>
-      <c r="O59" s="28"/>
-      <c r="P59" s="29"/>
+      <c r="O59" s="71">
+        <v>0</v>
+      </c>
+      <c r="P59" s="71">
+        <v>0</v>
+      </c>
       <c r="Q59" s="29"/>
       <c r="R59" s="29"/>
       <c r="S59" s="29"/>
@@ -4801,9 +5042,9 @@
       <c r="V59" s="29"/>
       <c r="W59" s="30"/>
     </row>
-    <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="100"/>
-      <c r="C60" s="129"/>
+    <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="107"/>
+      <c r="C60" s="103"/>
       <c r="D60" s="49" t="s">
         <v>83</v>
       </c>
@@ -4836,8 +5077,12 @@
       <c r="N60" s="71">
         <v>0</v>
       </c>
-      <c r="O60" s="28"/>
-      <c r="P60" s="29"/>
+      <c r="O60" s="71">
+        <v>0</v>
+      </c>
+      <c r="P60" s="71">
+        <v>0</v>
+      </c>
       <c r="Q60" s="29"/>
       <c r="R60" s="29"/>
       <c r="S60" s="29"/>
@@ -4846,9 +5091,9 @@
       <c r="V60" s="29"/>
       <c r="W60" s="30"/>
     </row>
-    <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="100"/>
-      <c r="C61" s="129"/>
+    <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="107"/>
+      <c r="C61" s="103"/>
       <c r="D61" s="49" t="s">
         <v>84</v>
       </c>
@@ -4881,8 +5126,12 @@
       <c r="N61" s="71">
         <v>0</v>
       </c>
-      <c r="O61" s="28"/>
-      <c r="P61" s="29"/>
+      <c r="O61" s="71">
+        <v>0</v>
+      </c>
+      <c r="P61" s="71">
+        <v>0</v>
+      </c>
       <c r="Q61" s="29"/>
       <c r="R61" s="29"/>
       <c r="S61" s="29"/>
@@ -4891,9 +5140,9 @@
       <c r="V61" s="29"/>
       <c r="W61" s="30"/>
     </row>
-    <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="100"/>
-      <c r="C62" s="129"/>
+    <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="107"/>
+      <c r="C62" s="103"/>
       <c r="D62" s="49" t="s">
         <v>85</v>
       </c>
@@ -4926,8 +5175,12 @@
       <c r="N62" s="71">
         <v>0</v>
       </c>
-      <c r="O62" s="28"/>
-      <c r="P62" s="29"/>
+      <c r="O62" s="71">
+        <v>0</v>
+      </c>
+      <c r="P62" s="71">
+        <v>0</v>
+      </c>
       <c r="Q62" s="29"/>
       <c r="R62" s="29"/>
       <c r="S62" s="29"/>
@@ -4936,9 +5189,9 @@
       <c r="V62" s="29"/>
       <c r="W62" s="30"/>
     </row>
-    <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="100"/>
-      <c r="C63" s="129"/>
+    <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="107"/>
+      <c r="C63" s="103"/>
       <c r="D63" s="49" t="s">
         <v>86</v>
       </c>
@@ -4971,8 +5224,12 @@
       <c r="N63" s="71">
         <v>0</v>
       </c>
-      <c r="O63" s="28"/>
-      <c r="P63" s="29"/>
+      <c r="O63" s="71">
+        <v>0</v>
+      </c>
+      <c r="P63" s="71">
+        <v>0</v>
+      </c>
       <c r="Q63" s="29"/>
       <c r="R63" s="29"/>
       <c r="S63" s="29"/>
@@ -4981,9 +5238,9 @@
       <c r="V63" s="29"/>
       <c r="W63" s="30"/>
     </row>
-    <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="100"/>
-      <c r="C64" s="129"/>
+    <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="107"/>
+      <c r="C64" s="103"/>
       <c r="D64" s="49" t="s">
         <v>87</v>
       </c>
@@ -5016,8 +5273,12 @@
       <c r="N64" s="71">
         <v>0</v>
       </c>
-      <c r="O64" s="28"/>
-      <c r="P64" s="29"/>
+      <c r="O64" s="71">
+        <v>0</v>
+      </c>
+      <c r="P64" s="71">
+        <v>0</v>
+      </c>
       <c r="Q64" s="29"/>
       <c r="R64" s="29"/>
       <c r="S64" s="29"/>
@@ -5026,9 +5287,9 @@
       <c r="V64" s="29"/>
       <c r="W64" s="30"/>
     </row>
-    <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="100"/>
-      <c r="C65" s="129"/>
+    <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="107"/>
+      <c r="C65" s="103"/>
       <c r="D65" s="49" t="s">
         <v>88</v>
       </c>
@@ -5061,8 +5322,12 @@
       <c r="N65" s="71">
         <v>0</v>
       </c>
-      <c r="O65" s="28"/>
-      <c r="P65" s="29"/>
+      <c r="O65" s="71">
+        <v>0</v>
+      </c>
+      <c r="P65" s="71">
+        <v>0</v>
+      </c>
       <c r="Q65" s="29"/>
       <c r="R65" s="29"/>
       <c r="S65" s="29"/>
@@ -5071,9 +5336,9 @@
       <c r="V65" s="29"/>
       <c r="W65" s="30"/>
     </row>
-    <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="100"/>
-      <c r="C66" s="129"/>
+    <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="107"/>
+      <c r="C66" s="103"/>
       <c r="D66" s="49" t="s">
         <v>89</v>
       </c>
@@ -5106,8 +5371,12 @@
       <c r="N66" s="71">
         <v>0</v>
       </c>
-      <c r="O66" s="28"/>
-      <c r="P66" s="29"/>
+      <c r="O66" s="71">
+        <v>0</v>
+      </c>
+      <c r="P66" s="71">
+        <v>0</v>
+      </c>
       <c r="Q66" s="29"/>
       <c r="R66" s="29"/>
       <c r="S66" s="29"/>
@@ -5116,9 +5385,9 @@
       <c r="V66" s="29"/>
       <c r="W66" s="30"/>
     </row>
-    <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="100"/>
-      <c r="C67" s="129"/>
+    <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="107"/>
+      <c r="C67" s="103"/>
       <c r="D67" s="49" t="s">
         <v>94</v>
       </c>
@@ -5151,8 +5420,12 @@
       <c r="N67" s="71">
         <v>0</v>
       </c>
-      <c r="O67" s="28"/>
-      <c r="P67" s="29"/>
+      <c r="O67" s="71">
+        <v>0</v>
+      </c>
+      <c r="P67" s="71">
+        <v>0</v>
+      </c>
       <c r="Q67" s="29"/>
       <c r="R67" s="29"/>
       <c r="S67" s="29"/>
@@ -5161,9 +5434,9 @@
       <c r="V67" s="29"/>
       <c r="W67" s="30"/>
     </row>
-    <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="100"/>
-      <c r="C68" s="129"/>
+    <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="107"/>
+      <c r="C68" s="103"/>
       <c r="D68" s="49" t="s">
         <v>95</v>
       </c>
@@ -5196,8 +5469,12 @@
       <c r="N68" s="71">
         <v>0</v>
       </c>
-      <c r="O68" s="28"/>
-      <c r="P68" s="29"/>
+      <c r="O68" s="71">
+        <v>0</v>
+      </c>
+      <c r="P68" s="71">
+        <v>0</v>
+      </c>
       <c r="Q68" s="29"/>
       <c r="R68" s="29"/>
       <c r="S68" s="29"/>
@@ -5206,9 +5483,9 @@
       <c r="V68" s="29"/>
       <c r="W68" s="30"/>
     </row>
-    <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="100"/>
-      <c r="C69" s="129"/>
+    <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="107"/>
+      <c r="C69" s="103"/>
       <c r="D69" s="49" t="s">
         <v>96</v>
       </c>
@@ -5241,8 +5518,12 @@
       <c r="N69" s="71">
         <v>0</v>
       </c>
-      <c r="O69" s="28"/>
-      <c r="P69" s="29"/>
+      <c r="O69" s="71">
+        <v>0</v>
+      </c>
+      <c r="P69" s="71">
+        <v>0</v>
+      </c>
       <c r="Q69" s="29"/>
       <c r="R69" s="29"/>
       <c r="S69" s="29"/>
@@ -5251,9 +5532,9 @@
       <c r="V69" s="29"/>
       <c r="W69" s="30"/>
     </row>
-    <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="100"/>
-      <c r="C70" s="129"/>
+    <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="107"/>
+      <c r="C70" s="103"/>
       <c r="D70" s="49" t="s">
         <v>97</v>
       </c>
@@ -5286,8 +5567,12 @@
       <c r="N70" s="71">
         <v>0</v>
       </c>
-      <c r="O70" s="28"/>
-      <c r="P70" s="29"/>
+      <c r="O70" s="71">
+        <v>0</v>
+      </c>
+      <c r="P70" s="71">
+        <v>0</v>
+      </c>
       <c r="Q70" s="29"/>
       <c r="R70" s="29"/>
       <c r="S70" s="29"/>
@@ -5296,9 +5581,9 @@
       <c r="V70" s="29"/>
       <c r="W70" s="30"/>
     </row>
-    <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="100"/>
-      <c r="C71" s="129"/>
+    <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="107"/>
+      <c r="C71" s="103"/>
       <c r="D71" s="49" t="s">
         <v>98</v>
       </c>
@@ -5331,8 +5616,12 @@
       <c r="N71" s="71">
         <v>0</v>
       </c>
-      <c r="O71" s="28"/>
-      <c r="P71" s="29"/>
+      <c r="O71" s="71">
+        <v>0</v>
+      </c>
+      <c r="P71" s="71">
+        <v>0</v>
+      </c>
       <c r="Q71" s="29"/>
       <c r="R71" s="29"/>
       <c r="S71" s="29"/>
@@ -5341,9 +5630,9 @@
       <c r="V71" s="29"/>
       <c r="W71" s="30"/>
     </row>
-    <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="100"/>
-      <c r="C72" s="129"/>
+    <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="107"/>
+      <c r="C72" s="103"/>
       <c r="D72" s="49" t="s">
         <v>99</v>
       </c>
@@ -5376,8 +5665,12 @@
       <c r="N72" s="71">
         <v>0</v>
       </c>
-      <c r="O72" s="28"/>
-      <c r="P72" s="29"/>
+      <c r="O72" s="71">
+        <v>0</v>
+      </c>
+      <c r="P72" s="71">
+        <v>0</v>
+      </c>
       <c r="Q72" s="29"/>
       <c r="R72" s="29"/>
       <c r="S72" s="29"/>
@@ -5386,9 +5679,9 @@
       <c r="V72" s="29"/>
       <c r="W72" s="30"/>
     </row>
-    <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="100"/>
-      <c r="C73" s="129"/>
+    <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="107"/>
+      <c r="C73" s="103"/>
       <c r="D73" s="49" t="s">
         <v>100</v>
       </c>
@@ -5421,8 +5714,12 @@
       <c r="N73" s="71">
         <v>0</v>
       </c>
-      <c r="O73" s="28"/>
-      <c r="P73" s="29"/>
+      <c r="O73" s="71">
+        <v>0</v>
+      </c>
+      <c r="P73" s="71">
+        <v>0</v>
+      </c>
       <c r="Q73" s="29"/>
       <c r="R73" s="29"/>
       <c r="S73" s="29"/>
@@ -5431,9 +5728,9 @@
       <c r="V73" s="29"/>
       <c r="W73" s="30"/>
     </row>
-    <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="100"/>
-      <c r="C74" s="129"/>
+    <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="107"/>
+      <c r="C74" s="103"/>
       <c r="D74" s="49" t="s">
         <v>101</v>
       </c>
@@ -5466,8 +5763,12 @@
       <c r="N74" s="71">
         <v>0</v>
       </c>
-      <c r="O74" s="28"/>
-      <c r="P74" s="29"/>
+      <c r="O74" s="71">
+        <v>0</v>
+      </c>
+      <c r="P74" s="71">
+        <v>0</v>
+      </c>
       <c r="Q74" s="29"/>
       <c r="R74" s="29"/>
       <c r="S74" s="29"/>
@@ -5476,9 +5777,9 @@
       <c r="V74" s="29"/>
       <c r="W74" s="30"/>
     </row>
-    <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="100"/>
-      <c r="C75" s="129"/>
+    <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="107"/>
+      <c r="C75" s="103"/>
       <c r="D75" s="49" t="s">
         <v>102</v>
       </c>
@@ -5511,8 +5812,12 @@
       <c r="N75" s="71">
         <v>0</v>
       </c>
-      <c r="O75" s="28"/>
-      <c r="P75" s="29"/>
+      <c r="O75" s="71">
+        <v>0</v>
+      </c>
+      <c r="P75" s="71">
+        <v>0</v>
+      </c>
       <c r="Q75" s="29"/>
       <c r="R75" s="29"/>
       <c r="S75" s="29"/>
@@ -5521,9 +5826,9 @@
       <c r="V75" s="29"/>
       <c r="W75" s="30"/>
     </row>
-    <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="100"/>
-      <c r="C76" s="129"/>
+    <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="107"/>
+      <c r="C76" s="103"/>
       <c r="D76" s="49" t="s">
         <v>103</v>
       </c>
@@ -5556,8 +5861,12 @@
       <c r="N76" s="71">
         <v>0</v>
       </c>
-      <c r="O76" s="28"/>
-      <c r="P76" s="29"/>
+      <c r="O76" s="71">
+        <v>0</v>
+      </c>
+      <c r="P76" s="71">
+        <v>0</v>
+      </c>
       <c r="Q76" s="29"/>
       <c r="R76" s="29"/>
       <c r="S76" s="29"/>
@@ -5566,9 +5875,9 @@
       <c r="V76" s="29"/>
       <c r="W76" s="30"/>
     </row>
-    <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="100"/>
-      <c r="C77" s="129"/>
+    <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="107"/>
+      <c r="C77" s="103"/>
       <c r="D77" s="49" t="s">
         <v>104</v>
       </c>
@@ -5601,8 +5910,12 @@
       <c r="N77" s="71">
         <v>0</v>
       </c>
-      <c r="O77" s="28"/>
-      <c r="P77" s="29"/>
+      <c r="O77" s="71">
+        <v>0</v>
+      </c>
+      <c r="P77" s="71">
+        <v>0</v>
+      </c>
       <c r="Q77" s="29"/>
       <c r="R77" s="29"/>
       <c r="S77" s="29"/>
@@ -5611,9 +5924,9 @@
       <c r="V77" s="29"/>
       <c r="W77" s="30"/>
     </row>
-    <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="100"/>
-      <c r="C78" s="129"/>
+    <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="107"/>
+      <c r="C78" s="103"/>
       <c r="D78" s="49" t="s">
         <v>105</v>
       </c>
@@ -5646,8 +5959,12 @@
       <c r="N78" s="71">
         <v>0</v>
       </c>
-      <c r="O78" s="28"/>
-      <c r="P78" s="29"/>
+      <c r="O78" s="71">
+        <v>0</v>
+      </c>
+      <c r="P78" s="71">
+        <v>0</v>
+      </c>
       <c r="Q78" s="29"/>
       <c r="R78" s="29"/>
       <c r="S78" s="29"/>
@@ -5656,9 +5973,9 @@
       <c r="V78" s="29"/>
       <c r="W78" s="30"/>
     </row>
-    <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="100"/>
-      <c r="C79" s="129"/>
+    <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="107"/>
+      <c r="C79" s="103"/>
       <c r="D79" s="49" t="s">
         <v>106</v>
       </c>
@@ -5691,8 +6008,12 @@
       <c r="N79" s="71">
         <v>0</v>
       </c>
-      <c r="O79" s="28"/>
-      <c r="P79" s="29"/>
+      <c r="O79" s="71">
+        <v>0</v>
+      </c>
+      <c r="P79" s="71">
+        <v>0</v>
+      </c>
       <c r="Q79" s="29"/>
       <c r="R79" s="29"/>
       <c r="S79" s="29"/>
@@ -5701,9 +6022,9 @@
       <c r="V79" s="29"/>
       <c r="W79" s="30"/>
     </row>
-    <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="100"/>
-      <c r="C80" s="129"/>
+    <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="107"/>
+      <c r="C80" s="103"/>
       <c r="D80" s="49" t="s">
         <v>107</v>
       </c>
@@ -5736,8 +6057,12 @@
       <c r="N80" s="71">
         <v>0</v>
       </c>
-      <c r="O80" s="28"/>
-      <c r="P80" s="29"/>
+      <c r="O80" s="71">
+        <v>0</v>
+      </c>
+      <c r="P80" s="71">
+        <v>0</v>
+      </c>
       <c r="Q80" s="29"/>
       <c r="R80" s="29"/>
       <c r="S80" s="29"/>
@@ -5746,9 +6071,9 @@
       <c r="V80" s="29"/>
       <c r="W80" s="30"/>
     </row>
-    <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="100"/>
-      <c r="C81" s="129"/>
+    <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="107"/>
+      <c r="C81" s="103"/>
       <c r="D81" s="49" t="s">
         <v>90</v>
       </c>
@@ -5781,8 +6106,12 @@
       <c r="N81" s="71">
         <v>0</v>
       </c>
-      <c r="O81" s="28"/>
-      <c r="P81" s="29"/>
+      <c r="O81" s="71">
+        <v>0</v>
+      </c>
+      <c r="P81" s="71">
+        <v>0</v>
+      </c>
       <c r="Q81" s="29"/>
       <c r="R81" s="29"/>
       <c r="S81" s="29"/>
@@ -5791,9 +6120,9 @@
       <c r="V81" s="29"/>
       <c r="W81" s="30"/>
     </row>
-    <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="100"/>
-      <c r="C82" s="129"/>
+    <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="107"/>
+      <c r="C82" s="103"/>
       <c r="D82" s="49" t="s">
         <v>91</v>
       </c>
@@ -5826,8 +6155,12 @@
       <c r="N82" s="71">
         <v>0</v>
       </c>
-      <c r="O82" s="28"/>
-      <c r="P82" s="29"/>
+      <c r="O82" s="71">
+        <v>0</v>
+      </c>
+      <c r="P82" s="71">
+        <v>0</v>
+      </c>
       <c r="Q82" s="29"/>
       <c r="R82" s="29"/>
       <c r="S82" s="29"/>
@@ -5836,9 +6169,9 @@
       <c r="V82" s="29"/>
       <c r="W82" s="30"/>
     </row>
-    <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="100"/>
-      <c r="C83" s="129"/>
+    <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="107"/>
+      <c r="C83" s="103"/>
       <c r="D83" s="49" t="s">
         <v>114</v>
       </c>
@@ -5899,9 +6232,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="100"/>
-      <c r="C84" s="101" t="s">
+    <row r="84" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="107"/>
+      <c r="C84" s="108" t="s">
         <v>37</v>
       </c>
       <c r="D84" s="46" t="s">
@@ -5936,8 +6269,12 @@
       <c r="N84" s="71">
         <v>0</v>
       </c>
-      <c r="O84" s="28"/>
-      <c r="P84" s="28"/>
+      <c r="O84" s="71">
+        <v>0</v>
+      </c>
+      <c r="P84" s="71">
+        <v>0</v>
+      </c>
       <c r="Q84" s="28"/>
       <c r="R84" s="29"/>
       <c r="S84" s="29"/>
@@ -5946,9 +6283,9 @@
       <c r="V84" s="29"/>
       <c r="W84" s="30"/>
     </row>
-    <row r="85" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="100"/>
-      <c r="C85" s="101"/>
+    <row r="85" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="107"/>
+      <c r="C85" s="108"/>
       <c r="D85" s="52" t="s">
         <v>70</v>
       </c>
@@ -5981,8 +6318,12 @@
       <c r="N85" s="71">
         <v>0</v>
       </c>
-      <c r="O85" s="28"/>
-      <c r="P85" s="28"/>
+      <c r="O85" s="71">
+        <v>0</v>
+      </c>
+      <c r="P85" s="71">
+        <v>0</v>
+      </c>
       <c r="Q85" s="28"/>
       <c r="R85" s="29"/>
       <c r="S85" s="29"/>
@@ -5991,9 +6332,9 @@
       <c r="V85" s="29"/>
       <c r="W85" s="30"/>
     </row>
-    <row r="86" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="100"/>
-      <c r="C86" s="101"/>
+    <row r="86" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="107"/>
+      <c r="C86" s="108"/>
       <c r="D86" s="52" t="s">
         <v>71</v>
       </c>
@@ -6026,8 +6367,12 @@
       <c r="N86" s="71">
         <v>0</v>
       </c>
-      <c r="O86" s="28"/>
-      <c r="P86" s="28"/>
+      <c r="O86" s="71">
+        <v>0</v>
+      </c>
+      <c r="P86" s="71">
+        <v>0</v>
+      </c>
       <c r="Q86" s="28"/>
       <c r="R86" s="29"/>
       <c r="S86" s="29"/>
@@ -6036,9 +6381,9 @@
       <c r="V86" s="29"/>
       <c r="W86" s="30"/>
     </row>
-    <row r="87" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="100"/>
-      <c r="C87" s="101"/>
+    <row r="87" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="107"/>
+      <c r="C87" s="108"/>
       <c r="D87" s="52" t="s">
         <v>72</v>
       </c>
@@ -6071,8 +6416,12 @@
       <c r="N87" s="71">
         <v>0</v>
       </c>
-      <c r="O87" s="28"/>
-      <c r="P87" s="28"/>
+      <c r="O87" s="71">
+        <v>0</v>
+      </c>
+      <c r="P87" s="71">
+        <v>0</v>
+      </c>
       <c r="Q87" s="28"/>
       <c r="R87" s="28"/>
       <c r="S87" s="29"/>
@@ -6081,9 +6430,9 @@
       <c r="V87" s="29"/>
       <c r="W87" s="30"/>
     </row>
-    <row r="88" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="100"/>
-      <c r="C88" s="101"/>
+    <row r="88" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="107"/>
+      <c r="C88" s="108"/>
       <c r="D88" s="52" t="s">
         <v>73</v>
       </c>
@@ -6116,8 +6465,12 @@
       <c r="N88" s="71">
         <v>0</v>
       </c>
-      <c r="O88" s="28"/>
-      <c r="P88" s="28"/>
+      <c r="O88" s="71">
+        <v>0</v>
+      </c>
+      <c r="P88" s="71">
+        <v>0</v>
+      </c>
       <c r="Q88" s="28"/>
       <c r="R88" s="28"/>
       <c r="S88" s="28"/>
@@ -6126,9 +6479,9 @@
       <c r="V88" s="28"/>
       <c r="W88" s="58"/>
     </row>
-    <row r="89" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="100"/>
-      <c r="C89" s="101"/>
+    <row r="89" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="107"/>
+      <c r="C89" s="108"/>
       <c r="D89" s="52" t="s">
         <v>74</v>
       </c>
@@ -6161,8 +6514,12 @@
       <c r="N89" s="71">
         <v>0</v>
       </c>
-      <c r="O89" s="28"/>
-      <c r="P89" s="28"/>
+      <c r="O89" s="71">
+        <v>0</v>
+      </c>
+      <c r="P89" s="71">
+        <v>0</v>
+      </c>
       <c r="Q89" s="28"/>
       <c r="R89" s="29"/>
       <c r="S89" s="29"/>
@@ -6171,8 +6528,8 @@
       <c r="V89" s="29"/>
       <c r="W89" s="30"/>
     </row>
-    <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="100"/>
+    <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="107"/>
       <c r="C90" s="83" t="s">
         <v>125</v>
       </c>
@@ -6230,12 +6587,12 @@
       <c r="V90" s="48">
         <v>0</v>
       </c>
-      <c r="W90" s="86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="100"/>
+      <c r="W90" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="107"/>
       <c r="C91" s="75" t="s">
         <v>113</v>
       </c>
@@ -6269,8 +6626,12 @@
       <c r="N91" s="71">
         <v>0</v>
       </c>
-      <c r="O91" s="28"/>
-      <c r="P91" s="28"/>
+      <c r="O91" s="71">
+        <v>0</v>
+      </c>
+      <c r="P91" s="71">
+        <v>0</v>
+      </c>
       <c r="Q91" s="28"/>
       <c r="R91" s="29"/>
       <c r="S91" s="29"/>
@@ -6279,8 +6640,8 @@
       <c r="V91" s="29"/>
       <c r="W91" s="30"/>
     </row>
-    <row r="92" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="119" t="s">
+    <row r="92" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="126" t="s">
         <v>92</v>
       </c>
       <c r="C92" s="38" t="s">
@@ -6316,8 +6677,12 @@
       <c r="N92" s="70">
         <v>0</v>
       </c>
-      <c r="O92" s="25"/>
-      <c r="P92" s="25"/>
+      <c r="O92" s="70">
+        <v>0</v>
+      </c>
+      <c r="P92" s="70">
+        <v>0</v>
+      </c>
       <c r="Q92" s="25"/>
       <c r="R92" s="25"/>
       <c r="S92" s="25"/>
@@ -6326,8 +6691,8 @@
       <c r="V92" s="25"/>
       <c r="W92" s="67"/>
     </row>
-    <row r="93" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="120"/>
+    <row r="93" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="127"/>
       <c r="C93" s="41" t="s">
         <v>119</v>
       </c>
@@ -6361,8 +6726,12 @@
       <c r="N93" s="73">
         <v>0</v>
       </c>
-      <c r="O93" s="35"/>
-      <c r="P93" s="35"/>
+      <c r="O93" s="73">
+        <v>0</v>
+      </c>
+      <c r="P93" s="73">
+        <v>0</v>
+      </c>
       <c r="Q93" s="35"/>
       <c r="R93" s="35"/>
       <c r="S93" s="35"/>
@@ -6371,9 +6740,9 @@
       <c r="V93" s="35"/>
       <c r="W93" s="66"/>
     </row>
-    <row r="94" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="121"/>
-      <c r="C94" s="131" t="s">
+    <row r="94" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="128"/>
+      <c r="C94" s="105" t="s">
         <v>108</v>
       </c>
       <c r="D94" s="42" t="s">
@@ -6408,8 +6777,12 @@
       <c r="N94" s="71">
         <v>0</v>
       </c>
-      <c r="O94" s="28"/>
-      <c r="P94" s="28"/>
+      <c r="O94" s="71">
+        <v>0</v>
+      </c>
+      <c r="P94" s="71">
+        <v>0</v>
+      </c>
       <c r="Q94" s="28"/>
       <c r="R94" s="28"/>
       <c r="S94" s="28"/>
@@ -6418,9 +6791,9 @@
       <c r="V94" s="28"/>
       <c r="W94" s="58"/>
     </row>
-    <row r="95" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B95" s="122"/>
-      <c r="C95" s="131"/>
+    <row r="95" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B95" s="129"/>
+      <c r="C95" s="105"/>
       <c r="D95" s="42" t="s">
         <v>109</v>
       </c>
@@ -6453,8 +6826,12 @@
       <c r="N95" s="71">
         <v>0</v>
       </c>
-      <c r="O95" s="28"/>
-      <c r="P95" s="28"/>
+      <c r="O95" s="71">
+        <v>0</v>
+      </c>
+      <c r="P95" s="71">
+        <v>0</v>
+      </c>
       <c r="Q95" s="28"/>
       <c r="R95" s="28"/>
       <c r="S95" s="28"/>
@@ -6463,8 +6840,8 @@
       <c r="V95" s="29"/>
       <c r="W95" s="58"/>
     </row>
-    <row r="96" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="123"/>
+    <row r="96" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="130"/>
       <c r="C96" s="44" t="s">
         <v>116</v>
       </c>
@@ -6492,14 +6869,18 @@
       <c r="L96" s="72">
         <v>0</v>
       </c>
-      <c r="M96" s="96">
+      <c r="M96" s="94">
         <v>0.75</v>
       </c>
-      <c r="N96" s="96">
-        <v>0</v>
-      </c>
-      <c r="O96" s="32"/>
-      <c r="P96" s="32"/>
+      <c r="N96" s="94">
+        <v>0</v>
+      </c>
+      <c r="O96" s="94">
+        <v>0</v>
+      </c>
+      <c r="P96" s="94">
+        <v>0</v>
+      </c>
       <c r="Q96" s="32"/>
       <c r="R96" s="32"/>
       <c r="S96" s="32"/>
@@ -6508,8 +6889,8 @@
       <c r="V96" s="32"/>
       <c r="W96" s="64"/>
     </row>
-    <row r="97" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="99" t="s">
+    <row r="97" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="106" t="s">
         <v>93</v>
       </c>
       <c r="C97" s="63" t="s">
@@ -6539,14 +6920,18 @@
       <c r="L97" s="70">
         <v>0</v>
       </c>
-      <c r="M97" s="87">
+      <c r="M97" s="86">
         <v>0.46700000000000003</v>
       </c>
-      <c r="N97" s="87">
-        <v>0</v>
-      </c>
-      <c r="O97" s="26"/>
-      <c r="P97" s="26"/>
+      <c r="N97" s="86">
+        <v>0</v>
+      </c>
+      <c r="O97" s="86">
+        <v>0</v>
+      </c>
+      <c r="P97" s="86">
+        <v>0</v>
+      </c>
       <c r="Q97" s="26"/>
       <c r="R97" s="26"/>
       <c r="S97" s="26"/>
@@ -6555,8 +6940,8 @@
       <c r="V97" s="26"/>
       <c r="W97" s="27"/>
     </row>
-    <row r="98" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B98" s="122"/>
+    <row r="98" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B98" s="129"/>
       <c r="C98" s="54" t="s">
         <v>131</v>
       </c>
@@ -6584,16 +6969,18 @@
       <c r="L98" s="71">
         <v>0</v>
       </c>
-      <c r="M98" s="97">
-        <v>0</v>
-      </c>
-      <c r="N98" s="97">
-        <v>0</v>
-      </c>
-      <c r="O98" s="134">
-        <v>0</v>
-      </c>
-      <c r="P98" s="29"/>
+      <c r="M98" s="95">
+        <v>0</v>
+      </c>
+      <c r="N98" s="95">
+        <v>0</v>
+      </c>
+      <c r="O98" s="131">
+        <v>0</v>
+      </c>
+      <c r="P98" s="131">
+        <v>0</v>
+      </c>
       <c r="Q98" s="29"/>
       <c r="R98" s="29"/>
       <c r="S98" s="29"/>
@@ -6602,8 +6989,8 @@
       <c r="V98" s="29"/>
       <c r="W98" s="30"/>
     </row>
-    <row r="99" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B99" s="122"/>
+    <row r="99" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B99" s="129"/>
       <c r="C99" s="54" t="s">
         <v>130</v>
       </c>
@@ -6631,16 +7018,18 @@
       <c r="L99" s="71">
         <v>0</v>
       </c>
-      <c r="M99" s="97">
-        <v>0</v>
-      </c>
-      <c r="N99" s="97">
-        <v>0</v>
-      </c>
-      <c r="O99" s="133">
+      <c r="M99" s="95">
+        <v>0</v>
+      </c>
+      <c r="N99" s="95">
+        <v>0</v>
+      </c>
+      <c r="O99" s="97">
         <v>1</v>
       </c>
-      <c r="P99" s="29"/>
+      <c r="P99" s="135">
+        <v>0</v>
+      </c>
       <c r="Q99" s="29"/>
       <c r="R99" s="29"/>
       <c r="S99" s="29"/>
@@ -6649,8 +7038,8 @@
       <c r="V99" s="29"/>
       <c r="W99" s="30"/>
     </row>
-    <row r="100" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B100" s="122"/>
+    <row r="100" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B100" s="129"/>
       <c r="C100" s="54" t="s">
         <v>129</v>
       </c>
@@ -6678,16 +7067,18 @@
       <c r="L100" s="71">
         <v>0</v>
       </c>
-      <c r="M100" s="97">
-        <v>0</v>
-      </c>
-      <c r="N100" s="97">
-        <v>0</v>
-      </c>
-      <c r="O100" s="133">
+      <c r="M100" s="95">
+        <v>0</v>
+      </c>
+      <c r="N100" s="95">
+        <v>0</v>
+      </c>
+      <c r="O100" s="97">
         <v>0.1</v>
       </c>
-      <c r="P100" s="29"/>
+      <c r="P100" s="97">
+        <v>0</v>
+      </c>
       <c r="Q100" s="29"/>
       <c r="R100" s="29"/>
       <c r="S100" s="29"/>
@@ -6696,8 +7087,8 @@
       <c r="V100" s="29"/>
       <c r="W100" s="30"/>
     </row>
-    <row r="101" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B101" s="122"/>
+    <row r="101" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B101" s="129"/>
       <c r="C101" s="54" t="s">
         <v>128</v>
       </c>
@@ -6731,8 +7122,12 @@
       <c r="N101" s="71">
         <v>0</v>
       </c>
-      <c r="O101" s="29"/>
-      <c r="P101" s="29"/>
+      <c r="O101" s="71">
+        <v>0</v>
+      </c>
+      <c r="P101" s="71">
+        <v>0</v>
+      </c>
       <c r="Q101" s="29"/>
       <c r="R101" s="29"/>
       <c r="S101" s="29"/>
@@ -6741,8 +7136,8 @@
       <c r="V101" s="29"/>
       <c r="W101" s="30"/>
     </row>
-    <row r="102" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="123"/>
+    <row r="102" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="130"/>
       <c r="C102" s="44" t="s">
         <v>127</v>
       </c>
@@ -6773,11 +7168,15 @@
       <c r="M102" s="72">
         <v>0</v>
       </c>
-      <c r="N102" s="132" t="s">
+      <c r="N102" s="136" t="s">
         <v>132</v>
       </c>
-      <c r="O102" s="32"/>
-      <c r="P102" s="33"/>
+      <c r="O102" s="136">
+        <v>0</v>
+      </c>
+      <c r="P102" s="137">
+        <v>0</v>
+      </c>
       <c r="Q102" s="33"/>
       <c r="R102" s="33"/>
       <c r="S102" s="33"/>
@@ -6786,22 +7185,22 @@
       <c r="V102" s="33"/>
       <c r="W102" s="34"/>
     </row>
-    <row r="103" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="114" t="s">
+    <row r="103" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="C103" s="115"/>
-      <c r="D103" s="115"/>
-      <c r="E103" s="115"/>
-      <c r="F103" s="115"/>
-      <c r="G103" s="115"/>
+      <c r="C103" s="122"/>
+      <c r="D103" s="122"/>
+      <c r="E103" s="122"/>
+      <c r="F103" s="122"/>
+      <c r="G103" s="122"/>
       <c r="H103" s="17">
         <f t="shared" ref="H103:W103" si="4">SUM(H4:H102)</f>
         <v>48.72</v>
       </c>
       <c r="I103" s="17">
         <f t="shared" si="4"/>
-        <v>18.993000000000002</v>
+        <v>19.023000000000003</v>
       </c>
       <c r="J103" s="17">
         <f t="shared" si="4"/>
@@ -6829,7 +7228,7 @@
       </c>
       <c r="P103" s="17">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="Q103" s="17">
         <f t="shared" si="4"/>
@@ -6860,7 +7259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -6869,24 +7268,24 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
-      <c r="J104" s="105" t="s">
+      <c r="J104" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="K104" s="106"/>
-      <c r="L104" s="106"/>
-      <c r="M104" s="106"/>
-      <c r="N104" s="106"/>
-      <c r="O104" s="106"/>
-      <c r="P104" s="106"/>
-      <c r="Q104" s="106"/>
-      <c r="R104" s="106"/>
-      <c r="S104" s="106"/>
-      <c r="T104" s="106"/>
-      <c r="U104" s="106"/>
-      <c r="V104" s="106"/>
-      <c r="W104" s="107"/>
-    </row>
-    <row r="105" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K104" s="113"/>
+      <c r="L104" s="113"/>
+      <c r="M104" s="113"/>
+      <c r="N104" s="113"/>
+      <c r="O104" s="113"/>
+      <c r="P104" s="113"/>
+      <c r="Q104" s="113"/>
+      <c r="R104" s="113"/>
+      <c r="S104" s="113"/>
+      <c r="T104" s="113"/>
+      <c r="U104" s="113"/>
+      <c r="V104" s="113"/>
+      <c r="W104" s="114"/>
+    </row>
+    <row r="105" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B105" s="76" t="s">
         <v>124</v>
       </c>
@@ -6910,7 +7309,7 @@
       <c r="O105" s="9"/>
       <c r="P105" s="9"/>
     </row>
-    <row r="106" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B106" s="82" t="s">
         <v>16</v>
       </c>
@@ -6928,10 +7327,10 @@
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="124" t="s">
+      <c r="H106" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="I106" s="127"/>
+      <c r="I106" s="101"/>
       <c r="J106" s="10">
         <f>H103-J103</f>
         <v>46.769999999999996</v>
@@ -6958,38 +7357,38 @@
       </c>
       <c r="P106" s="10">
         <f t="shared" si="5"/>
-        <v>29.726999999999997</v>
+        <v>29.696999999999996</v>
       </c>
       <c r="Q106" s="10">
         <f t="shared" si="5"/>
-        <v>29.726999999999997</v>
+        <v>29.696999999999996</v>
       </c>
       <c r="R106" s="10">
         <f t="shared" si="5"/>
-        <v>29.726999999999997</v>
+        <v>29.696999999999996</v>
       </c>
       <c r="S106" s="10">
         <f t="shared" si="5"/>
-        <v>29.726999999999997</v>
+        <v>29.696999999999996</v>
       </c>
       <c r="T106" s="10">
         <f t="shared" si="5"/>
-        <v>29.726999999999997</v>
+        <v>29.696999999999996</v>
       </c>
       <c r="U106" s="10">
         <f t="shared" si="5"/>
-        <v>29.726999999999997</v>
+        <v>29.696999999999996</v>
       </c>
       <c r="V106" s="10">
         <f t="shared" si="5"/>
-        <v>29.726999999999997</v>
+        <v>29.696999999999996</v>
       </c>
       <c r="W106" s="10">
         <f t="shared" si="5"/>
-        <v>29.726999999999997</v>
-      </c>
-    </row>
-    <row r="107" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29.696999999999996</v>
+      </c>
+    </row>
+    <row r="107" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B107" s="80" t="s">
         <v>15</v>
       </c>
@@ -6999,11 +7398,11 @@
       </c>
       <c r="D107" s="5">
         <f>SUM(I97,I84:I89,I17:I36,I10:I15,I8,I5:I6,I90,I4)</f>
-        <v>5.8929999999999998</v>
+        <v>5.923</v>
       </c>
       <c r="E107" s="5">
         <f>SUM(C107,-D107)</f>
-        <v>12.306999999999992</v>
+        <v>12.276999999999992</v>
       </c>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
@@ -7014,7 +7413,7 @@
       <c r="L107" s="3"/>
       <c r="M107" s="3"/>
     </row>
-    <row r="108" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="80" t="s">
         <v>17</v>
       </c>
@@ -7031,29 +7430,29 @@
         <v>5.5</v>
       </c>
       <c r="F108" s="3"/>
-      <c r="H108" s="124" t="s">
+      <c r="H108" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="I108" s="125"/>
-      <c r="J108" s="124">
+      <c r="I108" s="99"/>
+      <c r="J108" s="98">
         <f>H103-I103</f>
-        <v>29.726999999999997</v>
-      </c>
-      <c r="K108" s="125"/>
-      <c r="L108" s="125"/>
-      <c r="M108" s="125"/>
-      <c r="N108" s="125"/>
-      <c r="O108" s="125"/>
-      <c r="P108" s="125"/>
-      <c r="Q108" s="125"/>
-      <c r="R108" s="125"/>
-      <c r="S108" s="125"/>
-      <c r="T108" s="125"/>
-      <c r="U108" s="125"/>
-      <c r="V108" s="125"/>
-      <c r="W108" s="126"/>
-    </row>
-    <row r="109" spans="2:23" x14ac:dyDescent="0.25">
+        <v>29.696999999999996</v>
+      </c>
+      <c r="K108" s="99"/>
+      <c r="L108" s="99"/>
+      <c r="M108" s="99"/>
+      <c r="N108" s="99"/>
+      <c r="O108" s="99"/>
+      <c r="P108" s="99"/>
+      <c r="Q108" s="99"/>
+      <c r="R108" s="99"/>
+      <c r="S108" s="99"/>
+      <c r="T108" s="99"/>
+      <c r="U108" s="99"/>
+      <c r="V108" s="99"/>
+      <c r="W108" s="100"/>
+    </row>
+    <row r="109" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
@@ -7067,7 +7466,7 @@
       <c r="L109" s="3"/>
       <c r="M109" s="3"/>
     </row>
-    <row r="110" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -7081,7 +7480,7 @@
       <c r="L110" s="3"/>
       <c r="M110" s="3"/>
     </row>
-    <row r="111" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
@@ -7095,48 +7494,42 @@
       <c r="L111" s="3"/>
       <c r="M111" s="3"/>
     </row>
-    <row r="112" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B117" s="7"/>
     </row>
-    <row r="118" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B118" s="7"/>
     </row>
-    <row r="119" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B119" s="7"/>
     </row>
-    <row r="120" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B124" s="7"/>
     </row>
-    <row r="125" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B125" s="7"/>
     </row>
-    <row r="126" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B126" s="7"/>
     </row>
-    <row r="127" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B127" s="7"/>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J108:W108"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="C41:C83"/>
-    <mergeCell ref="C20:C36"/>
-    <mergeCell ref="C94:C95"/>
     <mergeCell ref="B41:B91"/>
     <mergeCell ref="C84:C89"/>
     <mergeCell ref="J2:W2"/>
@@ -7149,6 +7542,12 @@
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="B92:B96"/>
     <mergeCell ref="B97:B102"/>
+    <mergeCell ref="J108:W108"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="C41:C83"/>
+    <mergeCell ref="C20:C36"/>
+    <mergeCell ref="C94:C95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7162,7 +7561,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7174,7 +7573,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado excel, arreglndo cosas de los puntos de spawn en las salas del dungeon, establecidas las 5 primeras salas INACTIVAS
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
   <si>
     <t>Subtarea</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Enemigos</t>
   </si>
   <si>
-    <t>Introducir prefab</t>
-  </si>
-  <si>
     <t>Implementar datos comportamiento</t>
   </si>
   <si>
@@ -420,13 +417,19 @@
   </si>
   <si>
     <t>0.7</t>
+  </si>
+  <si>
+    <t>Crear entrada dungeon</t>
+  </si>
+  <si>
+    <t>Implementar Métodos de spawn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +526,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1102,7 +1112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1387,6 +1397,102 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1411,100 +1517,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1613,51 +1626,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$106:$W$106</c:f>
+              <c:f>Hoja1!$J$107:$W$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>46.769999999999996</c:v>
+                  <c:v>46.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.47</c:v>
+                  <c:v>42.870000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.32</c:v>
+                  <c:v>35.720000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.326999999999998</c:v>
+                  <c:v>31.727000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.826999999999998</c:v>
+                  <c:v>30.227000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.726999999999997</c:v>
+                  <c:v>29.127000000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.696999999999996</c:v>
+                  <c:v>29.097000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.696999999999996</c:v>
+                  <c:v>27.068000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.696999999999996</c:v>
+                  <c:v>27.068000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.696999999999996</c:v>
+                  <c:v>27.068000000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29.696999999999996</c:v>
+                  <c:v>27.068000000000005</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29.696999999999996</c:v>
+                  <c:v>27.068000000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.696999999999996</c:v>
+                  <c:v>27.068000000000005</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29.696999999999996</c:v>
+                  <c:v>27.068000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2093,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W128"/>
+  <dimension ref="A1:W129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R59" sqref="R59"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2118,7 +2131,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" s="84" t="s">
         <v>12</v>
@@ -2212,13 +2225,13 @@
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="88" t="s">
-        <v>58</v>
-      </c>
       <c r="D4" s="88" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="88"/>
       <c r="F4" s="88" t="s">
@@ -2280,7 +2293,7 @@
     <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="116"/>
       <c r="C5" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="46"/>
       <c r="E5" s="52"/>
@@ -2343,7 +2356,7 @@
     <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="116"/>
       <c r="C6" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="46"/>
       <c r="E6" s="52"/>
@@ -2391,11 +2404,11 @@
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="116"/>
-      <c r="C7" s="124" t="s">
-        <v>54</v>
+      <c r="C7" s="123" t="s">
+        <v>53</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="54"/>
       <c r="F7" s="54" t="s">
@@ -2442,9 +2455,9 @@
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="116"/>
-      <c r="C8" s="124"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="52"/>
       <c r="F8" s="52" t="s">
@@ -2491,9 +2504,9 @@
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="120"/>
-      <c r="C9" s="125"/>
+      <c r="C9" s="124"/>
       <c r="D9" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="44"/>
       <c r="F9" s="44" t="s">
@@ -2540,10 +2553,10 @@
     </row>
     <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="117" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="51" t="s">
         <v>64</v>
-      </c>
-      <c r="C10" s="51" t="s">
-        <v>65</v>
       </c>
       <c r="D10" s="51"/>
       <c r="E10" s="47"/>
@@ -2592,7 +2605,7 @@
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="118"/>
       <c r="C11" s="46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="52"/>
@@ -2641,7 +2654,7 @@
     <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="118"/>
       <c r="C12" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="52"/>
@@ -2690,7 +2703,7 @@
     <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="119"/>
       <c r="C13" s="45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="53"/>
@@ -2739,7 +2752,7 @@
     <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="119"/>
       <c r="C14" s="45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="53"/>
@@ -2788,7 +2801,7 @@
     <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="119"/>
       <c r="C15" s="45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="53"/>
@@ -2839,7 +2852,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="50"/>
       <c r="E16" s="50"/>
@@ -2859,10 +2872,10 @@
       <c r="J16" s="70">
         <v>0</v>
       </c>
-      <c r="K16" s="134">
+      <c r="K16" s="102">
         <v>2</v>
       </c>
-      <c r="L16" s="134">
+      <c r="L16" s="102">
         <v>6.5</v>
       </c>
       <c r="M16" s="86">
@@ -2948,9 +2961,9 @@
       <c r="V17" s="29"/>
       <c r="W17" s="30"/>
     </row>
-    <row r="18" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="116"/>
-      <c r="C18" s="123" t="s">
+      <c r="C18" s="98" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="46" t="s">
@@ -2964,11 +2977,11 @@
         <v>1</v>
       </c>
       <c r="H18" s="4">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="I18" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J18" s="71">
         <v>0</v>
@@ -2979,16 +2992,16 @@
       <c r="L18" s="71">
         <v>0</v>
       </c>
-      <c r="M18" s="71">
-        <v>0</v>
-      </c>
-      <c r="N18" s="71">
-        <v>0</v>
-      </c>
-      <c r="O18" s="71">
-        <v>0</v>
-      </c>
-      <c r="P18" s="71">
+      <c r="M18" s="48">
+        <v>0.15</v>
+      </c>
+      <c r="N18" s="48">
+        <v>0</v>
+      </c>
+      <c r="O18" s="48">
+        <v>0</v>
+      </c>
+      <c r="P18" s="48">
         <v>0</v>
       </c>
       <c r="Q18" s="29"/>
@@ -3001,23 +3014,25 @@
     </row>
     <row r="19" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="116"/>
-      <c r="C19" s="123"/>
+      <c r="C19" s="136" t="s">
+        <v>37</v>
+      </c>
       <c r="D19" s="46" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E19" s="46"/>
       <c r="F19" s="46" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="4">
+        <v>3</v>
+      </c>
+      <c r="H19" s="4">
         <v>1</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0.5</v>
       </c>
       <c r="I19" s="55">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J19" s="71">
         <v>0</v>
@@ -3028,11 +3043,11 @@
       <c r="L19" s="71">
         <v>0</v>
       </c>
-      <c r="M19" s="48">
-        <v>0.15</v>
+      <c r="M19" s="71">
+        <v>0</v>
       </c>
       <c r="N19" s="48">
-        <v>0</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="O19" s="48">
         <v>0</v>
@@ -3050,25 +3065,23 @@
     </row>
     <row r="20" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="116"/>
-      <c r="C20" s="104" t="s">
-        <v>37</v>
-      </c>
+      <c r="C20" s="136"/>
       <c r="D20" s="46" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="E20" s="46"/>
       <c r="F20" s="46" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H20" s="4">
         <v>1</v>
       </c>
       <c r="I20" s="55">
         <f t="shared" si="0"/>
-        <v>1.1499999999999999</v>
+        <v>0</v>
       </c>
       <c r="J20" s="71">
         <v>0</v>
@@ -3082,13 +3095,13 @@
       <c r="M20" s="71">
         <v>0</v>
       </c>
-      <c r="N20" s="48">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="O20" s="48">
-        <v>0</v>
-      </c>
-      <c r="P20" s="48">
+      <c r="N20" s="71">
+        <v>0</v>
+      </c>
+      <c r="O20" s="71">
+        <v>0</v>
+      </c>
+      <c r="P20" s="71">
         <v>0</v>
       </c>
       <c r="Q20" s="29"/>
@@ -3101,7 +3114,7 @@
     </row>
     <row r="21" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="116"/>
-      <c r="C21" s="104"/>
+      <c r="C21" s="136"/>
       <c r="D21" s="46" t="s">
         <v>34</v>
       </c>
@@ -3150,7 +3163,7 @@
     </row>
     <row r="22" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="116"/>
-      <c r="C22" s="104"/>
+      <c r="C22" s="136"/>
       <c r="D22" s="46" t="s">
         <v>35</v>
       </c>
@@ -3166,7 +3179,7 @@
       </c>
       <c r="I22" s="55">
         <f t="shared" si="0"/>
-        <v>0.38</v>
+        <v>1.2469999999999999</v>
       </c>
       <c r="J22" s="71">
         <v>0</v>
@@ -3180,16 +3193,18 @@
       <c r="M22" s="71">
         <v>0</v>
       </c>
-      <c r="N22" s="132">
+      <c r="N22" s="100">
         <v>0.35</v>
       </c>
-      <c r="O22" s="132">
-        <v>0</v>
-      </c>
-      <c r="P22" s="133">
+      <c r="O22" s="100">
+        <v>0</v>
+      </c>
+      <c r="P22" s="101">
         <v>0.03</v>
       </c>
-      <c r="Q22" s="29"/>
+      <c r="Q22" s="97">
+        <v>0.86699999999999999</v>
+      </c>
       <c r="R22" s="29"/>
       <c r="S22" s="29"/>
       <c r="T22" s="29"/>
@@ -3199,9 +3214,9 @@
     </row>
     <row r="23" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="116"/>
-      <c r="C23" s="104"/>
+      <c r="C23" s="136"/>
       <c r="D23" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="46"/>
       <c r="F23" s="46" t="s">
@@ -3211,11 +3226,11 @@
         <v>4</v>
       </c>
       <c r="H23" s="4">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="I23" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="J23" s="71">
         <v>0</v>
@@ -3238,7 +3253,9 @@
       <c r="P23" s="71">
         <v>0</v>
       </c>
-      <c r="Q23" s="29"/>
+      <c r="Q23" s="97">
+        <v>0.33</v>
+      </c>
       <c r="R23" s="29"/>
       <c r="S23" s="29"/>
       <c r="T23" s="29"/>
@@ -3248,9 +3265,9 @@
     </row>
     <row r="24" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="116"/>
-      <c r="C24" s="104"/>
+      <c r="C24" s="136"/>
       <c r="D24" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="46"/>
       <c r="F24" s="46" t="s">
@@ -3264,7 +3281,7 @@
       </c>
       <c r="I24" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="J24" s="71">
         <v>0</v>
@@ -3287,7 +3304,9 @@
       <c r="P24" s="71">
         <v>0</v>
       </c>
-      <c r="Q24" s="29"/>
+      <c r="Q24" s="97">
+        <v>0.11600000000000001</v>
+      </c>
       <c r="R24" s="29"/>
       <c r="S24" s="29"/>
       <c r="T24" s="29"/>
@@ -3297,9 +3316,9 @@
     </row>
     <row r="25" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="116"/>
-      <c r="C25" s="104"/>
+      <c r="C25" s="136"/>
       <c r="D25" s="46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="46"/>
       <c r="F25" s="46" t="s">
@@ -3313,7 +3332,7 @@
       </c>
       <c r="I25" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="J25" s="71">
         <v>0</v>
@@ -3336,7 +3355,9 @@
       <c r="P25" s="71">
         <v>0</v>
       </c>
-      <c r="Q25" s="29"/>
+      <c r="Q25" s="97">
+        <v>0.3</v>
+      </c>
       <c r="R25" s="29"/>
       <c r="S25" s="29"/>
       <c r="T25" s="29"/>
@@ -3346,9 +3367,9 @@
     </row>
     <row r="26" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="116"/>
-      <c r="C26" s="104"/>
+      <c r="C26" s="136"/>
       <c r="D26" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" s="46"/>
       <c r="F26" s="46" t="s">
@@ -3362,7 +3383,7 @@
       </c>
       <c r="I26" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="J26" s="71">
         <v>0</v>
@@ -3385,7 +3406,9 @@
       <c r="P26" s="71">
         <v>0</v>
       </c>
-      <c r="Q26" s="29"/>
+      <c r="Q26" s="97">
+        <v>0.11600000000000001</v>
+      </c>
       <c r="R26" s="29"/>
       <c r="S26" s="29"/>
       <c r="T26" s="29"/>
@@ -3395,9 +3418,9 @@
     </row>
     <row r="27" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="116"/>
-      <c r="C27" s="104"/>
+      <c r="C27" s="136"/>
       <c r="D27" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" s="46"/>
       <c r="F27" s="46" t="s">
@@ -3411,7 +3434,7 @@
       </c>
       <c r="I27" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J27" s="71">
         <v>0</v>
@@ -3434,7 +3457,9 @@
       <c r="P27" s="71">
         <v>0</v>
       </c>
-      <c r="Q27" s="29"/>
+      <c r="Q27" s="97">
+        <v>0.05</v>
+      </c>
       <c r="R27" s="29"/>
       <c r="S27" s="29"/>
       <c r="T27" s="29"/>
@@ -3444,9 +3469,9 @@
     </row>
     <row r="28" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="116"/>
-      <c r="C28" s="104"/>
+      <c r="C28" s="136"/>
       <c r="D28" s="46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" s="46"/>
       <c r="F28" s="46" t="s">
@@ -3493,9 +3518,9 @@
     </row>
     <row r="29" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="116"/>
-      <c r="C29" s="104"/>
+      <c r="C29" s="136"/>
       <c r="D29" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29" s="46"/>
       <c r="F29" s="46" t="s">
@@ -3542,9 +3567,9 @@
     </row>
     <row r="30" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="116"/>
-      <c r="C30" s="104"/>
+      <c r="C30" s="136"/>
       <c r="D30" s="46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" s="46"/>
       <c r="F30" s="46" t="s">
@@ -3591,9 +3616,9 @@
     </row>
     <row r="31" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="116"/>
-      <c r="C31" s="104"/>
+      <c r="C31" s="136"/>
       <c r="D31" s="46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="46"/>
       <c r="F31" s="46" t="s">
@@ -3640,9 +3665,9 @@
     </row>
     <row r="32" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="116"/>
-      <c r="C32" s="104"/>
+      <c r="C32" s="136"/>
       <c r="D32" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" s="46"/>
       <c r="F32" s="46" t="s">
@@ -3689,9 +3714,9 @@
     </row>
     <row r="33" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="116"/>
-      <c r="C33" s="104"/>
+      <c r="C33" s="136"/>
       <c r="D33" s="46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33" s="46"/>
       <c r="F33" s="46" t="s">
@@ -3738,9 +3763,9 @@
     </row>
     <row r="34" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="116"/>
-      <c r="C34" s="104"/>
+      <c r="C34" s="136"/>
       <c r="D34" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34" s="46"/>
       <c r="F34" s="46" t="s">
@@ -3787,9 +3812,9 @@
     </row>
     <row r="35" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="116"/>
-      <c r="C35" s="104"/>
+      <c r="C35" s="136"/>
       <c r="D35" s="46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" s="46"/>
       <c r="F35" s="46" t="s">
@@ -3836,9 +3861,9 @@
     </row>
     <row r="36" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="116"/>
-      <c r="C36" s="104"/>
+      <c r="C36" s="136"/>
       <c r="D36" s="52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E36" s="52"/>
       <c r="F36" s="52" t="s">
@@ -3886,7 +3911,7 @@
     <row r="37" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="116"/>
       <c r="C37" s="49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D37" s="49"/>
       <c r="E37" s="49"/>
@@ -3935,7 +3960,7 @@
     <row r="38" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="116"/>
       <c r="C38" s="49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" s="49"/>
       <c r="E38" s="49"/>
@@ -3984,7 +4009,7 @@
     <row r="39" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="116"/>
       <c r="C39" s="49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" s="49"/>
       <c r="E39" s="49"/>
@@ -4007,7 +4032,7 @@
       <c r="K39" s="71">
         <v>0</v>
       </c>
-      <c r="L39" s="132">
+      <c r="L39" s="100">
         <v>0.5</v>
       </c>
       <c r="M39" s="48">
@@ -4047,7 +4072,7 @@
     <row r="40" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="116"/>
       <c r="C40" s="56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
@@ -4097,7 +4122,7 @@
       <c r="B41" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="102" t="s">
+      <c r="C41" s="134" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="50" t="s">
@@ -4114,10 +4139,10 @@
         <v>0.5</v>
       </c>
       <c r="I41" s="57">
-        <f t="shared" ref="I41:I101" si="1">SUM(J41:W41)</f>
+        <f t="shared" ref="I41:I102" si="1">SUM(J41:W41)</f>
         <v>0.95</v>
       </c>
-      <c r="J41" s="134">
+      <c r="J41" s="102">
         <v>0.45</v>
       </c>
       <c r="K41" s="86">
@@ -4162,7 +4187,7 @@
     </row>
     <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="107"/>
-      <c r="C42" s="103"/>
+      <c r="C42" s="135"/>
       <c r="D42" s="49" t="s">
         <v>21</v>
       </c>
@@ -4211,7 +4236,7 @@
     </row>
     <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="107"/>
-      <c r="C43" s="103"/>
+      <c r="C43" s="135"/>
       <c r="D43" s="49" t="s">
         <v>22</v>
       </c>
@@ -4260,7 +4285,7 @@
     </row>
     <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="107"/>
-      <c r="C44" s="103"/>
+      <c r="C44" s="135"/>
       <c r="D44" s="49" t="s">
         <v>23</v>
       </c>
@@ -4309,7 +4334,7 @@
     </row>
     <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="107"/>
-      <c r="C45" s="103"/>
+      <c r="C45" s="135"/>
       <c r="D45" s="49" t="s">
         <v>24</v>
       </c>
@@ -4358,7 +4383,7 @@
     </row>
     <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="107"/>
-      <c r="C46" s="103"/>
+      <c r="C46" s="135"/>
       <c r="D46" s="49" t="s">
         <v>25</v>
       </c>
@@ -4407,7 +4432,7 @@
     </row>
     <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="107"/>
-      <c r="C47" s="103"/>
+      <c r="C47" s="135"/>
       <c r="D47" s="49" t="s">
         <v>26</v>
       </c>
@@ -4456,7 +4481,7 @@
     </row>
     <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="107"/>
-      <c r="C48" s="103"/>
+      <c r="C48" s="135"/>
       <c r="D48" s="49" t="s">
         <v>27</v>
       </c>
@@ -4505,7 +4530,7 @@
     </row>
     <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="107"/>
-      <c r="C49" s="103"/>
+      <c r="C49" s="135"/>
       <c r="D49" s="49" t="s">
         <v>28</v>
       </c>
@@ -4554,7 +4579,7 @@
     </row>
     <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="107"/>
-      <c r="C50" s="103"/>
+      <c r="C50" s="135"/>
       <c r="D50" s="49" t="s">
         <v>29</v>
       </c>
@@ -4603,7 +4628,7 @@
     </row>
     <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="107"/>
-      <c r="C51" s="103"/>
+      <c r="C51" s="135"/>
       <c r="D51" s="49" t="s">
         <v>30</v>
       </c>
@@ -4652,7 +4677,7 @@
     </row>
     <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="107"/>
-      <c r="C52" s="103"/>
+      <c r="C52" s="135"/>
       <c r="D52" s="49" t="s">
         <v>31</v>
       </c>
@@ -4701,9 +4726,9 @@
     </row>
     <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="107"/>
-      <c r="C53" s="103"/>
+      <c r="C53" s="135"/>
       <c r="D53" s="49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E53" s="49"/>
       <c r="F53" s="49" t="s">
@@ -4750,9 +4775,9 @@
     </row>
     <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="107"/>
-      <c r="C54" s="103"/>
+      <c r="C54" s="135"/>
       <c r="D54" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E54" s="49"/>
       <c r="F54" s="49" t="s">
@@ -4799,9 +4824,9 @@
     </row>
     <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="107"/>
-      <c r="C55" s="103"/>
+      <c r="C55" s="135"/>
       <c r="D55" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E55" s="49"/>
       <c r="F55" s="49" t="s">
@@ -4848,9 +4873,9 @@
     </row>
     <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="107"/>
-      <c r="C56" s="103"/>
+      <c r="C56" s="135"/>
       <c r="D56" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E56" s="49"/>
       <c r="F56" s="49" t="s">
@@ -4897,9 +4922,9 @@
     </row>
     <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="107"/>
-      <c r="C57" s="103"/>
+      <c r="C57" s="135"/>
       <c r="D57" s="49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E57" s="49"/>
       <c r="F57" s="49" t="s">
@@ -4946,9 +4971,9 @@
     </row>
     <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="107"/>
-      <c r="C58" s="103"/>
+      <c r="C58" s="135"/>
       <c r="D58" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E58" s="49"/>
       <c r="F58" s="49" t="s">
@@ -4995,9 +5020,9 @@
     </row>
     <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="107"/>
-      <c r="C59" s="103"/>
+      <c r="C59" s="135"/>
       <c r="D59" s="49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E59" s="49"/>
       <c r="F59" s="49" t="s">
@@ -5044,9 +5069,9 @@
     </row>
     <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="107"/>
-      <c r="C60" s="103"/>
+      <c r="C60" s="135"/>
       <c r="D60" s="49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E60" s="49"/>
       <c r="F60" s="49" t="s">
@@ -5093,9 +5118,9 @@
     </row>
     <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="107"/>
-      <c r="C61" s="103"/>
+      <c r="C61" s="135"/>
       <c r="D61" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E61" s="49"/>
       <c r="F61" s="49" t="s">
@@ -5142,9 +5167,9 @@
     </row>
     <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="107"/>
-      <c r="C62" s="103"/>
+      <c r="C62" s="135"/>
       <c r="D62" s="49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E62" s="49"/>
       <c r="F62" s="49" t="s">
@@ -5191,9 +5216,9 @@
     </row>
     <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="107"/>
-      <c r="C63" s="103"/>
+      <c r="C63" s="135"/>
       <c r="D63" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E63" s="49"/>
       <c r="F63" s="49" t="s">
@@ -5240,9 +5265,9 @@
     </row>
     <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="107"/>
-      <c r="C64" s="103"/>
+      <c r="C64" s="135"/>
       <c r="D64" s="49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E64" s="49"/>
       <c r="F64" s="49" t="s">
@@ -5289,9 +5314,9 @@
     </row>
     <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="107"/>
-      <c r="C65" s="103"/>
+      <c r="C65" s="135"/>
       <c r="D65" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E65" s="49"/>
       <c r="F65" s="49" t="s">
@@ -5338,9 +5363,9 @@
     </row>
     <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="107"/>
-      <c r="C66" s="103"/>
+      <c r="C66" s="135"/>
       <c r="D66" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E66" s="49"/>
       <c r="F66" s="49" t="s">
@@ -5387,9 +5412,9 @@
     </row>
     <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="107"/>
-      <c r="C67" s="103"/>
+      <c r="C67" s="135"/>
       <c r="D67" s="49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E67" s="49"/>
       <c r="F67" s="49" t="s">
@@ -5436,9 +5461,9 @@
     </row>
     <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="107"/>
-      <c r="C68" s="103"/>
+      <c r="C68" s="135"/>
       <c r="D68" s="49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E68" s="49"/>
       <c r="F68" s="49" t="s">
@@ -5485,9 +5510,9 @@
     </row>
     <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="107"/>
-      <c r="C69" s="103"/>
+      <c r="C69" s="135"/>
       <c r="D69" s="49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E69" s="49"/>
       <c r="F69" s="49" t="s">
@@ -5534,9 +5559,9 @@
     </row>
     <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="107"/>
-      <c r="C70" s="103"/>
+      <c r="C70" s="135"/>
       <c r="D70" s="49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E70" s="49"/>
       <c r="F70" s="49" t="s">
@@ -5583,9 +5608,9 @@
     </row>
     <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="107"/>
-      <c r="C71" s="103"/>
+      <c r="C71" s="135"/>
       <c r="D71" s="49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E71" s="49"/>
       <c r="F71" s="49" t="s">
@@ -5632,9 +5657,9 @@
     </row>
     <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="107"/>
-      <c r="C72" s="103"/>
+      <c r="C72" s="135"/>
       <c r="D72" s="49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E72" s="49"/>
       <c r="F72" s="49" t="s">
@@ -5681,9 +5706,9 @@
     </row>
     <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="107"/>
-      <c r="C73" s="103"/>
+      <c r="C73" s="135"/>
       <c r="D73" s="49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E73" s="49"/>
       <c r="F73" s="49" t="s">
@@ -5730,9 +5755,9 @@
     </row>
     <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="107"/>
-      <c r="C74" s="103"/>
+      <c r="C74" s="135"/>
       <c r="D74" s="49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E74" s="49"/>
       <c r="F74" s="49" t="s">
@@ -5779,9 +5804,9 @@
     </row>
     <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="107"/>
-      <c r="C75" s="103"/>
+      <c r="C75" s="135"/>
       <c r="D75" s="49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E75" s="49"/>
       <c r="F75" s="49" t="s">
@@ -5828,9 +5853,9 @@
     </row>
     <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="107"/>
-      <c r="C76" s="103"/>
+      <c r="C76" s="135"/>
       <c r="D76" s="49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E76" s="49"/>
       <c r="F76" s="49" t="s">
@@ -5877,9 +5902,9 @@
     </row>
     <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="107"/>
-      <c r="C77" s="103"/>
+      <c r="C77" s="135"/>
       <c r="D77" s="49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E77" s="49"/>
       <c r="F77" s="49" t="s">
@@ -5926,9 +5951,9 @@
     </row>
     <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="107"/>
-      <c r="C78" s="103"/>
+      <c r="C78" s="135"/>
       <c r="D78" s="49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E78" s="49"/>
       <c r="F78" s="49" t="s">
@@ -5975,9 +6000,9 @@
     </row>
     <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="107"/>
-      <c r="C79" s="103"/>
+      <c r="C79" s="135"/>
       <c r="D79" s="49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E79" s="49"/>
       <c r="F79" s="49" t="s">
@@ -6024,9 +6049,9 @@
     </row>
     <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="107"/>
-      <c r="C80" s="103"/>
+      <c r="C80" s="135"/>
       <c r="D80" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E80" s="49"/>
       <c r="F80" s="49" t="s">
@@ -6039,7 +6064,7 @@
         <v>0.25</v>
       </c>
       <c r="I80" s="55">
-        <f t="shared" ref="I80:I89" si="2">SUM(J80:W80)</f>
+        <f t="shared" ref="I80:I90" si="2">SUM(J80:W80)</f>
         <v>0</v>
       </c>
       <c r="J80" s="71">
@@ -6073,9 +6098,9 @@
     </row>
     <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="107"/>
-      <c r="C81" s="103"/>
+      <c r="C81" s="135"/>
       <c r="D81" s="49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E81" s="49"/>
       <c r="F81" s="49" t="s">
@@ -6122,9 +6147,9 @@
     </row>
     <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="107"/>
-      <c r="C82" s="103"/>
+      <c r="C82" s="135"/>
       <c r="D82" s="49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E82" s="49"/>
       <c r="F82" s="49" t="s">
@@ -6171,9 +6196,9 @@
     </row>
     <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="107"/>
-      <c r="C83" s="103"/>
+      <c r="C83" s="135"/>
       <c r="D83" s="49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E83" s="49"/>
       <c r="F83" s="49" t="s">
@@ -6238,7 +6263,7 @@
         <v>37</v>
       </c>
       <c r="D84" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E84" s="52"/>
       <c r="F84" s="52" t="s">
@@ -6287,7 +6312,7 @@
       <c r="B85" s="107"/>
       <c r="C85" s="108"/>
       <c r="D85" s="52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E85" s="52"/>
       <c r="F85" s="52" t="s">
@@ -6336,7 +6361,7 @@
       <c r="B86" s="107"/>
       <c r="C86" s="108"/>
       <c r="D86" s="52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E86" s="52"/>
       <c r="F86" s="52" t="s">
@@ -6385,7 +6410,7 @@
       <c r="B87" s="107"/>
       <c r="C87" s="108"/>
       <c r="D87" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E87" s="52"/>
       <c r="F87" s="52" t="s">
@@ -6434,7 +6459,7 @@
       <c r="B88" s="107"/>
       <c r="C88" s="108"/>
       <c r="D88" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E88" s="52"/>
       <c r="F88" s="52" t="s">
@@ -6483,7 +6508,7 @@
       <c r="B89" s="107"/>
       <c r="C89" s="108"/>
       <c r="D89" s="52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E89" s="52"/>
       <c r="F89" s="46" t="s">
@@ -6530,8 +6555,8 @@
     </row>
     <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="107"/>
-      <c r="C90" s="83" t="s">
-        <v>125</v>
+      <c r="C90" s="138" t="s">
+        <v>132</v>
       </c>
       <c r="D90" s="52"/>
       <c r="E90" s="52"/>
@@ -6539,261 +6564,263 @@
         <v>15</v>
       </c>
       <c r="G90" s="4">
+        <v>3</v>
+      </c>
+      <c r="H90" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I90" s="55">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="J90" s="71">
+        <v>0</v>
+      </c>
+      <c r="K90" s="71">
+        <v>0</v>
+      </c>
+      <c r="L90" s="71">
+        <v>0</v>
+      </c>
+      <c r="M90" s="71">
+        <v>0</v>
+      </c>
+      <c r="N90" s="71">
+        <v>0</v>
+      </c>
+      <c r="O90" s="71">
+        <v>0</v>
+      </c>
+      <c r="P90" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q90" s="48">
+        <v>0.25</v>
+      </c>
+      <c r="R90" s="29"/>
+      <c r="S90" s="29"/>
+      <c r="T90" s="29"/>
+      <c r="U90" s="29"/>
+      <c r="V90" s="29"/>
+      <c r="W90" s="30"/>
+    </row>
+    <row r="91" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="107"/>
+      <c r="C91" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="D91" s="52"/>
+      <c r="E91" s="52"/>
+      <c r="F91" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="G91" s="4">
         <v>1</v>
       </c>
-      <c r="H90" s="4">
+      <c r="H91" s="4">
         <v>2</v>
       </c>
-      <c r="I90" s="55">
+      <c r="I91" s="55">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="J90" s="48">
+      <c r="J91" s="48">
         <v>1.5</v>
       </c>
-      <c r="K90" s="48">
-        <v>0</v>
-      </c>
-      <c r="L90" s="48">
-        <v>0</v>
-      </c>
-      <c r="M90" s="48">
-        <v>0</v>
-      </c>
-      <c r="N90" s="48">
-        <v>0</v>
-      </c>
-      <c r="O90" s="48">
-        <v>0</v>
-      </c>
-      <c r="P90" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q90" s="48">
-        <v>0</v>
-      </c>
-      <c r="R90" s="48">
-        <v>0</v>
-      </c>
-      <c r="S90" s="48">
-        <v>0</v>
-      </c>
-      <c r="T90" s="48">
-        <v>0</v>
-      </c>
-      <c r="U90" s="48">
-        <v>0</v>
-      </c>
-      <c r="V90" s="48">
-        <v>0</v>
-      </c>
-      <c r="W90" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="107"/>
-      <c r="C91" s="75" t="s">
-        <v>113</v>
-      </c>
-      <c r="D91" s="42"/>
-      <c r="E91" s="54"/>
-      <c r="F91" s="54" t="s">
+      <c r="K91" s="48">
+        <v>0</v>
+      </c>
+      <c r="L91" s="48">
+        <v>0</v>
+      </c>
+      <c r="M91" s="48">
+        <v>0</v>
+      </c>
+      <c r="N91" s="48">
+        <v>0</v>
+      </c>
+      <c r="O91" s="48">
+        <v>0</v>
+      </c>
+      <c r="P91" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q91" s="48">
+        <v>0</v>
+      </c>
+      <c r="R91" s="48">
+        <v>0</v>
+      </c>
+      <c r="S91" s="48">
+        <v>0</v>
+      </c>
+      <c r="T91" s="48">
+        <v>0</v>
+      </c>
+      <c r="U91" s="48">
+        <v>0</v>
+      </c>
+      <c r="V91" s="48">
+        <v>0</v>
+      </c>
+      <c r="W91" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="107"/>
+      <c r="C92" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="D92" s="42"/>
+      <c r="E92" s="54"/>
+      <c r="F92" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="G91" s="4">
+      <c r="G92" s="4">
         <v>4</v>
       </c>
-      <c r="H91" s="4">
+      <c r="H92" s="4">
         <v>1</v>
       </c>
-      <c r="I91" s="55">
-        <f>SUM(J91:W91)</f>
-        <v>0</v>
-      </c>
-      <c r="J91" s="71">
-        <v>0</v>
-      </c>
-      <c r="K91" s="71">
-        <v>0</v>
-      </c>
-      <c r="L91" s="71">
-        <v>0</v>
-      </c>
-      <c r="M91" s="71">
-        <v>0</v>
-      </c>
-      <c r="N91" s="71">
-        <v>0</v>
-      </c>
-      <c r="O91" s="71">
-        <v>0</v>
-      </c>
-      <c r="P91" s="71">
-        <v>0</v>
-      </c>
-      <c r="Q91" s="28"/>
-      <c r="R91" s="29"/>
-      <c r="S91" s="29"/>
-      <c r="T91" s="29"/>
-      <c r="U91" s="29"/>
-      <c r="V91" s="29"/>
-      <c r="W91" s="30"/>
-    </row>
-    <row r="92" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="126" t="s">
-        <v>92</v>
-      </c>
-      <c r="C92" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="D92" s="39"/>
-      <c r="E92" s="38"/>
-      <c r="F92" s="38" t="s">
+      <c r="I92" s="55">
+        <f>SUM(J92:W92)</f>
+        <v>0</v>
+      </c>
+      <c r="J92" s="71">
+        <v>0</v>
+      </c>
+      <c r="K92" s="71">
+        <v>0</v>
+      </c>
+      <c r="L92" s="71">
+        <v>0</v>
+      </c>
+      <c r="M92" s="71">
+        <v>0</v>
+      </c>
+      <c r="N92" s="71">
+        <v>0</v>
+      </c>
+      <c r="O92" s="71">
+        <v>0</v>
+      </c>
+      <c r="P92" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="28"/>
+      <c r="R92" s="29"/>
+      <c r="S92" s="29"/>
+      <c r="T92" s="29"/>
+      <c r="U92" s="29"/>
+      <c r="V92" s="29"/>
+      <c r="W92" s="30"/>
+    </row>
+    <row r="93" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="125" t="s">
+        <v>91</v>
+      </c>
+      <c r="C93" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" s="39"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G92" s="12">
+      <c r="G93" s="12">
         <v>6</v>
       </c>
-      <c r="H92" s="12">
+      <c r="H93" s="12">
         <v>0.75</v>
-      </c>
-      <c r="I92" s="57">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J92" s="70">
-        <v>0</v>
-      </c>
-      <c r="K92" s="70">
-        <v>0</v>
-      </c>
-      <c r="L92" s="70">
-        <v>0</v>
-      </c>
-      <c r="M92" s="70">
-        <v>0</v>
-      </c>
-      <c r="N92" s="70">
-        <v>0</v>
-      </c>
-      <c r="O92" s="70">
-        <v>0</v>
-      </c>
-      <c r="P92" s="70">
-        <v>0</v>
-      </c>
-      <c r="Q92" s="25"/>
-      <c r="R92" s="25"/>
-      <c r="S92" s="25"/>
-      <c r="T92" s="25"/>
-      <c r="U92" s="25"/>
-      <c r="V92" s="25"/>
-      <c r="W92" s="67"/>
-    </row>
-    <row r="93" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="127"/>
-      <c r="C93" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="D93" s="40"/>
-      <c r="E93" s="41"/>
-      <c r="F93" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="G93" s="36">
-        <v>6</v>
-      </c>
-      <c r="H93" s="36">
-        <v>1.5</v>
       </c>
       <c r="I93" s="57">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J93" s="73">
-        <v>0</v>
-      </c>
-      <c r="K93" s="73">
-        <v>0</v>
-      </c>
-      <c r="L93" s="73">
-        <v>0</v>
-      </c>
-      <c r="M93" s="73">
-        <v>0</v>
-      </c>
-      <c r="N93" s="73">
-        <v>0</v>
-      </c>
-      <c r="O93" s="73">
-        <v>0</v>
-      </c>
-      <c r="P93" s="73">
-        <v>0</v>
-      </c>
-      <c r="Q93" s="35"/>
-      <c r="R93" s="35"/>
-      <c r="S93" s="35"/>
-      <c r="T93" s="35"/>
-      <c r="U93" s="35"/>
-      <c r="V93" s="35"/>
-      <c r="W93" s="66"/>
+      <c r="J93" s="70">
+        <v>0</v>
+      </c>
+      <c r="K93" s="70">
+        <v>0</v>
+      </c>
+      <c r="L93" s="70">
+        <v>0</v>
+      </c>
+      <c r="M93" s="70">
+        <v>0</v>
+      </c>
+      <c r="N93" s="70">
+        <v>0</v>
+      </c>
+      <c r="O93" s="70">
+        <v>0</v>
+      </c>
+      <c r="P93" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="25"/>
+      <c r="R93" s="25"/>
+      <c r="S93" s="25"/>
+      <c r="T93" s="25"/>
+      <c r="U93" s="25"/>
+      <c r="V93" s="25"/>
+      <c r="W93" s="67"/>
     </row>
     <row r="94" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="128"/>
-      <c r="C94" s="105" t="s">
-        <v>108</v>
-      </c>
-      <c r="D94" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="E94" s="54"/>
-      <c r="F94" s="54" t="s">
+      <c r="B94" s="126"/>
+      <c r="C94" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D94" s="40"/>
+      <c r="E94" s="41"/>
+      <c r="F94" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="G94" s="4">
+      <c r="G94" s="36">
         <v>6</v>
       </c>
-      <c r="H94" s="4">
-        <v>1</v>
-      </c>
-      <c r="I94" s="55">
+      <c r="H94" s="36">
+        <v>1.5</v>
+      </c>
+      <c r="I94" s="57">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J94" s="71">
-        <v>0</v>
-      </c>
-      <c r="K94" s="71">
-        <v>0</v>
-      </c>
-      <c r="L94" s="71">
-        <v>0</v>
-      </c>
-      <c r="M94" s="71">
-        <v>0</v>
-      </c>
-      <c r="N94" s="71">
-        <v>0</v>
-      </c>
-      <c r="O94" s="71">
-        <v>0</v>
-      </c>
-      <c r="P94" s="71">
-        <v>0</v>
-      </c>
-      <c r="Q94" s="28"/>
-      <c r="R94" s="28"/>
-      <c r="S94" s="28"/>
-      <c r="T94" s="28"/>
-      <c r="U94" s="28"/>
-      <c r="V94" s="28"/>
-      <c r="W94" s="58"/>
-    </row>
-    <row r="95" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B95" s="129"/>
-      <c r="C95" s="105"/>
+      <c r="J94" s="73">
+        <v>0</v>
+      </c>
+      <c r="K94" s="73">
+        <v>0</v>
+      </c>
+      <c r="L94" s="73">
+        <v>0</v>
+      </c>
+      <c r="M94" s="73">
+        <v>0</v>
+      </c>
+      <c r="N94" s="73">
+        <v>0</v>
+      </c>
+      <c r="O94" s="73">
+        <v>0</v>
+      </c>
+      <c r="P94" s="73">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="35"/>
+      <c r="R94" s="35"/>
+      <c r="S94" s="35"/>
+      <c r="T94" s="35"/>
+      <c r="U94" s="35"/>
+      <c r="V94" s="35"/>
+      <c r="W94" s="66"/>
+    </row>
+    <row r="95" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="127"/>
+      <c r="C95" s="137" t="s">
+        <v>107</v>
+      </c>
       <c r="D95" s="42" t="s">
         <v>109</v>
       </c>
@@ -6805,7 +6832,7 @@
         <v>6</v>
       </c>
       <c r="H95" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I95" s="55">
         <f t="shared" si="1"/>
@@ -6835,162 +6862,162 @@
       <c r="Q95" s="28"/>
       <c r="R95" s="28"/>
       <c r="S95" s="28"/>
-      <c r="T95" s="29"/>
-      <c r="U95" s="29"/>
-      <c r="V95" s="29"/>
+      <c r="T95" s="28"/>
+      <c r="U95" s="28"/>
+      <c r="V95" s="28"/>
       <c r="W95" s="58"/>
     </row>
-    <row r="96" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="130"/>
-      <c r="C96" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="D96" s="43"/>
-      <c r="E96" s="44"/>
-      <c r="F96" s="44" t="s">
+    <row r="96" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B96" s="128"/>
+      <c r="C96" s="137"/>
+      <c r="D96" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E96" s="54"/>
+      <c r="F96" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="G96" s="11">
+      <c r="G96" s="4">
+        <v>6</v>
+      </c>
+      <c r="H96" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I96" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J96" s="71">
+        <v>0</v>
+      </c>
+      <c r="K96" s="71">
+        <v>0</v>
+      </c>
+      <c r="L96" s="71">
+        <v>0</v>
+      </c>
+      <c r="M96" s="71">
+        <v>0</v>
+      </c>
+      <c r="N96" s="71">
+        <v>0</v>
+      </c>
+      <c r="O96" s="71">
+        <v>0</v>
+      </c>
+      <c r="P96" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="28"/>
+      <c r="R96" s="28"/>
+      <c r="S96" s="28"/>
+      <c r="T96" s="29"/>
+      <c r="U96" s="29"/>
+      <c r="V96" s="29"/>
+      <c r="W96" s="58"/>
+    </row>
+    <row r="97" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="129"/>
+      <c r="C97" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="D97" s="43"/>
+      <c r="E97" s="44"/>
+      <c r="F97" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G97" s="11">
         <v>1</v>
       </c>
-      <c r="H96" s="11">
+      <c r="H97" s="11">
         <v>1</v>
       </c>
-      <c r="I96" s="59">
+      <c r="I97" s="59">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="J96" s="72">
-        <v>0</v>
-      </c>
-      <c r="K96" s="72">
-        <v>0</v>
-      </c>
-      <c r="L96" s="72">
-        <v>0</v>
-      </c>
-      <c r="M96" s="94">
+      <c r="J97" s="72">
+        <v>0</v>
+      </c>
+      <c r="K97" s="72">
+        <v>0</v>
+      </c>
+      <c r="L97" s="72">
+        <v>0</v>
+      </c>
+      <c r="M97" s="94">
         <v>0.75</v>
       </c>
-      <c r="N96" s="94">
-        <v>0</v>
-      </c>
-      <c r="O96" s="94">
-        <v>0</v>
-      </c>
-      <c r="P96" s="94">
-        <v>0</v>
-      </c>
-      <c r="Q96" s="32"/>
-      <c r="R96" s="32"/>
-      <c r="S96" s="32"/>
-      <c r="T96" s="32"/>
-      <c r="U96" s="32"/>
-      <c r="V96" s="32"/>
-      <c r="W96" s="64"/>
-    </row>
-    <row r="97" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="106" t="s">
-        <v>93</v>
-      </c>
-      <c r="C97" s="63" t="s">
-        <v>117</v>
-      </c>
-      <c r="D97" s="62"/>
-      <c r="E97" s="63"/>
-      <c r="F97" s="63" t="s">
+      <c r="N97" s="94">
+        <v>0</v>
+      </c>
+      <c r="O97" s="94">
+        <v>0</v>
+      </c>
+      <c r="P97" s="94">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="32"/>
+      <c r="R97" s="32"/>
+      <c r="S97" s="32"/>
+      <c r="T97" s="32"/>
+      <c r="U97" s="32"/>
+      <c r="V97" s="32"/>
+      <c r="W97" s="64"/>
+    </row>
+    <row r="98" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="106" t="s">
+        <v>92</v>
+      </c>
+      <c r="C98" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="D98" s="62"/>
+      <c r="E98" s="63"/>
+      <c r="F98" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="G97" s="12">
+      <c r="G98" s="12">
         <v>1</v>
       </c>
-      <c r="H97" s="12">
+      <c r="H98" s="12">
         <v>1.5</v>
       </c>
-      <c r="I97" s="57">
+      <c r="I98" s="57">
         <f t="shared" si="1"/>
         <v>0.46700000000000003</v>
       </c>
-      <c r="J97" s="70">
-        <v>0</v>
-      </c>
-      <c r="K97" s="70">
-        <v>0</v>
-      </c>
-      <c r="L97" s="70">
-        <v>0</v>
-      </c>
-      <c r="M97" s="86">
+      <c r="J98" s="70">
+        <v>0</v>
+      </c>
+      <c r="K98" s="70">
+        <v>0</v>
+      </c>
+      <c r="L98" s="70">
+        <v>0</v>
+      </c>
+      <c r="M98" s="86">
         <v>0.46700000000000003</v>
       </c>
-      <c r="N97" s="86">
-        <v>0</v>
-      </c>
-      <c r="O97" s="86">
-        <v>0</v>
-      </c>
-      <c r="P97" s="86">
-        <v>0</v>
-      </c>
-      <c r="Q97" s="26"/>
-      <c r="R97" s="26"/>
-      <c r="S97" s="26"/>
-      <c r="T97" s="26"/>
-      <c r="U97" s="26"/>
-      <c r="V97" s="26"/>
-      <c r="W97" s="27"/>
-    </row>
-    <row r="98" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B98" s="129"/>
-      <c r="C98" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="D98" s="42"/>
-      <c r="E98" s="54"/>
-      <c r="F98" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="G98" s="4">
-        <v>1</v>
-      </c>
-      <c r="H98" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="I98" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J98" s="71">
-        <v>0</v>
-      </c>
-      <c r="K98" s="71">
-        <v>0</v>
-      </c>
-      <c r="L98" s="71">
-        <v>0</v>
-      </c>
-      <c r="M98" s="95">
-        <v>0</v>
-      </c>
-      <c r="N98" s="95">
-        <v>0</v>
-      </c>
-      <c r="O98" s="131">
-        <v>0</v>
-      </c>
-      <c r="P98" s="131">
-        <v>0</v>
-      </c>
-      <c r="Q98" s="29"/>
-      <c r="R98" s="29"/>
-      <c r="S98" s="29"/>
-      <c r="T98" s="29"/>
-      <c r="U98" s="29"/>
-      <c r="V98" s="29"/>
-      <c r="W98" s="30"/>
+      <c r="N98" s="86">
+        <v>0</v>
+      </c>
+      <c r="O98" s="86">
+        <v>0</v>
+      </c>
+      <c r="P98" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q98" s="26"/>
+      <c r="R98" s="26"/>
+      <c r="S98" s="26"/>
+      <c r="T98" s="26"/>
+      <c r="U98" s="26"/>
+      <c r="V98" s="26"/>
+      <c r="W98" s="27"/>
     </row>
     <row r="99" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B99" s="129"/>
+      <c r="B99" s="128"/>
       <c r="C99" s="54" t="s">
         <v>130</v>
       </c>
@@ -7007,7 +7034,7 @@
       </c>
       <c r="I99" s="55">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J99" s="71">
         <v>0</v>
@@ -7024,10 +7051,10 @@
       <c r="N99" s="95">
         <v>0</v>
       </c>
-      <c r="O99" s="97">
-        <v>1</v>
-      </c>
-      <c r="P99" s="135">
+      <c r="O99" s="99">
+        <v>0</v>
+      </c>
+      <c r="P99" s="99">
         <v>0</v>
       </c>
       <c r="Q99" s="29"/>
@@ -7039,7 +7066,7 @@
       <c r="W99" s="30"/>
     </row>
     <row r="100" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B100" s="129"/>
+      <c r="B100" s="128"/>
       <c r="C100" s="54" t="s">
         <v>129</v>
       </c>
@@ -7056,7 +7083,7 @@
       </c>
       <c r="I100" s="55">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J100" s="71">
         <v>0</v>
@@ -7074,9 +7101,9 @@
         <v>0</v>
       </c>
       <c r="O100" s="97">
-        <v>0.1</v>
-      </c>
-      <c r="P100" s="97">
+        <v>1</v>
+      </c>
+      <c r="P100" s="103">
         <v>0</v>
       </c>
       <c r="Q100" s="29"/>
@@ -7088,7 +7115,7 @@
       <c r="W100" s="30"/>
     </row>
     <row r="101" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B101" s="129"/>
+      <c r="B101" s="128"/>
       <c r="C101" s="54" t="s">
         <v>128</v>
       </c>
@@ -7098,14 +7125,14 @@
         <v>16</v>
       </c>
       <c r="G101" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H101" s="4">
         <v>0.33</v>
       </c>
       <c r="I101" s="55">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J101" s="71">
         <v>0</v>
@@ -7116,16 +7143,16 @@
       <c r="L101" s="71">
         <v>0</v>
       </c>
-      <c r="M101" s="71">
-        <v>0</v>
-      </c>
-      <c r="N101" s="71">
-        <v>0</v>
-      </c>
-      <c r="O101" s="71">
-        <v>0</v>
-      </c>
-      <c r="P101" s="71">
+      <c r="M101" s="95">
+        <v>0</v>
+      </c>
+      <c r="N101" s="95">
+        <v>0</v>
+      </c>
+      <c r="O101" s="97">
+        <v>0.1</v>
+      </c>
+      <c r="P101" s="97">
         <v>0</v>
       </c>
       <c r="Q101" s="29"/>
@@ -7136,335 +7163,370 @@
       <c r="V101" s="29"/>
       <c r="W101" s="30"/>
     </row>
-    <row r="102" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="130"/>
-      <c r="C102" s="44" t="s">
+    <row r="102" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B102" s="128"/>
+      <c r="C102" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="D102" s="43"/>
-      <c r="E102" s="44"/>
-      <c r="F102" s="44" t="s">
+      <c r="D102" s="42"/>
+      <c r="E102" s="54"/>
+      <c r="F102" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="G102" s="11">
+      <c r="G102" s="4">
+        <v>3</v>
+      </c>
+      <c r="H102" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="I102" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J102" s="71">
+        <v>0</v>
+      </c>
+      <c r="K102" s="71">
+        <v>0</v>
+      </c>
+      <c r="L102" s="71">
+        <v>0</v>
+      </c>
+      <c r="M102" s="71">
+        <v>0</v>
+      </c>
+      <c r="N102" s="71">
+        <v>0</v>
+      </c>
+      <c r="O102" s="71">
+        <v>0</v>
+      </c>
+      <c r="P102" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q102" s="29"/>
+      <c r="R102" s="29"/>
+      <c r="S102" s="29"/>
+      <c r="T102" s="29"/>
+      <c r="U102" s="29"/>
+      <c r="V102" s="29"/>
+      <c r="W102" s="30"/>
+    </row>
+    <row r="103" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="129"/>
+      <c r="C103" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D103" s="43"/>
+      <c r="E103" s="44"/>
+      <c r="F103" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G103" s="11">
         <v>1</v>
       </c>
-      <c r="H102" s="11">
+      <c r="H103" s="11">
         <v>3</v>
       </c>
-      <c r="I102" s="59">
-        <f t="shared" ref="I102" si="3">SUM(J102:W102)</f>
-        <v>0</v>
-      </c>
-      <c r="J102" s="72">
-        <v>0</v>
-      </c>
-      <c r="K102" s="72">
-        <v>0</v>
-      </c>
-      <c r="L102" s="72">
-        <v>0</v>
-      </c>
-      <c r="M102" s="72">
-        <v>0</v>
-      </c>
-      <c r="N102" s="136" t="s">
-        <v>132</v>
-      </c>
-      <c r="O102" s="136">
-        <v>0</v>
-      </c>
-      <c r="P102" s="137">
-        <v>0</v>
-      </c>
-      <c r="Q102" s="33"/>
-      <c r="R102" s="33"/>
-      <c r="S102" s="33"/>
-      <c r="T102" s="33"/>
-      <c r="U102" s="33"/>
-      <c r="V102" s="33"/>
-      <c r="W102" s="34"/>
-    </row>
-    <row r="103" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="121" t="s">
+      <c r="I103" s="59">
+        <f t="shared" ref="I103" si="3">SUM(J103:W103)</f>
+        <v>0</v>
+      </c>
+      <c r="J103" s="72">
+        <v>0</v>
+      </c>
+      <c r="K103" s="72">
+        <v>0</v>
+      </c>
+      <c r="L103" s="72">
+        <v>0</v>
+      </c>
+      <c r="M103" s="72">
+        <v>0</v>
+      </c>
+      <c r="N103" s="104" t="s">
+        <v>131</v>
+      </c>
+      <c r="O103" s="104">
+        <v>0</v>
+      </c>
+      <c r="P103" s="105">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="33"/>
+      <c r="R103" s="33"/>
+      <c r="S103" s="33"/>
+      <c r="T103" s="33"/>
+      <c r="U103" s="33"/>
+      <c r="V103" s="33"/>
+      <c r="W103" s="34"/>
+    </row>
+    <row r="104" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B104" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="C103" s="122"/>
-      <c r="D103" s="122"/>
-      <c r="E103" s="122"/>
-      <c r="F103" s="122"/>
-      <c r="G103" s="122"/>
-      <c r="H103" s="17">
-        <f t="shared" ref="H103:W103" si="4">SUM(H4:H102)</f>
-        <v>48.72</v>
-      </c>
-      <c r="I103" s="17">
-        <f t="shared" si="4"/>
-        <v>19.023000000000003</v>
-      </c>
-      <c r="J103" s="17">
-        <f t="shared" si="4"/>
+      <c r="C104" s="122"/>
+      <c r="D104" s="122"/>
+      <c r="E104" s="122"/>
+      <c r="F104" s="122"/>
+      <c r="G104" s="122"/>
+      <c r="H104" s="17">
+        <f>SUM(H4:H103)</f>
+        <v>48.120000000000005</v>
+      </c>
+      <c r="I104" s="17">
+        <f>SUM(I4:I103)</f>
+        <v>21.052000000000003</v>
+      </c>
+      <c r="J104" s="17">
+        <f>SUM(J4:J103)</f>
         <v>1.95</v>
       </c>
-      <c r="K103" s="17">
-        <f t="shared" si="4"/>
+      <c r="K104" s="17">
+        <f>SUM(K4:K103)</f>
         <v>3.3</v>
       </c>
-      <c r="L103" s="17">
-        <f>SUM(L4:L102)</f>
+      <c r="L104" s="17">
+        <f>SUM(L4:L103)</f>
         <v>7.15</v>
       </c>
-      <c r="M103" s="17">
-        <f t="shared" si="4"/>
+      <c r="M104" s="17">
+        <f>SUM(M4:M103)</f>
         <v>3.9929999999999999</v>
       </c>
-      <c r="N103" s="17">
-        <f t="shared" si="4"/>
+      <c r="N104" s="17">
+        <f>SUM(N4:N103)</f>
         <v>1.5</v>
       </c>
-      <c r="O103" s="17">
-        <f t="shared" si="4"/>
+      <c r="O104" s="17">
+        <f>SUM(O4:O103)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="P103" s="17">
-        <f t="shared" si="4"/>
+      <c r="P104" s="17">
+        <f>SUM(P4:P103)</f>
         <v>0.03</v>
       </c>
-      <c r="Q103" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R103" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S103" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T103" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="U103" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V103" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="W103" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="112" t="s">
-        <v>11</v>
-      </c>
-      <c r="K104" s="113"/>
-      <c r="L104" s="113"/>
-      <c r="M104" s="113"/>
-      <c r="N104" s="113"/>
-      <c r="O104" s="113"/>
-      <c r="P104" s="113"/>
-      <c r="Q104" s="113"/>
-      <c r="R104" s="113"/>
-      <c r="S104" s="113"/>
-      <c r="T104" s="113"/>
-      <c r="U104" s="113"/>
-      <c r="V104" s="113"/>
-      <c r="W104" s="114"/>
+      <c r="Q104" s="17">
+        <f>SUM(Q4:Q103)</f>
+        <v>2.0290000000000004</v>
+      </c>
+      <c r="R104" s="17">
+        <f>SUM(R4:R103)</f>
+        <v>0</v>
+      </c>
+      <c r="S104" s="17">
+        <f>SUM(S4:S103)</f>
+        <v>0</v>
+      </c>
+      <c r="T104" s="17">
+        <f>SUM(T4:T103)</f>
+        <v>0</v>
+      </c>
+      <c r="U104" s="17">
+        <f>SUM(U4:U103)</f>
+        <v>0</v>
+      </c>
+      <c r="V104" s="17">
+        <f>SUM(V4:V103)</f>
+        <v>0</v>
+      </c>
+      <c r="W104" s="18">
+        <f>SUM(W4:W103)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="105" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="C105" s="77" t="s">
-        <v>121</v>
-      </c>
-      <c r="D105" s="77" t="s">
-        <v>122</v>
-      </c>
-      <c r="E105" s="78" t="s">
-        <v>123</v>
-      </c>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
-      <c r="J105" s="3"/>
-      <c r="K105" s="3"/>
-      <c r="L105" s="3"/>
-      <c r="M105" s="3"/>
-      <c r="O105" s="9"/>
-      <c r="P105" s="9"/>
+      <c r="J105" s="112" t="s">
+        <v>11</v>
+      </c>
+      <c r="K105" s="113"/>
+      <c r="L105" s="113"/>
+      <c r="M105" s="113"/>
+      <c r="N105" s="113"/>
+      <c r="O105" s="113"/>
+      <c r="P105" s="113"/>
+      <c r="Q105" s="113"/>
+      <c r="R105" s="113"/>
+      <c r="S105" s="113"/>
+      <c r="T105" s="113"/>
+      <c r="U105" s="113"/>
+      <c r="V105" s="113"/>
+      <c r="W105" s="114"/>
     </row>
     <row r="106" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="C106" s="81">
-        <f>SUM(H7,H9,H40,H91,H92,H93,H94,H95,H96,H98:H102,H40)</f>
-        <v>12.27</v>
-      </c>
-      <c r="D106" s="36">
-        <f>SUM(I98:I102,I91:I96,I9,I7,I40)</f>
-        <v>1.85</v>
-      </c>
-      <c r="E106" s="36">
-        <f>SUM(C106,-D106)</f>
-        <v>10.42</v>
+      <c r="B106" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="C106" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="D106" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="E106" s="78" t="s">
+        <v>122</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="98" t="s">
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="O106" s="9"/>
+      <c r="P106" s="9"/>
+    </row>
+    <row r="107" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B107" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="C107" s="81">
+        <f>SUM(H7,H9,H40,H92,H93,H94,H95,H96,H97,H99:H103,H40)</f>
+        <v>12.27</v>
+      </c>
+      <c r="D107" s="36">
+        <f>SUM(I99:I103,I92:I97,I9,I7,I40)</f>
+        <v>1.85</v>
+      </c>
+      <c r="E107" s="36">
+        <f>SUM(C107,-D107)</f>
+        <v>10.42</v>
+      </c>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="130" t="s">
         <v>9</v>
       </c>
-      <c r="I106" s="101"/>
-      <c r="J106" s="10">
-        <f>H103-J103</f>
-        <v>46.769999999999996</v>
-      </c>
-      <c r="K106" s="10">
-        <f>J106-K103</f>
-        <v>43.47</v>
-      </c>
-      <c r="L106" s="10">
-        <f>K106-L103</f>
-        <v>36.32</v>
-      </c>
-      <c r="M106" s="10">
-        <f>L106-M103</f>
-        <v>32.326999999999998</v>
-      </c>
-      <c r="N106" s="10">
-        <f t="shared" ref="N106:W106" si="5">M106-N103</f>
-        <v>30.826999999999998</v>
-      </c>
-      <c r="O106" s="10">
-        <f t="shared" si="5"/>
-        <v>29.726999999999997</v>
-      </c>
-      <c r="P106" s="10">
-        <f t="shared" si="5"/>
-        <v>29.696999999999996</v>
-      </c>
-      <c r="Q106" s="10">
-        <f t="shared" si="5"/>
-        <v>29.696999999999996</v>
-      </c>
-      <c r="R106" s="10">
-        <f t="shared" si="5"/>
-        <v>29.696999999999996</v>
-      </c>
-      <c r="S106" s="10">
-        <f t="shared" si="5"/>
-        <v>29.696999999999996</v>
-      </c>
-      <c r="T106" s="10">
-        <f t="shared" si="5"/>
-        <v>29.696999999999996</v>
-      </c>
-      <c r="U106" s="10">
-        <f t="shared" si="5"/>
-        <v>29.696999999999996</v>
-      </c>
-      <c r="V106" s="10">
-        <f t="shared" si="5"/>
-        <v>29.696999999999996</v>
-      </c>
-      <c r="W106" s="10">
-        <f t="shared" si="5"/>
-        <v>29.696999999999996</v>
-      </c>
-    </row>
-    <row r="107" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="80" t="s">
-        <v>15</v>
-      </c>
-      <c r="C107" s="79">
-        <f>SUM(H4,H84:H89,H97,H17:H36,H10:H15,H8,H6,H5,H90)</f>
-        <v>18.199999999999992</v>
-      </c>
-      <c r="D107" s="5">
-        <f>SUM(I97,I84:I89,I17:I36,I10:I15,I8,I5:I6,I90,I4)</f>
-        <v>5.923</v>
-      </c>
-      <c r="E107" s="5">
-        <f>SUM(C107,-D107)</f>
-        <v>12.276999999999992</v>
-      </c>
-      <c r="F107" s="3"/>
-      <c r="G107" s="3"/>
-      <c r="H107" s="3"/>
-      <c r="I107" s="3"/>
-      <c r="J107" s="3"/>
-      <c r="K107" s="3"/>
-      <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
+      <c r="I107" s="133"/>
+      <c r="J107" s="10">
+        <f>H104-J104</f>
+        <v>46.17</v>
+      </c>
+      <c r="K107" s="10">
+        <f>J107-K104</f>
+        <v>42.870000000000005</v>
+      </c>
+      <c r="L107" s="10">
+        <f>K107-L104</f>
+        <v>35.720000000000006</v>
+      </c>
+      <c r="M107" s="10">
+        <f>L107-M104</f>
+        <v>31.727000000000007</v>
+      </c>
+      <c r="N107" s="10">
+        <f t="shared" ref="N107:W107" si="4">M107-N104</f>
+        <v>30.227000000000007</v>
+      </c>
+      <c r="O107" s="10">
+        <f t="shared" si="4"/>
+        <v>29.127000000000006</v>
+      </c>
+      <c r="P107" s="10">
+        <f t="shared" si="4"/>
+        <v>29.097000000000005</v>
+      </c>
+      <c r="Q107" s="10">
+        <f t="shared" si="4"/>
+        <v>27.068000000000005</v>
+      </c>
+      <c r="R107" s="10">
+        <f t="shared" si="4"/>
+        <v>27.068000000000005</v>
+      </c>
+      <c r="S107" s="10">
+        <f t="shared" si="4"/>
+        <v>27.068000000000005</v>
+      </c>
+      <c r="T107" s="10">
+        <f t="shared" si="4"/>
+        <v>27.068000000000005</v>
+      </c>
+      <c r="U107" s="10">
+        <f t="shared" si="4"/>
+        <v>27.068000000000005</v>
+      </c>
+      <c r="V107" s="10">
+        <f t="shared" si="4"/>
+        <v>27.068000000000005</v>
+      </c>
+      <c r="W107" s="10">
+        <f t="shared" si="4"/>
+        <v>27.068000000000005</v>
+      </c>
     </row>
     <row r="108" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C108" s="79">
+        <f>SUM(H4,H84:H89,H98,H17:H36,H10:H15,H8,H6,H5,H91)</f>
+        <v>17.399999999999991</v>
+      </c>
+      <c r="D108" s="5">
+        <f>SUM(I98,I84:I89,I17:I36,I10:I15,I8,I5:I6,I91,I4)</f>
+        <v>7.7019999999999991</v>
+      </c>
+      <c r="E108" s="5">
+        <f>SUM(C108,-D108)</f>
+        <v>9.6979999999999933</v>
+      </c>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+    </row>
+    <row r="109" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B109" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C108" s="79">
+      <c r="C109" s="79">
         <f>SUM(H41:H83,H37:H39)</f>
         <v>16.75</v>
       </c>
-      <c r="D108" s="5">
+      <c r="D109" s="5">
         <f>SUM(I41:I83,I37:I39,I16)</f>
         <v>11.25</v>
       </c>
-      <c r="E108" s="5">
-        <f>SUM(C108,-D108)</f>
+      <c r="E109" s="5">
+        <f>SUM(C109,-D109)</f>
         <v>5.5</v>
       </c>
-      <c r="F108" s="3"/>
-      <c r="H108" s="98" t="s">
+      <c r="F109" s="3"/>
+      <c r="H109" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="I108" s="99"/>
-      <c r="J108" s="98">
-        <f>H103-I103</f>
-        <v>29.696999999999996</v>
-      </c>
-      <c r="K108" s="99"/>
-      <c r="L108" s="99"/>
-      <c r="M108" s="99"/>
-      <c r="N108" s="99"/>
-      <c r="O108" s="99"/>
-      <c r="P108" s="99"/>
-      <c r="Q108" s="99"/>
-      <c r="R108" s="99"/>
-      <c r="S108" s="99"/>
-      <c r="T108" s="99"/>
-      <c r="U108" s="99"/>
-      <c r="V108" s="99"/>
-      <c r="W108" s="100"/>
-    </row>
-    <row r="109" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
-      <c r="F109" s="3"/>
-      <c r="G109" s="3"/>
-      <c r="H109" s="3"/>
-      <c r="I109" s="3"/>
-      <c r="J109" s="3"/>
-      <c r="K109" s="3"/>
-      <c r="L109" s="3"/>
-      <c r="M109" s="3"/>
+      <c r="I109" s="131"/>
+      <c r="J109" s="130">
+        <f>H104-I104</f>
+        <v>27.068000000000001</v>
+      </c>
+      <c r="K109" s="131"/>
+      <c r="L109" s="131"/>
+      <c r="M109" s="131"/>
+      <c r="N109" s="131"/>
+      <c r="O109" s="131"/>
+      <c r="P109" s="131"/>
+      <c r="Q109" s="131"/>
+      <c r="R109" s="131"/>
+      <c r="S109" s="131"/>
+      <c r="T109" s="131"/>
+      <c r="U109" s="131"/>
+      <c r="V109" s="131"/>
+      <c r="W109" s="132"/>
     </row>
     <row r="110" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B110" s="3"/>
@@ -7494,60 +7556,73 @@
       <c r="L111" s="3"/>
       <c r="M111" s="3"/>
     </row>
-    <row r="112" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="7"/>
-    </row>
-    <row r="118" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="3"/>
+      <c r="M112" s="3"/>
+    </row>
+    <row r="113" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B118" s="7"/>
     </row>
-    <row r="119" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B119" s="7"/>
     </row>
-    <row r="120" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="7"/>
-    </row>
-    <row r="125" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B120" s="7"/>
+    </row>
+    <row r="121" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B125" s="7"/>
     </row>
-    <row r="126" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B126" s="7"/>
     </row>
-    <row r="127" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B127" s="7"/>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B128" s="6"/>
-      <c r="C128" s="6"/>
+    <row r="128" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B128" s="7"/>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B41:B91"/>
+  <mergeCells count="17">
+    <mergeCell ref="J109:W109"/>
+    <mergeCell ref="H107:I107"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="C41:C83"/>
+    <mergeCell ref="C19:C36"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="B41:B92"/>
     <mergeCell ref="C84:C89"/>
     <mergeCell ref="J2:W2"/>
-    <mergeCell ref="J104:W104"/>
+    <mergeCell ref="J105:W105"/>
     <mergeCell ref="B16:B40"/>
     <mergeCell ref="B10:B15"/>
     <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B104:G104"/>
     <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="B97:B102"/>
-    <mergeCell ref="J108:W108"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="C41:C83"/>
-    <mergeCell ref="C20:C36"/>
-    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="B93:B97"/>
+    <mergeCell ref="B98:B103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Establecida animación de muerte de enemigos (OVERWORLD)  actualizado excel
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="130">
   <si>
     <t>Subtarea</t>
   </si>
@@ -227,24 +227,6 @@
     <t>Introducir sonido encontrar secreto</t>
   </si>
   <si>
-    <t>Introducir animación morir Oktorok</t>
-  </si>
-  <si>
-    <t>Introducir animación morir Leever</t>
-  </si>
-  <si>
-    <t>Introducir animación morir Tektite</t>
-  </si>
-  <si>
-    <t>Introducir animación morir River Zola</t>
-  </si>
-  <si>
-    <t>Introducir animación morir Moblin</t>
-  </si>
-  <si>
-    <t>Introducir animación morir Peahat</t>
-  </si>
-  <si>
     <t>Crear prefab Trifuerza</t>
   </si>
   <si>
@@ -426,6 +408,9 @@
   </si>
   <si>
     <t>Introducir spawns sala 14</t>
+  </si>
+  <si>
+    <t>Introducir animación morir</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1418,6 +1403,84 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1440,87 +1503,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1629,51 +1611,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$108:$W$108</c:f>
+              <c:f>Hoja1!$J$103:$W$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>46.370000000000005</c:v>
+                  <c:v>47.169999999999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.070000000000007</c:v>
+                  <c:v>43.86999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.920000000000009</c:v>
+                  <c:v>36.719999999999992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.92700000000001</c:v>
+                  <c:v>32.72699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.42700000000001</c:v>
+                  <c:v>31.22699999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.327000000000009</c:v>
+                  <c:v>30.126999999999988</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.297000000000008</c:v>
+                  <c:v>30.096999999999987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.268000000000008</c:v>
+                  <c:v>28.067999999999987</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25.785300000000007</c:v>
+                  <c:v>26.585299999999986</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.068300000000008</c:v>
+                  <c:v>21.868299999999984</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.918300000000009</c:v>
+                  <c:v>15.238299999999985</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15.918300000000009</c:v>
+                  <c:v>15.238299999999985</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15.918300000000009</c:v>
+                  <c:v>15.238299999999985</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15.918300000000009</c:v>
+                  <c:v>15.238299999999985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2109,10 +2091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W130"/>
+  <dimension ref="A1:W125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q104" sqref="Q104:T104"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T85" sqref="T85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2134,29 +2116,29 @@
   <sheetData>
     <row r="1" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B1" s="74" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="113" t="s">
+      <c r="J2" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="114"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="114"/>
-      <c r="R2" s="114"/>
-      <c r="S2" s="114"/>
-      <c r="T2" s="114"/>
-      <c r="U2" s="114"/>
-      <c r="V2" s="114"/>
-      <c r="W2" s="115"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="108"/>
+      <c r="Q2" s="108"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="108"/>
+      <c r="T2" s="108"/>
+      <c r="U2" s="108"/>
+      <c r="V2" s="108"/>
+      <c r="W2" s="109"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
@@ -2227,7 +2209,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="113" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="78" t="s">
@@ -2294,7 +2276,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="120"/>
+      <c r="B5" s="114"/>
       <c r="C5" s="37" t="s">
         <v>58</v>
       </c>
@@ -2357,9 +2339,9 @@
       </c>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="120"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="37" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="43"/>
@@ -2420,8 +2402,8 @@
       </c>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="120"/>
-      <c r="C7" s="127" t="s">
+      <c r="B7" s="114"/>
+      <c r="C7" s="121" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="33" t="s">
@@ -2485,8 +2467,8 @@
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="120"/>
-      <c r="C8" s="127"/>
+      <c r="B8" s="114"/>
+      <c r="C8" s="121"/>
       <c r="D8" s="37" t="s">
         <v>61</v>
       </c>
@@ -2548,8 +2530,8 @@
       </c>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="124"/>
-      <c r="C9" s="128"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="122"/>
       <c r="D9" s="34" t="s">
         <v>62</v>
       </c>
@@ -2606,12 +2588,12 @@
       <c r="V9" s="97">
         <v>0</v>
       </c>
-      <c r="W9" s="135">
+      <c r="W9" s="103">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="121" t="s">
+      <c r="B10" s="115" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="42" t="s">
@@ -2676,7 +2658,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="122"/>
+      <c r="B11" s="116"/>
       <c r="C11" s="37" t="s">
         <v>65</v>
       </c>
@@ -2730,7 +2712,7 @@
       <c r="W11" s="26"/>
     </row>
     <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="122"/>
+      <c r="B12" s="116"/>
       <c r="C12" s="37" t="s">
         <v>66</v>
       </c>
@@ -2793,9 +2775,9 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="123"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="36" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="44"/>
@@ -2842,7 +2824,7 @@
       <c r="S13" s="64">
         <v>0</v>
       </c>
-      <c r="T13" s="136">
+      <c r="T13" s="104">
         <v>0.15</v>
       </c>
       <c r="U13" s="83">
@@ -2856,9 +2838,9 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="123"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="36" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="44"/>
@@ -2911,7 +2893,7 @@
       <c r="W14" s="59"/>
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="123"/>
+      <c r="B15" s="117"/>
       <c r="C15" s="36" t="s">
         <v>67</v>
       </c>
@@ -2966,11 +2948,11 @@
       <c r="W15" s="59"/>
     </row>
     <row r="16" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="119" t="s">
+      <c r="B16" s="113" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
@@ -3031,7 +3013,7 @@
       </c>
     </row>
     <row r="17" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="120"/>
+      <c r="B17" s="114"/>
       <c r="C17" s="37" t="s">
         <v>36</v>
       </c>
@@ -3094,7 +3076,7 @@
       </c>
     </row>
     <row r="18" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="120"/>
+      <c r="B18" s="114"/>
       <c r="C18" s="88" t="s">
         <v>14</v>
       </c>
@@ -3159,8 +3141,8 @@
       </c>
     </row>
     <row r="19" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="120"/>
-      <c r="C19" s="108" t="s">
+      <c r="B19" s="114"/>
+      <c r="C19" s="134" t="s">
         <v>37</v>
       </c>
       <c r="D19" s="37" t="s">
@@ -3224,10 +3206,10 @@
       </c>
     </row>
     <row r="20" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="120"/>
-      <c r="C20" s="108"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="134"/>
       <c r="D20" s="37" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="37" t="s">
@@ -3287,8 +3269,8 @@
       </c>
     </row>
     <row r="21" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="120"/>
-      <c r="C21" s="108"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="37" t="s">
         <v>34</v>
       </c>
@@ -3342,8 +3324,8 @@
       <c r="W21" s="22"/>
     </row>
     <row r="22" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="120"/>
-      <c r="C22" s="108"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="134"/>
       <c r="D22" s="37" t="s">
         <v>35</v>
       </c>
@@ -3405,8 +3387,8 @@
       </c>
     </row>
     <row r="23" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="120"/>
-      <c r="C23" s="108"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="134"/>
       <c r="D23" s="37" t="s">
         <v>39</v>
       </c>
@@ -3468,8 +3450,8 @@
       </c>
     </row>
     <row r="24" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="120"/>
-      <c r="C24" s="108"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="134"/>
       <c r="D24" s="37" t="s">
         <v>40</v>
       </c>
@@ -3531,8 +3513,8 @@
       </c>
     </row>
     <row r="25" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="120"/>
-      <c r="C25" s="108"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="134"/>
       <c r="D25" s="37" t="s">
         <v>41</v>
       </c>
@@ -3594,8 +3576,8 @@
       </c>
     </row>
     <row r="26" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="120"/>
-      <c r="C26" s="108"/>
+      <c r="B26" s="114"/>
+      <c r="C26" s="134"/>
       <c r="D26" s="37" t="s">
         <v>42</v>
       </c>
@@ -3657,8 +3639,8 @@
       </c>
     </row>
     <row r="27" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="120"/>
-      <c r="C27" s="108"/>
+      <c r="B27" s="114"/>
+      <c r="C27" s="134"/>
       <c r="D27" s="37" t="s">
         <v>43</v>
       </c>
@@ -3720,8 +3702,8 @@
       </c>
     </row>
     <row r="28" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="120"/>
-      <c r="C28" s="108"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="134"/>
       <c r="D28" s="37" t="s">
         <v>44</v>
       </c>
@@ -3783,8 +3765,8 @@
       </c>
     </row>
     <row r="29" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="120"/>
-      <c r="C29" s="108"/>
+      <c r="B29" s="114"/>
+      <c r="C29" s="134"/>
       <c r="D29" s="37" t="s">
         <v>45</v>
       </c>
@@ -3846,8 +3828,8 @@
       </c>
     </row>
     <row r="30" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="120"/>
-      <c r="C30" s="108"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="134"/>
       <c r="D30" s="37" t="s">
         <v>46</v>
       </c>
@@ -3909,8 +3891,8 @@
       </c>
     </row>
     <row r="31" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="120"/>
-      <c r="C31" s="108"/>
+      <c r="B31" s="114"/>
+      <c r="C31" s="134"/>
       <c r="D31" s="37" t="s">
         <v>47</v>
       </c>
@@ -3972,8 +3954,8 @@
       </c>
     </row>
     <row r="32" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="120"/>
-      <c r="C32" s="108"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="134"/>
       <c r="D32" s="37" t="s">
         <v>48</v>
       </c>
@@ -4035,8 +4017,8 @@
       </c>
     </row>
     <row r="33" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="120"/>
-      <c r="C33" s="108"/>
+      <c r="B33" s="114"/>
+      <c r="C33" s="134"/>
       <c r="D33" s="37" t="s">
         <v>49</v>
       </c>
@@ -4098,8 +4080,8 @@
       </c>
     </row>
     <row r="34" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="120"/>
-      <c r="C34" s="108"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="134"/>
       <c r="D34" s="37" t="s">
         <v>50</v>
       </c>
@@ -4161,8 +4143,8 @@
       </c>
     </row>
     <row r="35" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="120"/>
-      <c r="C35" s="108"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="134"/>
       <c r="D35" s="37" t="s">
         <v>51</v>
       </c>
@@ -4224,10 +4206,10 @@
       </c>
     </row>
     <row r="36" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="120"/>
-      <c r="C36" s="108"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="134"/>
       <c r="D36" s="37" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E36" s="37"/>
       <c r="F36" s="37" t="s">
@@ -4287,10 +4269,10 @@
       </c>
     </row>
     <row r="37" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="120"/>
-      <c r="C37" s="108"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="134"/>
       <c r="D37" s="43" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E37" s="43"/>
       <c r="F37" s="43" t="s">
@@ -4333,7 +4315,7 @@
       <c r="R37" s="61">
         <v>0</v>
       </c>
-      <c r="S37" s="134">
+      <c r="S37" s="102">
         <v>0.317</v>
       </c>
       <c r="T37" s="87">
@@ -4350,7 +4332,7 @@
       </c>
     </row>
     <row r="38" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="120"/>
+      <c r="B38" s="114"/>
       <c r="C38" s="40" t="s">
         <v>52</v>
       </c>
@@ -4405,7 +4387,7 @@
       <c r="W38" s="22"/>
     </row>
     <row r="39" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="120"/>
+      <c r="B39" s="114"/>
       <c r="C39" s="40" t="s">
         <v>54</v>
       </c>
@@ -4460,7 +4442,7 @@
       <c r="W39" s="22"/>
     </row>
     <row r="40" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="120"/>
+      <c r="B40" s="114"/>
       <c r="C40" s="40" t="s">
         <v>55</v>
       </c>
@@ -4523,9 +4505,9 @@
       </c>
     </row>
     <row r="41" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="120"/>
+      <c r="B41" s="114"/>
       <c r="C41" s="47" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D41" s="47"/>
       <c r="E41" s="47"/>
@@ -4578,10 +4560,10 @@
       <c r="W41" s="22"/>
     </row>
     <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="110" t="s">
+      <c r="B42" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="106" t="s">
+      <c r="C42" s="132" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="41" t="s">
@@ -4598,7 +4580,7 @@
         <v>0.5</v>
       </c>
       <c r="I42" s="48">
-        <f t="shared" ref="I42:I103" si="2">SUM(J42:W42)</f>
+        <f t="shared" ref="I42:I98" si="2">SUM(J42:W42)</f>
         <v>0.95</v>
       </c>
       <c r="J42" s="92">
@@ -4645,8 +4627,8 @@
       </c>
     </row>
     <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="111"/>
-      <c r="C43" s="107"/>
+      <c r="B43" s="106"/>
+      <c r="C43" s="133"/>
       <c r="D43" s="40" t="s">
         <v>21</v>
       </c>
@@ -4700,8 +4682,8 @@
       <c r="W43" s="22"/>
     </row>
     <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="111"/>
-      <c r="C44" s="107"/>
+      <c r="B44" s="106"/>
+      <c r="C44" s="133"/>
       <c r="D44" s="40" t="s">
         <v>22</v>
       </c>
@@ -4755,8 +4737,8 @@
       <c r="W44" s="22"/>
     </row>
     <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="111"/>
-      <c r="C45" s="107"/>
+      <c r="B45" s="106"/>
+      <c r="C45" s="133"/>
       <c r="D45" s="40" t="s">
         <v>23</v>
       </c>
@@ -4810,8 +4792,8 @@
       <c r="W45" s="22"/>
     </row>
     <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="111"/>
-      <c r="C46" s="107"/>
+      <c r="B46" s="106"/>
+      <c r="C46" s="133"/>
       <c r="D46" s="40" t="s">
         <v>24</v>
       </c>
@@ -4865,8 +4847,8 @@
       <c r="W46" s="22"/>
     </row>
     <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="111"/>
-      <c r="C47" s="107"/>
+      <c r="B47" s="106"/>
+      <c r="C47" s="133"/>
       <c r="D47" s="40" t="s">
         <v>25</v>
       </c>
@@ -4920,8 +4902,8 @@
       <c r="W47" s="22"/>
     </row>
     <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="111"/>
-      <c r="C48" s="107"/>
+      <c r="B48" s="106"/>
+      <c r="C48" s="133"/>
       <c r="D48" s="40" t="s">
         <v>26</v>
       </c>
@@ -4975,8 +4957,8 @@
       <c r="W48" s="22"/>
     </row>
     <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="111"/>
-      <c r="C49" s="107"/>
+      <c r="B49" s="106"/>
+      <c r="C49" s="133"/>
       <c r="D49" s="40" t="s">
         <v>27</v>
       </c>
@@ -5030,8 +5012,8 @@
       <c r="W49" s="22"/>
     </row>
     <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="111"/>
-      <c r="C50" s="107"/>
+      <c r="B50" s="106"/>
+      <c r="C50" s="133"/>
       <c r="D50" s="40" t="s">
         <v>28</v>
       </c>
@@ -5085,8 +5067,8 @@
       <c r="W50" s="22"/>
     </row>
     <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="111"/>
-      <c r="C51" s="107"/>
+      <c r="B51" s="106"/>
+      <c r="C51" s="133"/>
       <c r="D51" s="40" t="s">
         <v>29</v>
       </c>
@@ -5140,8 +5122,8 @@
       <c r="W51" s="22"/>
     </row>
     <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="111"/>
-      <c r="C52" s="107"/>
+      <c r="B52" s="106"/>
+      <c r="C52" s="133"/>
       <c r="D52" s="40" t="s">
         <v>30</v>
       </c>
@@ -5195,8 +5177,8 @@
       <c r="W52" s="22"/>
     </row>
     <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="111"/>
-      <c r="C53" s="107"/>
+      <c r="B53" s="106"/>
+      <c r="C53" s="133"/>
       <c r="D53" s="40" t="s">
         <v>31</v>
       </c>
@@ -5250,10 +5232,10 @@
       <c r="W53" s="22"/>
     </row>
     <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="111"/>
-      <c r="C54" s="107"/>
+      <c r="B54" s="106"/>
+      <c r="C54" s="133"/>
       <c r="D54" s="40" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E54" s="40"/>
       <c r="F54" s="40" t="s">
@@ -5305,10 +5287,10 @@
       <c r="W54" s="22"/>
     </row>
     <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="111"/>
-      <c r="C55" s="107"/>
+      <c r="B55" s="106"/>
+      <c r="C55" s="133"/>
       <c r="D55" s="40" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E55" s="40"/>
       <c r="F55" s="40" t="s">
@@ -5360,10 +5342,10 @@
       <c r="W55" s="22"/>
     </row>
     <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="111"/>
-      <c r="C56" s="107"/>
+      <c r="B56" s="106"/>
+      <c r="C56" s="133"/>
       <c r="D56" s="40" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E56" s="40"/>
       <c r="F56" s="40" t="s">
@@ -5415,10 +5397,10 @@
       <c r="W56" s="22"/>
     </row>
     <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="111"/>
-      <c r="C57" s="107"/>
+      <c r="B57" s="106"/>
+      <c r="C57" s="133"/>
       <c r="D57" s="40" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E57" s="40"/>
       <c r="F57" s="40" t="s">
@@ -5470,10 +5452,10 @@
       <c r="W57" s="22"/>
     </row>
     <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="111"/>
-      <c r="C58" s="107"/>
+      <c r="B58" s="106"/>
+      <c r="C58" s="133"/>
       <c r="D58" s="40" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E58" s="40"/>
       <c r="F58" s="40" t="s">
@@ -5525,10 +5507,10 @@
       <c r="W58" s="22"/>
     </row>
     <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="111"/>
-      <c r="C59" s="107"/>
+      <c r="B59" s="106"/>
+      <c r="C59" s="133"/>
       <c r="D59" s="40" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E59" s="40"/>
       <c r="F59" s="40" t="s">
@@ -5580,10 +5562,10 @@
       <c r="W59" s="22"/>
     </row>
     <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="111"/>
-      <c r="C60" s="107"/>
+      <c r="B60" s="106"/>
+      <c r="C60" s="133"/>
       <c r="D60" s="40" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E60" s="40"/>
       <c r="F60" s="40" t="s">
@@ -5635,10 +5617,10 @@
       <c r="W60" s="22"/>
     </row>
     <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="111"/>
-      <c r="C61" s="107"/>
+      <c r="B61" s="106"/>
+      <c r="C61" s="133"/>
       <c r="D61" s="40" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E61" s="40"/>
       <c r="F61" s="40" t="s">
@@ -5690,10 +5672,10 @@
       <c r="W61" s="22"/>
     </row>
     <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="111"/>
-      <c r="C62" s="107"/>
+      <c r="B62" s="106"/>
+      <c r="C62" s="133"/>
       <c r="D62" s="40" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E62" s="40"/>
       <c r="F62" s="40" t="s">
@@ -5745,10 +5727,10 @@
       <c r="W62" s="22"/>
     </row>
     <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="111"/>
-      <c r="C63" s="107"/>
+      <c r="B63" s="106"/>
+      <c r="C63" s="133"/>
       <c r="D63" s="40" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E63" s="40"/>
       <c r="F63" s="40" t="s">
@@ -5800,10 +5782,10 @@
       <c r="W63" s="22"/>
     </row>
     <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="111"/>
-      <c r="C64" s="107"/>
+      <c r="B64" s="106"/>
+      <c r="C64" s="133"/>
       <c r="D64" s="40" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E64" s="40"/>
       <c r="F64" s="40" t="s">
@@ -5855,10 +5837,10 @@
       <c r="W64" s="22"/>
     </row>
     <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="111"/>
-      <c r="C65" s="107"/>
+      <c r="B65" s="106"/>
+      <c r="C65" s="133"/>
       <c r="D65" s="40" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E65" s="40"/>
       <c r="F65" s="40" t="s">
@@ -5910,10 +5892,10 @@
       <c r="W65" s="22"/>
     </row>
     <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="111"/>
-      <c r="C66" s="107"/>
+      <c r="B66" s="106"/>
+      <c r="C66" s="133"/>
       <c r="D66" s="40" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E66" s="40"/>
       <c r="F66" s="40" t="s">
@@ -5965,10 +5947,10 @@
       <c r="W66" s="22"/>
     </row>
     <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="111"/>
-      <c r="C67" s="107"/>
+      <c r="B67" s="106"/>
+      <c r="C67" s="133"/>
       <c r="D67" s="40" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E67" s="40"/>
       <c r="F67" s="40" t="s">
@@ -6020,10 +6002,10 @@
       <c r="W67" s="22"/>
     </row>
     <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="111"/>
-      <c r="C68" s="107"/>
+      <c r="B68" s="106"/>
+      <c r="C68" s="133"/>
       <c r="D68" s="40" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E68" s="40"/>
       <c r="F68" s="40" t="s">
@@ -6075,10 +6057,10 @@
       <c r="W68" s="22"/>
     </row>
     <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="111"/>
-      <c r="C69" s="107"/>
+      <c r="B69" s="106"/>
+      <c r="C69" s="133"/>
       <c r="D69" s="40" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E69" s="40"/>
       <c r="F69" s="40" t="s">
@@ -6130,10 +6112,10 @@
       <c r="W69" s="22"/>
     </row>
     <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="111"/>
-      <c r="C70" s="107"/>
+      <c r="B70" s="106"/>
+      <c r="C70" s="133"/>
       <c r="D70" s="40" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E70" s="40"/>
       <c r="F70" s="40" t="s">
@@ -6185,10 +6167,10 @@
       <c r="W70" s="22"/>
     </row>
     <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="111"/>
-      <c r="C71" s="107"/>
+      <c r="B71" s="106"/>
+      <c r="C71" s="133"/>
       <c r="D71" s="40" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E71" s="40"/>
       <c r="F71" s="40" t="s">
@@ -6240,10 +6222,10 @@
       <c r="W71" s="22"/>
     </row>
     <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="111"/>
-      <c r="C72" s="107"/>
+      <c r="B72" s="106"/>
+      <c r="C72" s="133"/>
       <c r="D72" s="40" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E72" s="40"/>
       <c r="F72" s="40" t="s">
@@ -6295,10 +6277,10 @@
       <c r="W72" s="22"/>
     </row>
     <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="111"/>
-      <c r="C73" s="107"/>
+      <c r="B73" s="106"/>
+      <c r="C73" s="133"/>
       <c r="D73" s="40" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E73" s="40"/>
       <c r="F73" s="40" t="s">
@@ -6350,10 +6332,10 @@
       <c r="W73" s="22"/>
     </row>
     <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="111"/>
-      <c r="C74" s="107"/>
+      <c r="B74" s="106"/>
+      <c r="C74" s="133"/>
       <c r="D74" s="40" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E74" s="40"/>
       <c r="F74" s="40" t="s">
@@ -6405,10 +6387,10 @@
       <c r="W74" s="22"/>
     </row>
     <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="111"/>
-      <c r="C75" s="107"/>
+      <c r="B75" s="106"/>
+      <c r="C75" s="133"/>
       <c r="D75" s="40" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E75" s="40"/>
       <c r="F75" s="40" t="s">
@@ -6460,10 +6442,10 @@
       <c r="W75" s="22"/>
     </row>
     <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="111"/>
-      <c r="C76" s="107"/>
+      <c r="B76" s="106"/>
+      <c r="C76" s="133"/>
       <c r="D76" s="40" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E76" s="40"/>
       <c r="F76" s="40" t="s">
@@ -6515,10 +6497,10 @@
       <c r="W76" s="22"/>
     </row>
     <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="111"/>
-      <c r="C77" s="107"/>
+      <c r="B77" s="106"/>
+      <c r="C77" s="133"/>
       <c r="D77" s="40" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E77" s="40"/>
       <c r="F77" s="40" t="s">
@@ -6570,10 +6552,10 @@
       <c r="W77" s="22"/>
     </row>
     <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="111"/>
-      <c r="C78" s="107"/>
+      <c r="B78" s="106"/>
+      <c r="C78" s="133"/>
       <c r="D78" s="40" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E78" s="40"/>
       <c r="F78" s="40" t="s">
@@ -6625,10 +6607,10 @@
       <c r="W78" s="22"/>
     </row>
     <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="111"/>
-      <c r="C79" s="107"/>
+      <c r="B79" s="106"/>
+      <c r="C79" s="133"/>
       <c r="D79" s="40" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E79" s="40"/>
       <c r="F79" s="40" t="s">
@@ -6680,10 +6662,10 @@
       <c r="W79" s="22"/>
     </row>
     <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="111"/>
-      <c r="C80" s="107"/>
+      <c r="B80" s="106"/>
+      <c r="C80" s="133"/>
       <c r="D80" s="40" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E80" s="40"/>
       <c r="F80" s="40" t="s">
@@ -6735,10 +6717,10 @@
       <c r="W80" s="22"/>
     </row>
     <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="111"/>
-      <c r="C81" s="107"/>
+      <c r="B81" s="106"/>
+      <c r="C81" s="133"/>
       <c r="D81" s="40" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E81" s="40"/>
       <c r="F81" s="40" t="s">
@@ -6751,7 +6733,7 @@
         <v>0.25</v>
       </c>
       <c r="I81" s="46">
-        <f t="shared" ref="I81:I91" si="3">SUM(J81:W81)</f>
+        <f t="shared" ref="I81:I86" si="3">SUM(J81:W81)</f>
         <v>0</v>
       </c>
       <c r="J81" s="61">
@@ -6790,10 +6772,10 @@
       <c r="W81" s="22"/>
     </row>
     <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="111"/>
-      <c r="C82" s="107"/>
+      <c r="B82" s="106"/>
+      <c r="C82" s="133"/>
       <c r="D82" s="40" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E82" s="40"/>
       <c r="F82" s="40" t="s">
@@ -6845,10 +6827,10 @@
       <c r="W82" s="22"/>
     </row>
     <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="111"/>
-      <c r="C83" s="107"/>
+      <c r="B83" s="106"/>
+      <c r="C83" s="133"/>
       <c r="D83" s="40" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E83" s="40"/>
       <c r="F83" s="40" t="s">
@@ -6900,10 +6882,10 @@
       <c r="W83" s="22"/>
     </row>
     <row r="84" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="111"/>
-      <c r="C84" s="107"/>
+      <c r="B84" s="106"/>
+      <c r="C84" s="133"/>
       <c r="D84" s="40" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E84" s="40"/>
       <c r="F84" s="40" t="s">
@@ -6963,12 +6945,12 @@
       </c>
     </row>
     <row r="85" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="111"/>
-      <c r="C85" s="112" t="s">
+      <c r="B85" s="106"/>
+      <c r="C85" s="96" t="s">
         <v>37</v>
       </c>
       <c r="D85" s="37" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="E85" s="43"/>
       <c r="F85" s="43" t="s">
@@ -6978,11 +6960,11 @@
         <v>5</v>
       </c>
       <c r="H85" s="4">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="I85" s="46">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.48</v>
       </c>
       <c r="J85" s="61">
         <v>0</v>
@@ -7014,30 +6996,32 @@
       <c r="S85" s="61">
         <v>0</v>
       </c>
-      <c r="T85" s="21"/>
+      <c r="T85" s="87">
+        <v>1.48</v>
+      </c>
       <c r="U85" s="21"/>
       <c r="V85" s="21"/>
       <c r="W85" s="22"/>
     </row>
     <row r="86" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="111"/>
-      <c r="C86" s="112"/>
-      <c r="D86" s="43" t="s">
-        <v>69</v>
-      </c>
+      <c r="B86" s="106"/>
+      <c r="C86" s="96" t="s">
+        <v>126</v>
+      </c>
+      <c r="D86" s="43"/>
       <c r="E86" s="43"/>
-      <c r="F86" s="43" t="s">
+      <c r="F86" s="37" t="s">
         <v>15</v>
       </c>
       <c r="G86" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H86" s="4">
         <v>0.2</v>
       </c>
       <c r="I86" s="46">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J86" s="61">
         <v>0</v>
@@ -7060,93 +7044,109 @@
       <c r="P86" s="61">
         <v>0</v>
       </c>
-      <c r="Q86" s="61">
-        <v>0</v>
-      </c>
-      <c r="R86" s="61">
-        <v>0</v>
-      </c>
-      <c r="S86" s="61">
-        <v>0</v>
-      </c>
-      <c r="T86" s="21"/>
-      <c r="U86" s="21"/>
-      <c r="V86" s="21"/>
-      <c r="W86" s="22"/>
+      <c r="Q86" s="39">
+        <v>0.25</v>
+      </c>
+      <c r="R86" s="39">
+        <v>0</v>
+      </c>
+      <c r="S86" s="39">
+        <v>0</v>
+      </c>
+      <c r="T86" s="39">
+        <v>0</v>
+      </c>
+      <c r="U86" s="39">
+        <v>0</v>
+      </c>
+      <c r="V86" s="39">
+        <v>0</v>
+      </c>
+      <c r="W86" s="75">
+        <v>0</v>
+      </c>
     </row>
     <row r="87" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="111"/>
-      <c r="C87" s="112"/>
-      <c r="D87" s="43" t="s">
-        <v>70</v>
-      </c>
+      <c r="B87" s="106"/>
+      <c r="C87" s="73" t="s">
+        <v>118</v>
+      </c>
+      <c r="D87" s="43"/>
       <c r="E87" s="43"/>
-      <c r="F87" s="43" t="s">
+      <c r="F87" s="37" t="s">
         <v>15</v>
       </c>
       <c r="G87" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H87" s="4">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="I87" s="46">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J87" s="61">
-        <v>0</v>
-      </c>
-      <c r="K87" s="61">
-        <v>0</v>
-      </c>
-      <c r="L87" s="61">
-        <v>0</v>
-      </c>
-      <c r="M87" s="61">
-        <v>0</v>
-      </c>
-      <c r="N87" s="61">
-        <v>0</v>
-      </c>
-      <c r="O87" s="61">
-        <v>0</v>
-      </c>
-      <c r="P87" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q87" s="61">
-        <v>0</v>
-      </c>
-      <c r="R87" s="61">
-        <v>0</v>
-      </c>
-      <c r="S87" s="61">
-        <v>0</v>
-      </c>
-      <c r="T87" s="21"/>
-      <c r="U87" s="21"/>
-      <c r="V87" s="21"/>
-      <c r="W87" s="22"/>
-    </row>
-    <row r="88" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="111"/>
-      <c r="C88" s="112"/>
-      <c r="D88" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="E88" s="43"/>
-      <c r="F88" s="43" t="s">
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="J87" s="39">
+        <v>1.5</v>
+      </c>
+      <c r="K87" s="39">
+        <v>0</v>
+      </c>
+      <c r="L87" s="39">
+        <v>0</v>
+      </c>
+      <c r="M87" s="39">
+        <v>0</v>
+      </c>
+      <c r="N87" s="39">
+        <v>0</v>
+      </c>
+      <c r="O87" s="39">
+        <v>0</v>
+      </c>
+      <c r="P87" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="39">
+        <v>0</v>
+      </c>
+      <c r="R87" s="39">
+        <v>0</v>
+      </c>
+      <c r="S87" s="39">
+        <v>0</v>
+      </c>
+      <c r="T87" s="39">
+        <v>0</v>
+      </c>
+      <c r="U87" s="39">
+        <v>0</v>
+      </c>
+      <c r="V87" s="39">
+        <v>0</v>
+      </c>
+      <c r="W87" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="106"/>
+      <c r="C88" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="D88" s="33"/>
+      <c r="E88" s="45"/>
+      <c r="F88" s="45" t="s">
+        <v>16</v>
       </c>
       <c r="G88" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H88" s="4">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I88" s="46">
-        <f t="shared" si="3"/>
+        <f>SUM(J88:W88)</f>
         <v>0</v>
       </c>
       <c r="J88" s="61">
@@ -7184,135 +7184,139 @@
       <c r="V88" s="21"/>
       <c r="W88" s="22"/>
     </row>
-    <row r="89" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="111"/>
-      <c r="C89" s="112"/>
-      <c r="D89" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="E89" s="43"/>
-      <c r="F89" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="G89" s="4">
-        <v>5</v>
-      </c>
-      <c r="H89" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="I89" s="46">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J89" s="61">
-        <v>0</v>
-      </c>
-      <c r="K89" s="61">
-        <v>0</v>
-      </c>
-      <c r="L89" s="61">
-        <v>0</v>
-      </c>
-      <c r="M89" s="61">
-        <v>0</v>
-      </c>
-      <c r="N89" s="61">
-        <v>0</v>
-      </c>
-      <c r="O89" s="61">
-        <v>0</v>
-      </c>
-      <c r="P89" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q89" s="61">
-        <v>0</v>
-      </c>
-      <c r="R89" s="61">
-        <v>0</v>
-      </c>
-      <c r="S89" s="61">
-        <v>0</v>
-      </c>
-      <c r="T89" s="20"/>
-      <c r="U89" s="20"/>
-      <c r="V89" s="20"/>
-      <c r="W89" s="49"/>
+    <row r="89" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="123" t="s">
+        <v>85</v>
+      </c>
+      <c r="C89" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D89" s="30"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" s="12">
+        <v>6</v>
+      </c>
+      <c r="H89" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="I89" s="48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J89" s="60">
+        <v>0</v>
+      </c>
+      <c r="K89" s="60">
+        <v>0</v>
+      </c>
+      <c r="L89" s="60">
+        <v>0</v>
+      </c>
+      <c r="M89" s="60">
+        <v>0</v>
+      </c>
+      <c r="N89" s="60">
+        <v>0</v>
+      </c>
+      <c r="O89" s="60">
+        <v>0</v>
+      </c>
+      <c r="P89" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="60">
+        <v>0</v>
+      </c>
+      <c r="R89" s="60">
+        <v>0</v>
+      </c>
+      <c r="S89" s="60">
+        <v>0</v>
+      </c>
+      <c r="T89" s="19"/>
+      <c r="U89" s="19"/>
+      <c r="V89" s="19"/>
+      <c r="W89" s="57"/>
     </row>
     <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="111"/>
-      <c r="C90" s="112"/>
-      <c r="D90" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="E90" s="43"/>
-      <c r="F90" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G90" s="4">
-        <v>5</v>
-      </c>
-      <c r="H90" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="I90" s="46">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J90" s="61">
-        <v>0</v>
-      </c>
-      <c r="K90" s="61">
-        <v>0</v>
-      </c>
-      <c r="L90" s="61">
-        <v>0</v>
-      </c>
-      <c r="M90" s="61">
-        <v>0</v>
-      </c>
-      <c r="N90" s="61">
-        <v>0</v>
-      </c>
-      <c r="O90" s="61">
-        <v>0</v>
-      </c>
-      <c r="P90" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q90" s="61">
-        <v>0</v>
-      </c>
-      <c r="R90" s="61">
-        <v>0</v>
-      </c>
-      <c r="S90" s="61">
-        <v>0</v>
-      </c>
-      <c r="T90" s="21"/>
-      <c r="U90" s="21"/>
-      <c r="V90" s="21"/>
-      <c r="W90" s="22"/>
+      <c r="B90" s="124"/>
+      <c r="C90" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D90" s="31"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" s="27">
+        <v>6</v>
+      </c>
+      <c r="H90" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="I90" s="48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J90" s="63">
+        <v>0</v>
+      </c>
+      <c r="K90" s="63">
+        <v>0</v>
+      </c>
+      <c r="L90" s="63">
+        <v>0</v>
+      </c>
+      <c r="M90" s="63">
+        <v>0</v>
+      </c>
+      <c r="N90" s="63">
+        <v>0</v>
+      </c>
+      <c r="O90" s="63">
+        <v>0</v>
+      </c>
+      <c r="P90" s="63">
+        <v>0</v>
+      </c>
+      <c r="Q90" s="63">
+        <v>0</v>
+      </c>
+      <c r="R90" s="63">
+        <v>0</v>
+      </c>
+      <c r="S90" s="63">
+        <v>0</v>
+      </c>
+      <c r="T90" s="26"/>
+      <c r="U90" s="26"/>
+      <c r="V90" s="26"/>
+      <c r="W90" s="56"/>
     </row>
     <row r="91" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="111"/>
-      <c r="C91" s="96" t="s">
-        <v>132</v>
-      </c>
-      <c r="D91" s="43"/>
-      <c r="E91" s="43"/>
-      <c r="F91" s="37" t="s">
-        <v>15</v>
+      <c r="B91" s="125"/>
+      <c r="C91" s="135" t="s">
+        <v>101</v>
+      </c>
+      <c r="D91" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E91" s="45"/>
+      <c r="F91" s="45" t="s">
+        <v>16</v>
       </c>
       <c r="G91" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H91" s="4">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="I91" s="46">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J91" s="61">
         <v>0</v>
@@ -7335,167 +7339,159 @@
       <c r="P91" s="61">
         <v>0</v>
       </c>
-      <c r="Q91" s="39">
-        <v>0.25</v>
-      </c>
-      <c r="R91" s="39">
-        <v>0</v>
-      </c>
-      <c r="S91" s="39">
-        <v>0</v>
-      </c>
-      <c r="T91" s="39">
-        <v>0</v>
-      </c>
-      <c r="U91" s="39">
-        <v>0</v>
-      </c>
-      <c r="V91" s="39">
-        <v>0</v>
-      </c>
-      <c r="W91" s="75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="111"/>
-      <c r="C92" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="D92" s="43"/>
-      <c r="E92" s="43"/>
-      <c r="F92" s="37" t="s">
-        <v>15</v>
+      <c r="Q91" s="61">
+        <v>0</v>
+      </c>
+      <c r="R91" s="61">
+        <v>0</v>
+      </c>
+      <c r="S91" s="61">
+        <v>0</v>
+      </c>
+      <c r="T91" s="20"/>
+      <c r="U91" s="20"/>
+      <c r="V91" s="20"/>
+      <c r="W91" s="49"/>
+    </row>
+    <row r="92" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B92" s="126"/>
+      <c r="C92" s="135"/>
+      <c r="D92" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E92" s="45"/>
+      <c r="F92" s="45" t="s">
+        <v>16</v>
       </c>
       <c r="G92" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H92" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I92" s="46">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J92" s="61">
+        <v>0</v>
+      </c>
+      <c r="K92" s="61">
+        <v>0</v>
+      </c>
+      <c r="L92" s="61">
+        <v>0</v>
+      </c>
+      <c r="M92" s="61">
+        <v>0</v>
+      </c>
+      <c r="N92" s="61">
+        <v>0</v>
+      </c>
+      <c r="O92" s="61">
+        <v>0</v>
+      </c>
+      <c r="P92" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="61">
+        <v>0</v>
+      </c>
+      <c r="R92" s="61">
+        <v>0</v>
+      </c>
+      <c r="S92" s="61">
+        <v>0</v>
+      </c>
+      <c r="T92" s="21"/>
+      <c r="U92" s="21"/>
+      <c r="V92" s="21"/>
+      <c r="W92" s="49"/>
+    </row>
+    <row r="93" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="127"/>
+      <c r="C93" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D93" s="34"/>
+      <c r="E93" s="35"/>
+      <c r="F93" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="11">
+        <v>1</v>
+      </c>
+      <c r="H93" s="11">
+        <v>1</v>
+      </c>
+      <c r="I93" s="50">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="J93" s="62">
+        <v>0</v>
+      </c>
+      <c r="K93" s="62">
+        <v>0</v>
+      </c>
+      <c r="L93" s="62">
+        <v>0</v>
+      </c>
+      <c r="M93" s="84">
+        <v>0.75</v>
+      </c>
+      <c r="N93" s="84">
+        <v>0</v>
+      </c>
+      <c r="O93" s="84">
+        <v>0</v>
+      </c>
+      <c r="P93" s="84">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="84">
+        <v>0</v>
+      </c>
+      <c r="R93" s="84">
+        <v>0</v>
+      </c>
+      <c r="S93" s="84">
+        <v>0</v>
+      </c>
+      <c r="T93" s="84">
+        <v>0</v>
+      </c>
+      <c r="U93" s="84">
+        <v>0</v>
+      </c>
+      <c r="V93" s="84">
+        <v>0</v>
+      </c>
+      <c r="W93" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="105" t="s">
+        <v>86</v>
+      </c>
+      <c r="C94" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="D94" s="53"/>
+      <c r="E94" s="54"/>
+      <c r="F94" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" s="12">
+        <v>1</v>
+      </c>
+      <c r="H94" s="12">
         <v>1.5</v>
-      </c>
-      <c r="J92" s="39">
-        <v>1.5</v>
-      </c>
-      <c r="K92" s="39">
-        <v>0</v>
-      </c>
-      <c r="L92" s="39">
-        <v>0</v>
-      </c>
-      <c r="M92" s="39">
-        <v>0</v>
-      </c>
-      <c r="N92" s="39">
-        <v>0</v>
-      </c>
-      <c r="O92" s="39">
-        <v>0</v>
-      </c>
-      <c r="P92" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q92" s="39">
-        <v>0</v>
-      </c>
-      <c r="R92" s="39">
-        <v>0</v>
-      </c>
-      <c r="S92" s="39">
-        <v>0</v>
-      </c>
-      <c r="T92" s="39">
-        <v>0</v>
-      </c>
-      <c r="U92" s="39">
-        <v>0</v>
-      </c>
-      <c r="V92" s="39">
-        <v>0</v>
-      </c>
-      <c r="W92" s="75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="111"/>
-      <c r="C93" s="65" t="s">
-        <v>112</v>
-      </c>
-      <c r="D93" s="33"/>
-      <c r="E93" s="45"/>
-      <c r="F93" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="G93" s="4">
-        <v>4</v>
-      </c>
-      <c r="H93" s="4">
-        <v>1</v>
-      </c>
-      <c r="I93" s="46">
-        <f>SUM(J93:W93)</f>
-        <v>0</v>
-      </c>
-      <c r="J93" s="61">
-        <v>0</v>
-      </c>
-      <c r="K93" s="61">
-        <v>0</v>
-      </c>
-      <c r="L93" s="61">
-        <v>0</v>
-      </c>
-      <c r="M93" s="61">
-        <v>0</v>
-      </c>
-      <c r="N93" s="61">
-        <v>0</v>
-      </c>
-      <c r="O93" s="61">
-        <v>0</v>
-      </c>
-      <c r="P93" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q93" s="61">
-        <v>0</v>
-      </c>
-      <c r="R93" s="61">
-        <v>0</v>
-      </c>
-      <c r="S93" s="61">
-        <v>0</v>
-      </c>
-      <c r="T93" s="21"/>
-      <c r="U93" s="21"/>
-      <c r="V93" s="21"/>
-      <c r="W93" s="22"/>
-    </row>
-    <row r="94" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="129" t="s">
-        <v>91</v>
-      </c>
-      <c r="C94" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="D94" s="30"/>
-      <c r="E94" s="29"/>
-      <c r="F94" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G94" s="12">
-        <v>6</v>
-      </c>
-      <c r="H94" s="12">
-        <v>0.75</v>
       </c>
       <c r="I94" s="48">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="J94" s="60">
         <v>0</v>
@@ -7506,108 +7502,122 @@
       <c r="L94" s="60">
         <v>0</v>
       </c>
-      <c r="M94" s="60">
-        <v>0</v>
-      </c>
-      <c r="N94" s="60">
-        <v>0</v>
-      </c>
-      <c r="O94" s="60">
-        <v>0</v>
-      </c>
-      <c r="P94" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q94" s="60">
-        <v>0</v>
-      </c>
-      <c r="R94" s="60">
-        <v>0</v>
-      </c>
-      <c r="S94" s="60">
-        <v>0</v>
-      </c>
-      <c r="T94" s="19"/>
-      <c r="U94" s="19"/>
-      <c r="V94" s="19"/>
-      <c r="W94" s="57"/>
-    </row>
-    <row r="95" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="130"/>
-      <c r="C95" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="D95" s="31"/>
-      <c r="E95" s="32"/>
-      <c r="F95" s="32" t="s">
+      <c r="M94" s="76">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="N94" s="76">
+        <v>0</v>
+      </c>
+      <c r="O94" s="76">
+        <v>0</v>
+      </c>
+      <c r="P94" s="76">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="76">
+        <v>0</v>
+      </c>
+      <c r="R94" s="76">
+        <v>0</v>
+      </c>
+      <c r="S94" s="76">
+        <v>0</v>
+      </c>
+      <c r="T94" s="76">
+        <v>0</v>
+      </c>
+      <c r="U94" s="76">
+        <v>0</v>
+      </c>
+      <c r="V94" s="76">
+        <v>0</v>
+      </c>
+      <c r="W94" s="76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B95" s="126"/>
+      <c r="C95" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="D95" s="33"/>
+      <c r="E95" s="45"/>
+      <c r="F95" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="G95" s="27">
-        <v>6</v>
-      </c>
-      <c r="H95" s="27">
-        <v>1.5</v>
-      </c>
-      <c r="I95" s="48">
+      <c r="G95" s="4">
+        <v>1</v>
+      </c>
+      <c r="H95" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="I95" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J95" s="63">
-        <v>0</v>
-      </c>
-      <c r="K95" s="63">
-        <v>0</v>
-      </c>
-      <c r="L95" s="63">
-        <v>0</v>
-      </c>
-      <c r="M95" s="63">
-        <v>0</v>
-      </c>
-      <c r="N95" s="63">
-        <v>0</v>
-      </c>
-      <c r="O95" s="63">
-        <v>0</v>
-      </c>
-      <c r="P95" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q95" s="63">
-        <v>0</v>
-      </c>
-      <c r="R95" s="63">
-        <v>0</v>
-      </c>
-      <c r="S95" s="63">
-        <v>0</v>
-      </c>
-      <c r="T95" s="26"/>
-      <c r="U95" s="26"/>
-      <c r="V95" s="26"/>
-      <c r="W95" s="56"/>
-    </row>
-    <row r="96" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="131"/>
-      <c r="C96" s="109" t="s">
-        <v>107</v>
-      </c>
-      <c r="D96" s="33" t="s">
-        <v>109</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="J95" s="61">
+        <v>0</v>
+      </c>
+      <c r="K95" s="61">
+        <v>0</v>
+      </c>
+      <c r="L95" s="61">
+        <v>0</v>
+      </c>
+      <c r="M95" s="85">
+        <v>0</v>
+      </c>
+      <c r="N95" s="85">
+        <v>0</v>
+      </c>
+      <c r="O95" s="89">
+        <v>0</v>
+      </c>
+      <c r="P95" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="89">
+        <v>0</v>
+      </c>
+      <c r="R95" s="87">
+        <v>0.1</v>
+      </c>
+      <c r="S95" s="87">
+        <v>0</v>
+      </c>
+      <c r="T95" s="87">
+        <v>0</v>
+      </c>
+      <c r="U95" s="87">
+        <v>0</v>
+      </c>
+      <c r="V95" s="87">
+        <v>0</v>
+      </c>
+      <c r="W95" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B96" s="126"/>
+      <c r="C96" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D96" s="33"/>
       <c r="E96" s="45"/>
       <c r="F96" s="45" t="s">
         <v>16</v>
       </c>
       <c r="G96" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H96" s="4">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="I96" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J96" s="61">
         <v>0</v>
@@ -7618,51 +7628,59 @@
       <c r="L96" s="61">
         <v>0</v>
       </c>
-      <c r="M96" s="61">
-        <v>0</v>
-      </c>
-      <c r="N96" s="61">
-        <v>0</v>
-      </c>
-      <c r="O96" s="61">
-        <v>0</v>
-      </c>
-      <c r="P96" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q96" s="61">
-        <v>0</v>
-      </c>
-      <c r="R96" s="61">
-        <v>0</v>
-      </c>
-      <c r="S96" s="61">
-        <v>0</v>
-      </c>
-      <c r="T96" s="20"/>
-      <c r="U96" s="20"/>
-      <c r="V96" s="20"/>
-      <c r="W96" s="49"/>
+      <c r="M96" s="85">
+        <v>0</v>
+      </c>
+      <c r="N96" s="85">
+        <v>0</v>
+      </c>
+      <c r="O96" s="87">
+        <v>1</v>
+      </c>
+      <c r="P96" s="93">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="87">
+        <v>0</v>
+      </c>
+      <c r="R96" s="87">
+        <v>0</v>
+      </c>
+      <c r="S96" s="87">
+        <v>0</v>
+      </c>
+      <c r="T96" s="87">
+        <v>0</v>
+      </c>
+      <c r="U96" s="87">
+        <v>0</v>
+      </c>
+      <c r="V96" s="87">
+        <v>0</v>
+      </c>
+      <c r="W96" s="87">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B97" s="132"/>
-      <c r="C97" s="109"/>
-      <c r="D97" s="33" t="s">
-        <v>108</v>
-      </c>
+      <c r="B97" s="126"/>
+      <c r="C97" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D97" s="33"/>
       <c r="E97" s="45"/>
       <c r="F97" s="45" t="s">
         <v>16</v>
       </c>
       <c r="G97" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H97" s="4">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="I97" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J97" s="61">
         <v>0</v>
@@ -7673,827 +7691,517 @@
       <c r="L97" s="61">
         <v>0</v>
       </c>
-      <c r="M97" s="61">
-        <v>0</v>
-      </c>
-      <c r="N97" s="61">
-        <v>0</v>
-      </c>
-      <c r="O97" s="61">
-        <v>0</v>
-      </c>
-      <c r="P97" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q97" s="61">
-        <v>0</v>
-      </c>
-      <c r="R97" s="61">
-        <v>0</v>
-      </c>
-      <c r="S97" s="61">
-        <v>0</v>
-      </c>
-      <c r="T97" s="21"/>
-      <c r="U97" s="21"/>
-      <c r="V97" s="21"/>
-      <c r="W97" s="49"/>
-    </row>
-    <row r="98" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="133"/>
-      <c r="C98" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="D98" s="34"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="35" t="s">
+      <c r="M97" s="85">
+        <v>0</v>
+      </c>
+      <c r="N97" s="85">
+        <v>0</v>
+      </c>
+      <c r="O97" s="87">
+        <v>0.1</v>
+      </c>
+      <c r="P97" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="87">
+        <v>0</v>
+      </c>
+      <c r="R97" s="87">
+        <v>0</v>
+      </c>
+      <c r="S97" s="87">
+        <v>0</v>
+      </c>
+      <c r="T97" s="87">
+        <v>0</v>
+      </c>
+      <c r="U97" s="87">
+        <v>0</v>
+      </c>
+      <c r="V97" s="87">
+        <v>0</v>
+      </c>
+      <c r="W97" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B98" s="126"/>
+      <c r="C98" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D98" s="33"/>
+      <c r="E98" s="45"/>
+      <c r="F98" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="G98" s="11">
-        <v>1</v>
-      </c>
-      <c r="H98" s="11">
-        <v>1</v>
-      </c>
-      <c r="I98" s="50">
-        <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
-      <c r="J98" s="62">
-        <v>0</v>
-      </c>
-      <c r="K98" s="62">
-        <v>0</v>
-      </c>
-      <c r="L98" s="62">
-        <v>0</v>
-      </c>
-      <c r="M98" s="84">
-        <v>0.75</v>
-      </c>
-      <c r="N98" s="84">
-        <v>0</v>
-      </c>
-      <c r="O98" s="84">
-        <v>0</v>
-      </c>
-      <c r="P98" s="84">
-        <v>0</v>
-      </c>
-      <c r="Q98" s="84">
-        <v>0</v>
-      </c>
-      <c r="R98" s="84">
-        <v>0</v>
-      </c>
-      <c r="S98" s="84">
-        <v>0</v>
-      </c>
-      <c r="T98" s="84">
-        <v>0</v>
-      </c>
-      <c r="U98" s="84">
-        <v>0</v>
-      </c>
-      <c r="V98" s="84">
-        <v>0</v>
-      </c>
-      <c r="W98" s="84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="110" t="s">
-        <v>92</v>
-      </c>
-      <c r="C99" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="D99" s="53"/>
-      <c r="E99" s="54"/>
-      <c r="F99" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="G99" s="12">
-        <v>1</v>
-      </c>
-      <c r="H99" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="I99" s="48">
-        <f t="shared" si="2"/>
-        <v>0.46700000000000003</v>
-      </c>
-      <c r="J99" s="60">
-        <v>0</v>
-      </c>
-      <c r="K99" s="60">
-        <v>0</v>
-      </c>
-      <c r="L99" s="60">
-        <v>0</v>
-      </c>
-      <c r="M99" s="76">
-        <v>0.46700000000000003</v>
-      </c>
-      <c r="N99" s="76">
-        <v>0</v>
-      </c>
-      <c r="O99" s="76">
-        <v>0</v>
-      </c>
-      <c r="P99" s="76">
-        <v>0</v>
-      </c>
-      <c r="Q99" s="76">
-        <v>0</v>
-      </c>
-      <c r="R99" s="76">
-        <v>0</v>
-      </c>
-      <c r="S99" s="76">
-        <v>0</v>
-      </c>
-      <c r="T99" s="76">
-        <v>0</v>
-      </c>
-      <c r="U99" s="76">
-        <v>0</v>
-      </c>
-      <c r="V99" s="76">
-        <v>0</v>
-      </c>
-      <c r="W99" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B100" s="132"/>
-      <c r="C100" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="D100" s="33"/>
-      <c r="E100" s="45"/>
-      <c r="F100" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="G100" s="4">
-        <v>1</v>
-      </c>
-      <c r="H100" s="4">
+      <c r="G98" s="4">
+        <v>3</v>
+      </c>
+      <c r="H98" s="4">
         <v>0.33</v>
       </c>
-      <c r="I100" s="46">
+      <c r="I98" s="46">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="J100" s="61">
-        <v>0</v>
-      </c>
-      <c r="K100" s="61">
-        <v>0</v>
-      </c>
-      <c r="L100" s="61">
-        <v>0</v>
-      </c>
-      <c r="M100" s="85">
-        <v>0</v>
-      </c>
-      <c r="N100" s="85">
-        <v>0</v>
-      </c>
-      <c r="O100" s="89">
-        <v>0</v>
-      </c>
-      <c r="P100" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q100" s="89">
-        <v>0</v>
-      </c>
-      <c r="R100" s="87">
+      <c r="J98" s="61">
+        <v>0</v>
+      </c>
+      <c r="K98" s="61">
+        <v>0</v>
+      </c>
+      <c r="L98" s="61">
+        <v>0</v>
+      </c>
+      <c r="M98" s="61">
+        <v>0</v>
+      </c>
+      <c r="N98" s="61">
+        <v>0</v>
+      </c>
+      <c r="O98" s="61">
+        <v>0</v>
+      </c>
+      <c r="P98" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q98" s="61">
+        <v>0</v>
+      </c>
+      <c r="R98" s="101"/>
+      <c r="S98" s="101"/>
+      <c r="T98" s="87">
         <v>0.1</v>
       </c>
-      <c r="S100" s="87">
-        <v>0</v>
-      </c>
-      <c r="T100" s="87">
-        <v>0</v>
-      </c>
-      <c r="U100" s="87">
-        <v>0</v>
-      </c>
-      <c r="V100" s="87">
-        <v>0</v>
-      </c>
-      <c r="W100" s="87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B101" s="132"/>
-      <c r="C101" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="D101" s="33"/>
-      <c r="E101" s="45"/>
-      <c r="F101" s="45" t="s">
+      <c r="U98" s="87">
+        <v>0</v>
+      </c>
+      <c r="V98" s="87">
+        <v>0</v>
+      </c>
+      <c r="W98" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B99" s="127"/>
+      <c r="C99" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D99" s="34"/>
+      <c r="E99" s="35"/>
+      <c r="F99" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="G101" s="4">
+      <c r="G99" s="11">
         <v>1</v>
       </c>
-      <c r="H101" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="I101" s="46">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J101" s="61">
-        <v>0</v>
-      </c>
-      <c r="K101" s="61">
-        <v>0</v>
-      </c>
-      <c r="L101" s="61">
-        <v>0</v>
-      </c>
-      <c r="M101" s="85">
-        <v>0</v>
-      </c>
-      <c r="N101" s="85">
-        <v>0</v>
-      </c>
-      <c r="O101" s="87">
-        <v>1</v>
-      </c>
-      <c r="P101" s="93">
-        <v>0</v>
-      </c>
-      <c r="Q101" s="87">
-        <v>0</v>
-      </c>
-      <c r="R101" s="87">
-        <v>0</v>
-      </c>
-      <c r="S101" s="87">
-        <v>0</v>
-      </c>
-      <c r="T101" s="87">
-        <v>0</v>
-      </c>
-      <c r="U101" s="87">
-        <v>0</v>
-      </c>
-      <c r="V101" s="87">
-        <v>0</v>
-      </c>
-      <c r="W101" s="87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B102" s="132"/>
-      <c r="C102" s="45" t="s">
-        <v>128</v>
-      </c>
-      <c r="D102" s="33"/>
-      <c r="E102" s="45"/>
-      <c r="F102" s="45" t="s">
+      <c r="H99" s="11">
+        <v>3</v>
+      </c>
+      <c r="I99" s="50">
+        <f t="shared" ref="I99" si="4">SUM(J99:W99)</f>
+        <v>0</v>
+      </c>
+      <c r="J99" s="62">
+        <v>0</v>
+      </c>
+      <c r="K99" s="62">
+        <v>0</v>
+      </c>
+      <c r="L99" s="62">
+        <v>0</v>
+      </c>
+      <c r="M99" s="62">
+        <v>0</v>
+      </c>
+      <c r="N99" s="94" t="s">
+        <v>125</v>
+      </c>
+      <c r="O99" s="94">
+        <v>0</v>
+      </c>
+      <c r="P99" s="95">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="95">
+        <v>0</v>
+      </c>
+      <c r="R99" s="95">
+        <v>0</v>
+      </c>
+      <c r="S99" s="95">
+        <v>0</v>
+      </c>
+      <c r="T99" s="95">
+        <v>0</v>
+      </c>
+      <c r="U99" s="24"/>
+      <c r="V99" s="24"/>
+      <c r="W99" s="25"/>
+    </row>
+    <row r="100" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="119" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" s="120"/>
+      <c r="D100" s="120"/>
+      <c r="E100" s="120"/>
+      <c r="F100" s="120"/>
+      <c r="G100" s="120"/>
+      <c r="H100" s="17">
+        <f>SUM(H4:H99)</f>
+        <v>49.11999999999999</v>
+      </c>
+      <c r="I100" s="17">
+        <f>SUM(I4:I99)</f>
+        <v>33.881700000000002</v>
+      </c>
+      <c r="J100" s="17">
+        <f>SUM(J4:J99)</f>
+        <v>1.95</v>
+      </c>
+      <c r="K100" s="17">
+        <f>SUM(K4:K99)</f>
+        <v>3.3</v>
+      </c>
+      <c r="L100" s="17">
+        <f>SUM(L4:L99)</f>
+        <v>7.15</v>
+      </c>
+      <c r="M100" s="17">
+        <f>SUM(M4:M99)</f>
+        <v>3.9929999999999999</v>
+      </c>
+      <c r="N100" s="17">
+        <f>SUM(N4:N99)</f>
+        <v>1.5</v>
+      </c>
+      <c r="O100" s="17">
+        <f>SUM(O4:O99)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P100" s="17">
+        <f>SUM(P4:P99)</f>
+        <v>0.03</v>
+      </c>
+      <c r="Q100" s="17">
+        <f>SUM(Q4:Q99)</f>
+        <v>2.0290000000000004</v>
+      </c>
+      <c r="R100" s="17">
+        <f>SUM(R4:R99)</f>
+        <v>1.4826999999999999</v>
+      </c>
+      <c r="S100" s="17">
+        <f>SUM(S4:S99)</f>
+        <v>4.7170000000000005</v>
+      </c>
+      <c r="T100" s="17">
+        <f>SUM(T4:T99)</f>
+        <v>6.629999999999999</v>
+      </c>
+      <c r="U100" s="17">
+        <f>SUM(U4:U99)</f>
+        <v>0</v>
+      </c>
+      <c r="V100" s="17">
+        <f>SUM(V4:V99)</f>
+        <v>0</v>
+      </c>
+      <c r="W100" s="18">
+        <f>SUM(W4:W99)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="110" t="s">
+        <v>11</v>
+      </c>
+      <c r="K101" s="111"/>
+      <c r="L101" s="111"/>
+      <c r="M101" s="111"/>
+      <c r="N101" s="111"/>
+      <c r="O101" s="111"/>
+      <c r="P101" s="111"/>
+      <c r="Q101" s="111"/>
+      <c r="R101" s="111"/>
+      <c r="S101" s="111"/>
+      <c r="T101" s="111"/>
+      <c r="U101" s="111"/>
+      <c r="V101" s="111"/>
+      <c r="W101" s="112"/>
+    </row>
+    <row r="102" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="C102" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="E102" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="3"/>
+      <c r="O102" s="9"/>
+      <c r="P102" s="9"/>
+    </row>
+    <row r="103" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="G102" s="4">
-        <v>1</v>
-      </c>
-      <c r="H102" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="I102" s="46">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="J102" s="61">
-        <v>0</v>
-      </c>
-      <c r="K102" s="61">
-        <v>0</v>
-      </c>
-      <c r="L102" s="61">
-        <v>0</v>
-      </c>
-      <c r="M102" s="85">
-        <v>0</v>
-      </c>
-      <c r="N102" s="85">
-        <v>0</v>
-      </c>
-      <c r="O102" s="87">
-        <v>0.1</v>
-      </c>
-      <c r="P102" s="87">
-        <v>0</v>
-      </c>
-      <c r="Q102" s="87">
-        <v>0</v>
-      </c>
-      <c r="R102" s="87">
-        <v>0</v>
-      </c>
-      <c r="S102" s="87">
-        <v>0</v>
-      </c>
-      <c r="T102" s="87">
-        <v>0</v>
-      </c>
-      <c r="U102" s="87">
-        <v>0</v>
-      </c>
-      <c r="V102" s="87">
-        <v>0</v>
-      </c>
-      <c r="W102" s="87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B103" s="132"/>
-      <c r="C103" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="D103" s="33"/>
-      <c r="E103" s="45"/>
-      <c r="F103" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="G103" s="4">
-        <v>3</v>
-      </c>
-      <c r="H103" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="I103" s="46">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="J103" s="61">
-        <v>0</v>
-      </c>
-      <c r="K103" s="61">
-        <v>0</v>
-      </c>
-      <c r="L103" s="61">
-        <v>0</v>
-      </c>
-      <c r="M103" s="61">
-        <v>0</v>
-      </c>
-      <c r="N103" s="61">
-        <v>0</v>
-      </c>
-      <c r="O103" s="61">
-        <v>0</v>
-      </c>
-      <c r="P103" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q103" s="61">
-        <v>0</v>
-      </c>
-      <c r="R103" s="101"/>
-      <c r="S103" s="101"/>
-      <c r="T103" s="87">
-        <v>0.1</v>
-      </c>
-      <c r="U103" s="87">
-        <v>0</v>
-      </c>
-      <c r="V103" s="87">
-        <v>0</v>
-      </c>
-      <c r="W103" s="87">
-        <v>0</v>
+      <c r="C103" s="71">
+        <f>SUM(H7,H9,H41,H88,H89,H90,H91,H92,H93,H95:H99,H41)</f>
+        <v>12.27</v>
+      </c>
+      <c r="D103" s="27">
+        <f>SUM(I95:I99,I88:I93,I9,I7,I41)</f>
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="E103" s="27">
+        <f>SUM(C103,-D103)</f>
+        <v>4.2199999999999989</v>
+      </c>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="I103" s="131"/>
+      <c r="J103" s="10">
+        <f>H100-J100</f>
+        <v>47.169999999999987</v>
+      </c>
+      <c r="K103" s="10">
+        <f>J103-K100</f>
+        <v>43.86999999999999</v>
+      </c>
+      <c r="L103" s="10">
+        <f>K103-L100</f>
+        <v>36.719999999999992</v>
+      </c>
+      <c r="M103" s="10">
+        <f>L103-M100</f>
+        <v>32.72699999999999</v>
+      </c>
+      <c r="N103" s="10">
+        <f t="shared" ref="N103:W103" si="5">M103-N100</f>
+        <v>31.22699999999999</v>
+      </c>
+      <c r="O103" s="10">
+        <f t="shared" si="5"/>
+        <v>30.126999999999988</v>
+      </c>
+      <c r="P103" s="10">
+        <f t="shared" si="5"/>
+        <v>30.096999999999987</v>
+      </c>
+      <c r="Q103" s="10">
+        <f t="shared" si="5"/>
+        <v>28.067999999999987</v>
+      </c>
+      <c r="R103" s="10">
+        <f t="shared" si="5"/>
+        <v>26.585299999999986</v>
+      </c>
+      <c r="S103" s="10">
+        <f t="shared" si="5"/>
+        <v>21.868299999999984</v>
+      </c>
+      <c r="T103" s="10">
+        <f t="shared" si="5"/>
+        <v>15.238299999999985</v>
+      </c>
+      <c r="U103" s="10">
+        <f t="shared" si="5"/>
+        <v>15.238299999999985</v>
+      </c>
+      <c r="V103" s="10">
+        <f t="shared" si="5"/>
+        <v>15.238299999999985</v>
+      </c>
+      <c r="W103" s="10">
+        <f t="shared" si="5"/>
+        <v>15.238299999999985</v>
       </c>
     </row>
     <row r="104" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="133"/>
-      <c r="C104" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="D104" s="34"/>
-      <c r="E104" s="35"/>
-      <c r="F104" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="G104" s="11">
-        <v>1</v>
-      </c>
-      <c r="H104" s="11">
-        <v>3</v>
-      </c>
-      <c r="I104" s="50">
-        <f t="shared" ref="I104" si="4">SUM(J104:W104)</f>
-        <v>0</v>
-      </c>
-      <c r="J104" s="62">
-        <v>0</v>
-      </c>
-      <c r="K104" s="62">
-        <v>0</v>
-      </c>
-      <c r="L104" s="62">
-        <v>0</v>
-      </c>
-      <c r="M104" s="62">
-        <v>0</v>
-      </c>
-      <c r="N104" s="94" t="s">
-        <v>131</v>
-      </c>
-      <c r="O104" s="94">
-        <v>0</v>
-      </c>
-      <c r="P104" s="95">
-        <v>0</v>
-      </c>
-      <c r="Q104" s="95">
-        <v>0</v>
-      </c>
-      <c r="R104" s="95">
-        <v>0</v>
-      </c>
-      <c r="S104" s="95">
-        <v>0</v>
-      </c>
-      <c r="T104" s="95">
-        <v>0</v>
-      </c>
-      <c r="U104" s="24"/>
-      <c r="V104" s="24"/>
-      <c r="W104" s="25"/>
-    </row>
-    <row r="105" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="125" t="s">
-        <v>8</v>
-      </c>
-      <c r="C105" s="126"/>
-      <c r="D105" s="126"/>
-      <c r="E105" s="126"/>
-      <c r="F105" s="126"/>
-      <c r="G105" s="126"/>
-      <c r="H105" s="17">
-        <f t="shared" ref="H105:W105" si="5">SUM(H4:H104)</f>
-        <v>48.320000000000007</v>
-      </c>
-      <c r="I105" s="17">
-        <f t="shared" si="5"/>
-        <v>32.401700000000005</v>
-      </c>
-      <c r="J105" s="17">
-        <f t="shared" si="5"/>
-        <v>1.95</v>
-      </c>
-      <c r="K105" s="17">
-        <f t="shared" si="5"/>
-        <v>3.3</v>
-      </c>
-      <c r="L105" s="17">
-        <f t="shared" si="5"/>
-        <v>7.15</v>
-      </c>
-      <c r="M105" s="17">
-        <f t="shared" si="5"/>
-        <v>3.9929999999999999</v>
-      </c>
-      <c r="N105" s="17">
-        <f t="shared" si="5"/>
-        <v>1.5</v>
-      </c>
-      <c r="O105" s="17">
-        <f t="shared" si="5"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P105" s="17">
-        <f t="shared" si="5"/>
-        <v>0.03</v>
-      </c>
-      <c r="Q105" s="17">
-        <f t="shared" si="5"/>
-        <v>2.0290000000000004</v>
-      </c>
-      <c r="R105" s="17">
-        <f t="shared" si="5"/>
-        <v>1.4826999999999999</v>
-      </c>
-      <c r="S105" s="17">
-        <f t="shared" si="5"/>
-        <v>4.7170000000000005</v>
-      </c>
-      <c r="T105" s="17">
-        <f t="shared" si="5"/>
-        <v>5.1499999999999995</v>
-      </c>
-      <c r="U105" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V105" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W105" s="18">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="116" t="s">
-        <v>11</v>
-      </c>
-      <c r="K106" s="117"/>
-      <c r="L106" s="117"/>
-      <c r="M106" s="117"/>
-      <c r="N106" s="117"/>
-      <c r="O106" s="117"/>
-      <c r="P106" s="117"/>
-      <c r="Q106" s="117"/>
-      <c r="R106" s="117"/>
-      <c r="S106" s="117"/>
-      <c r="T106" s="117"/>
-      <c r="U106" s="117"/>
-      <c r="V106" s="117"/>
-      <c r="W106" s="118"/>
-    </row>
-    <row r="107" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="66" t="s">
-        <v>123</v>
-      </c>
-      <c r="C107" s="67" t="s">
-        <v>120</v>
-      </c>
-      <c r="D107" s="67" t="s">
-        <v>121</v>
-      </c>
-      <c r="E107" s="68" t="s">
-        <v>122</v>
-      </c>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
+      <c r="B104" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" s="69">
+        <f>SUM(H4,H85:H85,H94,H17:H37,H10:H15,H8,H6,H5,H87)</f>
+        <v>18.399999999999991</v>
+      </c>
+      <c r="D104" s="5">
+        <f>SUM(I94,I85:I85,I17:I37,I10:I15,I8,I5:I6,I87,I4)</f>
+        <v>14.3317</v>
+      </c>
+      <c r="E104" s="5">
+        <f>SUM(C104,-D104)</f>
+        <v>4.0682999999999918</v>
+      </c>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="3"/>
+    </row>
+    <row r="105" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B105" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105" s="69">
+        <f>SUM(H42:H84,H38:H40)</f>
+        <v>16.75</v>
+      </c>
+      <c r="D105" s="5">
+        <f>SUM(I42:I84,I38:I40,I16)</f>
+        <v>11.25</v>
+      </c>
+      <c r="E105" s="5">
+        <f>SUM(C105,-D105)</f>
+        <v>5.5</v>
+      </c>
+      <c r="F105" s="3"/>
+      <c r="H105" s="128" t="s">
+        <v>10</v>
+      </c>
+      <c r="I105" s="129"/>
+      <c r="J105" s="128">
+        <f>H100-I100</f>
+        <v>15.238299999999988</v>
+      </c>
+      <c r="K105" s="129"/>
+      <c r="L105" s="129"/>
+      <c r="M105" s="129"/>
+      <c r="N105" s="129"/>
+      <c r="O105" s="129"/>
+      <c r="P105" s="129"/>
+      <c r="Q105" s="129"/>
+      <c r="R105" s="129"/>
+      <c r="S105" s="129"/>
+      <c r="T105" s="129"/>
+      <c r="U105" s="129"/>
+      <c r="V105" s="129"/>
+      <c r="W105" s="130"/>
+    </row>
+    <row r="106" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+    </row>
+    <row r="107" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+      <c r="I107" s="3"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
       <c r="M107" s="3"/>
-      <c r="O107" s="9"/>
-      <c r="P107" s="9"/>
-    </row>
-    <row r="108" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B108" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C108" s="71">
-        <f>SUM(H7,H9,H41,H93,H94,H95,H96,H97,H98,H100:H104,H41)</f>
-        <v>12.27</v>
-      </c>
-      <c r="D108" s="27">
-        <f>SUM(I100:I104,I93:I98,I9,I7,I41)</f>
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="E108" s="27">
-        <f>SUM(C108,-D108)</f>
-        <v>4.2199999999999989</v>
-      </c>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="I108" s="105"/>
-      <c r="J108" s="10">
-        <f>H105-J105</f>
-        <v>46.370000000000005</v>
-      </c>
-      <c r="K108" s="10">
-        <f>J108-K105</f>
-        <v>43.070000000000007</v>
-      </c>
-      <c r="L108" s="10">
-        <f>K108-L105</f>
-        <v>35.920000000000009</v>
-      </c>
-      <c r="M108" s="10">
-        <f>L108-M105</f>
-        <v>31.92700000000001</v>
-      </c>
-      <c r="N108" s="10">
-        <f t="shared" ref="N108:W108" si="6">M108-N105</f>
-        <v>30.42700000000001</v>
-      </c>
-      <c r="O108" s="10">
-        <f t="shared" si="6"/>
-        <v>29.327000000000009</v>
-      </c>
-      <c r="P108" s="10">
-        <f t="shared" si="6"/>
-        <v>29.297000000000008</v>
-      </c>
-      <c r="Q108" s="10">
-        <f t="shared" si="6"/>
-        <v>27.268000000000008</v>
-      </c>
-      <c r="R108" s="10">
-        <f t="shared" si="6"/>
-        <v>25.785300000000007</v>
-      </c>
-      <c r="S108" s="10">
-        <f t="shared" si="6"/>
-        <v>21.068300000000008</v>
-      </c>
-      <c r="T108" s="10">
-        <f t="shared" si="6"/>
-        <v>15.918300000000009</v>
-      </c>
-      <c r="U108" s="10">
-        <f t="shared" si="6"/>
-        <v>15.918300000000009</v>
-      </c>
-      <c r="V108" s="10">
-        <f t="shared" si="6"/>
-        <v>15.918300000000009</v>
-      </c>
-      <c r="W108" s="10">
-        <f t="shared" si="6"/>
-        <v>15.918300000000009</v>
-      </c>
-    </row>
-    <row r="109" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B109" s="70" t="s">
-        <v>15</v>
-      </c>
-      <c r="C109" s="69">
-        <f>SUM(H4,H85:H90,H99,H17:H37,H10:H15,H8,H6,H5,H92)</f>
-        <v>17.599999999999994</v>
-      </c>
-      <c r="D109" s="5">
-        <f>SUM(I99,I85:I90,I17:I37,I10:I15,I8,I5:I6,I92,I4)</f>
-        <v>12.851699999999999</v>
-      </c>
-      <c r="E109" s="5">
-        <f>SUM(C109,-D109)</f>
-        <v>4.7482999999999951</v>
-      </c>
-      <c r="F109" s="3"/>
-      <c r="G109" s="3"/>
-      <c r="H109" s="3"/>
-      <c r="I109" s="3"/>
-      <c r="J109" s="3"/>
-      <c r="K109" s="3"/>
-      <c r="L109" s="3"/>
-      <c r="M109" s="3"/>
-    </row>
-    <row r="110" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B110" s="70" t="s">
-        <v>17</v>
-      </c>
-      <c r="C110" s="69">
-        <f>SUM(H42:H84,H38:H40)</f>
-        <v>16.75</v>
-      </c>
-      <c r="D110" s="5">
-        <f>SUM(I42:I84,I38:I40,I16)</f>
-        <v>11.25</v>
-      </c>
-      <c r="E110" s="5">
-        <f>SUM(C110,-D110)</f>
-        <v>5.5</v>
-      </c>
-      <c r="F110" s="3"/>
-      <c r="H110" s="102" t="s">
-        <v>10</v>
-      </c>
-      <c r="I110" s="103"/>
-      <c r="J110" s="102">
-        <f>H105-I105</f>
-        <v>15.918300000000002</v>
-      </c>
-      <c r="K110" s="103"/>
-      <c r="L110" s="103"/>
-      <c r="M110" s="103"/>
-      <c r="N110" s="103"/>
-      <c r="O110" s="103"/>
-      <c r="P110" s="103"/>
-      <c r="Q110" s="103"/>
-      <c r="R110" s="103"/>
-      <c r="S110" s="103"/>
-      <c r="T110" s="103"/>
-      <c r="U110" s="103"/>
-      <c r="V110" s="103"/>
-      <c r="W110" s="104"/>
-    </row>
-    <row r="111" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B111" s="3"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="3"/>
-      <c r="F111" s="3"/>
-      <c r="G111" s="3"/>
-      <c r="H111" s="3"/>
-      <c r="I111" s="3"/>
-      <c r="J111" s="3"/>
-      <c r="K111" s="3"/>
-      <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
-    </row>
-    <row r="112" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B112" s="3"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="3"/>
-      <c r="F112" s="3"/>
-      <c r="G112" s="3"/>
-      <c r="H112" s="3"/>
-      <c r="I112" s="3"/>
-      <c r="J112" s="3"/>
-      <c r="K112" s="3"/>
-      <c r="L112" s="3"/>
-      <c r="M112" s="3"/>
-    </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
-      <c r="G113" s="3"/>
-      <c r="H113" s="3"/>
-      <c r="I113" s="3"/>
-      <c r="J113" s="3"/>
-      <c r="K113" s="3"/>
-      <c r="L113" s="3"/>
-      <c r="M113" s="3"/>
-    </row>
-    <row r="114" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="7"/>
-    </row>
-    <row r="120" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="7"/>
-    </row>
-    <row r="121" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+    </row>
+    <row r="109" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="7"/>
+    </row>
+    <row r="115" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="7"/>
+    </row>
+    <row r="116" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="7"/>
+    </row>
+    <row r="117" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B121" s="7"/>
     </row>
-    <row r="122" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="7"/>
-    </row>
-    <row r="127" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="7"/>
-    </row>
-    <row r="128" spans="2:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="7"/>
-    </row>
-    <row r="129" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="7"/>
-    </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B130" s="6"/>
-      <c r="C130" s="6"/>
+    <row r="122" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="7"/>
+    </row>
+    <row r="123" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="7"/>
+    </row>
+    <row r="124" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B124" s="7"/>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B42:B93"/>
-    <mergeCell ref="C85:C90"/>
+  <mergeCells count="16">
+    <mergeCell ref="J105:W105"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="C42:C84"/>
+    <mergeCell ref="C19:C37"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="B42:B88"/>
     <mergeCell ref="J2:W2"/>
-    <mergeCell ref="J106:W106"/>
+    <mergeCell ref="J101:W101"/>
     <mergeCell ref="B16:B41"/>
     <mergeCell ref="B10:B15"/>
     <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B100:G100"/>
     <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B94:B98"/>
-    <mergeCell ref="B99:B104"/>
-    <mergeCell ref="J110:W110"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="H110:I110"/>
-    <mergeCell ref="C42:C84"/>
-    <mergeCell ref="C19:C37"/>
-    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="B94:B99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Screenshot dia 10 + Actualización del excel + pequeños ajustes para visualización en 2 salas secretas
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 4 SampleTextStudio.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iriag\Desktop\Alex\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MSI-D\Documents\MAP_LegendOfRadev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="130">
   <si>
     <t>Subtarea</t>
   </si>
@@ -1412,6 +1412,75 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1434,75 +1503,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1525,7 +1525,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1611,51 +1611,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$103:$W$103</c:f>
+              <c:f>Hoja1!$J$102:$W$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>47.169999999999987</c:v>
+                  <c:v>46.919999999999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.86999999999999</c:v>
+                  <c:v>43.61999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.719999999999992</c:v>
+                  <c:v>36.469999999999992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.72699999999999</c:v>
+                  <c:v>32.47699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.22699999999999</c:v>
+                  <c:v>30.97699999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.126999999999988</c:v>
+                  <c:v>29.876999999999988</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.096999999999987</c:v>
+                  <c:v>29.846999999999987</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.067999999999987</c:v>
+                  <c:v>27.817999999999987</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.585299999999986</c:v>
+                  <c:v>26.335299999999986</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.868299999999984</c:v>
+                  <c:v>21.618299999999984</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.228299999999985</c:v>
+                  <c:v>13.748299999999984</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.078299999999984</c:v>
+                  <c:v>10.658299999999985</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.078299999999984</c:v>
+                  <c:v>10.658299999999985</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12.078299999999984</c:v>
+                  <c:v>10.658299999999985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1771,7 +1771,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2091,30 +2091,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W125"/>
+  <dimension ref="A1:W124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V44" sqref="V44:V53"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C14" sqref="C13:O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>119</v>
       </c>
@@ -2122,25 +2122,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="115" t="s">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="116"/>
-      <c r="Q2" s="116"/>
-      <c r="R2" s="116"/>
-      <c r="S2" s="116"/>
-      <c r="T2" s="116"/>
-      <c r="U2" s="116"/>
-      <c r="V2" s="116"/>
-      <c r="W2" s="117"/>
-    </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="108"/>
+      <c r="Q2" s="108"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="108"/>
+      <c r="T2" s="108"/>
+      <c r="U2" s="108"/>
+      <c r="V2" s="108"/>
+      <c r="W2" s="109"/>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
@@ -2208,8 +2208,8 @@
         <v>43081</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="121" t="s">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="113" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="78" t="s">
@@ -2275,8 +2275,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="122"/>
+    <row r="5" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="114"/>
       <c r="C5" s="37" t="s">
         <v>58</v>
       </c>
@@ -2338,8 +2338,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="122"/>
+    <row r="6" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="114"/>
       <c r="C6" s="37" t="s">
         <v>68</v>
       </c>
@@ -2401,9 +2401,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="122"/>
-      <c r="C7" s="129" t="s">
+    <row r="7" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="114"/>
+      <c r="C7" s="121" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="33" t="s">
@@ -2466,9 +2466,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="122"/>
-      <c r="C8" s="129"/>
+    <row r="8" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="114"/>
+      <c r="C8" s="121"/>
       <c r="D8" s="37" t="s">
         <v>61</v>
       </c>
@@ -2529,9 +2529,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="126"/>
-      <c r="C9" s="130"/>
+    <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="118"/>
+      <c r="C9" s="122"/>
       <c r="D9" s="34" t="s">
         <v>62</v>
       </c>
@@ -2592,8 +2592,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="123" t="s">
+    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="115" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="42" t="s">
@@ -2657,8 +2657,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="124"/>
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="116"/>
       <c r="C11" s="37" t="s">
         <v>65</v>
       </c>
@@ -2711,8 +2711,8 @@
       <c r="V11" s="26"/>
       <c r="W11" s="26"/>
     </row>
-    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="124"/>
+    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="116"/>
       <c r="C12" s="37" t="s">
         <v>66</v>
       </c>
@@ -2774,8 +2774,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="125"/>
+    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="117"/>
       <c r="C13" s="36" t="s">
         <v>113</v>
       </c>
@@ -2837,8 +2837,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="125"/>
+    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="117"/>
       <c r="C14" s="36" t="s">
         <v>111</v>
       </c>
@@ -2892,8 +2892,8 @@
       <c r="V14" s="23"/>
       <c r="W14" s="59"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="125"/>
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="117"/>
       <c r="C15" s="36" t="s">
         <v>67</v>
       </c>
@@ -2947,8 +2947,8 @@
       <c r="V15" s="23"/>
       <c r="W15" s="59"/>
     </row>
-    <row r="16" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="121" t="s">
+    <row r="16" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="113" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="55" t="s">
@@ -3012,8 +3012,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="122"/>
+    <row r="17" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="114"/>
       <c r="C17" s="37" t="s">
         <v>36</v>
       </c>
@@ -3075,8 +3075,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="122"/>
+    <row r="18" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="114"/>
       <c r="C18" s="88" t="s">
         <v>14</v>
       </c>
@@ -3140,9 +3140,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="122"/>
-      <c r="C19" s="111" t="s">
+    <row r="19" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="114"/>
+      <c r="C19" s="134" t="s">
         <v>37</v>
       </c>
       <c r="D19" s="37" t="s">
@@ -3205,9 +3205,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="122"/>
-      <c r="C20" s="111"/>
+    <row r="20" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="114"/>
+      <c r="C20" s="134"/>
       <c r="D20" s="37" t="s">
         <v>127</v>
       </c>
@@ -3268,9 +3268,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="122"/>
-      <c r="C21" s="111"/>
+    <row r="21" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="114"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="37" t="s">
         <v>34</v>
       </c>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="I21" s="46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="J21" s="61">
         <v>0</v>
@@ -3318,14 +3318,16 @@
       <c r="S21" s="61">
         <v>0</v>
       </c>
-      <c r="T21" s="21"/>
+      <c r="T21" s="91">
+        <v>0.23</v>
+      </c>
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
       <c r="W21" s="22"/>
     </row>
-    <row r="22" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="122"/>
-      <c r="C22" s="111"/>
+    <row r="22" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="114"/>
+      <c r="C22" s="134"/>
       <c r="D22" s="37" t="s">
         <v>35</v>
       </c>
@@ -3386,9 +3388,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="122"/>
-      <c r="C23" s="111"/>
+    <row r="23" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="114"/>
+      <c r="C23" s="134"/>
       <c r="D23" s="37" t="s">
         <v>39</v>
       </c>
@@ -3449,9 +3451,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="122"/>
-      <c r="C24" s="111"/>
+    <row r="24" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="114"/>
+      <c r="C24" s="134"/>
       <c r="D24" s="37" t="s">
         <v>40</v>
       </c>
@@ -3512,9 +3514,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="122"/>
-      <c r="C25" s="111"/>
+    <row r="25" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="114"/>
+      <c r="C25" s="134"/>
       <c r="D25" s="37" t="s">
         <v>41</v>
       </c>
@@ -3575,9 +3577,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="122"/>
-      <c r="C26" s="111"/>
+    <row r="26" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="114"/>
+      <c r="C26" s="134"/>
       <c r="D26" s="37" t="s">
         <v>42</v>
       </c>
@@ -3638,9 +3640,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="122"/>
-      <c r="C27" s="111"/>
+    <row r="27" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="114"/>
+      <c r="C27" s="134"/>
       <c r="D27" s="37" t="s">
         <v>43</v>
       </c>
@@ -3701,9 +3703,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="122"/>
-      <c r="C28" s="111"/>
+    <row r="28" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="114"/>
+      <c r="C28" s="134"/>
       <c r="D28" s="37" t="s">
         <v>44</v>
       </c>
@@ -3764,9 +3766,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="122"/>
-      <c r="C29" s="111"/>
+    <row r="29" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="114"/>
+      <c r="C29" s="134"/>
       <c r="D29" s="37" t="s">
         <v>45</v>
       </c>
@@ -3827,9 +3829,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="122"/>
-      <c r="C30" s="111"/>
+    <row r="30" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="114"/>
+      <c r="C30" s="134"/>
       <c r="D30" s="37" t="s">
         <v>46</v>
       </c>
@@ -3890,9 +3892,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="122"/>
-      <c r="C31" s="111"/>
+    <row r="31" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="114"/>
+      <c r="C31" s="134"/>
       <c r="D31" s="37" t="s">
         <v>47</v>
       </c>
@@ -3953,9 +3955,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="122"/>
-      <c r="C32" s="111"/>
+    <row r="32" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="114"/>
+      <c r="C32" s="134"/>
       <c r="D32" s="37" t="s">
         <v>48</v>
       </c>
@@ -4016,9 +4018,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="122"/>
-      <c r="C33" s="111"/>
+    <row r="33" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="114"/>
+      <c r="C33" s="134"/>
       <c r="D33" s="37" t="s">
         <v>49</v>
       </c>
@@ -4079,9 +4081,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="122"/>
-      <c r="C34" s="111"/>
+    <row r="34" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="114"/>
+      <c r="C34" s="134"/>
       <c r="D34" s="37" t="s">
         <v>50</v>
       </c>
@@ -4142,9 +4144,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="122"/>
-      <c r="C35" s="111"/>
+    <row r="35" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="114"/>
+      <c r="C35" s="134"/>
       <c r="D35" s="37" t="s">
         <v>51</v>
       </c>
@@ -4205,9 +4207,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="122"/>
-      <c r="C36" s="111"/>
+    <row r="36" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="114"/>
+      <c r="C36" s="134"/>
       <c r="D36" s="37" t="s">
         <v>128</v>
       </c>
@@ -4268,9 +4270,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="122"/>
-      <c r="C37" s="111"/>
+    <row r="37" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="114"/>
+      <c r="C37" s="134"/>
       <c r="D37" s="43" t="s">
         <v>104</v>
       </c>
@@ -4331,8 +4333,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="122"/>
+    <row r="38" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="114"/>
       <c r="C38" s="40" t="s">
         <v>52</v>
       </c>
@@ -4386,8 +4388,8 @@
       <c r="V38" s="21"/>
       <c r="W38" s="22"/>
     </row>
-    <row r="39" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="122"/>
+    <row r="39" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="114"/>
       <c r="C39" s="40" t="s">
         <v>54</v>
       </c>
@@ -4441,8 +4443,8 @@
       <c r="V39" s="21"/>
       <c r="W39" s="22"/>
     </row>
-    <row r="40" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="122"/>
+    <row r="40" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="114"/>
       <c r="C40" s="40" t="s">
         <v>55</v>
       </c>
@@ -4504,8 +4506,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="122"/>
+    <row r="41" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="114"/>
       <c r="C41" s="47" t="s">
         <v>105</v>
       </c>
@@ -4559,11 +4561,11 @@
       <c r="V41" s="21"/>
       <c r="W41" s="22"/>
     </row>
-    <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="113" t="s">
+    <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="109" t="s">
+      <c r="C42" s="132" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="41" t="s">
@@ -4580,7 +4582,7 @@
         <v>0.5</v>
       </c>
       <c r="I42" s="48">
-        <f t="shared" ref="I42:I98" si="2">SUM(J42:W42)</f>
+        <f t="shared" ref="I42:I97" si="2">SUM(J42:W42)</f>
         <v>0.95</v>
       </c>
       <c r="J42" s="92">
@@ -4626,9 +4628,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="114"/>
-      <c r="C43" s="110"/>
+    <row r="43" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="106"/>
+      <c r="C43" s="133"/>
       <c r="D43" s="40" t="s">
         <v>21</v>
       </c>
@@ -4689,9 +4691,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="114"/>
-      <c r="C44" s="110"/>
+    <row r="44" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="106"/>
+      <c r="C44" s="133"/>
       <c r="D44" s="40" t="s">
         <v>22</v>
       </c>
@@ -4752,9 +4754,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="114"/>
-      <c r="C45" s="110"/>
+    <row r="45" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="106"/>
+      <c r="C45" s="133"/>
       <c r="D45" s="40" t="s">
         <v>23</v>
       </c>
@@ -4815,9 +4817,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="114"/>
-      <c r="C46" s="110"/>
+    <row r="46" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="106"/>
+      <c r="C46" s="133"/>
       <c r="D46" s="40" t="s">
         <v>24</v>
       </c>
@@ -4878,9 +4880,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="114"/>
-      <c r="C47" s="110"/>
+    <row r="47" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="106"/>
+      <c r="C47" s="133"/>
       <c r="D47" s="40" t="s">
         <v>25</v>
       </c>
@@ -4941,9 +4943,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="114"/>
-      <c r="C48" s="110"/>
+    <row r="48" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="106"/>
+      <c r="C48" s="133"/>
       <c r="D48" s="40" t="s">
         <v>26</v>
       </c>
@@ -5004,9 +5006,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="114"/>
-      <c r="C49" s="110"/>
+    <row r="49" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="106"/>
+      <c r="C49" s="133"/>
       <c r="D49" s="40" t="s">
         <v>27</v>
       </c>
@@ -5067,9 +5069,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="114"/>
-      <c r="C50" s="110"/>
+    <row r="50" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="106"/>
+      <c r="C50" s="133"/>
       <c r="D50" s="40" t="s">
         <v>28</v>
       </c>
@@ -5130,9 +5132,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="114"/>
-      <c r="C51" s="110"/>
+    <row r="51" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="106"/>
+      <c r="C51" s="133"/>
       <c r="D51" s="40" t="s">
         <v>29</v>
       </c>
@@ -5193,9 +5195,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="114"/>
-      <c r="C52" s="110"/>
+    <row r="52" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="106"/>
+      <c r="C52" s="133"/>
       <c r="D52" s="40" t="s">
         <v>30</v>
       </c>
@@ -5256,9 +5258,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="114"/>
-      <c r="C53" s="110"/>
+    <row r="53" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="106"/>
+      <c r="C53" s="133"/>
       <c r="D53" s="40" t="s">
         <v>31</v>
       </c>
@@ -5319,9 +5321,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="114"/>
-      <c r="C54" s="110"/>
+    <row r="54" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="106"/>
+      <c r="C54" s="133"/>
       <c r="D54" s="40" t="s">
         <v>70</v>
       </c>
@@ -5337,7 +5339,7 @@
       </c>
       <c r="I54" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="J54" s="61">
         <v>0</v>
@@ -5372,13 +5374,19 @@
       <c r="T54" s="101">
         <v>0</v>
       </c>
-      <c r="U54" s="21"/>
-      <c r="V54" s="21"/>
-      <c r="W54" s="22"/>
-    </row>
-    <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="114"/>
-      <c r="C55" s="110"/>
+      <c r="U54" s="87">
+        <v>0.12</v>
+      </c>
+      <c r="V54" s="87">
+        <v>0</v>
+      </c>
+      <c r="W54" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="106"/>
+      <c r="C55" s="133"/>
       <c r="D55" s="40" t="s">
         <v>71</v>
       </c>
@@ -5394,7 +5402,7 @@
       </c>
       <c r="I55" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="J55" s="61">
         <v>0</v>
@@ -5429,15 +5437,21 @@
       <c r="T55" s="101">
         <v>0</v>
       </c>
-      <c r="U55" s="21"/>
-      <c r="V55" s="21"/>
-      <c r="W55" s="22"/>
-    </row>
-    <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="114"/>
-      <c r="C56" s="110"/>
+      <c r="U55" s="87">
+        <v>0.17</v>
+      </c>
+      <c r="V55" s="87">
+        <v>0</v>
+      </c>
+      <c r="W55" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="106"/>
+      <c r="C56" s="133"/>
       <c r="D56" s="40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E56" s="40"/>
       <c r="F56" s="40" t="s">
@@ -5451,7 +5465,7 @@
       </c>
       <c r="I56" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="J56" s="61">
         <v>0</v>
@@ -5486,15 +5500,21 @@
       <c r="T56" s="101">
         <v>0</v>
       </c>
-      <c r="U56" s="21"/>
-      <c r="V56" s="21"/>
-      <c r="W56" s="22"/>
-    </row>
-    <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="114"/>
-      <c r="C57" s="110"/>
+      <c r="U56" s="87">
+        <v>0.17</v>
+      </c>
+      <c r="V56" s="87">
+        <v>0</v>
+      </c>
+      <c r="W56" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="106"/>
+      <c r="C57" s="133"/>
       <c r="D57" s="40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E57" s="40"/>
       <c r="F57" s="40" t="s">
@@ -5508,7 +5528,7 @@
       </c>
       <c r="I57" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J57" s="61">
         <v>0</v>
@@ -5543,15 +5563,21 @@
       <c r="T57" s="101">
         <v>0</v>
       </c>
-      <c r="U57" s="21"/>
-      <c r="V57" s="21"/>
-      <c r="W57" s="22"/>
-    </row>
-    <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="114"/>
-      <c r="C58" s="110"/>
+      <c r="U57" s="87">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V57" s="87">
+        <v>0</v>
+      </c>
+      <c r="W57" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="106"/>
+      <c r="C58" s="133"/>
       <c r="D58" s="40" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E58" s="40"/>
       <c r="F58" s="40" t="s">
@@ -5565,7 +5591,7 @@
       </c>
       <c r="I58" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="J58" s="61">
         <v>0</v>
@@ -5600,15 +5626,21 @@
       <c r="T58" s="101">
         <v>0</v>
       </c>
-      <c r="U58" s="21"/>
-      <c r="V58" s="21"/>
-      <c r="W58" s="22"/>
-    </row>
-    <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="114"/>
-      <c r="C59" s="110"/>
+      <c r="U58" s="87">
+        <v>0.12</v>
+      </c>
+      <c r="V58" s="87">
+        <v>0</v>
+      </c>
+      <c r="W58" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="106"/>
+      <c r="C59" s="133"/>
       <c r="D59" s="40" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E59" s="40"/>
       <c r="F59" s="40" t="s">
@@ -5622,7 +5654,7 @@
       </c>
       <c r="I59" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="J59" s="61">
         <v>0</v>
@@ -5657,15 +5689,21 @@
       <c r="T59" s="101">
         <v>0</v>
       </c>
-      <c r="U59" s="21"/>
-      <c r="V59" s="21"/>
-      <c r="W59" s="22"/>
-    </row>
-    <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="114"/>
-      <c r="C60" s="110"/>
+      <c r="U59" s="87">
+        <v>0.06</v>
+      </c>
+      <c r="V59" s="87">
+        <v>0</v>
+      </c>
+      <c r="W59" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="106"/>
+      <c r="C60" s="133"/>
       <c r="D60" s="40" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E60" s="40"/>
       <c r="F60" s="40" t="s">
@@ -5679,7 +5717,7 @@
       </c>
       <c r="I60" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J60" s="61">
         <v>0</v>
@@ -5714,15 +5752,21 @@
       <c r="T60" s="101">
         <v>0</v>
       </c>
-      <c r="U60" s="21"/>
-      <c r="V60" s="21"/>
-      <c r="W60" s="22"/>
-    </row>
-    <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="114"/>
-      <c r="C61" s="110"/>
+      <c r="U60" s="87">
+        <v>0.04</v>
+      </c>
+      <c r="V60" s="87">
+        <v>0</v>
+      </c>
+      <c r="W60" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="106"/>
+      <c r="C61" s="133"/>
       <c r="D61" s="40" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E61" s="40"/>
       <c r="F61" s="40" t="s">
@@ -5736,7 +5780,7 @@
       </c>
       <c r="I61" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J61" s="61">
         <v>0</v>
@@ -5771,15 +5815,21 @@
       <c r="T61" s="101">
         <v>0</v>
       </c>
-      <c r="U61" s="21"/>
-      <c r="V61" s="21"/>
-      <c r="W61" s="22"/>
-    </row>
-    <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="114"/>
-      <c r="C62" s="110"/>
+      <c r="U61" s="87">
+        <v>0.05</v>
+      </c>
+      <c r="V61" s="87">
+        <v>0</v>
+      </c>
+      <c r="W61" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="106"/>
+      <c r="C62" s="133"/>
       <c r="D62" s="40" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E62" s="40"/>
       <c r="F62" s="40" t="s">
@@ -5793,7 +5843,7 @@
       </c>
       <c r="I62" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J62" s="61">
         <v>0</v>
@@ -5828,15 +5878,21 @@
       <c r="T62" s="101">
         <v>0</v>
       </c>
-      <c r="U62" s="21"/>
-      <c r="V62" s="21"/>
-      <c r="W62" s="22"/>
-    </row>
-    <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="114"/>
-      <c r="C63" s="110"/>
+      <c r="U62" s="87">
+        <v>0.04</v>
+      </c>
+      <c r="V62" s="87">
+        <v>0</v>
+      </c>
+      <c r="W62" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="106"/>
+      <c r="C63" s="133"/>
       <c r="D63" s="40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E63" s="40"/>
       <c r="F63" s="40" t="s">
@@ -5850,7 +5906,7 @@
       </c>
       <c r="I63" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J63" s="61">
         <v>0</v>
@@ -5885,15 +5941,21 @@
       <c r="T63" s="101">
         <v>0</v>
       </c>
-      <c r="U63" s="21"/>
-      <c r="V63" s="21"/>
-      <c r="W63" s="22"/>
-    </row>
-    <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="114"/>
-      <c r="C64" s="110"/>
+      <c r="U63" s="87">
+        <v>0.1</v>
+      </c>
+      <c r="V63" s="87">
+        <v>0</v>
+      </c>
+      <c r="W63" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="106"/>
+      <c r="C64" s="133"/>
       <c r="D64" s="40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E64" s="40"/>
       <c r="F64" s="40" t="s">
@@ -5946,11 +6008,11 @@
       <c r="V64" s="21"/>
       <c r="W64" s="22"/>
     </row>
-    <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="114"/>
-      <c r="C65" s="110"/>
+    <row r="65" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="106"/>
+      <c r="C65" s="133"/>
       <c r="D65" s="40" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E65" s="40"/>
       <c r="F65" s="40" t="s">
@@ -6003,11 +6065,11 @@
       <c r="V65" s="21"/>
       <c r="W65" s="22"/>
     </row>
-    <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="114"/>
-      <c r="C66" s="110"/>
+    <row r="66" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="106"/>
+      <c r="C66" s="133"/>
       <c r="D66" s="40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E66" s="40"/>
       <c r="F66" s="40" t="s">
@@ -6060,11 +6122,11 @@
       <c r="V66" s="21"/>
       <c r="W66" s="22"/>
     </row>
-    <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="114"/>
-      <c r="C67" s="110"/>
+    <row r="67" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="106"/>
+      <c r="C67" s="133"/>
       <c r="D67" s="40" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E67" s="40"/>
       <c r="F67" s="40" t="s">
@@ -6117,11 +6179,11 @@
       <c r="V67" s="21"/>
       <c r="W67" s="22"/>
     </row>
-    <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="114"/>
-      <c r="C68" s="110"/>
+    <row r="68" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="106"/>
+      <c r="C68" s="133"/>
       <c r="D68" s="40" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E68" s="40"/>
       <c r="F68" s="40" t="s">
@@ -6174,11 +6236,11 @@
       <c r="V68" s="21"/>
       <c r="W68" s="22"/>
     </row>
-    <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="114"/>
-      <c r="C69" s="110"/>
+    <row r="69" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="106"/>
+      <c r="C69" s="133"/>
       <c r="D69" s="40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E69" s="40"/>
       <c r="F69" s="40" t="s">
@@ -6231,11 +6293,11 @@
       <c r="V69" s="21"/>
       <c r="W69" s="22"/>
     </row>
-    <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="114"/>
-      <c r="C70" s="110"/>
+    <row r="70" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="106"/>
+      <c r="C70" s="133"/>
       <c r="D70" s="40" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E70" s="40"/>
       <c r="F70" s="40" t="s">
@@ -6288,11 +6350,11 @@
       <c r="V70" s="21"/>
       <c r="W70" s="22"/>
     </row>
-    <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="114"/>
-      <c r="C71" s="110"/>
+    <row r="71" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="106"/>
+      <c r="C71" s="133"/>
       <c r="D71" s="40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E71" s="40"/>
       <c r="F71" s="40" t="s">
@@ -6345,11 +6407,11 @@
       <c r="V71" s="21"/>
       <c r="W71" s="22"/>
     </row>
-    <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="114"/>
-      <c r="C72" s="110"/>
+    <row r="72" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="106"/>
+      <c r="C72" s="133"/>
       <c r="D72" s="40" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E72" s="40"/>
       <c r="F72" s="40" t="s">
@@ -6402,11 +6464,11 @@
       <c r="V72" s="21"/>
       <c r="W72" s="22"/>
     </row>
-    <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="114"/>
-      <c r="C73" s="110"/>
+    <row r="73" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="106"/>
+      <c r="C73" s="133"/>
       <c r="D73" s="40" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E73" s="40"/>
       <c r="F73" s="40" t="s">
@@ -6459,11 +6521,11 @@
       <c r="V73" s="21"/>
       <c r="W73" s="22"/>
     </row>
-    <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="114"/>
-      <c r="C74" s="110"/>
+    <row r="74" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="106"/>
+      <c r="C74" s="133"/>
       <c r="D74" s="40" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E74" s="40"/>
       <c r="F74" s="40" t="s">
@@ -6516,11 +6578,11 @@
       <c r="V74" s="21"/>
       <c r="W74" s="22"/>
     </row>
-    <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="114"/>
-      <c r="C75" s="110"/>
+    <row r="75" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="106"/>
+      <c r="C75" s="133"/>
       <c r="D75" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E75" s="40"/>
       <c r="F75" s="40" t="s">
@@ -6573,11 +6635,11 @@
       <c r="V75" s="21"/>
       <c r="W75" s="22"/>
     </row>
-    <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="114"/>
-      <c r="C76" s="110"/>
+    <row r="76" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="106"/>
+      <c r="C76" s="133"/>
       <c r="D76" s="40" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E76" s="40"/>
       <c r="F76" s="40" t="s">
@@ -6630,11 +6692,11 @@
       <c r="V76" s="21"/>
       <c r="W76" s="22"/>
     </row>
-    <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="114"/>
-      <c r="C77" s="110"/>
+    <row r="77" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="106"/>
+      <c r="C77" s="133"/>
       <c r="D77" s="40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E77" s="40"/>
       <c r="F77" s="40" t="s">
@@ -6687,11 +6749,11 @@
       <c r="V77" s="21"/>
       <c r="W77" s="22"/>
     </row>
-    <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="114"/>
-      <c r="C78" s="110"/>
+    <row r="78" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="106"/>
+      <c r="C78" s="133"/>
       <c r="D78" s="40" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E78" s="40"/>
       <c r="F78" s="40" t="s">
@@ -6744,11 +6806,11 @@
       <c r="V78" s="21"/>
       <c r="W78" s="22"/>
     </row>
-    <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="114"/>
-      <c r="C79" s="110"/>
+    <row r="79" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="106"/>
+      <c r="C79" s="133"/>
       <c r="D79" s="40" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E79" s="40"/>
       <c r="F79" s="40" t="s">
@@ -6801,11 +6863,11 @@
       <c r="V79" s="21"/>
       <c r="W79" s="22"/>
     </row>
-    <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="114"/>
-      <c r="C80" s="110"/>
+    <row r="80" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="106"/>
+      <c r="C80" s="133"/>
       <c r="D80" s="40" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E80" s="40"/>
       <c r="F80" s="40" t="s">
@@ -6818,7 +6880,7 @@
         <v>0.25</v>
       </c>
       <c r="I80" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I80:I85" si="3">SUM(J80:W80)</f>
         <v>0</v>
       </c>
       <c r="J80" s="61">
@@ -6858,11 +6920,11 @@
       <c r="V80" s="21"/>
       <c r="W80" s="22"/>
     </row>
-    <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="114"/>
-      <c r="C81" s="110"/>
+    <row r="81" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="106"/>
+      <c r="C81" s="133"/>
       <c r="D81" s="40" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="E81" s="40"/>
       <c r="F81" s="40" t="s">
@@ -6875,7 +6937,7 @@
         <v>0.25</v>
       </c>
       <c r="I81" s="46">
-        <f t="shared" ref="I81:I86" si="3">SUM(J81:W81)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J81" s="61">
@@ -6915,11 +6977,11 @@
       <c r="V81" s="21"/>
       <c r="W81" s="22"/>
     </row>
-    <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="114"/>
-      <c r="C82" s="110"/>
+    <row r="82" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="106"/>
+      <c r="C82" s="133"/>
       <c r="D82" s="40" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E82" s="40"/>
       <c r="F82" s="40" t="s">
@@ -6972,147 +7034,147 @@
       <c r="V82" s="21"/>
       <c r="W82" s="22"/>
     </row>
-    <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="114"/>
-      <c r="C83" s="110"/>
+    <row r="83" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="106"/>
+      <c r="C83" s="133"/>
       <c r="D83" s="40" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="E83" s="40"/>
       <c r="F83" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G83" s="4">
-        <v>2</v>
-      </c>
-      <c r="H83" s="4">
-        <v>0.25</v>
+      <c r="G83" s="16">
+        <v>1</v>
+      </c>
+      <c r="H83" s="16">
+        <v>1</v>
       </c>
       <c r="I83" s="46">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J83" s="61">
         <v>0</v>
       </c>
-      <c r="K83" s="61">
-        <v>0</v>
-      </c>
-      <c r="L83" s="61">
-        <v>0</v>
-      </c>
-      <c r="M83" s="61">
-        <v>0</v>
-      </c>
-      <c r="N83" s="61">
-        <v>0</v>
-      </c>
-      <c r="O83" s="61">
-        <v>0</v>
-      </c>
-      <c r="P83" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q83" s="61">
-        <v>0</v>
-      </c>
-      <c r="R83" s="61">
-        <v>0</v>
-      </c>
-      <c r="S83" s="61">
-        <v>0</v>
-      </c>
-      <c r="T83" s="101">
-        <v>0</v>
-      </c>
-      <c r="U83" s="21"/>
-      <c r="V83" s="21"/>
-      <c r="W83" s="22"/>
-    </row>
-    <row r="84" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="114"/>
-      <c r="C84" s="110"/>
-      <c r="D84" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E84" s="40"/>
-      <c r="F84" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="G84" s="16">
-        <v>1</v>
-      </c>
-      <c r="H84" s="16">
-        <v>1</v>
+      <c r="K83" s="39">
+        <v>0.8</v>
+      </c>
+      <c r="L83" s="39">
+        <v>0</v>
+      </c>
+      <c r="M83" s="39">
+        <v>0</v>
+      </c>
+      <c r="N83" s="39">
+        <v>0</v>
+      </c>
+      <c r="O83" s="39">
+        <v>0</v>
+      </c>
+      <c r="P83" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="39">
+        <v>0</v>
+      </c>
+      <c r="R83" s="39">
+        <v>0</v>
+      </c>
+      <c r="S83" s="39">
+        <v>0</v>
+      </c>
+      <c r="T83" s="39">
+        <v>0</v>
+      </c>
+      <c r="U83" s="39">
+        <v>0</v>
+      </c>
+      <c r="V83" s="39">
+        <v>0</v>
+      </c>
+      <c r="W83" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="106"/>
+      <c r="C84" s="96" t="s">
+        <v>37</v>
+      </c>
+      <c r="D84" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="E84" s="43"/>
+      <c r="F84" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" s="4">
+        <v>5</v>
+      </c>
+      <c r="H84" s="4">
+        <v>2</v>
       </c>
       <c r="I84" s="46">
         <f t="shared" si="3"/>
-        <v>0.8</v>
+        <v>1.48</v>
       </c>
       <c r="J84" s="61">
         <v>0</v>
       </c>
-      <c r="K84" s="39">
-        <v>0.8</v>
-      </c>
-      <c r="L84" s="39">
-        <v>0</v>
-      </c>
-      <c r="M84" s="39">
-        <v>0</v>
-      </c>
-      <c r="N84" s="39">
-        <v>0</v>
-      </c>
-      <c r="O84" s="39">
-        <v>0</v>
-      </c>
-      <c r="P84" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q84" s="39">
-        <v>0</v>
-      </c>
-      <c r="R84" s="39">
-        <v>0</v>
-      </c>
-      <c r="S84" s="39">
-        <v>0</v>
-      </c>
-      <c r="T84" s="39">
-        <v>0</v>
-      </c>
-      <c r="U84" s="39">
-        <v>0</v>
-      </c>
-      <c r="V84" s="39">
-        <v>0</v>
-      </c>
-      <c r="W84" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="114"/>
+      <c r="K84" s="61">
+        <v>0</v>
+      </c>
+      <c r="L84" s="61">
+        <v>0</v>
+      </c>
+      <c r="M84" s="61">
+        <v>0</v>
+      </c>
+      <c r="N84" s="61">
+        <v>0</v>
+      </c>
+      <c r="O84" s="61">
+        <v>0</v>
+      </c>
+      <c r="P84" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="61">
+        <v>0</v>
+      </c>
+      <c r="R84" s="61">
+        <v>0</v>
+      </c>
+      <c r="S84" s="61">
+        <v>0</v>
+      </c>
+      <c r="T84" s="87">
+        <v>1.48</v>
+      </c>
+      <c r="U84" s="21"/>
+      <c r="V84" s="21"/>
+      <c r="W84" s="22"/>
+    </row>
+    <row r="85" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="106"/>
       <c r="C85" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="D85" s="37" t="s">
-        <v>129</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D85" s="43"/>
       <c r="E85" s="43"/>
-      <c r="F85" s="43" t="s">
+      <c r="F85" s="37" t="s">
         <v>15</v>
       </c>
       <c r="G85" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H85" s="4">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="I85" s="46">
         <f t="shared" si="3"/>
-        <v>1.48</v>
+        <v>0.25</v>
       </c>
       <c r="J85" s="61">
         <v>0</v>
@@ -7135,26 +7197,32 @@
       <c r="P85" s="61">
         <v>0</v>
       </c>
-      <c r="Q85" s="61">
-        <v>0</v>
-      </c>
-      <c r="R85" s="61">
-        <v>0</v>
-      </c>
-      <c r="S85" s="61">
-        <v>0</v>
-      </c>
-      <c r="T85" s="87">
-        <v>1.48</v>
-      </c>
-      <c r="U85" s="21"/>
-      <c r="V85" s="21"/>
-      <c r="W85" s="22"/>
-    </row>
-    <row r="86" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="114"/>
-      <c r="C86" s="96" t="s">
-        <v>126</v>
+      <c r="Q85" s="39">
+        <v>0.25</v>
+      </c>
+      <c r="R85" s="39">
+        <v>0</v>
+      </c>
+      <c r="S85" s="39">
+        <v>0</v>
+      </c>
+      <c r="T85" s="39">
+        <v>0</v>
+      </c>
+      <c r="U85" s="39">
+        <v>0</v>
+      </c>
+      <c r="V85" s="39">
+        <v>0</v>
+      </c>
+      <c r="W85" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="106"/>
+      <c r="C86" s="73" t="s">
+        <v>118</v>
       </c>
       <c r="D86" s="43"/>
       <c r="E86" s="43"/>
@@ -7162,295 +7230,287 @@
         <v>15</v>
       </c>
       <c r="G86" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H86" s="4">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="I86" s="46">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="J86" s="61">
-        <v>0</v>
-      </c>
-      <c r="K86" s="61">
-        <v>0</v>
-      </c>
-      <c r="L86" s="61">
-        <v>0</v>
-      </c>
-      <c r="M86" s="61">
-        <v>0</v>
-      </c>
-      <c r="N86" s="61">
-        <v>0</v>
-      </c>
-      <c r="O86" s="61">
-        <v>0</v>
-      </c>
-      <c r="P86" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q86" s="39">
-        <v>0.25</v>
-      </c>
-      <c r="R86" s="39">
-        <v>0</v>
-      </c>
-      <c r="S86" s="39">
-        <v>0</v>
-      </c>
-      <c r="T86" s="39">
-        <v>0</v>
-      </c>
-      <c r="U86" s="39">
-        <v>0</v>
-      </c>
-      <c r="V86" s="39">
-        <v>0</v>
-      </c>
-      <c r="W86" s="75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="114"/>
-      <c r="C87" s="73" t="s">
-        <v>118</v>
-      </c>
-      <c r="D87" s="43"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G87" s="4">
-        <v>1</v>
-      </c>
-      <c r="H87" s="4">
-        <v>2</v>
-      </c>
-      <c r="I87" s="46">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="J87" s="39">
+      <c r="J86" s="39">
         <v>1.5</v>
       </c>
-      <c r="K87" s="39">
-        <v>0</v>
-      </c>
-      <c r="L87" s="39">
-        <v>0</v>
-      </c>
-      <c r="M87" s="39">
-        <v>0</v>
-      </c>
-      <c r="N87" s="39">
-        <v>0</v>
-      </c>
-      <c r="O87" s="39">
-        <v>0</v>
-      </c>
-      <c r="P87" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q87" s="39">
-        <v>0</v>
-      </c>
-      <c r="R87" s="39">
-        <v>0</v>
-      </c>
-      <c r="S87" s="39">
-        <v>0</v>
-      </c>
-      <c r="T87" s="39">
-        <v>0</v>
-      </c>
-      <c r="U87" s="39">
-        <v>0</v>
-      </c>
-      <c r="V87" s="39">
-        <v>0</v>
-      </c>
-      <c r="W87" s="75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="114"/>
-      <c r="C88" s="65" t="s">
+      <c r="K86" s="39">
+        <v>0</v>
+      </c>
+      <c r="L86" s="39">
+        <v>0</v>
+      </c>
+      <c r="M86" s="39">
+        <v>0</v>
+      </c>
+      <c r="N86" s="39">
+        <v>0</v>
+      </c>
+      <c r="O86" s="39">
+        <v>0</v>
+      </c>
+      <c r="P86" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q86" s="39">
+        <v>0</v>
+      </c>
+      <c r="R86" s="39">
+        <v>0</v>
+      </c>
+      <c r="S86" s="39">
+        <v>0</v>
+      </c>
+      <c r="T86" s="39">
+        <v>0</v>
+      </c>
+      <c r="U86" s="39">
+        <v>0</v>
+      </c>
+      <c r="V86" s="39">
+        <v>0</v>
+      </c>
+      <c r="W86" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:23" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B87" s="106"/>
+      <c r="C87" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="D88" s="33"/>
-      <c r="E88" s="45"/>
-      <c r="F88" s="45" t="s">
+      <c r="D87" s="33"/>
+      <c r="E87" s="45"/>
+      <c r="F87" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="G88" s="4">
+      <c r="G87" s="4">
         <v>4</v>
       </c>
-      <c r="H88" s="4">
+      <c r="H87" s="4">
         <v>1</v>
       </c>
-      <c r="I88" s="46">
-        <f>SUM(J88:W88)</f>
-        <v>0</v>
-      </c>
-      <c r="J88" s="61">
-        <v>0</v>
-      </c>
-      <c r="K88" s="61">
-        <v>0</v>
-      </c>
-      <c r="L88" s="61">
-        <v>0</v>
-      </c>
-      <c r="M88" s="61">
-        <v>0</v>
-      </c>
-      <c r="N88" s="61">
-        <v>0</v>
-      </c>
-      <c r="O88" s="61">
-        <v>0</v>
-      </c>
-      <c r="P88" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q88" s="61">
-        <v>0</v>
-      </c>
-      <c r="R88" s="61">
-        <v>0</v>
-      </c>
-      <c r="S88" s="61">
-        <v>0</v>
-      </c>
-      <c r="T88" s="21"/>
-      <c r="U88" s="21"/>
-      <c r="V88" s="21"/>
-      <c r="W88" s="22"/>
-    </row>
-    <row r="89" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="131" t="s">
+      <c r="I87" s="46">
+        <f>SUM(J87:W87)</f>
+        <v>0</v>
+      </c>
+      <c r="J87" s="61">
+        <v>0</v>
+      </c>
+      <c r="K87" s="61">
+        <v>0</v>
+      </c>
+      <c r="L87" s="61">
+        <v>0</v>
+      </c>
+      <c r="M87" s="61">
+        <v>0</v>
+      </c>
+      <c r="N87" s="61">
+        <v>0</v>
+      </c>
+      <c r="O87" s="61">
+        <v>0</v>
+      </c>
+      <c r="P87" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="61">
+        <v>0</v>
+      </c>
+      <c r="R87" s="61">
+        <v>0</v>
+      </c>
+      <c r="S87" s="61">
+        <v>0</v>
+      </c>
+      <c r="T87" s="21"/>
+      <c r="U87" s="21"/>
+      <c r="V87" s="21"/>
+      <c r="W87" s="22"/>
+    </row>
+    <row r="88" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="123" t="s">
         <v>85</v>
       </c>
-      <c r="C89" s="29" t="s">
+      <c r="C88" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D89" s="30"/>
-      <c r="E89" s="29"/>
-      <c r="F89" s="29" t="s">
+      <c r="D88" s="30"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G89" s="12">
+      <c r="G88" s="12">
         <v>6</v>
       </c>
-      <c r="H89" s="12">
+      <c r="H88" s="12">
         <v>0.75</v>
+      </c>
+      <c r="I88" s="48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J88" s="60">
+        <v>0</v>
+      </c>
+      <c r="K88" s="60">
+        <v>0</v>
+      </c>
+      <c r="L88" s="60">
+        <v>0</v>
+      </c>
+      <c r="M88" s="60">
+        <v>0</v>
+      </c>
+      <c r="N88" s="60">
+        <v>0</v>
+      </c>
+      <c r="O88" s="60">
+        <v>0</v>
+      </c>
+      <c r="P88" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q88" s="60">
+        <v>0</v>
+      </c>
+      <c r="R88" s="60">
+        <v>0</v>
+      </c>
+      <c r="S88" s="60">
+        <v>0</v>
+      </c>
+      <c r="T88" s="19"/>
+      <c r="U88" s="19"/>
+      <c r="V88" s="19"/>
+      <c r="W88" s="57"/>
+    </row>
+    <row r="89" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="124"/>
+      <c r="C89" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D89" s="31"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" s="27">
+        <v>6</v>
+      </c>
+      <c r="H89" s="27">
+        <v>1.5</v>
       </c>
       <c r="I89" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J89" s="60">
-        <v>0</v>
-      </c>
-      <c r="K89" s="60">
-        <v>0</v>
-      </c>
-      <c r="L89" s="60">
-        <v>0</v>
-      </c>
-      <c r="M89" s="60">
-        <v>0</v>
-      </c>
-      <c r="N89" s="60">
-        <v>0</v>
-      </c>
-      <c r="O89" s="60">
-        <v>0</v>
-      </c>
-      <c r="P89" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q89" s="60">
-        <v>0</v>
-      </c>
-      <c r="R89" s="60">
-        <v>0</v>
-      </c>
-      <c r="S89" s="60">
-        <v>0</v>
-      </c>
-      <c r="T89" s="19"/>
-      <c r="U89" s="19"/>
-      <c r="V89" s="19"/>
-      <c r="W89" s="57"/>
-    </row>
-    <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="132"/>
-      <c r="C90" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D90" s="31"/>
-      <c r="E90" s="32"/>
-      <c r="F90" s="32" t="s">
+      <c r="J89" s="63">
+        <v>0</v>
+      </c>
+      <c r="K89" s="63">
+        <v>0</v>
+      </c>
+      <c r="L89" s="63">
+        <v>0</v>
+      </c>
+      <c r="M89" s="63">
+        <v>0</v>
+      </c>
+      <c r="N89" s="63">
+        <v>0</v>
+      </c>
+      <c r="O89" s="63">
+        <v>0</v>
+      </c>
+      <c r="P89" s="63">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="63">
+        <v>0</v>
+      </c>
+      <c r="R89" s="63">
+        <v>0</v>
+      </c>
+      <c r="S89" s="63">
+        <v>0</v>
+      </c>
+      <c r="T89" s="26"/>
+      <c r="U89" s="26"/>
+      <c r="V89" s="26"/>
+      <c r="W89" s="56"/>
+    </row>
+    <row r="90" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="125"/>
+      <c r="C90" s="135" t="s">
+        <v>101</v>
+      </c>
+      <c r="D90" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E90" s="45"/>
+      <c r="F90" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="G90" s="27">
+      <c r="G90" s="4">
         <v>6</v>
       </c>
-      <c r="H90" s="27">
-        <v>1.5</v>
-      </c>
-      <c r="I90" s="48">
+      <c r="H90" s="4">
+        <v>1</v>
+      </c>
+      <c r="I90" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J90" s="63">
-        <v>0</v>
-      </c>
-      <c r="K90" s="63">
-        <v>0</v>
-      </c>
-      <c r="L90" s="63">
-        <v>0</v>
-      </c>
-      <c r="M90" s="63">
-        <v>0</v>
-      </c>
-      <c r="N90" s="63">
-        <v>0</v>
-      </c>
-      <c r="O90" s="63">
-        <v>0</v>
-      </c>
-      <c r="P90" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q90" s="63">
-        <v>0</v>
-      </c>
-      <c r="R90" s="63">
-        <v>0</v>
-      </c>
-      <c r="S90" s="63">
-        <v>0</v>
-      </c>
-      <c r="T90" s="26"/>
-      <c r="U90" s="26"/>
-      <c r="V90" s="26"/>
-      <c r="W90" s="56"/>
-    </row>
-    <row r="91" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="133"/>
-      <c r="C91" s="112" t="s">
-        <v>101</v>
-      </c>
+      <c r="J90" s="61">
+        <v>0</v>
+      </c>
+      <c r="K90" s="61">
+        <v>0</v>
+      </c>
+      <c r="L90" s="61">
+        <v>0</v>
+      </c>
+      <c r="M90" s="61">
+        <v>0</v>
+      </c>
+      <c r="N90" s="61">
+        <v>0</v>
+      </c>
+      <c r="O90" s="61">
+        <v>0</v>
+      </c>
+      <c r="P90" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q90" s="61">
+        <v>0</v>
+      </c>
+      <c r="R90" s="61">
+        <v>0</v>
+      </c>
+      <c r="S90" s="61">
+        <v>0</v>
+      </c>
+      <c r="T90" s="20"/>
+      <c r="U90" s="20"/>
+      <c r="V90" s="20"/>
+      <c r="W90" s="49"/>
+    </row>
+    <row r="91" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B91" s="126"/>
+      <c r="C91" s="135"/>
       <c r="D91" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E91" s="45"/>
       <c r="F91" s="45" t="s">
@@ -7460,7 +7520,7 @@
         <v>6</v>
       </c>
       <c r="H91" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I91" s="46">
         <f t="shared" si="2"/>
@@ -7496,198 +7556,206 @@
       <c r="S91" s="61">
         <v>0</v>
       </c>
-      <c r="T91" s="20"/>
-      <c r="U91" s="20"/>
-      <c r="V91" s="20"/>
+      <c r="T91" s="21"/>
+      <c r="U91" s="21"/>
+      <c r="V91" s="21"/>
       <c r="W91" s="49"/>
     </row>
-    <row r="92" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B92" s="134"/>
-      <c r="C92" s="112"/>
-      <c r="D92" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="E92" s="45"/>
-      <c r="F92" s="45" t="s">
+    <row r="92" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="127"/>
+      <c r="C92" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D92" s="34"/>
+      <c r="E92" s="35"/>
+      <c r="F92" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="G92" s="4">
-        <v>6</v>
-      </c>
-      <c r="H92" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="I92" s="46">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J92" s="61">
-        <v>0</v>
-      </c>
-      <c r="K92" s="61">
-        <v>0</v>
-      </c>
-      <c r="L92" s="61">
-        <v>0</v>
-      </c>
-      <c r="M92" s="61">
-        <v>0</v>
-      </c>
-      <c r="N92" s="61">
-        <v>0</v>
-      </c>
-      <c r="O92" s="61">
-        <v>0</v>
-      </c>
-      <c r="P92" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q92" s="61">
-        <v>0</v>
-      </c>
-      <c r="R92" s="61">
-        <v>0</v>
-      </c>
-      <c r="S92" s="61">
-        <v>0</v>
-      </c>
-      <c r="T92" s="21"/>
-      <c r="U92" s="21"/>
-      <c r="V92" s="21"/>
-      <c r="W92" s="49"/>
-    </row>
-    <row r="93" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="135"/>
-      <c r="C93" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="D93" s="34"/>
-      <c r="E93" s="35"/>
-      <c r="F93" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="G93" s="11">
+      <c r="G92" s="11">
         <v>1</v>
       </c>
-      <c r="H93" s="11">
+      <c r="H92" s="11">
         <v>1</v>
       </c>
-      <c r="I93" s="50">
+      <c r="I92" s="50">
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
-      <c r="J93" s="62">
-        <v>0</v>
-      </c>
-      <c r="K93" s="62">
-        <v>0</v>
-      </c>
-      <c r="L93" s="62">
-        <v>0</v>
-      </c>
-      <c r="M93" s="84">
+      <c r="J92" s="62">
+        <v>0</v>
+      </c>
+      <c r="K92" s="62">
+        <v>0</v>
+      </c>
+      <c r="L92" s="62">
+        <v>0</v>
+      </c>
+      <c r="M92" s="84">
         <v>0.75</v>
       </c>
-      <c r="N93" s="84">
-        <v>0</v>
-      </c>
-      <c r="O93" s="84">
-        <v>0</v>
-      </c>
-      <c r="P93" s="84">
-        <v>0</v>
-      </c>
-      <c r="Q93" s="84">
-        <v>0</v>
-      </c>
-      <c r="R93" s="84">
-        <v>0</v>
-      </c>
-      <c r="S93" s="84">
-        <v>0</v>
-      </c>
-      <c r="T93" s="84">
-        <v>0</v>
-      </c>
-      <c r="U93" s="84">
-        <v>0</v>
-      </c>
-      <c r="V93" s="84">
-        <v>0</v>
-      </c>
-      <c r="W93" s="84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="113" t="s">
+      <c r="N92" s="84">
+        <v>0</v>
+      </c>
+      <c r="O92" s="84">
+        <v>0</v>
+      </c>
+      <c r="P92" s="84">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="84">
+        <v>0</v>
+      </c>
+      <c r="R92" s="84">
+        <v>0</v>
+      </c>
+      <c r="S92" s="84">
+        <v>0</v>
+      </c>
+      <c r="T92" s="84">
+        <v>0</v>
+      </c>
+      <c r="U92" s="84">
+        <v>0</v>
+      </c>
+      <c r="V92" s="84">
+        <v>0</v>
+      </c>
+      <c r="W92" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="C94" s="54" t="s">
+      <c r="C93" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="D94" s="53"/>
-      <c r="E94" s="54"/>
-      <c r="F94" s="54" t="s">
+      <c r="D93" s="53"/>
+      <c r="E93" s="54"/>
+      <c r="F93" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="G94" s="12">
+      <c r="G93" s="12">
         <v>1</v>
       </c>
-      <c r="H94" s="12">
+      <c r="H93" s="12">
         <v>1.5</v>
       </c>
-      <c r="I94" s="48">
+      <c r="I93" s="48">
         <f t="shared" si="2"/>
         <v>0.46700000000000003</v>
       </c>
-      <c r="J94" s="60">
-        <v>0</v>
-      </c>
-      <c r="K94" s="60">
-        <v>0</v>
-      </c>
-      <c r="L94" s="60">
-        <v>0</v>
-      </c>
-      <c r="M94" s="76">
+      <c r="J93" s="60">
+        <v>0</v>
+      </c>
+      <c r="K93" s="60">
+        <v>0</v>
+      </c>
+      <c r="L93" s="60">
+        <v>0</v>
+      </c>
+      <c r="M93" s="76">
         <v>0.46700000000000003</v>
       </c>
-      <c r="N94" s="76">
-        <v>0</v>
-      </c>
-      <c r="O94" s="76">
-        <v>0</v>
-      </c>
-      <c r="P94" s="76">
-        <v>0</v>
-      </c>
-      <c r="Q94" s="76">
-        <v>0</v>
-      </c>
-      <c r="R94" s="76">
-        <v>0</v>
-      </c>
-      <c r="S94" s="76">
-        <v>0</v>
-      </c>
-      <c r="T94" s="76">
-        <v>0</v>
-      </c>
-      <c r="U94" s="76">
-        <v>0</v>
-      </c>
-      <c r="V94" s="76">
-        <v>0</v>
-      </c>
-      <c r="W94" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B95" s="134"/>
+      <c r="N93" s="76">
+        <v>0</v>
+      </c>
+      <c r="O93" s="76">
+        <v>0</v>
+      </c>
+      <c r="P93" s="76">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="76">
+        <v>0</v>
+      </c>
+      <c r="R93" s="76">
+        <v>0</v>
+      </c>
+      <c r="S93" s="76">
+        <v>0</v>
+      </c>
+      <c r="T93" s="76">
+        <v>0</v>
+      </c>
+      <c r="U93" s="76">
+        <v>0</v>
+      </c>
+      <c r="V93" s="76">
+        <v>0</v>
+      </c>
+      <c r="W93" s="76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B94" s="126"/>
+      <c r="C94" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="D94" s="33"/>
+      <c r="E94" s="45"/>
+      <c r="F94" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G94" s="4">
+        <v>1</v>
+      </c>
+      <c r="H94" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="I94" s="46">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="J94" s="61">
+        <v>0</v>
+      </c>
+      <c r="K94" s="61">
+        <v>0</v>
+      </c>
+      <c r="L94" s="61">
+        <v>0</v>
+      </c>
+      <c r="M94" s="85">
+        <v>0</v>
+      </c>
+      <c r="N94" s="85">
+        <v>0</v>
+      </c>
+      <c r="O94" s="89">
+        <v>0</v>
+      </c>
+      <c r="P94" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="89">
+        <v>0</v>
+      </c>
+      <c r="R94" s="87">
+        <v>0.1</v>
+      </c>
+      <c r="S94" s="87">
+        <v>0</v>
+      </c>
+      <c r="T94" s="87">
+        <v>0</v>
+      </c>
+      <c r="U94" s="87">
+        <v>0</v>
+      </c>
+      <c r="V94" s="87">
+        <v>0</v>
+      </c>
+      <c r="W94" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B95" s="126"/>
       <c r="C95" s="45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D95" s="33"/>
       <c r="E95" s="45"/>
@@ -7702,7 +7770,7 @@
       </c>
       <c r="I95" s="46">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J95" s="61">
         <v>0</v>
@@ -7719,17 +7787,17 @@
       <c r="N95" s="85">
         <v>0</v>
       </c>
-      <c r="O95" s="89">
-        <v>0</v>
-      </c>
-      <c r="P95" s="89">
-        <v>0</v>
-      </c>
-      <c r="Q95" s="89">
+      <c r="O95" s="87">
+        <v>1</v>
+      </c>
+      <c r="P95" s="93">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="87">
         <v>0</v>
       </c>
       <c r="R95" s="87">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="S95" s="87">
         <v>0</v>
@@ -7747,10 +7815,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B96" s="134"/>
+    <row r="96" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B96" s="126"/>
       <c r="C96" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D96" s="33"/>
       <c r="E96" s="45"/>
@@ -7765,7 +7833,7 @@
       </c>
       <c r="I96" s="46">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="J96" s="61">
         <v>0</v>
@@ -7783,9 +7851,9 @@
         <v>0</v>
       </c>
       <c r="O96" s="87">
-        <v>1</v>
-      </c>
-      <c r="P96" s="93">
+        <v>0.1</v>
+      </c>
+      <c r="P96" s="87">
         <v>0</v>
       </c>
       <c r="Q96" s="87">
@@ -7810,10 +7878,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B97" s="134"/>
+    <row r="97" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B97" s="126"/>
       <c r="C97" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D97" s="33"/>
       <c r="E97" s="45"/>
@@ -7821,7 +7889,7 @@
         <v>16</v>
       </c>
       <c r="G97" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H97" s="4">
         <v>0.33</v>
@@ -7839,30 +7907,26 @@
       <c r="L97" s="61">
         <v>0</v>
       </c>
-      <c r="M97" s="85">
-        <v>0</v>
-      </c>
-      <c r="N97" s="85">
-        <v>0</v>
-      </c>
-      <c r="O97" s="87">
+      <c r="M97" s="61">
+        <v>0</v>
+      </c>
+      <c r="N97" s="61">
+        <v>0</v>
+      </c>
+      <c r="O97" s="61">
+        <v>0</v>
+      </c>
+      <c r="P97" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="61">
+        <v>0</v>
+      </c>
+      <c r="R97" s="101"/>
+      <c r="S97" s="101"/>
+      <c r="T97" s="87">
         <v>0.1</v>
       </c>
-      <c r="P97" s="87">
-        <v>0</v>
-      </c>
-      <c r="Q97" s="87">
-        <v>0</v>
-      </c>
-      <c r="R97" s="87">
-        <v>0</v>
-      </c>
-      <c r="S97" s="87">
-        <v>0</v>
-      </c>
-      <c r="T97" s="87">
-        <v>0</v>
-      </c>
       <c r="U97" s="87">
         <v>0</v>
       </c>
@@ -7873,390 +7937,345 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B98" s="134"/>
-      <c r="C98" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="D98" s="33"/>
-      <c r="E98" s="45"/>
-      <c r="F98" s="45" t="s">
+    <row r="98" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="127"/>
+      <c r="C98" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D98" s="34"/>
+      <c r="E98" s="35"/>
+      <c r="F98" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="G98" s="4">
+      <c r="G98" s="11">
+        <v>1</v>
+      </c>
+      <c r="H98" s="11">
         <v>3</v>
       </c>
-      <c r="H98" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="I98" s="46">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="J98" s="61">
-        <v>0</v>
-      </c>
-      <c r="K98" s="61">
-        <v>0</v>
-      </c>
-      <c r="L98" s="61">
-        <v>0</v>
-      </c>
-      <c r="M98" s="61">
-        <v>0</v>
-      </c>
-      <c r="N98" s="61">
-        <v>0</v>
-      </c>
-      <c r="O98" s="61">
-        <v>0</v>
-      </c>
-      <c r="P98" s="61">
-        <v>0</v>
-      </c>
-      <c r="Q98" s="61">
-        <v>0</v>
-      </c>
-      <c r="R98" s="101"/>
-      <c r="S98" s="101"/>
-      <c r="T98" s="87">
-        <v>0.1</v>
-      </c>
-      <c r="U98" s="87">
-        <v>0</v>
-      </c>
-      <c r="V98" s="87">
-        <v>0</v>
-      </c>
-      <c r="W98" s="87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="135"/>
-      <c r="C99" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="D99" s="34"/>
-      <c r="E99" s="35"/>
-      <c r="F99" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="G99" s="11">
-        <v>1</v>
-      </c>
-      <c r="H99" s="11">
-        <v>3</v>
-      </c>
-      <c r="I99" s="50">
-        <f t="shared" ref="I99" si="4">SUM(J99:W99)</f>
-        <v>0</v>
-      </c>
-      <c r="J99" s="62">
-        <v>0</v>
-      </c>
-      <c r="K99" s="62">
-        <v>0</v>
-      </c>
-      <c r="L99" s="62">
-        <v>0</v>
-      </c>
-      <c r="M99" s="62">
-        <v>0</v>
-      </c>
-      <c r="N99" s="94" t="s">
+      <c r="I98" s="50">
+        <f t="shared" ref="I98" si="4">SUM(J98:W98)</f>
+        <v>0</v>
+      </c>
+      <c r="J98" s="62">
+        <v>0</v>
+      </c>
+      <c r="K98" s="62">
+        <v>0</v>
+      </c>
+      <c r="L98" s="62">
+        <v>0</v>
+      </c>
+      <c r="M98" s="62">
+        <v>0</v>
+      </c>
+      <c r="N98" s="94" t="s">
         <v>125</v>
       </c>
-      <c r="O99" s="94">
-        <v>0</v>
-      </c>
-      <c r="P99" s="95">
-        <v>0</v>
-      </c>
-      <c r="Q99" s="95">
-        <v>0</v>
-      </c>
-      <c r="R99" s="95">
-        <v>0</v>
-      </c>
-      <c r="S99" s="95">
-        <v>0</v>
-      </c>
-      <c r="T99" s="95">
-        <v>0</v>
-      </c>
-      <c r="U99" s="24"/>
-      <c r="V99" s="24"/>
-      <c r="W99" s="25"/>
-    </row>
-    <row r="100" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="127" t="s">
+      <c r="O98" s="94">
+        <v>0</v>
+      </c>
+      <c r="P98" s="95">
+        <v>0</v>
+      </c>
+      <c r="Q98" s="95">
+        <v>0</v>
+      </c>
+      <c r="R98" s="95">
+        <v>0</v>
+      </c>
+      <c r="S98" s="95">
+        <v>0</v>
+      </c>
+      <c r="T98" s="95">
+        <v>0</v>
+      </c>
+      <c r="U98" s="24"/>
+      <c r="V98" s="24"/>
+      <c r="W98" s="25"/>
+    </row>
+    <row r="99" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B99" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="C100" s="128"/>
-      <c r="D100" s="128"/>
-      <c r="E100" s="128"/>
-      <c r="F100" s="128"/>
-      <c r="G100" s="128"/>
-      <c r="H100" s="17">
-        <f t="shared" ref="H100:W100" si="5">SUM(H4:H99)</f>
-        <v>49.11999999999999</v>
-      </c>
-      <c r="I100" s="17">
-        <f t="shared" si="5"/>
-        <v>37.041699999999999</v>
-      </c>
-      <c r="J100" s="17">
-        <f t="shared" si="5"/>
+      <c r="C99" s="120"/>
+      <c r="D99" s="120"/>
+      <c r="E99" s="120"/>
+      <c r="F99" s="120"/>
+      <c r="G99" s="120"/>
+      <c r="H99" s="17">
+        <f>SUM(H4:H98)</f>
+        <v>48.86999999999999</v>
+      </c>
+      <c r="I99" s="17">
+        <f>SUM(I4:I98)</f>
+        <v>38.2117</v>
+      </c>
+      <c r="J99" s="17">
+        <f>SUM(J4:J98)</f>
         <v>1.95</v>
       </c>
-      <c r="K100" s="17">
-        <f t="shared" si="5"/>
+      <c r="K99" s="17">
+        <f>SUM(K4:K98)</f>
         <v>3.3</v>
       </c>
-      <c r="L100" s="17">
-        <f t="shared" si="5"/>
+      <c r="L99" s="17">
+        <f>SUM(L4:L98)</f>
         <v>7.15</v>
       </c>
-      <c r="M100" s="17">
-        <f t="shared" si="5"/>
+      <c r="M99" s="17">
+        <f>SUM(M4:M98)</f>
         <v>3.9929999999999999</v>
       </c>
-      <c r="N100" s="17">
-        <f t="shared" si="5"/>
+      <c r="N99" s="17">
+        <f>SUM(N4:N98)</f>
         <v>1.5</v>
       </c>
-      <c r="O100" s="17">
-        <f t="shared" si="5"/>
+      <c r="O99" s="17">
+        <f>SUM(O4:O98)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="P100" s="17">
-        <f t="shared" si="5"/>
+      <c r="P99" s="17">
+        <f>SUM(P4:P98)</f>
         <v>0.03</v>
       </c>
-      <c r="Q100" s="17">
-        <f t="shared" si="5"/>
+      <c r="Q99" s="17">
+        <f>SUM(Q4:Q98)</f>
         <v>2.0290000000000004</v>
       </c>
-      <c r="R100" s="17">
-        <f t="shared" si="5"/>
+      <c r="R99" s="17">
+        <f>SUM(R4:R98)</f>
         <v>1.4826999999999999</v>
       </c>
-      <c r="S100" s="17">
-        <f t="shared" si="5"/>
+      <c r="S99" s="17">
+        <f>SUM(S4:S98)</f>
         <v>4.7170000000000005</v>
       </c>
-      <c r="T100" s="17">
-        <f t="shared" si="5"/>
-        <v>7.6399999999999988</v>
-      </c>
-      <c r="U100" s="17">
-        <f t="shared" si="5"/>
-        <v>2.15</v>
-      </c>
-      <c r="V100" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W100" s="18">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
+      <c r="T99" s="17">
+        <f>SUM(T4:T98)</f>
+        <v>7.8699999999999992</v>
+      </c>
+      <c r="U99" s="17">
+        <f>SUM(U4:U98)</f>
+        <v>3.09</v>
+      </c>
+      <c r="V99" s="17">
+        <f>SUM(V4:V98)</f>
+        <v>0</v>
+      </c>
+      <c r="W99" s="18">
+        <f>SUM(W4:W98)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="110" t="s">
+        <v>11</v>
+      </c>
+      <c r="K100" s="111"/>
+      <c r="L100" s="111"/>
+      <c r="M100" s="111"/>
+      <c r="N100" s="111"/>
+      <c r="O100" s="111"/>
+      <c r="P100" s="111"/>
+      <c r="Q100" s="111"/>
+      <c r="R100" s="111"/>
+      <c r="S100" s="111"/>
+      <c r="T100" s="111"/>
+      <c r="U100" s="111"/>
+      <c r="V100" s="111"/>
+      <c r="W100" s="112"/>
+    </row>
+    <row r="101" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="C101" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="D101" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="E101" s="68" t="s">
+        <v>116</v>
+      </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
-      <c r="J101" s="118" t="s">
-        <v>11</v>
-      </c>
-      <c r="K101" s="119"/>
-      <c r="L101" s="119"/>
-      <c r="M101" s="119"/>
-      <c r="N101" s="119"/>
-      <c r="O101" s="119"/>
-      <c r="P101" s="119"/>
-      <c r="Q101" s="119"/>
-      <c r="R101" s="119"/>
-      <c r="S101" s="119"/>
-      <c r="T101" s="119"/>
-      <c r="U101" s="119"/>
-      <c r="V101" s="119"/>
-      <c r="W101" s="120"/>
-    </row>
-    <row r="102" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="C102" s="67" t="s">
-        <v>114</v>
-      </c>
-      <c r="D102" s="67" t="s">
-        <v>115</v>
-      </c>
-      <c r="E102" s="68" t="s">
-        <v>116</v>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+      <c r="M101" s="3"/>
+      <c r="O101" s="9"/>
+      <c r="P101" s="9"/>
+    </row>
+    <row r="102" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" s="71">
+        <f>SUM(H7,H9,H41,H87,H88,H89,H90,H91,H92,H94:H98,H41)</f>
+        <v>12.27</v>
+      </c>
+      <c r="D102" s="27">
+        <f>SUM(I94:I98,I87:I92,I9,I7,I41)</f>
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="E102" s="27">
+        <f>SUM(C102,-D102)</f>
+        <v>4.2199999999999989</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="3"/>
-      <c r="K102" s="3"/>
-      <c r="L102" s="3"/>
-      <c r="M102" s="3"/>
-      <c r="O102" s="9"/>
-      <c r="P102" s="9"/>
-    </row>
-    <row r="103" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C103" s="71">
-        <f>SUM(H7,H9,H41,H88,H89,H90,H91,H92,H93,H95:H99,H41)</f>
-        <v>12.27</v>
-      </c>
-      <c r="D103" s="27">
-        <f>SUM(I95:I99,I88:I93,I9,I7,I41)</f>
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="E103" s="27">
+      <c r="H102" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="I102" s="131"/>
+      <c r="J102" s="10">
+        <f>H99-J99</f>
+        <v>46.919999999999987</v>
+      </c>
+      <c r="K102" s="10">
+        <f>J102-K99</f>
+        <v>43.61999999999999</v>
+      </c>
+      <c r="L102" s="10">
+        <f>K102-L99</f>
+        <v>36.469999999999992</v>
+      </c>
+      <c r="M102" s="10">
+        <f>L102-M99</f>
+        <v>32.47699999999999</v>
+      </c>
+      <c r="N102" s="10">
+        <f t="shared" ref="N102:W102" si="5">M102-N99</f>
+        <v>30.97699999999999</v>
+      </c>
+      <c r="O102" s="10">
+        <f t="shared" si="5"/>
+        <v>29.876999999999988</v>
+      </c>
+      <c r="P102" s="10">
+        <f t="shared" si="5"/>
+        <v>29.846999999999987</v>
+      </c>
+      <c r="Q102" s="10">
+        <f t="shared" si="5"/>
+        <v>27.817999999999987</v>
+      </c>
+      <c r="R102" s="10">
+        <f t="shared" si="5"/>
+        <v>26.335299999999986</v>
+      </c>
+      <c r="S102" s="10">
+        <f t="shared" si="5"/>
+        <v>21.618299999999984</v>
+      </c>
+      <c r="T102" s="10">
+        <f t="shared" si="5"/>
+        <v>13.748299999999984</v>
+      </c>
+      <c r="U102" s="10">
+        <f t="shared" si="5"/>
+        <v>10.658299999999985</v>
+      </c>
+      <c r="V102" s="10">
+        <f t="shared" si="5"/>
+        <v>10.658299999999985</v>
+      </c>
+      <c r="W102" s="10">
+        <f t="shared" si="5"/>
+        <v>10.658299999999985</v>
+      </c>
+    </row>
+    <row r="103" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="69">
+        <f>SUM(H4,H84:H84,H93,H17:H37,H10:H15,H8,H6,H5,H86)</f>
+        <v>18.399999999999991</v>
+      </c>
+      <c r="D103" s="5">
+        <f>SUM(I93,I84:I84,I17:I37,I10:I15,I8,I5:I6,I86,I4)</f>
+        <v>14.561700000000004</v>
+      </c>
+      <c r="E103" s="5">
         <f>SUM(C103,-D103)</f>
-        <v>4.2199999999999989</v>
-      </c>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="105" t="s">
-        <v>9</v>
-      </c>
-      <c r="I103" s="108"/>
-      <c r="J103" s="10">
-        <f>H100-J100</f>
-        <v>47.169999999999987</v>
-      </c>
-      <c r="K103" s="10">
-        <f>J103-K100</f>
-        <v>43.86999999999999</v>
-      </c>
-      <c r="L103" s="10">
-        <f>K103-L100</f>
-        <v>36.719999999999992</v>
-      </c>
-      <c r="M103" s="10">
-        <f>L103-M100</f>
-        <v>32.72699999999999</v>
-      </c>
-      <c r="N103" s="10">
-        <f t="shared" ref="N103:W103" si="6">M103-N100</f>
-        <v>31.22699999999999</v>
-      </c>
-      <c r="O103" s="10">
-        <f t="shared" si="6"/>
-        <v>30.126999999999988</v>
-      </c>
-      <c r="P103" s="10">
-        <f t="shared" si="6"/>
-        <v>30.096999999999987</v>
-      </c>
-      <c r="Q103" s="10">
-        <f t="shared" si="6"/>
-        <v>28.067999999999987</v>
-      </c>
-      <c r="R103" s="10">
-        <f t="shared" si="6"/>
-        <v>26.585299999999986</v>
-      </c>
-      <c r="S103" s="10">
-        <f t="shared" si="6"/>
-        <v>21.868299999999984</v>
-      </c>
-      <c r="T103" s="10">
-        <f t="shared" si="6"/>
-        <v>14.228299999999985</v>
-      </c>
-      <c r="U103" s="10">
-        <f t="shared" si="6"/>
-        <v>12.078299999999984</v>
-      </c>
-      <c r="V103" s="10">
-        <f t="shared" si="6"/>
-        <v>12.078299999999984</v>
-      </c>
-      <c r="W103" s="10">
-        <f t="shared" si="6"/>
-        <v>12.078299999999984</v>
-      </c>
-    </row>
-    <row r="104" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3.8382999999999878</v>
+      </c>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+      <c r="M103" s="3"/>
+    </row>
+    <row r="104" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B104" s="70" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C104" s="69">
-        <f>SUM(H4,H85:H85,H94,H17:H37,H10:H15,H8,H6,H5,H87)</f>
-        <v>18.399999999999991</v>
+        <f>SUM(H42:H83,H38:H40)</f>
+        <v>16.5</v>
       </c>
       <c r="D104" s="5">
-        <f>SUM(I94,I85:I85,I17:I37,I10:I15,I8,I5:I6,I87,I4)</f>
-        <v>14.3317</v>
+        <f>SUM(I42:I83,I38:I40,I16)</f>
+        <v>15.349999999999998</v>
       </c>
       <c r="E104" s="5">
         <f>SUM(C104,-D104)</f>
-        <v>4.0682999999999918</v>
+        <v>1.1500000000000021</v>
       </c>
       <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="3"/>
-      <c r="I104" s="3"/>
-      <c r="J104" s="3"/>
-      <c r="K104" s="3"/>
-      <c r="L104" s="3"/>
-      <c r="M104" s="3"/>
-    </row>
-    <row r="105" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="70" t="s">
-        <v>17</v>
-      </c>
-      <c r="C105" s="69">
-        <f>SUM(H42:H84,H38:H40)</f>
-        <v>16.75</v>
-      </c>
-      <c r="D105" s="5">
-        <f>SUM(I42:I84,I38:I40,I16)</f>
-        <v>14.41</v>
-      </c>
-      <c r="E105" s="5">
-        <f>SUM(C105,-D105)</f>
-        <v>2.34</v>
-      </c>
+      <c r="H104" s="128" t="s">
+        <v>10</v>
+      </c>
+      <c r="I104" s="129"/>
+      <c r="J104" s="128">
+        <f>H99-I99</f>
+        <v>10.65829999999999</v>
+      </c>
+      <c r="K104" s="129"/>
+      <c r="L104" s="129"/>
+      <c r="M104" s="129"/>
+      <c r="N104" s="129"/>
+      <c r="O104" s="129"/>
+      <c r="P104" s="129"/>
+      <c r="Q104" s="129"/>
+      <c r="R104" s="129"/>
+      <c r="S104" s="129"/>
+      <c r="T104" s="129"/>
+      <c r="U104" s="129"/>
+      <c r="V104" s="129"/>
+      <c r="W104" s="130"/>
+    </row>
+    <row r="105" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
       <c r="F105" s="3"/>
-      <c r="H105" s="105" t="s">
-        <v>10</v>
-      </c>
-      <c r="I105" s="106"/>
-      <c r="J105" s="105">
-        <f>H100-I100</f>
-        <v>12.078299999999992</v>
-      </c>
-      <c r="K105" s="106"/>
-      <c r="L105" s="106"/>
-      <c r="M105" s="106"/>
-      <c r="N105" s="106"/>
-      <c r="O105" s="106"/>
-      <c r="P105" s="106"/>
-      <c r="Q105" s="106"/>
-      <c r="R105" s="106"/>
-      <c r="S105" s="106"/>
-      <c r="T105" s="106"/>
-      <c r="U105" s="106"/>
-      <c r="V105" s="106"/>
-      <c r="W105" s="107"/>
-    </row>
-    <row r="106" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+      <c r="M105" s="3"/>
+    </row>
+    <row r="106" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
@@ -8270,7 +8289,7 @@
       <c r="L106" s="3"/>
       <c r="M106" s="3"/>
     </row>
-    <row r="107" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
@@ -8284,72 +8303,58 @@
       <c r="L107" s="3"/>
       <c r="M107" s="3"/>
     </row>
-    <row r="108" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
-      <c r="G108" s="3"/>
-      <c r="H108" s="3"/>
-      <c r="I108" s="3"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="3"/>
-      <c r="M108" s="3"/>
-    </row>
-    <row r="109" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="2:23" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="7"/>
+    </row>
+    <row r="114" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B114" s="7"/>
     </row>
-    <row r="115" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B115" s="7"/>
     </row>
-    <row r="116" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="7"/>
-    </row>
-    <row r="117" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B120" s="7"/>
+    </row>
+    <row r="121" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B121" s="7"/>
     </row>
-    <row r="122" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B122" s="7"/>
     </row>
-    <row r="123" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B123" s="7"/>
     </row>
-    <row r="124" spans="2:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="7"/>
-    </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B125" s="6"/>
-      <c r="C125" s="6"/>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B42:B88"/>
+    <mergeCell ref="J104:W104"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="C42:C83"/>
+    <mergeCell ref="C19:C37"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="B42:B87"/>
     <mergeCell ref="J2:W2"/>
-    <mergeCell ref="J101:W101"/>
+    <mergeCell ref="J100:W100"/>
     <mergeCell ref="B16:B41"/>
     <mergeCell ref="B10:B15"/>
     <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B100:G100"/>
+    <mergeCell ref="B99:G99"/>
     <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="B94:B99"/>
-    <mergeCell ref="J105:W105"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="C42:C84"/>
-    <mergeCell ref="C19:C37"/>
-    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="B88:B92"/>
+    <mergeCell ref="B93:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8363,7 +8368,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8375,7 +8380,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>